<commit_message>
working on spreadsheet loading
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="13545" tabRatio="863" activeTab="12"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="13545" tabRatio="863" firstSheet="4" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="148">
   <si>
     <t>Assumption</t>
   </si>
@@ -343,15 +343,6 @@
     <t>Government revenue</t>
   </si>
   <si>
-    <t>Total health expenditure</t>
-  </si>
-  <si>
-    <t>Domestic health expenditure</t>
-  </si>
-  <si>
-    <t>Total government expenditure</t>
-  </si>
-  <si>
     <t>AND AT LEAST ONE OF</t>
   </si>
   <si>
@@ -382,9 +373,6 @@
     <t>Average number of injections per person per year</t>
   </si>
   <si>
-    <t>Needle-syringe receptive sharing rate</t>
-  </si>
-  <si>
     <t>Disease progression rate (% per year)</t>
   </si>
   <si>
@@ -455,6 +443,33 @@
   </si>
   <si>
     <t>Risk-related population transitions (average number of years before movement)</t>
+  </si>
+  <si>
+    <t>Percentage of people who receptively shared a needle at last injection</t>
+  </si>
+  <si>
+    <t>Government expenditure</t>
+  </si>
+  <si>
+    <t>General government health expenditure</t>
+  </si>
+  <si>
+    <t>Domestic HIV spending</t>
+  </si>
+  <si>
+    <t>Global Fund HIV commitments</t>
+  </si>
+  <si>
+    <t>PEPFAR HIV commitments</t>
+  </si>
+  <si>
+    <t>Other international HIV commitments</t>
+  </si>
+  <si>
+    <t>Private HIV spending</t>
+  </si>
+  <si>
+    <t>Total domestic and international health expenditure</t>
   </si>
 </sst>
 </file>
@@ -464,10 +479,17 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -579,737 +601,739 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="663">
+  <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="655"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="655" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="655"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="655" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="655"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="655" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="655"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="655" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="11" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="662" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="662" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="663">
+  <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="13"/>
     <cellStyle name="Comma 2 2" xfId="661"/>
     <cellStyle name="Input" xfId="1" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal 10" xfId="663"/>
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Normal 2 2" xfId="656"/>
     <cellStyle name="Normal 3" xfId="5"/>
@@ -2507,14 +2531,14 @@
   <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2665,7 +2689,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2790,7 +2814,7 @@
   <sheetPr published="0"/>
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -2803,7 +2827,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2869,7 +2893,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C8" s="32">
         <v>0.05</v>
@@ -2879,7 +2903,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C9" s="32">
         <v>0.03</v>
@@ -2899,7 +2923,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2975,7 +2999,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B23" s="22"/>
     </row>
@@ -3042,7 +3066,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3101,7 +3125,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3147,7 +3171,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3263,7 +3287,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3368,7 +3392,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -3390,7 +3414,7 @@
     </row>
     <row r="3" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C3" s="31">
         <v>0.05</v>
@@ -3473,7 +3497,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -3550,7 +3574,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -3635,9 +3659,11 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0"/>
-  <dimension ref="A1:T27"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3855,7 +3881,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
@@ -3961,7 +3987,7 @@
     </row>
     <row r="19" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>105</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4047,7 +4073,7 @@
     <row r="24" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4128,8 +4154,431 @@
       </c>
       <c r="T27" s="27"/>
     </row>
+    <row r="31" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="22">
+        <v>2015</v>
+      </c>
+      <c r="D32" s="22">
+        <v>2016</v>
+      </c>
+      <c r="E32" s="22">
+        <v>2017</v>
+      </c>
+      <c r="F32" s="22">
+        <v>2018</v>
+      </c>
+      <c r="G32" s="22">
+        <v>2019</v>
+      </c>
+      <c r="H32" s="22">
+        <v>2020</v>
+      </c>
+      <c r="I32" s="22">
+        <v>2021</v>
+      </c>
+      <c r="J32" s="22">
+        <v>2022</v>
+      </c>
+      <c r="K32" s="22">
+        <v>2023</v>
+      </c>
+      <c r="L32" s="22">
+        <v>2024</v>
+      </c>
+      <c r="M32" s="22">
+        <v>2025</v>
+      </c>
+      <c r="N32" s="22">
+        <v>2026</v>
+      </c>
+      <c r="O32" s="22">
+        <v>2027</v>
+      </c>
+      <c r="P32" s="22">
+        <v>2028</v>
+      </c>
+      <c r="Q32" s="22">
+        <v>2029</v>
+      </c>
+      <c r="R32" s="22">
+        <v>2030</v>
+      </c>
+      <c r="T32" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="27"/>
+      <c r="N33" s="27"/>
+      <c r="O33" s="27"/>
+      <c r="P33" s="27"/>
+      <c r="Q33" s="27"/>
+      <c r="R33" s="27"/>
+      <c r="S33" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="T33" s="27"/>
+    </row>
+    <row r="34" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="22">
+        <v>2015</v>
+      </c>
+      <c r="D38" s="22">
+        <v>2016</v>
+      </c>
+      <c r="E38" s="22">
+        <v>2017</v>
+      </c>
+      <c r="F38" s="22">
+        <v>2018</v>
+      </c>
+      <c r="G38" s="22">
+        <v>2019</v>
+      </c>
+      <c r="H38" s="22">
+        <v>2020</v>
+      </c>
+      <c r="I38" s="22">
+        <v>2021</v>
+      </c>
+      <c r="J38" s="22">
+        <v>2022</v>
+      </c>
+      <c r="K38" s="22">
+        <v>2023</v>
+      </c>
+      <c r="L38" s="22">
+        <v>2024</v>
+      </c>
+      <c r="M38" s="22">
+        <v>2025</v>
+      </c>
+      <c r="N38" s="22">
+        <v>2026</v>
+      </c>
+      <c r="O38" s="22">
+        <v>2027</v>
+      </c>
+      <c r="P38" s="22">
+        <v>2028</v>
+      </c>
+      <c r="Q38" s="22">
+        <v>2029</v>
+      </c>
+      <c r="R38" s="22">
+        <v>2030</v>
+      </c>
+      <c r="T38" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="27"/>
+      <c r="R39" s="27"/>
+      <c r="S39" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="T39" s="27"/>
+    </row>
+    <row r="40" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="22">
+        <v>2015</v>
+      </c>
+      <c r="D44" s="22">
+        <v>2016</v>
+      </c>
+      <c r="E44" s="22">
+        <v>2017</v>
+      </c>
+      <c r="F44" s="22">
+        <v>2018</v>
+      </c>
+      <c r="G44" s="22">
+        <v>2019</v>
+      </c>
+      <c r="H44" s="22">
+        <v>2020</v>
+      </c>
+      <c r="I44" s="22">
+        <v>2021</v>
+      </c>
+      <c r="J44" s="22">
+        <v>2022</v>
+      </c>
+      <c r="K44" s="22">
+        <v>2023</v>
+      </c>
+      <c r="L44" s="22">
+        <v>2024</v>
+      </c>
+      <c r="M44" s="22">
+        <v>2025</v>
+      </c>
+      <c r="N44" s="22">
+        <v>2026</v>
+      </c>
+      <c r="O44" s="22">
+        <v>2027</v>
+      </c>
+      <c r="P44" s="22">
+        <v>2028</v>
+      </c>
+      <c r="Q44" s="22">
+        <v>2029</v>
+      </c>
+      <c r="R44" s="22">
+        <v>2030</v>
+      </c>
+      <c r="T44" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="27"/>
+      <c r="O45" s="27"/>
+      <c r="P45" s="27"/>
+      <c r="Q45" s="27"/>
+      <c r="R45" s="27"/>
+      <c r="S45" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="T45" s="27"/>
+    </row>
+    <row r="49" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="22">
+        <v>2015</v>
+      </c>
+      <c r="D50" s="22">
+        <v>2016</v>
+      </c>
+      <c r="E50" s="22">
+        <v>2017</v>
+      </c>
+      <c r="F50" s="22">
+        <v>2018</v>
+      </c>
+      <c r="G50" s="22">
+        <v>2019</v>
+      </c>
+      <c r="H50" s="22">
+        <v>2020</v>
+      </c>
+      <c r="I50" s="22">
+        <v>2021</v>
+      </c>
+      <c r="J50" s="22">
+        <v>2022</v>
+      </c>
+      <c r="K50" s="22">
+        <v>2023</v>
+      </c>
+      <c r="L50" s="22">
+        <v>2024</v>
+      </c>
+      <c r="M50" s="22">
+        <v>2025</v>
+      </c>
+      <c r="N50" s="22">
+        <v>2026</v>
+      </c>
+      <c r="O50" s="22">
+        <v>2027</v>
+      </c>
+      <c r="P50" s="22">
+        <v>2028</v>
+      </c>
+      <c r="Q50" s="22">
+        <v>2029</v>
+      </c>
+      <c r="R50" s="22">
+        <v>2030</v>
+      </c>
+      <c r="T50" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="27"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="27"/>
+      <c r="L51" s="27"/>
+      <c r="M51" s="27"/>
+      <c r="N51" s="27"/>
+      <c r="O51" s="27"/>
+      <c r="P51" s="27"/>
+      <c r="Q51" s="27"/>
+      <c r="R51" s="27"/>
+      <c r="S51" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="T51" s="27"/>
+    </row>
+    <row r="52" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="22">
+        <v>2015</v>
+      </c>
+      <c r="D56" s="22">
+        <v>2016</v>
+      </c>
+      <c r="E56" s="22">
+        <v>2017</v>
+      </c>
+      <c r="F56" s="22">
+        <v>2018</v>
+      </c>
+      <c r="G56" s="22">
+        <v>2019</v>
+      </c>
+      <c r="H56" s="22">
+        <v>2020</v>
+      </c>
+      <c r="I56" s="22">
+        <v>2021</v>
+      </c>
+      <c r="J56" s="22">
+        <v>2022</v>
+      </c>
+      <c r="K56" s="22">
+        <v>2023</v>
+      </c>
+      <c r="L56" s="22">
+        <v>2024</v>
+      </c>
+      <c r="M56" s="22">
+        <v>2025</v>
+      </c>
+      <c r="N56" s="22">
+        <v>2026</v>
+      </c>
+      <c r="O56" s="22">
+        <v>2027</v>
+      </c>
+      <c r="P56" s="22">
+        <v>2028</v>
+      </c>
+      <c r="Q56" s="22">
+        <v>2029</v>
+      </c>
+      <c r="R56" s="22">
+        <v>2030</v>
+      </c>
+      <c r="T56" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="27"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="27"/>
+      <c r="L57" s="27"/>
+      <c r="M57" s="27"/>
+      <c r="N57" s="27"/>
+      <c r="O57" s="27"/>
+      <c r="P57" s="27"/>
+      <c r="Q57" s="27"/>
+      <c r="R57" s="27"/>
+      <c r="S57" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="T57" s="27"/>
+    </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4478,7 +4927,7 @@
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="24"/>
       <c r="K13" s="24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -6211,7 +6660,7 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -6589,7 +7038,7 @@
     <row r="11" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="X12" s="3"/>
       <c r="Y12" s="22" t="s">
@@ -7184,7 +7633,7 @@
       <c r="S30" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -7423,7 +7872,7 @@
     <row r="12" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -7531,7 +7980,7 @@
     <row r="18" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -7727,7 +8176,7 @@
     </row>
     <row r="31" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -7828,7 +8277,7 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -8207,7 +8656,7 @@
     <row r="11" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -8666,7 +9115,7 @@
     <row r="29" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -8818,7 +9267,7 @@
     <row r="35" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Y36" s="22" t="s">
         <v>93</v>
@@ -9087,7 +9536,7 @@
     </row>
     <row r="47" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="Y47" s="22" t="s">
         <v>93</v>
@@ -9198,7 +9647,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10180,7 +10629,7 @@
     <row r="33" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -10515,7 +10964,7 @@
     <row r="44" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -10844,7 +11293,7 @@
     <row r="55" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
@@ -11490,7 +11939,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -11502,7 +11951,7 @@
   <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11512,7 +11961,7 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -11768,7 +12217,7 @@
     <row r="11" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -12079,7 +12528,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12099,7 +12548,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -12403,7 +12852,7 @@
     <row r="11" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -12700,7 +13149,7 @@
     <row r="22" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -12859,7 +13308,7 @@
     <row r="33" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>

</xml_diff>

<commit_message>
forgot to lock sheets
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="13545" tabRatio="863" firstSheet="4" activeTab="12"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="13545" tabRatio="863"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -2301,9 +2301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2530,9 +2528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2804,6 +2800,7 @@
       <c r="H19" s="31"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -3661,9 +3658,7 @@
   <sheetPr published="0"/>
   <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4579,6 +4574,7 @@
       <c r="T57" s="27"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5499,9 +5495,7 @@
   <sheetPr published="0"/>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X46" sqref="X46"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6638,6 +6632,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -6648,9 +6643,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7633,6 +7626,7 @@
       <c r="S30" s="8"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7644,9 +7638,7 @@
   <sheetPr published="0"/>
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -8262,6 +8254,7 @@
       <c r="T33" s="27"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12537,9 +12530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
forgot about death rates
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="13545" tabRatio="863"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="13545" tabRatio="863" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
     <sheet name="Cost &amp; coverage" sheetId="16" r:id="rId2"/>
     <sheet name="Demographics &amp; HIV prevalence" sheetId="20" r:id="rId3"/>
-    <sheet name="Other prevalences" sheetId="1" r:id="rId4"/>
+    <sheet name="Other epidemiology" sheetId="1" r:id="rId4"/>
     <sheet name="Optional indicators" sheetId="19" r:id="rId5"/>
     <sheet name="Testing &amp; treatment" sheetId="2" r:id="rId6"/>
     <sheet name="Sexual behavior" sheetId="3" r:id="rId7"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="149">
   <si>
     <t>Assumption</t>
   </si>
@@ -178,12 +178,6 @@
     <t>Number of diagnoses</t>
   </si>
   <si>
-    <t>Number of people on 1st-line treatment</t>
-  </si>
-  <si>
-    <t>Number of people on 2nd-line treatment</t>
-  </si>
-  <si>
     <t>Number of HIV-related deaths</t>
   </si>
   <si>
@@ -334,18 +328,12 @@
     <t>Male circumcision prevalence</t>
   </si>
   <si>
-    <t>Number of people on opiate substitution therapy</t>
-  </si>
-  <si>
     <t>Gross domestic product</t>
   </si>
   <si>
     <t>Government revenue</t>
   </si>
   <si>
-    <t>AND AT LEAST ONE OF</t>
-  </si>
-  <si>
     <t>Prevalence of any ulcerative STIs</t>
   </si>
   <si>
@@ -470,6 +458,21 @@
   </si>
   <si>
     <t>Total domestic and international health expenditure</t>
+  </si>
+  <si>
+    <t>Percentage of people who die from non-HIV-related causes per year</t>
+  </si>
+  <si>
+    <t>AND EITHER</t>
+  </si>
+  <si>
+    <t>Percentage of people who inject drugs on opiate substitution therapy</t>
+  </si>
+  <si>
+    <t>Number of people on first-line treatment</t>
+  </si>
+  <si>
+    <t>Number of people on second-line treatment</t>
   </si>
 </sst>
 </file>
@@ -1324,7 +1327,7 @@
     <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="662" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2301,7 +2304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2314,15 +2317,15 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
@@ -2335,7 +2338,7 @@
         <v>40</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
@@ -2348,7 +2351,7 @@
         <v>41</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E4" s="26"/>
       <c r="F4" s="26"/>
@@ -2361,7 +2364,7 @@
         <v>42</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E5" s="26"/>
       <c r="F5" s="26"/>
@@ -2374,7 +2377,7 @@
         <v>43</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
@@ -2387,7 +2390,7 @@
         <v>44</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="26"/>
@@ -2400,7 +2403,7 @@
         <v>45</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
@@ -2423,10 +2426,10 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="26"/>
       <c r="C13" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2434,10 +2437,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2448,7 +2451,7 @@
         <v>42</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2456,10 +2459,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -2470,7 +2473,7 @@
         <v>44</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -2478,10 +2481,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -2492,7 +2495,7 @@
         <v>38</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -2503,7 +2506,7 @@
         <v>36</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -2514,7 +2517,7 @@
         <v>35</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2534,7 +2537,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2685,7 +2688,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2824,7 +2827,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2890,7 +2893,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C8" s="32">
         <v>0.05</v>
@@ -2900,7 +2903,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C9" s="32">
         <v>0.03</v>
@@ -2920,7 +2923,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2996,7 +2999,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B23" s="22"/>
     </row>
@@ -3033,7 +3036,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C27" s="32">
         <v>0.25</v>
@@ -3063,7 +3066,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3122,7 +3125,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3168,7 +3171,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3264,7 +3267,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B57" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C57" s="27">
         <v>2</v>
@@ -3284,7 +3287,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3320,7 +3323,7 @@
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C65" s="32">
         <v>0.65</v>
@@ -3389,7 +3392,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -3411,7 +3414,7 @@
     </row>
     <row r="3" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C3" s="31">
         <v>0.05</v>
@@ -3422,7 +3425,7 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4" s="31">
         <v>0.1</v>
@@ -3433,7 +3436,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C5" s="31">
         <v>0.15</v>
@@ -3444,7 +3447,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" s="31">
         <v>0.221</v>
@@ -3455,7 +3458,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" s="31">
         <v>0.54700000000000004</v>
@@ -3466,7 +3469,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" s="31">
         <v>5.2999999999999999E-2</v>
@@ -3494,7 +3497,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -3517,7 +3520,7 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C14" s="27">
         <v>0</v>
@@ -3528,7 +3531,7 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C15" s="27">
         <v>0</v>
@@ -3539,7 +3542,7 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16" s="27">
         <v>1000</v>
@@ -3550,7 +3553,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C17" s="27">
         <v>5000</v>
@@ -3561,7 +3564,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C18" s="27">
         <v>50000</v>
@@ -3571,7 +3574,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -3594,7 +3597,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C24" s="27">
         <v>0</v>
@@ -3605,7 +3608,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C25" s="27">
         <v>0</v>
@@ -3616,7 +3619,7 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C26" s="27">
         <v>0</v>
@@ -3627,7 +3630,7 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C27" s="27">
         <v>1000</v>
@@ -3638,7 +3641,7 @@
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C28" s="27">
         <v>8000</v>
@@ -3658,13 +3661,13 @@
   <sheetPr published="0"/>
   <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -3764,13 +3767,13 @@
       <c r="Q3" s="27"/>
       <c r="R3" s="27"/>
       <c r="S3" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T3" s="27"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -3870,13 +3873,13 @@
       <c r="Q9" s="27"/>
       <c r="R9" s="27"/>
       <c r="S9" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T9" s="27"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
@@ -3976,13 +3979,13 @@
       <c r="Q15" s="27"/>
       <c r="R15" s="27"/>
       <c r="S15" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T15" s="27"/>
     </row>
     <row r="19" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4059,7 +4062,7 @@
       <c r="Q21" s="27"/>
       <c r="R21" s="27"/>
       <c r="S21" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T21" s="27"/>
     </row>
@@ -4068,7 +4071,7 @@
     <row r="24" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4145,13 +4148,13 @@
       <c r="Q27" s="27"/>
       <c r="R27" s="27"/>
       <c r="S27" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T27" s="27"/>
     </row>
     <row r="31" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4228,7 +4231,7 @@
       <c r="Q33" s="27"/>
       <c r="R33" s="27"/>
       <c r="S33" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T33" s="27"/>
     </row>
@@ -4237,7 +4240,7 @@
     <row r="36" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4314,7 +4317,7 @@
       <c r="Q39" s="27"/>
       <c r="R39" s="27"/>
       <c r="S39" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T39" s="27"/>
     </row>
@@ -4323,7 +4326,7 @@
     <row r="42" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4400,13 +4403,13 @@
       <c r="Q45" s="27"/>
       <c r="R45" s="27"/>
       <c r="S45" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T45" s="27"/>
     </row>
     <row r="49" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4483,7 +4486,7 @@
       <c r="Q51" s="27"/>
       <c r="R51" s="27"/>
       <c r="S51" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T51" s="27"/>
     </row>
@@ -4492,7 +4495,7 @@
     <row r="54" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4569,7 +4572,7 @@
       <c r="Q57" s="27"/>
       <c r="R57" s="27"/>
       <c r="S57" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T57" s="27"/>
     </row>
@@ -4593,7 +4596,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -4671,7 +4674,7 @@
       <c r="Q3" s="27"/>
       <c r="R3" s="27"/>
       <c r="S3" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T3" s="32">
         <v>0.3</v>
@@ -4699,7 +4702,7 @@
       <c r="Q4" s="27"/>
       <c r="R4" s="27"/>
       <c r="S4" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T4" s="32">
         <v>0.5</v>
@@ -4727,7 +4730,7 @@
       <c r="Q5" s="27"/>
       <c r="R5" s="27"/>
       <c r="S5" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T5" s="32">
         <v>0.3</v>
@@ -4755,7 +4758,7 @@
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
       <c r="S6" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T6" s="32">
         <v>0.1</v>
@@ -4783,7 +4786,7 @@
       <c r="Q7" s="27"/>
       <c r="R7" s="27"/>
       <c r="S7" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T7" s="32">
         <v>0.5</v>
@@ -4811,7 +4814,7 @@
       <c r="Q8" s="27"/>
       <c r="R8" s="27"/>
       <c r="S8" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T8" s="32">
         <v>0.4</v>
@@ -4839,7 +4842,7 @@
       <c r="Q9" s="27"/>
       <c r="R9" s="27"/>
       <c r="S9" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T9" s="32">
         <v>0.8</v>
@@ -4868,7 +4871,7 @@
       <c r="Q10" s="27"/>
       <c r="R10" s="27"/>
       <c r="S10" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T10" s="32">
         <v>0.9</v>
@@ -4923,12 +4926,12 @@
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="24"/>
       <c r="K13" s="24" t="s">
-        <v>105</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -5007,7 +5010,7 @@
       <c r="Q17" s="27"/>
       <c r="R17" s="27"/>
       <c r="S17" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T17" s="29">
         <v>1200000</v>
@@ -5035,7 +5038,7 @@
       <c r="Q18" s="27"/>
       <c r="R18" s="27"/>
       <c r="S18" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T18" s="29">
         <v>300000</v>
@@ -5063,7 +5066,7 @@
       <c r="Q19" s="27"/>
       <c r="R19" s="27"/>
       <c r="S19" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T19" s="29">
         <v>5000000</v>
@@ -5091,7 +5094,7 @@
       <c r="Q20" s="27"/>
       <c r="R20" s="27"/>
       <c r="S20" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T20" s="29">
         <v>100000</v>
@@ -5119,7 +5122,7 @@
       <c r="Q21" s="27"/>
       <c r="R21" s="27"/>
       <c r="S21" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T21" s="29">
         <v>700000</v>
@@ -5147,7 +5150,7 @@
       <c r="Q22" s="27"/>
       <c r="R22" s="27"/>
       <c r="S22" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T22" s="29">
         <v>4000000</v>
@@ -5175,7 +5178,7 @@
       <c r="Q23" s="27"/>
       <c r="R23" s="27"/>
       <c r="S23" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T23" s="29"/>
     </row>
@@ -5201,7 +5204,7 @@
       <c r="Q24" s="27"/>
       <c r="R24" s="27"/>
       <c r="S24" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T24" s="29"/>
     </row>
@@ -5210,12 +5213,12 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="K26" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -5294,7 +5297,7 @@
       <c r="Q29" s="27"/>
       <c r="R29" s="27"/>
       <c r="S29" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T29" s="30"/>
     </row>
@@ -5320,7 +5323,7 @@
       <c r="Q30" s="27"/>
       <c r="R30" s="27"/>
       <c r="S30" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T30" s="30"/>
     </row>
@@ -5346,7 +5349,7 @@
       <c r="Q31" s="27"/>
       <c r="R31" s="27"/>
       <c r="S31" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T31" s="30"/>
     </row>
@@ -5372,7 +5375,7 @@
       <c r="Q32" s="27"/>
       <c r="R32" s="27"/>
       <c r="S32" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T32" s="30"/>
     </row>
@@ -5398,7 +5401,7 @@
       <c r="Q33" s="27"/>
       <c r="R33" s="27"/>
       <c r="S33" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T33" s="30"/>
     </row>
@@ -5424,7 +5427,7 @@
       <c r="Q34" s="27"/>
       <c r="R34" s="27"/>
       <c r="S34" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T34" s="30"/>
     </row>
@@ -5450,7 +5453,7 @@
       <c r="Q35" s="27"/>
       <c r="R35" s="27"/>
       <c r="S35" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T35" s="30">
         <v>1000</v>
@@ -5478,7 +5481,7 @@
       <c r="Q36" s="27"/>
       <c r="R36" s="27"/>
       <c r="S36" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T36" s="31">
         <v>2000</v>
@@ -5565,7 +5568,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C3" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
@@ -5584,7 +5587,7 @@
       <c r="R3" s="27"/>
       <c r="S3" s="27"/>
       <c r="T3" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U3" s="33"/>
     </row>
@@ -5623,13 +5626,13 @@
         <v>3000000</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U4" s="33"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C5" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
@@ -5648,13 +5651,13 @@
       <c r="R5" s="27"/>
       <c r="S5" s="27"/>
       <c r="T5" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U5" s="33"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C7" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
@@ -5673,7 +5676,7 @@
       <c r="R7" s="27"/>
       <c r="S7" s="27"/>
       <c r="T7" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U7" s="33"/>
     </row>
@@ -5708,13 +5711,13 @@
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
       <c r="T8" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U8" s="33"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C9" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
@@ -5733,13 +5736,13 @@
       <c r="R9" s="27"/>
       <c r="S9" s="27"/>
       <c r="T9" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U9" s="33"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C11" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
@@ -5758,7 +5761,7 @@
       <c r="R11" s="27"/>
       <c r="S11" s="27"/>
       <c r="T11" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U11" s="33"/>
     </row>
@@ -5791,13 +5794,13 @@
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
       <c r="T12" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U12" s="33"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C13" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
@@ -5816,13 +5819,13 @@
       <c r="R13" s="27"/>
       <c r="S13" s="27"/>
       <c r="T13" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U13" s="33"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C15" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
@@ -5841,7 +5844,7 @@
       <c r="R15" s="27"/>
       <c r="S15" s="27"/>
       <c r="T15" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U15" s="33"/>
     </row>
@@ -5870,7 +5873,7 @@
       <c r="R16" s="27"/>
       <c r="S16" s="27"/>
       <c r="T16" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U16" s="27">
         <v>300000</v>
@@ -5878,7 +5881,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C17" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
@@ -5897,13 +5900,13 @@
       <c r="R17" s="27"/>
       <c r="S17" s="27"/>
       <c r="T17" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U17" s="33"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C19" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
@@ -5922,7 +5925,7 @@
       <c r="R19" s="27"/>
       <c r="S19" s="27"/>
       <c r="T19" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U19" s="33"/>
     </row>
@@ -5951,7 +5954,7 @@
       <c r="R20" s="27"/>
       <c r="S20" s="27"/>
       <c r="T20" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U20" s="29">
         <v>75000</v>
@@ -5959,7 +5962,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C21" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
@@ -5978,13 +5981,13 @@
       <c r="R21" s="27"/>
       <c r="S21" s="27"/>
       <c r="T21" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U21" s="33"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C23" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -6003,7 +6006,7 @@
       <c r="R23" s="27"/>
       <c r="S23" s="27"/>
       <c r="T23" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U23" s="33"/>
     </row>
@@ -6034,13 +6037,13 @@
       <c r="R24" s="27"/>
       <c r="S24" s="27"/>
       <c r="T24" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U24" s="33"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C25" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -6059,13 +6062,13 @@
       <c r="R25" s="27"/>
       <c r="S25" s="27"/>
       <c r="T25" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U25" s="33"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -6123,7 +6126,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C31" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
@@ -6142,7 +6145,7 @@
       <c r="R31" s="27"/>
       <c r="S31" s="27"/>
       <c r="T31" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U31" s="33">
         <v>1E-3</v>
@@ -6173,7 +6176,7 @@
       <c r="R32" s="27"/>
       <c r="S32" s="27"/>
       <c r="T32" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U32" s="33">
         <v>1E-3</v>
@@ -6181,7 +6184,7 @@
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C33" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
@@ -6200,7 +6203,7 @@
       <c r="R33" s="27"/>
       <c r="S33" s="27"/>
       <c r="T33" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U33" s="33">
         <v>1E-3</v>
@@ -6208,7 +6211,7 @@
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C35" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
@@ -6227,7 +6230,7 @@
       <c r="R35" s="27"/>
       <c r="S35" s="27"/>
       <c r="T35" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U35" s="33">
         <v>1E-3</v>
@@ -6258,7 +6261,7 @@
       <c r="R36" s="27"/>
       <c r="S36" s="27"/>
       <c r="T36" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U36" s="33">
         <v>1E-3</v>
@@ -6266,7 +6269,7 @@
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C37" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
@@ -6285,7 +6288,7 @@
       <c r="R37" s="27"/>
       <c r="S37" s="27"/>
       <c r="T37" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U37" s="33">
         <v>1E-3</v>
@@ -6293,7 +6296,7 @@
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C39" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D39" s="27"/>
       <c r="E39" s="27"/>
@@ -6312,7 +6315,7 @@
       <c r="R39" s="27"/>
       <c r="S39" s="27"/>
       <c r="T39" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U39" s="33">
         <v>1E-3</v>
@@ -6343,7 +6346,7 @@
       <c r="R40" s="27"/>
       <c r="S40" s="27"/>
       <c r="T40" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U40" s="33">
         <v>1E-3</v>
@@ -6351,7 +6354,7 @@
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C41" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
@@ -6370,7 +6373,7 @@
       <c r="R41" s="27"/>
       <c r="S41" s="27"/>
       <c r="T41" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U41" s="33">
         <v>1E-3</v>
@@ -6378,7 +6381,7 @@
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C43" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
@@ -6397,7 +6400,7 @@
       <c r="R43" s="27"/>
       <c r="S43" s="27"/>
       <c r="T43" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U43" s="33">
         <v>1E-3</v>
@@ -6428,7 +6431,7 @@
       <c r="R44" s="27"/>
       <c r="S44" s="27"/>
       <c r="T44" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U44" s="33">
         <v>1E-3</v>
@@ -6436,7 +6439,7 @@
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C45" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
@@ -6455,7 +6458,7 @@
       <c r="R45" s="27"/>
       <c r="S45" s="27"/>
       <c r="T45" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U45" s="33">
         <v>1E-3</v>
@@ -6463,7 +6466,7 @@
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C47" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
@@ -6482,7 +6485,7 @@
       <c r="R47" s="27"/>
       <c r="S47" s="27"/>
       <c r="T47" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U47" s="33">
         <v>1E-3</v>
@@ -6513,7 +6516,7 @@
       <c r="R48" s="27"/>
       <c r="S48" s="27"/>
       <c r="T48" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U48" s="33">
         <v>1E-3</v>
@@ -6521,7 +6524,7 @@
     </row>
     <row r="49" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C49" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D49" s="27"/>
       <c r="E49" s="27"/>
@@ -6540,7 +6543,7 @@
       <c r="R49" s="27"/>
       <c r="S49" s="27"/>
       <c r="T49" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U49" s="33">
         <v>1E-3</v>
@@ -6548,7 +6551,7 @@
     </row>
     <row r="51" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C51" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D51" s="27"/>
       <c r="E51" s="27"/>
@@ -6567,7 +6570,7 @@
       <c r="R51" s="27"/>
       <c r="S51" s="27"/>
       <c r="T51" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U51" s="33">
         <v>1E-3</v>
@@ -6598,7 +6601,7 @@
       <c r="R52" s="27"/>
       <c r="S52" s="27"/>
       <c r="T52" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U52" s="33">
         <v>1E-3</v>
@@ -6606,7 +6609,7 @@
     </row>
     <row r="53" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C53" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D53" s="27"/>
       <c r="E53" s="27"/>
@@ -6625,7 +6628,7 @@
       <c r="R53" s="27"/>
       <c r="S53" s="27"/>
       <c r="T53" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U53" s="33">
         <v>1E-3</v>
@@ -6641,9 +6644,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AC30"/>
+  <dimension ref="A1:AC42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6651,113 +6656,87 @@
     <col min="22" max="22" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
+    <row r="1" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>144</v>
+      </c>
       <c r="X1" s="3"/>
       <c r="Y1" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AB1" s="22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="22">
         <v>2000</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="22">
         <v>2001</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="22">
         <v>2002</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="22">
         <v>2003</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="22">
         <v>2004</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="22">
         <v>2005</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="22">
         <v>2006</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="22">
         <v>2007</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="22">
         <v>2008</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="22">
         <v>2009</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="22">
         <v>2010</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="22">
         <v>2011</v>
       </c>
-      <c r="O2" s="11">
+      <c r="O2" s="22">
         <v>2012</v>
       </c>
-      <c r="P2" s="11">
+      <c r="P2" s="22">
         <v>2013</v>
       </c>
-      <c r="Q2" s="11">
+      <c r="Q2" s="22">
         <v>2014</v>
       </c>
-      <c r="R2" s="11">
+      <c r="R2" s="22">
         <v>2015</v>
       </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="11" t="s">
+      <c r="T2" s="22" t="s">
         <v>0</v>
       </c>
       <c r="W2" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="21"/>
-      <c r="Y2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>92</v>
+      <c r="Y2" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z2" s="21" t="s">
+        <v>90</v>
       </c>
       <c r="AB2" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC2" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>GM</v>
@@ -6779,30 +6758,18 @@
       <c r="Q3" s="27"/>
       <c r="R3" s="27"/>
       <c r="S3" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T3" s="32">
-        <v>0.1</v>
-      </c>
-      <c r="W3" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="32">
-        <v>0.2</v>
-      </c>
-      <c r="Z3" s="32">
-        <v>0.2</v>
-      </c>
-      <c r="AB3" s="32">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+        <v>0.01</v>
+      </c>
+      <c r="W3" s="27"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
+      <c r="AB3" s="32"/>
+      <c r="AC3" s="32"/>
+    </row>
+    <row r="4" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>GF</v>
@@ -6824,30 +6791,18 @@
       <c r="Q4" s="27"/>
       <c r="R4" s="27"/>
       <c r="S4" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T4" s="32">
-        <v>0.1</v>
-      </c>
-      <c r="W4" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="32">
-        <v>0.2</v>
-      </c>
-      <c r="Z4" s="32">
-        <v>0.2</v>
-      </c>
-      <c r="AB4" s="32">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+        <v>0.01</v>
+      </c>
+      <c r="W4" s="27"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="32"/>
+      <c r="AB4" s="32"/>
+      <c r="AC4" s="32"/>
+    </row>
+    <row r="5" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>FSW</v>
@@ -6869,30 +6824,18 @@
       <c r="Q5" s="27"/>
       <c r="R5" s="27"/>
       <c r="S5" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T5" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="W5" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="Z5" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="AB5" s="32">
-        <v>0.1</v>
-      </c>
-      <c r="AC5" s="32">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+        <v>0.01</v>
+      </c>
+      <c r="W5" s="27"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="32"/>
+      <c r="AB5" s="32"/>
+      <c r="AC5" s="32"/>
+    </row>
+    <row r="6" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>CSW</v>
@@ -6914,30 +6857,18 @@
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
       <c r="S6" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T6" s="32">
-        <v>0.2</v>
-      </c>
-      <c r="W6" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="32">
-        <v>0.3</v>
-      </c>
-      <c r="Z6" s="32">
-        <v>0.3</v>
-      </c>
-      <c r="AB6" s="32">
-        <v>0.03</v>
-      </c>
-      <c r="AC6" s="32">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+        <v>0.01</v>
+      </c>
+      <c r="W6" s="27"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="32"/>
+      <c r="AB6" s="32"/>
+      <c r="AC6" s="32"/>
+    </row>
+    <row r="7" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>MSM</v>
@@ -6959,30 +6890,18 @@
       <c r="Q7" s="27"/>
       <c r="R7" s="27"/>
       <c r="S7" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T7" s="32">
-        <v>0.2</v>
-      </c>
-      <c r="W7" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="32">
-        <v>0.7</v>
-      </c>
-      <c r="Z7" s="32">
-        <v>0.7</v>
-      </c>
-      <c r="AB7" s="32">
-        <v>0.05</v>
-      </c>
-      <c r="AC7" s="32">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+        <v>0.01</v>
+      </c>
+      <c r="W7" s="27"/>
+      <c r="Y7" s="32"/>
+      <c r="Z7" s="32"/>
+      <c r="AB7" s="32"/>
+      <c r="AC7" s="32"/>
+    </row>
+    <row r="8" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>PWID</v>
@@ -7004,112 +6923,127 @@
       <c r="Q8" s="27"/>
       <c r="R8" s="27"/>
       <c r="S8" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T8" s="32">
-        <v>0.2</v>
-      </c>
-      <c r="W8" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="32">
-        <v>0.3</v>
-      </c>
-      <c r="Z8" s="32">
-        <v>0.3</v>
-      </c>
-      <c r="AB8" s="32">
-        <v>0.05</v>
-      </c>
-      <c r="AC8" s="32">
-        <v>0.05</v>
-      </c>
+        <v>0.01</v>
+      </c>
+      <c r="W8" s="27"/>
+      <c r="Y8" s="32"/>
+      <c r="Z8" s="32"/>
+      <c r="AB8" s="32"/>
+      <c r="AC8" s="32"/>
     </row>
     <row r="9" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>136</v>
-      </c>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AB12" s="22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="22">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11">
         <v>2000</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="11">
         <v>2001</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="11">
         <v>2002</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="11">
         <v>2003</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="11">
         <v>2004</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="11">
         <v>2005</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="11">
         <v>2006</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="11">
         <v>2007</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="11">
         <v>2008</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="11">
         <v>2009</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="11">
         <v>2010</v>
       </c>
-      <c r="N13" s="22">
+      <c r="N13" s="11">
         <v>2011</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="11">
         <v>2012</v>
       </c>
-      <c r="P13" s="22">
+      <c r="P13" s="11">
         <v>2013</v>
       </c>
-      <c r="Q13" s="22">
+      <c r="Q13" s="11">
         <v>2014</v>
       </c>
-      <c r="R13" s="22">
+      <c r="R13" s="11">
         <v>2015</v>
       </c>
-      <c r="T13" s="22" t="s">
+      <c r="S13" s="10"/>
+      <c r="T13" s="11" t="s">
         <v>0</v>
       </c>
       <c r="W13" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="Y13" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z13" s="21" t="s">
-        <v>92</v>
+      <c r="X13" s="21"/>
+      <c r="Y13" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>90</v>
       </c>
       <c r="AB13" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC13" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
       <c r="B14" s="22" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>GM</v>
@@ -7131,14 +7065,15 @@
       <c r="Q14" s="27"/>
       <c r="R14" s="27"/>
       <c r="S14" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T14" s="32">
         <v>0.1</v>
       </c>
       <c r="W14" s="27" t="s">
-        <v>85</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="X14" s="21"/>
       <c r="Y14" s="32">
         <v>0.2</v>
       </c>
@@ -7152,7 +7087,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
       <c r="B15" s="22" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>GF</v>
@@ -7174,14 +7110,15 @@
       <c r="Q15" s="27"/>
       <c r="R15" s="27"/>
       <c r="S15" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T15" s="32">
         <v>0.1</v>
       </c>
       <c r="W15" s="27" t="s">
-        <v>85</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="X15" s="21"/>
       <c r="Y15" s="32">
         <v>0.2</v>
       </c>
@@ -7195,7 +7132,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
       <c r="B16" s="22" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>FSW</v>
@@ -7217,14 +7155,15 @@
       <c r="Q16" s="27"/>
       <c r="R16" s="27"/>
       <c r="S16" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T16" s="32">
         <v>0.5</v>
       </c>
       <c r="W16" s="27" t="s">
-        <v>85</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="X16" s="21"/>
       <c r="Y16" s="32">
         <v>0.8</v>
       </c>
@@ -7238,7 +7177,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
       <c r="B17" s="22" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>CSW</v>
@@ -7260,14 +7200,15 @@
       <c r="Q17" s="27"/>
       <c r="R17" s="27"/>
       <c r="S17" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T17" s="32">
         <v>0.2</v>
       </c>
       <c r="W17" s="27" t="s">
-        <v>85</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="X17" s="21"/>
       <c r="Y17" s="32">
         <v>0.3</v>
       </c>
@@ -7281,7 +7222,8 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="18" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
       <c r="B18" s="22" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>MSM</v>
@@ -7303,14 +7245,15 @@
       <c r="Q18" s="27"/>
       <c r="R18" s="27"/>
       <c r="S18" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T18" s="32">
         <v>0.2</v>
       </c>
       <c r="W18" s="27" t="s">
-        <v>85</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="X18" s="21"/>
       <c r="Y18" s="32">
         <v>0.7</v>
       </c>
@@ -7324,7 +7267,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
       <c r="B19" s="22" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>PWID</v>
@@ -7346,14 +7290,15 @@
       <c r="Q19" s="27"/>
       <c r="R19" s="27"/>
       <c r="S19" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T19" s="32">
         <v>0.2</v>
       </c>
       <c r="W19" s="27" t="s">
-        <v>85</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="X19" s="21"/>
       <c r="Y19" s="32">
         <v>0.3</v>
       </c>
@@ -7367,125 +7312,93 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="S20" s="8"/>
-    </row>
-    <row r="21" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="S21" s="8"/>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="11">
+    <row r="20" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB23" s="22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="22">
         <v>2000</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D24" s="22">
         <v>2001</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E24" s="22">
         <v>2002</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F24" s="22">
         <v>2003</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G24" s="22">
         <v>2004</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H24" s="22">
         <v>2005</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I24" s="22">
         <v>2006</v>
       </c>
-      <c r="J23" s="11">
+      <c r="J24" s="22">
         <v>2007</v>
       </c>
-      <c r="K23" s="11">
+      <c r="K24" s="22">
         <v>2008</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L24" s="22">
         <v>2009</v>
       </c>
-      <c r="M23" s="11">
+      <c r="M24" s="22">
         <v>2010</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N24" s="22">
         <v>2011</v>
       </c>
-      <c r="O23" s="11">
+      <c r="O24" s="22">
         <v>2012</v>
       </c>
-      <c r="P23" s="11">
+      <c r="P24" s="22">
         <v>2013</v>
       </c>
-      <c r="Q23" s="11">
+      <c r="Q24" s="22">
         <v>2014</v>
       </c>
-      <c r="R23" s="11">
+      <c r="R24" s="22">
         <v>2015</v>
       </c>
-      <c r="S23" s="10"/>
-      <c r="T23" s="11" t="s">
+      <c r="T24" s="22" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="22" t="str">
+      <c r="W24" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y24" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z24" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB24" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC24" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="22" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>GM</v>
-      </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="T24" s="32">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B25" s="22" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
-        <v>GF</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
@@ -7504,16 +7417,31 @@
       <c r="Q25" s="27"/>
       <c r="R25" s="27"/>
       <c r="S25" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T25" s="32">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+      <c r="W25" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y25" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="Z25" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="AB25" s="32">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="22" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
-        <v>FSW</v>
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>GF</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
@@ -7532,16 +7460,31 @@
       <c r="Q26" s="27"/>
       <c r="R26" s="27"/>
       <c r="S26" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T26" s="32">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+      <c r="W26" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y26" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="Z26" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="AB26" s="32">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="22" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
-        <v>CSW</v>
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>FSW</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
@@ -7560,16 +7503,31 @@
       <c r="Q27" s="27"/>
       <c r="R27" s="27"/>
       <c r="S27" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T27" s="32">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="W27" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y27" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="Z27" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="AB27" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="AC27" s="32">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="22" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
-        <v>MSM</v>
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>CSW</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="27"/>
@@ -7588,16 +7546,31 @@
       <c r="Q28" s="27"/>
       <c r="R28" s="27"/>
       <c r="S28" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T28" s="32">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+      <c r="W28" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y28" s="32">
+        <v>0.3</v>
+      </c>
+      <c r="Z28" s="32">
+        <v>0.3</v>
+      </c>
+      <c r="AB28" s="32">
+        <v>0.03</v>
+      </c>
+      <c r="AC28" s="32">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="22" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
-        <v>PWID</v>
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>MSM</v>
       </c>
       <c r="C29" s="27"/>
       <c r="D29" s="27"/>
@@ -7616,17 +7589,402 @@
       <c r="Q29" s="27"/>
       <c r="R29" s="27"/>
       <c r="S29" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T29" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="W29" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y29" s="32">
+        <v>0.7</v>
+      </c>
+      <c r="Z29" s="32">
+        <v>0.7</v>
+      </c>
+      <c r="AB29" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="AC29" s="32">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$8</f>
+        <v>PWID</v>
+      </c>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="27"/>
+      <c r="R30" s="27"/>
+      <c r="S30" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="T30" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="W30" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y30" s="32">
+        <v>0.3</v>
+      </c>
+      <c r="Z30" s="32">
+        <v>0.3</v>
+      </c>
+      <c r="AB30" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="AC30" s="32">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="S31" s="8"/>
+    </row>
+    <row r="32" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S32" s="8"/>
+    </row>
+    <row r="33" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S33" s="8"/>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="W34" s="21"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z34" s="21"/>
+      <c r="AA34" s="21"/>
+      <c r="AB34" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC34" s="21"/>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="11">
+        <v>2000</v>
+      </c>
+      <c r="D35" s="11">
+        <v>2001</v>
+      </c>
+      <c r="E35" s="11">
+        <v>2002</v>
+      </c>
+      <c r="F35" s="11">
+        <v>2003</v>
+      </c>
+      <c r="G35" s="11">
+        <v>2004</v>
+      </c>
+      <c r="H35" s="11">
+        <v>2005</v>
+      </c>
+      <c r="I35" s="11">
+        <v>2006</v>
+      </c>
+      <c r="J35" s="11">
+        <v>2007</v>
+      </c>
+      <c r="K35" s="11">
+        <v>2008</v>
+      </c>
+      <c r="L35" s="11">
+        <v>2009</v>
+      </c>
+      <c r="M35" s="11">
+        <v>2010</v>
+      </c>
+      <c r="N35" s="11">
+        <v>2011</v>
+      </c>
+      <c r="O35" s="11">
+        <v>2012</v>
+      </c>
+      <c r="P35" s="11">
+        <v>2013</v>
+      </c>
+      <c r="Q35" s="11">
+        <v>2014</v>
+      </c>
+      <c r="R35" s="11">
+        <v>2015</v>
+      </c>
+      <c r="S35" s="10"/>
+      <c r="T35" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="W35" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="X35" s="21"/>
+      <c r="Y35" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z35" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA35" s="21"/>
+      <c r="AB35" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC35" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>GM</v>
+      </c>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="27"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="27"/>
+      <c r="S36" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="T36" s="32">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="S30" s="8"/>
+      <c r="W36" s="27"/>
+      <c r="X36" s="21"/>
+      <c r="Y36" s="32"/>
+      <c r="Z36" s="32"/>
+      <c r="AA36" s="21"/>
+      <c r="AB36" s="32"/>
+      <c r="AC36" s="32"/>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B37" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>GF</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="27"/>
+      <c r="Q37" s="27"/>
+      <c r="R37" s="27"/>
+      <c r="S37" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="T37" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="W37" s="27"/>
+      <c r="X37" s="21"/>
+      <c r="Y37" s="32"/>
+      <c r="Z37" s="32"/>
+      <c r="AA37" s="21"/>
+      <c r="AB37" s="32"/>
+      <c r="AC37" s="32"/>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B38" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>FSW</v>
+      </c>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="27"/>
+      <c r="P38" s="27"/>
+      <c r="Q38" s="27"/>
+      <c r="R38" s="27"/>
+      <c r="S38" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="T38" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="W38" s="27"/>
+      <c r="X38" s="21"/>
+      <c r="Y38" s="32"/>
+      <c r="Z38" s="32"/>
+      <c r="AA38" s="21"/>
+      <c r="AB38" s="32"/>
+      <c r="AC38" s="32"/>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B39" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>CSW</v>
+      </c>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="27"/>
+      <c r="R39" s="27"/>
+      <c r="S39" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="T39" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="W39" s="27"/>
+      <c r="X39" s="21"/>
+      <c r="Y39" s="32"/>
+      <c r="Z39" s="32"/>
+      <c r="AA39" s="21"/>
+      <c r="AB39" s="32"/>
+      <c r="AC39" s="32"/>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B40" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>MSM</v>
+      </c>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="27"/>
+      <c r="R40" s="27"/>
+      <c r="S40" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="T40" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="W40" s="27"/>
+      <c r="X40" s="21"/>
+      <c r="Y40" s="32"/>
+      <c r="Z40" s="32"/>
+      <c r="AA40" s="21"/>
+      <c r="AB40" s="32"/>
+      <c r="AC40" s="32"/>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B41" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$8</f>
+        <v>PWID</v>
+      </c>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
+      <c r="N41" s="27"/>
+      <c r="O41" s="27"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="27"/>
+      <c r="R41" s="27"/>
+      <c r="S41" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="T41" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="W41" s="27"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="32"/>
+      <c r="Z41" s="32"/>
+      <c r="AA41" s="21"/>
+      <c r="AB41" s="32"/>
+      <c r="AC41" s="32"/>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="S42" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7744,7 +8102,7 @@
       <c r="Q3" s="27"/>
       <c r="R3" s="27"/>
       <c r="S3" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T3" s="27"/>
     </row>
@@ -7856,7 +8214,7 @@
       <c r="Q9" s="27"/>
       <c r="R9" s="27"/>
       <c r="S9" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T9" s="27"/>
     </row>
@@ -7864,7 +8222,7 @@
     <row r="12" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -7964,7 +8322,7 @@
       <c r="Q15" s="27"/>
       <c r="R15" s="27"/>
       <c r="S15" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T15" s="27"/>
     </row>
@@ -7972,7 +8330,7 @@
     <row r="18" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -8049,7 +8407,7 @@
       <c r="Q21" s="27"/>
       <c r="R21" s="27"/>
       <c r="S21" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T21" s="27"/>
     </row>
@@ -8058,7 +8416,7 @@
     <row r="24" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -8162,13 +8520,13 @@
       <c r="Q27" s="27"/>
       <c r="R27" s="27"/>
       <c r="S27" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T27" s="27"/>
     </row>
     <row r="31" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -8249,7 +8607,7 @@
       <c r="Q33" s="27"/>
       <c r="R33" s="27"/>
       <c r="S33" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T33" s="27"/>
     </row>
@@ -8270,7 +8628,7 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -8292,12 +8650,12 @@
       <c r="S1" s="12"/>
       <c r="T1" s="12"/>
       <c r="Y1" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z1" s="21"/>
       <c r="AA1" s="21"/>
       <c r="AB1" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC1" s="21"/>
     </row>
@@ -8360,17 +8718,17 @@
         <v>34</v>
       </c>
       <c r="Y2" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA2" s="21"/>
       <c r="AB2" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC2" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
@@ -8396,7 +8754,7 @@
       <c r="Q3" s="27"/>
       <c r="R3" s="27"/>
       <c r="S3" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T3" s="32">
         <v>0.03</v>
@@ -8440,7 +8798,7 @@
       <c r="Q4" s="27"/>
       <c r="R4" s="27"/>
       <c r="S4" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T4" s="32">
         <v>0.03</v>
@@ -8490,7 +8848,7 @@
       <c r="Q5" s="27"/>
       <c r="R5" s="27"/>
       <c r="S5" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T5" s="27"/>
       <c r="W5" s="27" t="s">
@@ -8532,7 +8890,7 @@
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
       <c r="S6" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T6" s="32">
         <v>0.1</v>
@@ -8582,7 +8940,7 @@
       </c>
       <c r="R7" s="27"/>
       <c r="S7" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T7" s="27"/>
       <c r="W7" s="27" t="s">
@@ -8624,7 +8982,7 @@
       <c r="Q8" s="27"/>
       <c r="R8" s="27"/>
       <c r="S8" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T8" s="32">
         <v>0.8</v>
@@ -8649,7 +9007,7 @@
     <row r="11" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -8671,12 +9029,12 @@
       <c r="S12" s="12"/>
       <c r="T12" s="12"/>
       <c r="Y12" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z12" s="21"/>
       <c r="AA12" s="21"/>
       <c r="AB12" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC12" s="21"/>
     </row>
@@ -8739,17 +9097,17 @@
         <v>34</v>
       </c>
       <c r="Y13" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z13" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA13" s="21"/>
       <c r="AB13" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC13" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -8774,7 +9132,7 @@
       <c r="Q14" s="27"/>
       <c r="R14" s="27"/>
       <c r="S14" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T14" s="32">
         <v>0.8</v>
@@ -8799,7 +9157,7 @@
     <row r="17" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>50</v>
+        <v>147</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -8821,12 +9179,12 @@
       <c r="S18" s="12"/>
       <c r="T18" s="12"/>
       <c r="Y18" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z18" s="21"/>
       <c r="AA18" s="21"/>
       <c r="AB18" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC18" s="21"/>
     </row>
@@ -8889,17 +9247,17 @@
         <v>34</v>
       </c>
       <c r="Y19" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z19" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA19" s="21"/>
       <c r="AB19" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC19" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
@@ -8930,7 +9288,7 @@
       </c>
       <c r="R20" s="27"/>
       <c r="S20" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T20" s="27"/>
       <c r="W20" s="27" t="s">
@@ -8953,7 +9311,7 @@
     <row r="22" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -8975,12 +9333,12 @@
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
       <c r="Y24" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z24" s="21"/>
       <c r="AA24" s="21"/>
       <c r="AB24" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC24" s="21"/>
     </row>
@@ -9043,17 +9401,17 @@
         <v>34</v>
       </c>
       <c r="Y25" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z25" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA25" s="21"/>
       <c r="AB25" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC25" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
@@ -9084,7 +9442,7 @@
       </c>
       <c r="R26" s="27"/>
       <c r="S26" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T26" s="27"/>
       <c r="W26" s="27" t="s">
@@ -9108,7 +9466,7 @@
     <row r="29" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -9130,12 +9488,12 @@
       <c r="S30" s="12"/>
       <c r="T30" s="12"/>
       <c r="Y30" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z30" s="21"/>
       <c r="AA30" s="21"/>
       <c r="AB30" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC30" s="21"/>
     </row>
@@ -9198,17 +9556,17 @@
         <v>34</v>
       </c>
       <c r="Y31" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z31" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA31" s="21"/>
       <c r="AB31" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC31" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
@@ -9235,7 +9593,7 @@
       <c r="Q32" s="27"/>
       <c r="R32" s="27"/>
       <c r="S32" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T32" s="27"/>
       <c r="W32" s="27" t="s">
@@ -9260,13 +9618,13 @@
     <row r="35" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Y36" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AB36" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -9325,16 +9683,16 @@
         <v>34</v>
       </c>
       <c r="Y37" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z37" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AB37" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC37" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -9359,7 +9717,7 @@
       <c r="Q38" s="27"/>
       <c r="R38" s="27"/>
       <c r="S38" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T38" s="31"/>
       <c r="W38" s="27"/>
@@ -9390,7 +9748,7 @@
       <c r="Q39" s="27"/>
       <c r="R39" s="27"/>
       <c r="S39" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T39" s="31">
         <v>0.1</v>
@@ -9423,7 +9781,7 @@
       <c r="Q40" s="27"/>
       <c r="R40" s="27"/>
       <c r="S40" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T40" s="31">
         <v>0.2</v>
@@ -9456,7 +9814,7 @@
       <c r="Q41" s="27"/>
       <c r="R41" s="27"/>
       <c r="S41" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T41" s="31"/>
       <c r="W41" s="27"/>
@@ -9487,7 +9845,7 @@
       <c r="Q42" s="32"/>
       <c r="R42" s="27"/>
       <c r="S42" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T42" s="31"/>
       <c r="W42" s="27"/>
@@ -9518,7 +9876,7 @@
       <c r="Q43" s="27"/>
       <c r="R43" s="27"/>
       <c r="S43" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T43" s="31"/>
       <c r="W43" s="27"/>
@@ -9529,13 +9887,13 @@
     </row>
     <row r="47" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Y47" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AB47" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -9594,16 +9952,16 @@
         <v>34</v>
       </c>
       <c r="Y48" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z48" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AB48" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC48" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="2:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -9629,7 +9987,7 @@
       <c r="Q49" s="27"/>
       <c r="R49" s="27"/>
       <c r="S49" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T49" s="27"/>
       <c r="W49" s="27"/>
@@ -9650,7 +10008,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AC74"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9659,7 +10017,7 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -9681,12 +10039,12 @@
       <c r="S1" s="14"/>
       <c r="T1" s="14"/>
       <c r="Y1" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z1" s="21"/>
       <c r="AA1" s="21"/>
       <c r="AB1" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC1" s="21"/>
     </row>
@@ -9749,17 +10107,17 @@
         <v>34</v>
       </c>
       <c r="Y2" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA2" s="21"/>
       <c r="AB2" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC2" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
@@ -9785,7 +10143,7 @@
       <c r="Q3" s="27"/>
       <c r="R3" s="27"/>
       <c r="S3" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T3" s="27">
         <v>60</v>
@@ -9820,7 +10178,7 @@
       <c r="Q4" s="27"/>
       <c r="R4" s="27"/>
       <c r="S4" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T4" s="27">
         <v>60</v>
@@ -9855,7 +10213,7 @@
       <c r="Q5" s="27"/>
       <c r="R5" s="27"/>
       <c r="S5" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T5" s="27">
         <v>40</v>
@@ -9890,7 +10248,7 @@
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
       <c r="S6" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T6" s="27">
         <v>50</v>
@@ -9925,7 +10283,7 @@
       <c r="Q7" s="27"/>
       <c r="R7" s="27"/>
       <c r="S7" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T7" s="27">
         <v>50</v>
@@ -9960,7 +10318,7 @@
       <c r="Q8" s="27"/>
       <c r="R8" s="27"/>
       <c r="S8" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T8" s="27">
         <v>50</v>
@@ -9976,7 +10334,7 @@
     <row r="11" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -9998,12 +10356,12 @@
       <c r="S12" s="14"/>
       <c r="T12" s="14"/>
       <c r="Y12" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z12" s="21"/>
       <c r="AA12" s="21"/>
       <c r="AB12" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC12" s="21"/>
     </row>
@@ -10066,17 +10424,17 @@
         <v>34</v>
       </c>
       <c r="Y13" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z13" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA13" s="21"/>
       <c r="AB13" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC13" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -10102,7 +10460,7 @@
       <c r="Q14" s="27"/>
       <c r="R14" s="27"/>
       <c r="S14" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T14" s="27">
         <v>10</v>
@@ -10138,7 +10496,7 @@
       <c r="Q15" s="27"/>
       <c r="R15" s="27"/>
       <c r="S15" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T15" s="27">
         <v>10</v>
@@ -10174,7 +10532,7 @@
       <c r="Q16" s="27"/>
       <c r="R16" s="27"/>
       <c r="S16" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T16" s="27">
         <v>20</v>
@@ -10210,7 +10568,7 @@
       <c r="Q17" s="27"/>
       <c r="R17" s="27"/>
       <c r="S17" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T17" s="27">
         <v>20</v>
@@ -10246,7 +10604,7 @@
       <c r="Q18" s="27"/>
       <c r="R18" s="27"/>
       <c r="S18" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T18" s="27">
         <v>100</v>
@@ -10282,7 +10640,7 @@
       <c r="Q19" s="27"/>
       <c r="R19" s="27"/>
       <c r="S19" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T19" s="27">
         <v>20</v>
@@ -10299,7 +10657,7 @@
     <row r="22" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -10321,12 +10679,12 @@
       <c r="S23" s="14"/>
       <c r="T23" s="14"/>
       <c r="Y23" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z23" s="21"/>
       <c r="AA23" s="21"/>
       <c r="AB23" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC23" s="21"/>
     </row>
@@ -10389,17 +10747,17 @@
         <v>34</v>
       </c>
       <c r="Y24" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z24" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA24" s="21"/>
       <c r="AB24" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC24" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
@@ -10425,7 +10783,7 @@
       <c r="Q25" s="27"/>
       <c r="R25" s="27"/>
       <c r="S25" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T25" s="27">
         <v>0</v>
@@ -10461,7 +10819,7 @@
       <c r="Q26" s="27"/>
       <c r="R26" s="27"/>
       <c r="S26" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T26" s="27">
         <v>0</v>
@@ -10497,7 +10855,7 @@
       <c r="Q27" s="27"/>
       <c r="R27" s="27"/>
       <c r="S27" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T27" s="27">
         <v>400</v>
@@ -10533,7 +10891,7 @@
       <c r="Q28" s="27"/>
       <c r="R28" s="27"/>
       <c r="S28" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T28" s="27">
         <v>40</v>
@@ -10569,7 +10927,7 @@
       <c r="Q29" s="27"/>
       <c r="R29" s="27"/>
       <c r="S29" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T29" s="27">
         <v>0</v>
@@ -10605,7 +10963,7 @@
       <c r="Q30" s="27"/>
       <c r="R30" s="27"/>
       <c r="S30" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T30" s="27">
         <v>10</v>
@@ -10622,7 +10980,7 @@
     <row r="33" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -10644,12 +11002,12 @@
       <c r="S34" s="14"/>
       <c r="T34" s="14"/>
       <c r="Y34" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z34" s="21"/>
       <c r="AA34" s="21"/>
       <c r="AB34" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC34" s="21"/>
     </row>
@@ -10712,17 +11070,17 @@
         <v>34</v>
       </c>
       <c r="Y35" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z35" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA35" s="21"/>
       <c r="AB35" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC35" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
@@ -10748,13 +11106,13 @@
       <c r="Q36" s="27"/>
       <c r="R36" s="27"/>
       <c r="S36" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T36" s="32">
         <v>0.05</v>
       </c>
       <c r="W36" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="X36" s="21"/>
       <c r="Y36" s="32"/>
@@ -10786,13 +11144,13 @@
       <c r="Q37" s="27"/>
       <c r="R37" s="27"/>
       <c r="S37" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T37" s="32">
         <v>0.05</v>
       </c>
       <c r="W37" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="X37" s="21"/>
       <c r="Y37" s="32"/>
@@ -10824,7 +11182,7 @@
       <c r="Q38" s="27"/>
       <c r="R38" s="27"/>
       <c r="S38" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T38" s="32">
         <v>0.2</v>
@@ -10862,7 +11220,7 @@
       <c r="Q39" s="27"/>
       <c r="R39" s="27"/>
       <c r="S39" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T39" s="32">
         <v>0.2</v>
@@ -10900,7 +11258,7 @@
       <c r="Q40" s="27"/>
       <c r="R40" s="27"/>
       <c r="S40" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T40" s="32">
         <v>0.2</v>
@@ -10938,13 +11296,13 @@
       <c r="Q41" s="27"/>
       <c r="R41" s="27"/>
       <c r="S41" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T41" s="32">
         <v>0.2</v>
       </c>
       <c r="W41" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="X41" s="21"/>
       <c r="Y41" s="32"/>
@@ -10957,7 +11315,7 @@
     <row r="44" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -10979,12 +11337,12 @@
       <c r="S45" s="14"/>
       <c r="T45" s="14"/>
       <c r="Y45" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z45" s="21"/>
       <c r="AA45" s="21"/>
       <c r="AB45" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC45" s="21"/>
     </row>
@@ -11047,17 +11405,17 @@
         <v>34</v>
       </c>
       <c r="Y46" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z46" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA46" s="21"/>
       <c r="AB46" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC46" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.25">
@@ -11083,13 +11441,13 @@
       <c r="Q47" s="27"/>
       <c r="R47" s="27"/>
       <c r="S47" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T47" s="32">
         <v>0.5</v>
       </c>
       <c r="W47" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Y47" s="32"/>
       <c r="Z47" s="32"/>
@@ -11120,13 +11478,13 @@
       <c r="Q48" s="27"/>
       <c r="R48" s="27"/>
       <c r="S48" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T48" s="32">
         <v>0.5</v>
       </c>
       <c r="W48" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Y48" s="32"/>
       <c r="Z48" s="32"/>
@@ -11157,7 +11515,7 @@
       <c r="Q49" s="27"/>
       <c r="R49" s="27"/>
       <c r="S49" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T49" s="32">
         <v>0.5</v>
@@ -11194,7 +11552,7 @@
       <c r="Q50" s="27"/>
       <c r="R50" s="27"/>
       <c r="S50" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T50" s="32">
         <v>0.5</v>
@@ -11231,7 +11589,7 @@
       <c r="Q51" s="27"/>
       <c r="R51" s="27"/>
       <c r="S51" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T51" s="32">
         <v>0.5</v>
@@ -11268,13 +11626,13 @@
       <c r="Q52" s="27"/>
       <c r="R52" s="27"/>
       <c r="S52" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T52" s="32">
         <v>0.5</v>
       </c>
       <c r="W52" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Y52" s="32"/>
       <c r="Z52" s="32"/>
@@ -11286,7 +11644,7 @@
     <row r="55" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
@@ -11308,12 +11666,12 @@
       <c r="S56" s="14"/>
       <c r="T56" s="14"/>
       <c r="Y56" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z56" s="21"/>
       <c r="AA56" s="21"/>
       <c r="AB56" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC56" s="21"/>
     </row>
@@ -11376,17 +11734,17 @@
         <v>34</v>
       </c>
       <c r="Y57" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z57" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA57" s="21"/>
       <c r="AB57" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC57" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.25">
@@ -11412,7 +11770,7 @@
       <c r="Q58" s="27"/>
       <c r="R58" s="27"/>
       <c r="S58" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T58" s="27">
         <v>0</v>
@@ -11447,7 +11805,7 @@
       <c r="Q59" s="27"/>
       <c r="R59" s="27"/>
       <c r="S59" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T59" s="27">
         <v>0</v>
@@ -11482,7 +11840,7 @@
       <c r="Q60" s="27"/>
       <c r="R60" s="27"/>
       <c r="S60" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T60" s="32">
         <v>0.8</v>
@@ -11519,7 +11877,7 @@
       <c r="Q61" s="27"/>
       <c r="R61" s="27"/>
       <c r="S61" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T61" s="32">
         <v>0.8</v>
@@ -11556,7 +11914,7 @@
       <c r="Q62" s="27"/>
       <c r="R62" s="27"/>
       <c r="S62" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T62" s="27">
         <v>0</v>
@@ -11591,7 +11949,7 @@
       <c r="Q63" s="27"/>
       <c r="R63" s="27"/>
       <c r="S63" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T63" s="32">
         <v>0.8</v>
@@ -11609,7 +11967,7 @@
     <row r="66" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
@@ -11631,12 +11989,12 @@
       <c r="S67" s="14"/>
       <c r="T67" s="14"/>
       <c r="Y67" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z67" s="21"/>
       <c r="AA67" s="21"/>
       <c r="AB67" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC67" s="21"/>
     </row>
@@ -11699,17 +12057,17 @@
         <v>34</v>
       </c>
       <c r="Y68" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z68" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA68" s="21"/>
       <c r="AB68" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC68" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:29" x14ac:dyDescent="0.25">
@@ -11735,7 +12093,7 @@
       <c r="Q69" s="27"/>
       <c r="R69" s="27"/>
       <c r="S69" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T69" s="32">
         <v>0.3</v>
@@ -11772,7 +12130,7 @@
       <c r="Q70" s="27"/>
       <c r="R70" s="27"/>
       <c r="S70" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T70" s="27">
         <v>0</v>
@@ -11807,7 +12165,7 @@
       <c r="Q71" s="27"/>
       <c r="R71" s="27"/>
       <c r="S71" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T71" s="27">
         <v>0</v>
@@ -11842,7 +12200,7 @@
       <c r="Q72" s="27"/>
       <c r="R72" s="27"/>
       <c r="S72" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T72" s="32">
         <v>0.3</v>
@@ -11879,7 +12237,7 @@
       <c r="Q73" s="27"/>
       <c r="R73" s="27"/>
       <c r="S73" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T73" s="32">
         <v>0.3</v>
@@ -11916,7 +12274,7 @@
       <c r="Q74" s="27"/>
       <c r="R74" s="27"/>
       <c r="S74" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T74" s="32">
         <v>0.3</v>
@@ -11944,7 +12302,7 @@
   <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11954,7 +12312,7 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -11975,6 +12333,17 @@
       <c r="R1" s="16"/>
       <c r="S1" s="16"/>
       <c r="T1" s="16"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC1" s="21"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
@@ -12030,6 +12399,23 @@
       <c r="S2" s="16"/>
       <c r="T2" s="17" t="s">
         <v>0</v>
+      </c>
+      <c r="W2" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z2" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC2" s="21" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
@@ -12055,11 +12441,18 @@
       <c r="Q3" s="27"/>
       <c r="R3" s="27"/>
       <c r="S3" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T3" s="27">
         <v>0</v>
       </c>
+      <c r="W3" s="27"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="32"/>
+      <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
@@ -12084,11 +12477,18 @@
       <c r="Q4" s="27"/>
       <c r="R4" s="27"/>
       <c r="S4" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T4" s="27">
         <v>0</v>
       </c>
+      <c r="W4" s="27"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="32"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="32"/>
+      <c r="AC4" s="32"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -12113,11 +12513,18 @@
       <c r="Q5" s="27"/>
       <c r="R5" s="27"/>
       <c r="S5" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T5" s="27">
         <v>0</v>
       </c>
+      <c r="W5" s="27"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="32"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="32"/>
+      <c r="AC5" s="32"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
@@ -12142,11 +12549,18 @@
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
       <c r="S6" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T6" s="27">
         <v>0</v>
       </c>
+      <c r="W6" s="27"/>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="32"/>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="32"/>
+      <c r="AC6" s="32"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
@@ -12171,11 +12585,18 @@
       <c r="Q7" s="27"/>
       <c r="R7" s="27"/>
       <c r="S7" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T7" s="27">
         <v>0</v>
       </c>
+      <c r="W7" s="27"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="32"/>
+      <c r="Z7" s="32"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="32"/>
+      <c r="AC7" s="32"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
@@ -12200,17 +12621,24 @@
       <c r="Q8" s="27"/>
       <c r="R8" s="27"/>
       <c r="S8" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T8" s="27">
         <v>400</v>
       </c>
+      <c r="W8" s="27"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="32"/>
+      <c r="Z8" s="32"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="32"/>
+      <c r="AC8" s="32"/>
     </row>
     <row r="10" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -12233,12 +12661,12 @@
       <c r="T12" s="16"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z12" s="21"/>
       <c r="AA12" s="21"/>
       <c r="AB12" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC12" s="21"/>
     </row>
@@ -12301,17 +12729,17 @@
         <v>34</v>
       </c>
       <c r="Y13" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z13" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA13" s="21"/>
       <c r="AB13" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC13" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -12344,11 +12772,11 @@
       <c r="Q14" s="27"/>
       <c r="R14" s="27"/>
       <c r="S14" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T14" s="27"/>
       <c r="W14" s="27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Y14" s="32">
         <v>0</v>
@@ -12368,7 +12796,7 @@
     <row r="17" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -12390,12 +12818,12 @@
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
       <c r="Y18" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z18" s="21"/>
       <c r="AA18" s="21"/>
       <c r="AB18" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AC18" s="21"/>
     </row>
@@ -12458,17 +12886,17 @@
         <v>34</v>
       </c>
       <c r="Y19" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z19" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA19" s="21"/>
       <c r="AB19" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC19" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
@@ -12478,17 +12906,17 @@
       </c>
       <c r="C20" s="34"/>
       <c r="D20" s="34">
-        <v>250</v>
+        <v>0.03</v>
       </c>
       <c r="E20" s="34"/>
       <c r="F20" s="34">
-        <v>1000</v>
+        <v>0.05</v>
       </c>
       <c r="G20" s="34"/>
       <c r="H20" s="34"/>
       <c r="I20" s="34"/>
       <c r="J20" s="34">
-        <v>2000</v>
+        <v>0.08</v>
       </c>
       <c r="K20" s="34"/>
       <c r="L20" s="34"/>
@@ -12499,11 +12927,11 @@
       <c r="Q20" s="34"/>
       <c r="R20" s="34"/>
       <c r="S20" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T20" s="27"/>
       <c r="W20" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Y20" s="32">
         <v>0</v>
@@ -12520,7 +12948,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12539,7 +12966,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -12843,7 +13270,7 @@
     <row r="11" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -13140,7 +13567,7 @@
     <row r="22" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -13299,7 +13726,7 @@
     <row r="33" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>

</xml_diff>

<commit_message>
trying to figure out what map lambda was before
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="13545" tabRatio="863" activeTab="10"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="13545" tabRatio="863" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="146">
   <si>
     <t>Assumption</t>
   </si>
@@ -284,12 +284,6 @@
   </si>
   <si>
     <t>Populations</t>
-  </si>
-  <si>
-    <t>lower</t>
-  </si>
-  <si>
-    <t>upper</t>
   </si>
   <si>
     <t>Min</t>
@@ -2534,7 +2528,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2685,7 +2679,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2811,8 +2805,8 @@
   <sheetPr published="0"/>
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2824,7 +2818,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2890,7 +2884,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C8" s="32">
         <v>0.05</v>
@@ -2900,7 +2894,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C9" s="32">
         <v>0.03</v>
@@ -2920,7 +2914,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2996,7 +2990,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B23" s="22"/>
     </row>
@@ -3063,7 +3057,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3122,7 +3116,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3168,7 +3162,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3264,7 +3258,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -3369,7 +3363,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -3391,7 +3385,7 @@
     </row>
     <row r="3" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C3" s="31">
         <v>0.05</v>
@@ -3474,7 +3468,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -3551,7 +3545,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -3644,7 +3638,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -3750,7 +3744,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -3856,7 +3850,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
@@ -3962,7 +3956,7 @@
     </row>
     <row r="19" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4048,7 +4042,7 @@
     <row r="24" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4131,7 +4125,7 @@
     </row>
     <row r="31" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4217,7 +4211,7 @@
     <row r="36" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4303,7 +4297,7 @@
     <row r="42" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4386,7 +4380,7 @@
     </row>
     <row r="49" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4472,7 +4466,7 @@
     <row r="54" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4903,12 +4897,12 @@
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="24"/>
       <c r="K13" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -5195,7 +5189,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -5475,7 +5469,9 @@
   <sheetPr published="0"/>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5545,7 +5541,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C3" s="21" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
@@ -5609,7 +5605,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C5" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
@@ -5634,7 +5630,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C7" s="21" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
@@ -5694,7 +5690,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C9" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
@@ -5719,7 +5715,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C11" s="21" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
@@ -5777,7 +5773,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C13" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
@@ -5802,7 +5798,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C15" s="21" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
@@ -5858,7 +5854,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C17" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
@@ -5883,7 +5879,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C19" s="21" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
@@ -5939,7 +5935,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C21" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
@@ -5964,7 +5960,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C23" s="21" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -6020,7 +6016,7 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C25" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -6045,7 +6041,7 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -6103,7 +6099,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C31" s="21" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
@@ -6161,7 +6157,7 @@
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C33" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
@@ -6188,7 +6184,7 @@
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C35" s="21" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
@@ -6246,7 +6242,7 @@
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C37" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
@@ -6273,7 +6269,7 @@
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C39" s="21" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D39" s="27"/>
       <c r="E39" s="27"/>
@@ -6331,7 +6327,7 @@
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C41" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
@@ -6358,7 +6354,7 @@
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C43" s="21" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
@@ -6416,7 +6412,7 @@
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C45" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
@@ -6443,7 +6439,7 @@
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C47" s="21" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
@@ -6501,7 +6497,7 @@
     </row>
     <row r="49" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C49" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D49" s="27"/>
       <c r="E49" s="27"/>
@@ -6528,7 +6524,7 @@
     </row>
     <row r="51" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C51" s="21" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D51" s="27"/>
       <c r="E51" s="27"/>
@@ -6586,7 +6582,7 @@
     </row>
     <row r="53" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C53" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D53" s="27"/>
       <c r="E53" s="27"/>
@@ -6635,14 +6631,14 @@
   <sheetData>
     <row r="1" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="X1" s="3"/>
       <c r="Y1" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AB1" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -6701,16 +6697,16 @@
         <v>33</v>
       </c>
       <c r="Y2" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AB2" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC2" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -6916,7 +6912,7 @@
     <row r="11" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -6941,10 +6937,10 @@
       <c r="W12" s="21"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AB12" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
@@ -7007,16 +7003,16 @@
       </c>
       <c r="X13" s="21"/>
       <c r="Y13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AB13" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC13" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -7294,14 +7290,14 @@
     <row r="22" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="X23" s="3"/>
       <c r="Y23" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AB23" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -7360,16 +7356,16 @@
         <v>33</v>
       </c>
       <c r="Y24" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z24" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AB24" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC24" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -7665,12 +7661,12 @@
       <c r="W34" s="21"/>
       <c r="X34" s="3"/>
       <c r="Y34" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z34" s="21"/>
       <c r="AA34" s="21"/>
       <c r="AB34" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC34" s="21"/>
     </row>
@@ -7734,17 +7730,17 @@
       </c>
       <c r="X35" s="21"/>
       <c r="Y35" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z35" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA35" s="21"/>
       <c r="AB35" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC35" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
@@ -8199,7 +8195,7 @@
     <row r="12" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -8307,7 +8303,7 @@
     <row r="18" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -8503,7 +8499,7 @@
     </row>
     <row r="31" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -8605,7 +8601,7 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -8627,12 +8623,12 @@
       <c r="S1" s="12"/>
       <c r="T1" s="12"/>
       <c r="Y1" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z1" s="21"/>
       <c r="AA1" s="21"/>
       <c r="AB1" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC1" s="21"/>
     </row>
@@ -8695,17 +8691,17 @@
         <v>33</v>
       </c>
       <c r="Y2" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA2" s="21"/>
       <c r="AB2" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC2" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
@@ -8984,7 +8980,7 @@
     <row r="11" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -9006,12 +9002,12 @@
       <c r="S12" s="12"/>
       <c r="T12" s="12"/>
       <c r="Y12" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z12" s="21"/>
       <c r="AA12" s="21"/>
       <c r="AB12" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC12" s="21"/>
     </row>
@@ -9074,17 +9070,17 @@
         <v>33</v>
       </c>
       <c r="Y13" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z13" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA13" s="21"/>
       <c r="AB13" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC13" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -9134,7 +9130,7 @@
     <row r="17" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -9156,12 +9152,12 @@
       <c r="S18" s="12"/>
       <c r="T18" s="12"/>
       <c r="Y18" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z18" s="21"/>
       <c r="AA18" s="21"/>
       <c r="AB18" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC18" s="21"/>
     </row>
@@ -9224,17 +9220,17 @@
         <v>33</v>
       </c>
       <c r="Y19" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z19" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA19" s="21"/>
       <c r="AB19" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC19" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
@@ -9288,7 +9284,7 @@
     <row r="22" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -9310,12 +9306,12 @@
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
       <c r="Y24" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z24" s="21"/>
       <c r="AA24" s="21"/>
       <c r="AB24" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC24" s="21"/>
     </row>
@@ -9378,17 +9374,17 @@
         <v>33</v>
       </c>
       <c r="Y25" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z25" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA25" s="21"/>
       <c r="AB25" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC25" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
@@ -9443,7 +9439,7 @@
     <row r="29" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -9465,12 +9461,12 @@
       <c r="S30" s="12"/>
       <c r="T30" s="12"/>
       <c r="Y30" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z30" s="21"/>
       <c r="AA30" s="21"/>
       <c r="AB30" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC30" s="21"/>
     </row>
@@ -9533,17 +9529,17 @@
         <v>33</v>
       </c>
       <c r="Y31" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z31" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA31" s="21"/>
       <c r="AB31" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC31" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
@@ -9595,13 +9591,13 @@
     <row r="35" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Y36" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AB36" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -9660,16 +9656,16 @@
         <v>33</v>
       </c>
       <c r="Y37" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z37" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AB37" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC37" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -9864,13 +9860,13 @@
     </row>
     <row r="47" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="Y47" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AB47" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -9929,16 +9925,16 @@
         <v>33</v>
       </c>
       <c r="Y48" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z48" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AB48" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC48" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="2:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -9994,7 +9990,7 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -10016,12 +10012,12 @@
       <c r="S1" s="14"/>
       <c r="T1" s="14"/>
       <c r="Y1" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z1" s="21"/>
       <c r="AA1" s="21"/>
       <c r="AB1" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC1" s="21"/>
     </row>
@@ -10084,17 +10080,17 @@
         <v>33</v>
       </c>
       <c r="Y2" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA2" s="21"/>
       <c r="AB2" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC2" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
@@ -10311,7 +10307,7 @@
     <row r="11" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -10333,12 +10329,12 @@
       <c r="S12" s="14"/>
       <c r="T12" s="14"/>
       <c r="Y12" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z12" s="21"/>
       <c r="AA12" s="21"/>
       <c r="AB12" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC12" s="21"/>
     </row>
@@ -10401,17 +10397,17 @@
         <v>33</v>
       </c>
       <c r="Y13" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z13" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA13" s="21"/>
       <c r="AB13" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC13" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -10634,7 +10630,7 @@
     <row r="22" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -10656,12 +10652,12 @@
       <c r="S23" s="14"/>
       <c r="T23" s="14"/>
       <c r="Y23" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z23" s="21"/>
       <c r="AA23" s="21"/>
       <c r="AB23" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC23" s="21"/>
     </row>
@@ -10724,17 +10720,17 @@
         <v>33</v>
       </c>
       <c r="Y24" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z24" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA24" s="21"/>
       <c r="AB24" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC24" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
@@ -10957,7 +10953,7 @@
     <row r="33" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -10979,12 +10975,12 @@
       <c r="S34" s="14"/>
       <c r="T34" s="14"/>
       <c r="Y34" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z34" s="21"/>
       <c r="AA34" s="21"/>
       <c r="AB34" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC34" s="21"/>
     </row>
@@ -11047,17 +11043,17 @@
         <v>33</v>
       </c>
       <c r="Y35" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z35" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA35" s="21"/>
       <c r="AB35" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC35" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
@@ -11292,7 +11288,7 @@
     <row r="44" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -11314,12 +11310,12 @@
       <c r="S45" s="14"/>
       <c r="T45" s="14"/>
       <c r="Y45" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z45" s="21"/>
       <c r="AA45" s="21"/>
       <c r="AB45" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC45" s="21"/>
     </row>
@@ -11382,17 +11378,17 @@
         <v>33</v>
       </c>
       <c r="Y46" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z46" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA46" s="21"/>
       <c r="AB46" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC46" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.25">
@@ -11621,7 +11617,7 @@
     <row r="55" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
@@ -11643,12 +11639,12 @@
       <c r="S56" s="14"/>
       <c r="T56" s="14"/>
       <c r="Y56" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z56" s="21"/>
       <c r="AA56" s="21"/>
       <c r="AB56" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC56" s="21"/>
     </row>
@@ -11711,17 +11707,17 @@
         <v>33</v>
       </c>
       <c r="Y57" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z57" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA57" s="21"/>
       <c r="AB57" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC57" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.25">
@@ -11944,7 +11940,7 @@
     <row r="66" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
@@ -11966,12 +11962,12 @@
       <c r="S67" s="14"/>
       <c r="T67" s="14"/>
       <c r="Y67" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z67" s="21"/>
       <c r="AA67" s="21"/>
       <c r="AB67" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC67" s="21"/>
     </row>
@@ -12034,17 +12030,17 @@
         <v>33</v>
       </c>
       <c r="Y68" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z68" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA68" s="21"/>
       <c r="AB68" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC68" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="69" spans="1:29" x14ac:dyDescent="0.25">
@@ -12287,7 +12283,7 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -12311,12 +12307,12 @@
       <c r="W1" s="21"/>
       <c r="X1" s="21"/>
       <c r="Y1" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z1" s="21"/>
       <c r="AA1" s="21"/>
       <c r="AB1" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC1" s="21"/>
     </row>
@@ -12380,17 +12376,17 @@
       </c>
       <c r="X2" s="21"/>
       <c r="Y2" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA2" s="21"/>
       <c r="AB2" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC2" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
@@ -12613,7 +12609,7 @@
     <row r="11" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -12636,12 +12632,12 @@
       <c r="T12" s="16"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z12" s="21"/>
       <c r="AA12" s="21"/>
       <c r="AB12" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC12" s="21"/>
     </row>
@@ -12704,17 +12700,17 @@
         <v>33</v>
       </c>
       <c r="Y13" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z13" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA13" s="21"/>
       <c r="AB13" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC13" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -12771,7 +12767,7 @@
     <row r="17" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -12793,12 +12789,12 @@
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
       <c r="Y18" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z18" s="21"/>
       <c r="AA18" s="21"/>
       <c r="AB18" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AC18" s="21"/>
     </row>
@@ -12861,17 +12857,17 @@
         <v>33</v>
       </c>
       <c r="Y19" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z19" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA19" s="21"/>
       <c r="AB19" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC19" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
@@ -12942,7 +12938,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -13246,7 +13242,7 @@
     <row r="11" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -13543,7 +13539,7 @@
     <row r="22" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -13702,7 +13698,7 @@
     <row r="33" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>

</xml_diff>

<commit_message>
reads in spreadsheet now
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="13545" tabRatio="863" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="13545" tabRatio="863" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="146">
   <si>
     <t>Assumption</t>
   </si>
@@ -473,10 +473,17 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -597,728 +604,731 @@
   </borders>
   <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="655"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="655" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="655"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="655" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="655"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="655" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="655"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="655" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="11" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="11" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="662" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="662" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="662" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="662" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -5469,8 +5479,8 @@
   <sheetPr published="0"/>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5540,6 +5550,10 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>GM</v>
+      </c>
       <c r="C3" s="21" t="s">
         <v>11</v>
       </c>
@@ -5592,9 +5606,15 @@
       <c r="O4" s="29">
         <v>2600000</v>
       </c>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
+      <c r="P4" s="29">
+        <v>2700000</v>
+      </c>
+      <c r="Q4" s="29">
+        <v>2800000</v>
+      </c>
+      <c r="R4" s="29">
+        <v>2900000</v>
+      </c>
       <c r="S4" s="29">
         <v>3000000</v>
       </c>
@@ -5604,6 +5624,10 @@
       <c r="U4" s="33"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>GM</v>
+      </c>
       <c r="C5" s="21" t="s">
         <v>10</v>
       </c>
@@ -5629,6 +5653,10 @@
       <c r="U5" s="33"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>GF</v>
+      </c>
       <c r="C7" s="21" t="s">
         <v>11</v>
       </c>
@@ -5689,6 +5717,10 @@
       <c r="U8" s="33"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>GF</v>
+      </c>
       <c r="C9" s="21" t="s">
         <v>10</v>
       </c>
@@ -5714,6 +5746,10 @@
       <c r="U9" s="33"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>FSW</v>
+      </c>
       <c r="C11" s="21" t="s">
         <v>11</v>
       </c>
@@ -5772,6 +5808,10 @@
       <c r="U12" s="33"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>FSW</v>
+      </c>
       <c r="C13" s="21" t="s">
         <v>10</v>
       </c>
@@ -5797,6 +5837,10 @@
       <c r="U13" s="33"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>CSW</v>
+      </c>
       <c r="C15" s="21" t="s">
         <v>11</v>
       </c>
@@ -5853,6 +5897,10 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>CSW</v>
+      </c>
       <c r="C17" s="21" t="s">
         <v>10</v>
       </c>
@@ -5878,6 +5926,10 @@
       <c r="U17" s="33"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>MSM</v>
+      </c>
       <c r="C19" s="21" t="s">
         <v>11</v>
       </c>
@@ -5934,6 +5986,10 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>MSM</v>
+      </c>
       <c r="C21" s="21" t="s">
         <v>10</v>
       </c>
@@ -5959,6 +6015,10 @@
       <c r="U21" s="33"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$8</f>
+        <v>PWID</v>
+      </c>
       <c r="C23" s="21" t="s">
         <v>11</v>
       </c>
@@ -6015,6 +6075,10 @@
       <c r="U24" s="33"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$8</f>
+        <v>PWID</v>
+      </c>
       <c r="C25" s="21" t="s">
         <v>10</v>
       </c>
@@ -6098,6 +6162,10 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>GM</v>
+      </c>
       <c r="C31" s="21" t="s">
         <v>11</v>
       </c>
@@ -6156,6 +6224,10 @@
       </c>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B33" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>GM</v>
+      </c>
       <c r="C33" s="21" t="s">
         <v>10</v>
       </c>
@@ -6183,6 +6255,10 @@
       </c>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B35" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>GF</v>
+      </c>
       <c r="C35" s="21" t="s">
         <v>11</v>
       </c>
@@ -6241,6 +6317,10 @@
       </c>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B37" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>GF</v>
+      </c>
       <c r="C37" s="21" t="s">
         <v>10</v>
       </c>
@@ -6268,6 +6348,10 @@
       </c>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B39" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>FSW</v>
+      </c>
       <c r="C39" s="21" t="s">
         <v>11</v>
       </c>
@@ -6326,6 +6410,10 @@
       </c>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B41" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>FSW</v>
+      </c>
       <c r="C41" s="21" t="s">
         <v>10</v>
       </c>
@@ -6353,6 +6441,10 @@
       </c>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B43" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>CSW</v>
+      </c>
       <c r="C43" s="21" t="s">
         <v>11</v>
       </c>
@@ -6411,6 +6503,10 @@
       </c>
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B45" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>CSW</v>
+      </c>
       <c r="C45" s="21" t="s">
         <v>10</v>
       </c>
@@ -6438,6 +6534,10 @@
       </c>
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B47" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>MSM</v>
+      </c>
       <c r="C47" s="21" t="s">
         <v>11</v>
       </c>
@@ -6496,6 +6596,10 @@
       </c>
     </row>
     <row r="49" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B49" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>MSM</v>
+      </c>
       <c r="C49" s="21" t="s">
         <v>10</v>
       </c>
@@ -6523,6 +6627,10 @@
       </c>
     </row>
     <row r="51" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B51" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$8</f>
+        <v>PWID</v>
+      </c>
       <c r="C51" s="21" t="s">
         <v>11</v>
       </c>
@@ -6581,6 +6689,10 @@
       </c>
     </row>
     <row r="53" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B53" s="22" t="str">
+        <f>'Populations &amp; programs'!$C$8</f>
+        <v>PWID</v>
+      </c>
       <c r="C53" s="21" t="s">
         <v>10</v>
       </c>
@@ -6619,8 +6731,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AC42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6714,8 +6826,12 @@
         <f>'Populations &amp; programs'!$C$3</f>
         <v>GM</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
+      <c r="C3" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="D3" s="32">
+        <v>0.01</v>
+      </c>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
@@ -6728,19 +6844,31 @@
       <c r="N3" s="27"/>
       <c r="O3" s="27"/>
       <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
+      <c r="Q3" s="32">
+        <v>0.02</v>
+      </c>
+      <c r="R3" s="32">
+        <v>0.02</v>
+      </c>
       <c r="S3" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="T3" s="32">
+      <c r="T3" s="32"/>
+      <c r="W3" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y3" s="32">
         <v>0.01</v>
       </c>
-      <c r="W3" s="27"/>
-      <c r="Y3" s="32"/>
-      <c r="Z3" s="32"/>
-      <c r="AB3" s="32"/>
-      <c r="AC3" s="32"/>
+      <c r="Z3" s="32">
+        <v>0.02</v>
+      </c>
+      <c r="AB3" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="AC3" s="32">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="4" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="str">
@@ -7958,7 +8086,7 @@
       <c r="S42" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -9971,7 +10099,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12263,7 +12391,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -12920,7 +13048,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
adding population metadata but spreadsheet keeps getting overwritten
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="40" windowWidth="19420" windowHeight="10960" tabRatio="863" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Disutilities &amp; costs" sheetId="14" r:id="rId12"/>
     <sheet name="Macroeconomics" sheetId="18" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="130000"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="146">
   <si>
     <t>Men who have sex with men</t>
   </si>
@@ -464,21 +464,39 @@
   <si>
     <t>Modeled estimate of HIV prevalence</t>
   </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Injects</t>
+  </si>
+  <si>
+    <t>Heterosexual</t>
+  </si>
+  <si>
+    <t>Homosexual</t>
+  </si>
+  <si>
+    <t>Sex worker</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="171" formatCode="0.00%"/>
-    <numFmt numFmtId="172" formatCode="0.00000%"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -640,7 +658,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -1288,11 +1306,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
@@ -1325,104 +1343,105 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="11" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="11" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="10" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="662" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="662" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="662" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="655" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1"/>
-    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="13"/>
@@ -2394,39 +2413,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="22"/>
+    <col min="1" max="1" width="9.140625" style="22"/>
     <col min="2" max="2" width="5" style="22" customWidth="1"/>
-    <col min="3" max="3" width="13.875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="40.875" style="22" customWidth="1"/>
-    <col min="5" max="16384" width="9.125" style="22"/>
+    <col min="3" max="3" width="13.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" style="22" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="22"/>
+    <col min="8" max="9" width="14.28515625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="22" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" s="23" t="s">
         <v>95</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="E2" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="23">
         <v>1</v>
       </c>
@@ -2436,10 +2477,29 @@
       <c r="D3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="23">
         <v>2</v>
       </c>
@@ -2449,10 +2509,29 @@
       <c r="D4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="E4" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="23">
         <v>3</v>
       </c>
@@ -2462,10 +2541,29 @@
       <c r="D5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="E5" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="23">
         <v>4</v>
       </c>
@@ -2475,10 +2573,29 @@
       <c r="D6" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="E6" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="23">
         <v>5</v>
       </c>
@@ -2488,10 +2605,29 @@
       <c r="D7" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="23">
         <v>6</v>
       </c>
@@ -2501,25 +2637,44 @@
       <c r="D8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="E8" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="23"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="23"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="23"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>91</v>
       </c>
       <c r="B12" s="23"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="23"/>
       <c r="C13" s="23" t="s">
         <v>95</v>
@@ -2528,7 +2683,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="23">
         <v>1</v>
       </c>
@@ -2539,7 +2694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="23">
         <v>2</v>
       </c>
@@ -2550,7 +2705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="23">
         <v>3</v>
       </c>
@@ -2561,7 +2716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="23">
         <v>4</v>
       </c>
@@ -2572,7 +2727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="23">
         <v>5</v>
       </c>
@@ -2583,7 +2738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="23">
         <v>6</v>
       </c>
@@ -2594,7 +2749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="23">
         <v>7</v>
       </c>
@@ -2605,7 +2760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="23">
         <v>8</v>
       </c>
@@ -2616,7 +2771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="23">
         <v>9</v>
       </c>
@@ -2630,7 +2785,7 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2640,7 +2795,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z19"/>
   <sheetViews>
@@ -2648,12 +2803,12 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="7"/>
+    <col min="2" max="2" width="8.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -2665,7 +2820,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:26" s="7" customFormat="1">
+    <row r="2" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43"/>
       <c r="B2" s="43"/>
       <c r="C2" s="5" t="str">
@@ -2693,7 +2848,7 @@
         <v>CSW</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -2705,7 +2860,7 @@
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -2717,7 +2872,7 @@
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>PWID</v>
@@ -2729,7 +2884,7 @@
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>GM</v>
@@ -2741,7 +2896,7 @@
       <c r="G6" s="26"/>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>GF</v>
@@ -2753,7 +2908,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>CSW</v>
@@ -2765,7 +2920,7 @@
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:26" s="19" customFormat="1">
+    <row r="9" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="43"/>
       <c r="C9" s="17"/>
@@ -2793,10 +2948,10 @@
       <c r="Y9" s="17"/>
       <c r="Z9" s="17"/>
     </row>
-    <row r="10" spans="1:26" s="19" customFormat="1">
+    <row r="10" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="43"/>
       <c r="C11" s="3"/>
@@ -2806,7 +2961,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>47</v>
       </c>
@@ -2818,7 +2973,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:26" s="7" customFormat="1">
+    <row r="13" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="43"/>
       <c r="B13" s="43"/>
       <c r="C13" s="5" t="str">
@@ -2846,7 +3001,7 @@
         <v>CSW</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -2858,7 +3013,7 @@
       <c r="G14" s="26"/>
       <c r="H14" s="26"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -2870,7 +3025,7 @@
       <c r="G15" s="26"/>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>PWID</v>
@@ -2882,7 +3037,7 @@
       <c r="G16" s="26"/>
       <c r="H16" s="26"/>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>GM</v>
@@ -2894,7 +3049,7 @@
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>GF</v>
@@ -2906,7 +3061,7 @@
       <c r="G18" s="26"/>
       <c r="H18" s="26"/>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>CSW</v>
@@ -2930,7 +3085,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H67"/>
   <sheetViews>
@@ -2938,19 +3093,19 @@
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="19"/>
-    <col min="2" max="2" width="33.25" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="9.125" style="19"/>
+    <col min="1" max="1" width="9.140625" style="19"/>
+    <col min="2" max="2" width="33.28515625" style="19" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1">
+    <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
         <v>83</v>
       </c>
@@ -2961,7 +3116,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>79</v>
       </c>
@@ -2971,7 +3126,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>80</v>
       </c>
@@ -2981,7 +3136,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
         <v>81</v>
       </c>
@@ -2991,7 +3146,7 @@
       <c r="D5" s="24"/>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>82</v>
       </c>
@@ -3001,7 +3156,7 @@
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
         <v>78</v>
       </c>
@@ -3011,7 +3166,7 @@
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>122</v>
       </c>
@@ -3021,7 +3176,7 @@
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>123</v>
       </c>
@@ -3031,7 +3186,7 @@
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
@@ -3041,12 +3196,12 @@
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="7" customFormat="1">
+    <row r="14" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
         <v>83</v>
       </c>
@@ -3057,7 +3212,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="20" t="s">
         <v>86</v>
       </c>
@@ -3067,7 +3222,7 @@
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="20" t="s">
         <v>57</v>
       </c>
@@ -3077,7 +3232,7 @@
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="20" t="s">
         <v>48</v>
       </c>
@@ -3087,7 +3242,7 @@
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="20" t="s">
         <v>49</v>
       </c>
@@ -3097,7 +3252,7 @@
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="20" t="s">
         <v>59</v>
       </c>
@@ -3107,7 +3262,7 @@
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -3117,13 +3272,13 @@
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>121</v>
       </c>
       <c r="B23" s="20"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C24" s="5" t="s">
         <v>83</v>
       </c>
@@ -3134,7 +3289,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="20" t="s">
         <v>50</v>
       </c>
@@ -3144,7 +3299,7 @@
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="20" t="s">
         <v>48</v>
       </c>
@@ -3154,7 +3309,7 @@
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="20" t="s">
         <v>51</v>
       </c>
@@ -3164,7 +3319,7 @@
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
         <v>60</v>
       </c>
@@ -3174,7 +3329,7 @@
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -3184,12 +3339,12 @@
       <c r="G31" s="17"/>
       <c r="H31" s="17"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" s="5" t="s">
         <v>83</v>
       </c>
@@ -3200,7 +3355,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="20" t="s">
         <v>52</v>
       </c>
@@ -3210,7 +3365,7 @@
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" s="20" t="s">
         <v>53</v>
       </c>
@@ -3220,7 +3375,7 @@
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="20" t="s">
         <v>54</v>
       </c>
@@ -3230,10 +3385,10 @@
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="20"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -3243,12 +3398,12 @@
       <c r="G39" s="17"/>
       <c r="H39" s="17"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="5" t="s">
         <v>83</v>
       </c>
@@ -3259,7 +3414,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" s="20" t="s">
         <v>55</v>
       </c>
@@ -3273,7 +3428,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="20" t="s">
         <v>56</v>
       </c>
@@ -3287,7 +3442,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="17"/>
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
@@ -3297,12 +3452,12 @@
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C48" s="5" t="s">
         <v>83</v>
       </c>
@@ -3313,7 +3468,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" s="20" t="s">
         <v>86</v>
       </c>
@@ -3323,7 +3478,7 @@
       <c r="D49" s="24"/>
       <c r="E49" s="24"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B50" s="20" t="s">
         <v>57</v>
       </c>
@@ -3333,7 +3488,7 @@
       <c r="D50" s="24"/>
       <c r="E50" s="24"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B51" s="20" t="s">
         <v>58</v>
       </c>
@@ -3343,7 +3498,7 @@
       <c r="D51" s="24"/>
       <c r="E51" s="24"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="20" t="s">
         <v>49</v>
       </c>
@@ -3353,7 +3508,7 @@
       <c r="D52" s="24"/>
       <c r="E52" s="24"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" s="20" t="s">
         <v>59</v>
       </c>
@@ -3363,7 +3518,7 @@
       <c r="D53" s="24"/>
       <c r="E53" s="24"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" s="20" t="s">
         <v>87</v>
       </c>
@@ -3373,7 +3528,7 @@
       <c r="D54" s="24"/>
       <c r="E54" s="24"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="20" t="s">
         <v>98</v>
       </c>
@@ -3383,7 +3538,7 @@
       <c r="D55" s="24"/>
       <c r="E55" s="24"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="17"/>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
@@ -3393,12 +3548,12 @@
       <c r="G58" s="17"/>
       <c r="H58" s="17"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C60" s="5" t="s">
         <v>83</v>
       </c>
@@ -3409,7 +3564,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" s="20" t="s">
         <v>37</v>
       </c>
@@ -3419,7 +3574,7 @@
       <c r="D61" s="24"/>
       <c r="E61" s="24"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" s="20" t="s">
         <v>88</v>
       </c>
@@ -3429,7 +3584,7 @@
       <c r="D62" s="24"/>
       <c r="E62" s="24"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B63" s="20" t="s">
         <v>99</v>
       </c>
@@ -3439,7 +3594,7 @@
       <c r="D63" s="24"/>
       <c r="E63" s="24"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" s="20" t="s">
         <v>89</v>
       </c>
@@ -3449,7 +3604,7 @@
       <c r="D64" s="24"/>
       <c r="E64" s="24"/>
     </row>
-    <row r="65" spans="2:5">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="20" t="s">
         <v>38</v>
       </c>
@@ -3459,7 +3614,7 @@
       <c r="D65" s="24"/>
       <c r="E65" s="24"/>
     </row>
-    <row r="66" spans="2:5">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="20" t="s">
         <v>90</v>
       </c>
@@ -3469,7 +3624,7 @@
       <c r="D66" s="24"/>
       <c r="E66" s="24"/>
     </row>
-    <row r="67" spans="2:5">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="20" t="s">
         <v>39</v>
       </c>
@@ -3491,7 +3646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
@@ -3499,12 +3654,12 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>128</v>
       </c>
@@ -3513,7 +3668,7 @@
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="19"/>
       <c r="C2" s="5" t="s">
@@ -3526,7 +3681,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="19" customFormat="1">
+    <row r="3" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>127</v>
       </c>
@@ -3536,7 +3691,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4" s="20" t="s">
         <v>61</v>
@@ -3547,7 +3702,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5" s="20" t="s">
         <v>62</v>
@@ -3558,7 +3713,7 @@
       <c r="D5" s="24"/>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6" s="20" t="s">
         <v>63</v>
@@ -3569,7 +3724,7 @@
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="20" t="s">
         <v>64</v>
@@ -3580,7 +3735,7 @@
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8" s="20" t="s">
         <v>102</v>
@@ -3591,15 +3746,15 @@
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
     </row>
-    <row r="10" spans="1:8" s="19" customFormat="1"/>
-    <row r="11" spans="1:8" s="19" customFormat="1">
+    <row r="10" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -3609,7 +3764,7 @@
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>126</v>
       </c>
@@ -3618,7 +3773,7 @@
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="5" t="s">
@@ -3631,7 +3786,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
       <c r="B14" s="20" t="s">
         <v>86</v>
@@ -3642,7 +3797,7 @@
       <c r="D14" s="24"/>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="B15" s="20" t="s">
         <v>57</v>
@@ -3653,7 +3808,7 @@
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" s="20" t="s">
         <v>58</v>
@@ -3664,7 +3819,7 @@
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="20" t="s">
         <v>49</v>
@@ -3675,7 +3830,7 @@
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="20" t="s">
         <v>59</v>
@@ -3686,7 +3841,7 @@
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>125</v>
       </c>
@@ -3695,7 +3850,7 @@
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="5" t="s">
@@ -3708,7 +3863,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="20" t="s">
         <v>86</v>
@@ -3719,7 +3874,7 @@
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="20" t="s">
         <v>57</v>
@@ -3730,7 +3885,7 @@
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="20" t="s">
         <v>58</v>
@@ -3741,7 +3896,7 @@
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="20" t="s">
         <v>49</v>
@@ -3752,7 +3907,7 @@
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="20" t="s">
         <v>59</v>
@@ -3775,7 +3930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T57"/>
   <sheetViews>
@@ -3783,15 +3938,15 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="7"/>
-    <col min="3" max="4" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="7"/>
+    <col min="3" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.25" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>112</v>
       </c>
@@ -3813,7 +3968,7 @@
       <c r="R1" s="19"/>
       <c r="S1" s="19"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="C2" s="20">
         <v>2015</v>
@@ -3868,7 +4023,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3" s="5" t="s">
         <v>93</v>
@@ -3941,7 +4096,7 @@
       </c>
       <c r="T3" s="34"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>113</v>
       </c>
@@ -3963,7 +4118,7 @@
       <c r="R7" s="19"/>
       <c r="S7" s="19"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="C8" s="20">
         <v>2015</v>
@@ -4018,7 +4173,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="5" t="s">
         <v>93</v>
@@ -4091,7 +4246,7 @@
       </c>
       <c r="T9" s="34"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>20</v>
       </c>
@@ -4113,7 +4268,7 @@
       <c r="R13" s="19"/>
       <c r="S13" s="19"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
       <c r="C14" s="20">
         <v>2015</v>
@@ -4168,7 +4323,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="B15" s="5" t="s">
         <v>93</v>
@@ -4241,14 +4396,14 @@
       </c>
       <c r="T15" s="34"/>
     </row>
-    <row r="19" spans="1:20" s="19" customFormat="1">
+    <row r="19" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="7"/>
       <c r="T19" s="7"/>
     </row>
-    <row r="20" spans="1:20" s="19" customFormat="1">
+    <row r="20" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="20">
         <v>2015</v>
@@ -4302,7 +4457,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="19" customFormat="1">
+    <row r="21" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>93</v>
       </c>
@@ -4327,27 +4482,27 @@
       </c>
       <c r="T21" s="34"/>
     </row>
-    <row r="22" spans="1:20" s="19" customFormat="1">
+    <row r="22" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="T22" s="7"/>
     </row>
-    <row r="23" spans="1:20" s="19" customFormat="1">
+    <row r="23" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="I23" s="53"/>
       <c r="T23" s="7"/>
     </row>
-    <row r="24" spans="1:20" s="19" customFormat="1">
+    <row r="24" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="T24" s="7"/>
     </row>
-    <row r="25" spans="1:20" s="19" customFormat="1">
+    <row r="25" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="7"/>
       <c r="T25" s="7"/>
     </row>
-    <row r="26" spans="1:20" s="19" customFormat="1">
+    <row r="26" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="20">
         <v>2015</v>
@@ -4401,7 +4556,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="19" customFormat="1">
+    <row r="27" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>93</v>
       </c>
@@ -4474,14 +4629,14 @@
       </c>
       <c r="T27" s="34"/>
     </row>
-    <row r="31" spans="1:20" s="19" customFormat="1">
+    <row r="31" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B31" s="7"/>
       <c r="T31" s="7"/>
     </row>
-    <row r="32" spans="1:20" s="19" customFormat="1">
+    <row r="32" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="20">
         <v>2015</v>
@@ -4535,7 +4690,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="19" customFormat="1">
+    <row r="33" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>93</v>
       </c>
@@ -4592,26 +4747,26 @@
       </c>
       <c r="T33" s="34"/>
     </row>
-    <row r="34" spans="1:20" s="19" customFormat="1">
+    <row r="34" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="T34" s="7"/>
     </row>
-    <row r="35" spans="1:20" s="19" customFormat="1">
+    <row r="35" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="T35" s="7"/>
     </row>
-    <row r="36" spans="1:20" s="19" customFormat="1">
+    <row r="36" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="T36" s="7"/>
     </row>
-    <row r="37" spans="1:20" s="19" customFormat="1">
+    <row r="37" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B37" s="7"/>
       <c r="T37" s="7"/>
     </row>
-    <row r="38" spans="1:20" s="19" customFormat="1">
+    <row r="38" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="20">
         <v>2015</v>
@@ -4665,7 +4820,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="19" customFormat="1">
+    <row r="39" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>93</v>
       </c>
@@ -4690,26 +4845,26 @@
       </c>
       <c r="T39" s="34"/>
     </row>
-    <row r="40" spans="1:20" s="19" customFormat="1">
+    <row r="40" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
       <c r="T40" s="7"/>
     </row>
-    <row r="41" spans="1:20" s="19" customFormat="1">
+    <row r="41" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
       <c r="T41" s="7"/>
     </row>
-    <row r="42" spans="1:20" s="19" customFormat="1">
+    <row r="42" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
       <c r="T42" s="7"/>
     </row>
-    <row r="43" spans="1:20" s="19" customFormat="1">
+    <row r="43" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B43" s="7"/>
       <c r="T43" s="7"/>
     </row>
-    <row r="44" spans="1:20" s="19" customFormat="1">
+    <row r="44" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
       <c r="C44" s="20">
         <v>2015</v>
@@ -4763,7 +4918,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:20" s="19" customFormat="1">
+    <row r="45" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>93</v>
       </c>
@@ -4788,14 +4943,14 @@
       </c>
       <c r="T45" s="34"/>
     </row>
-    <row r="49" spans="1:20" s="19" customFormat="1">
+    <row r="49" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>25</v>
       </c>
       <c r="B49" s="7"/>
       <c r="T49" s="7"/>
     </row>
-    <row r="50" spans="1:20" s="19" customFormat="1">
+    <row r="50" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
       <c r="C50" s="20">
         <v>2015</v>
@@ -4849,7 +5004,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:20" s="19" customFormat="1">
+    <row r="51" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>93</v>
       </c>
@@ -4874,26 +5029,26 @@
       </c>
       <c r="T51" s="34"/>
     </row>
-    <row r="52" spans="1:20" s="19" customFormat="1">
+    <row r="52" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
       <c r="T52" s="7"/>
     </row>
-    <row r="53" spans="1:20" s="19" customFormat="1">
+    <row r="53" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="7"/>
       <c r="T53" s="7"/>
     </row>
-    <row r="54" spans="1:20" s="19" customFormat="1">
+    <row r="54" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
       <c r="T54" s="7"/>
     </row>
-    <row r="55" spans="1:20" s="19" customFormat="1">
+    <row r="55" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
         <v>26</v>
       </c>
       <c r="B55" s="7"/>
       <c r="T55" s="7"/>
     </row>
-    <row r="56" spans="1:20" s="19" customFormat="1">
+    <row r="56" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
       <c r="C56" s="20">
         <v>2015</v>
@@ -4947,7 +5102,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="57" spans="1:20" s="19" customFormat="1">
+    <row r="57" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
         <v>93</v>
       </c>
@@ -4984,27 +5139,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="19" width="9.125" style="19"/>
-    <col min="20" max="20" width="15.25" style="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.125" style="19"/>
+    <col min="1" max="19" width="9.140625" style="19"/>
+    <col min="20" max="20" width="15.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C2" s="20">
         <v>2000</v>
       </c>
@@ -5057,7 +5212,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="str">
         <f>'Populations &amp; programs'!$C$14</f>
         <v>NSP</v>
@@ -5097,7 +5252,7 @@
       </c>
       <c r="T3" s="27"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="str">
         <f>'Populations &amp; programs'!$C$15</f>
         <v>OST</v>
@@ -5129,7 +5284,7 @@
       </c>
       <c r="T4" s="45"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>'Populations &amp; programs'!$C$16</f>
         <v>MSM</v>
@@ -5157,7 +5312,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="str">
         <f>'Populations &amp; programs'!$C$17</f>
         <v>FSW</v>
@@ -5193,7 +5348,7 @@
       </c>
       <c r="T6" s="27"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="str">
         <f>'Populations &amp; programs'!$C$18</f>
         <v>ART</v>
@@ -5221,7 +5376,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>'Populations &amp; programs'!$C$19</f>
         <v>HTC</v>
@@ -5249,7 +5404,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="str">
         <f>'Populations &amp; programs'!$C$20</f>
         <v>BCC</v>
@@ -5279,7 +5434,7 @@
       </c>
       <c r="T9" s="27"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="5" t="str">
         <f>'Populations &amp; programs'!$C$21</f>
@@ -5308,7 +5463,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="56" t="s">
         <v>13</v>
@@ -5336,7 +5491,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="5"/>
       <c r="C12" s="7"/>
@@ -5359,7 +5514,7 @@
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -5382,18 +5537,18 @@
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" s="21"/>
       <c r="K14" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="20">
         <v>2000</v>
@@ -5447,7 +5602,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="str">
         <f>'Populations &amp; programs'!$C$14</f>
         <v>NSP</v>
@@ -5477,7 +5632,7 @@
       </c>
       <c r="T18" s="30"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="str">
         <f>'Populations &amp; programs'!$C$15</f>
         <v>OST</v>
@@ -5507,7 +5662,7 @@
       </c>
       <c r="T19" s="30"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="str">
         <f>'Populations &amp; programs'!$C$16</f>
         <v>MSM</v>
@@ -5537,7 +5692,7 @@
       </c>
       <c r="T20" s="30"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="str">
         <f>'Populations &amp; programs'!$C$17</f>
         <v>FSW</v>
@@ -5567,7 +5722,7 @@
       </c>
       <c r="T21" s="30"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="str">
         <f>'Populations &amp; programs'!$C$18</f>
         <v>ART</v>
@@ -5597,7 +5752,7 @@
       </c>
       <c r="T22" s="30"/>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="str">
         <f>'Populations &amp; programs'!$C$19</f>
         <v>HTC</v>
@@ -5627,7 +5782,7 @@
       </c>
       <c r="T23" s="30"/>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="str">
         <f>'Populations &amp; programs'!$C$20</f>
         <v>BCC</v>
@@ -5657,7 +5812,7 @@
       </c>
       <c r="T24" s="30"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="str">
         <f>'Populations &amp; programs'!$C$21</f>
         <v>STI</v>
@@ -5687,7 +5842,7 @@
       </c>
       <c r="T25" s="30"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B26" s="56" t="s">
         <v>13</v>
       </c>
@@ -5716,20 +5871,20 @@
       </c>
       <c r="T26" s="30"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="K27" s="21" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="20">
         <v>2000</v>
@@ -5783,7 +5938,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="str">
         <f>'Populations &amp; programs'!$C$14</f>
         <v>NSP</v>
@@ -5809,7 +5964,7 @@
       </c>
       <c r="T31" s="31"/>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="str">
         <f>'Populations &amp; programs'!$C$15</f>
         <v>OST</v>
@@ -5835,7 +5990,7 @@
       </c>
       <c r="T32" s="31"/>
     </row>
-    <row r="33" spans="2:20">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="str">
         <f>'Populations &amp; programs'!$C$16</f>
         <v>MSM</v>
@@ -5861,7 +6016,7 @@
       </c>
       <c r="T33" s="31"/>
     </row>
-    <row r="34" spans="2:20">
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="str">
         <f>'Populations &amp; programs'!$C$17</f>
         <v>FSW</v>
@@ -5887,7 +6042,7 @@
       </c>
       <c r="T34" s="31"/>
     </row>
-    <row r="35" spans="2:20">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="str">
         <f>'Populations &amp; programs'!$C$18</f>
         <v>ART</v>
@@ -5913,7 +6068,7 @@
       </c>
       <c r="T35" s="31"/>
     </row>
-    <row r="36" spans="2:20">
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="str">
         <f>'Populations &amp; programs'!$C$19</f>
         <v>HTC</v>
@@ -5939,7 +6094,7 @@
       </c>
       <c r="T36" s="31"/>
     </row>
-    <row r="37" spans="2:20">
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="str">
         <f>'Populations &amp; programs'!$C$20</f>
         <v>BCC</v>
@@ -5965,7 +6120,7 @@
       </c>
       <c r="T37" s="31"/>
     </row>
-    <row r="38" spans="2:20">
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="str">
         <f>'Populations &amp; programs'!$C$21</f>
         <v>STI</v>
@@ -5991,7 +6146,7 @@
       </c>
       <c r="T38" s="30"/>
     </row>
-    <row r="39" spans="2:20">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B39" s="56" t="s">
         <v>13</v>
       </c>
@@ -6029,7 +6184,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U53"/>
   <sheetViews>
@@ -6037,22 +6192,22 @@
       <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.125" style="19"/>
-    <col min="4" max="4" width="9.375" style="19" customWidth="1"/>
-    <col min="5" max="20" width="9.125" style="19"/>
-    <col min="21" max="21" width="15.25" style="19" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.875" style="19" customWidth="1"/>
-    <col min="23" max="16384" width="9.125" style="19"/>
+    <col min="1" max="3" width="9.140625" style="19"/>
+    <col min="4" max="4" width="9.42578125" style="19" customWidth="1"/>
+    <col min="5" max="20" width="9.140625" style="19"/>
+    <col min="21" max="21" width="15.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" style="19" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D2" s="20">
         <v>2000</v>
       </c>
@@ -6105,7 +6260,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -6136,7 +6291,7 @@
         <v>37500</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -6167,7 +6322,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -6198,12 +6353,12 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="U6" s="33"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -6232,7 +6387,7 @@
       </c>
       <c r="U7" s="32"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -6263,7 +6418,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -6292,7 +6447,7 @@
       </c>
       <c r="U9" s="32"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="33"/>
@@ -6313,7 +6468,7 @@
       <c r="S10" s="33"/>
       <c r="U10" s="33"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>PWID</v>
@@ -6352,7 +6507,7 @@
       </c>
       <c r="U11" s="32"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>PWID</v>
@@ -6391,7 +6546,7 @@
       </c>
       <c r="U12" s="32"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>PWID</v>
@@ -6430,7 +6585,7 @@
       </c>
       <c r="U13" s="32"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="33"/>
@@ -6451,7 +6606,7 @@
       <c r="S14" s="33"/>
       <c r="U14" s="33"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>GM</v>
@@ -6480,7 +6635,7 @@
       </c>
       <c r="U15" s="32"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>GM</v>
@@ -6541,7 +6696,7 @@
       </c>
       <c r="U16" s="32"/>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>GM</v>
@@ -6570,7 +6725,7 @@
       </c>
       <c r="U17" s="32"/>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="33"/>
@@ -6591,7 +6746,7 @@
       <c r="S18" s="33"/>
       <c r="U18" s="33"/>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>GF</v>
@@ -6620,7 +6775,7 @@
       </c>
       <c r="U19" s="32"/>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>GF</v>
@@ -6681,7 +6836,7 @@
       </c>
       <c r="U20" s="32"/>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>GF</v>
@@ -6710,7 +6865,7 @@
       </c>
       <c r="U21" s="32"/>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="33"/>
@@ -6731,7 +6886,7 @@
       <c r="S22" s="33"/>
       <c r="U22" s="33"/>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>CSW</v>
@@ -6760,7 +6915,7 @@
       </c>
       <c r="U23" s="32"/>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>CSW</v>
@@ -6821,7 +6976,7 @@
       </c>
       <c r="U24" s="32"/>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>CSW</v>
@@ -6850,12 +7005,12 @@
       </c>
       <c r="U25" s="32"/>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D30" s="20">
         <v>2000</v>
       </c>
@@ -6908,7 +7063,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -6939,7 +7094,7 @@
       </c>
       <c r="U31" s="28"/>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -6970,7 +7125,7 @@
       </c>
       <c r="U32" s="28"/>
     </row>
-    <row r="33" spans="2:21">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -7001,11 +7156,11 @@
       </c>
       <c r="U33" s="28"/>
     </row>
-    <row r="34" spans="2:21">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
     </row>
-    <row r="35" spans="2:21">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -7040,7 +7195,7 @@
       </c>
       <c r="U35" s="28"/>
     </row>
-    <row r="36" spans="2:21">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -7075,7 +7230,7 @@
       </c>
       <c r="U36" s="28"/>
     </row>
-    <row r="37" spans="2:21">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -7110,11 +7265,11 @@
       </c>
       <c r="U37" s="28"/>
     </row>
-    <row r="38" spans="2:21">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
     </row>
-    <row r="39" spans="2:21">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>PWID</v>
@@ -7149,7 +7304,7 @@
       </c>
       <c r="U39" s="28"/>
     </row>
-    <row r="40" spans="2:21">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>PWID</v>
@@ -7184,7 +7339,7 @@
       </c>
       <c r="U40" s="28"/>
     </row>
-    <row r="41" spans="2:21">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>PWID</v>
@@ -7219,11 +7374,11 @@
       </c>
       <c r="U41" s="28"/>
     </row>
-    <row r="42" spans="2:21">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
     </row>
-    <row r="43" spans="2:21">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>GM</v>
@@ -7252,7 +7407,7 @@
       </c>
       <c r="U43" s="28"/>
     </row>
-    <row r="44" spans="2:21">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>GM</v>
@@ -7283,7 +7438,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="45" spans="2:21">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>GM</v>
@@ -7312,11 +7467,11 @@
       </c>
       <c r="U45" s="28"/>
     </row>
-    <row r="46" spans="2:21">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
     </row>
-    <row r="47" spans="2:21">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>GF</v>
@@ -7345,7 +7500,7 @@
       </c>
       <c r="U47" s="28"/>
     </row>
-    <row r="48" spans="2:21">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>GF</v>
@@ -7382,7 +7537,7 @@
       </c>
       <c r="U48" s="28"/>
     </row>
-    <row r="49" spans="2:21">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>GF</v>
@@ -7411,11 +7566,11 @@
       </c>
       <c r="U49" s="28"/>
     </row>
-    <row r="50" spans="2:21">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
     </row>
-    <row r="51" spans="2:21">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>CSW</v>
@@ -7444,7 +7599,7 @@
       </c>
       <c r="U51" s="28"/>
     </row>
-    <row r="52" spans="2:21">
+    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>CSW</v>
@@ -7475,7 +7630,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="53" spans="2:21">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>CSW</v>
@@ -7516,7 +7671,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AC42"/>
   <sheetViews>
@@ -7524,15 +7679,15 @@
       <selection activeCell="Y25" sqref="Y25:AC30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="7"/>
-    <col min="21" max="21" width="9.125" customWidth="1"/>
-    <col min="22" max="22" width="8.875" customWidth="1"/>
-    <col min="23" max="23" width="8.625" style="7"/>
+    <col min="2" max="2" width="8.5703125" style="7"/>
+    <col min="21" max="21" width="9.140625" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" customWidth="1"/>
+    <col min="23" max="23" width="8.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="19" customFormat="1">
+    <row r="1" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>40</v>
       </c>
@@ -7546,7 +7701,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="19" customFormat="1">
+    <row r="2" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="20">
         <v>2000</v>
@@ -7616,7 +7771,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="19" customFormat="1">
+    <row r="3" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -7649,7 +7804,7 @@
       <c r="AB3" s="27"/>
       <c r="AC3" s="27"/>
     </row>
-    <row r="4" spans="1:29" s="19" customFormat="1">
+    <row r="4" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -7682,7 +7837,7 @@
       <c r="AB4" s="27"/>
       <c r="AC4" s="27"/>
     </row>
-    <row r="5" spans="1:29" s="19" customFormat="1">
+    <row r="5" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>PWID</v>
@@ -7715,7 +7870,7 @@
       <c r="AB5" s="27"/>
       <c r="AC5" s="27"/>
     </row>
-    <row r="6" spans="1:29" s="19" customFormat="1">
+    <row r="6" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>GM</v>
@@ -7748,7 +7903,7 @@
       <c r="AB6" s="27"/>
       <c r="AC6" s="27"/>
     </row>
-    <row r="7" spans="1:29" s="19" customFormat="1">
+    <row r="7" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>GF</v>
@@ -7781,7 +7936,7 @@
       <c r="AB7" s="27"/>
       <c r="AC7" s="27"/>
     </row>
-    <row r="8" spans="1:29" s="19" customFormat="1">
+    <row r="8" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>CSW</v>
@@ -7814,19 +7969,19 @@
       <c r="AB8" s="27"/>
       <c r="AC8" s="27"/>
     </row>
-    <row r="9" spans="1:29" s="19" customFormat="1">
+    <row r="9" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="W9" s="7"/>
     </row>
-    <row r="10" spans="1:29" s="19" customFormat="1">
+    <row r="10" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="W10" s="7"/>
     </row>
-    <row r="11" spans="1:29" s="19" customFormat="1">
+    <row r="11" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="W11" s="7"/>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>114</v>
       </c>
@@ -7857,7 +8012,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="C13" s="9">
         <v>2000</v>
@@ -7929,7 +8084,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -7974,7 +8129,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -8019,7 +8174,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -8064,7 +8219,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -8109,7 +8264,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -8154,7 +8309,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -8199,19 +8354,19 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:29" s="19" customFormat="1">
+    <row r="20" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="W20" s="7"/>
     </row>
-    <row r="21" spans="1:29" s="19" customFormat="1">
+    <row r="21" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="W21" s="7"/>
     </row>
-    <row r="22" spans="1:29" s="19" customFormat="1">
+    <row r="22" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="W22" s="7"/>
     </row>
-    <row r="23" spans="1:29" s="19" customFormat="1">
+    <row r="23" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>17</v>
       </c>
@@ -8225,7 +8380,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:29" s="19" customFormat="1">
+    <row r="24" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="20">
         <v>2000</v>
@@ -8295,7 +8450,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:29" s="19" customFormat="1">
+    <row r="25" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -8338,7 +8493,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:29" s="19" customFormat="1">
+    <row r="26" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -8381,7 +8536,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="19" customFormat="1">
+    <row r="27" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>PWID</v>
@@ -8424,7 +8579,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:29" s="19" customFormat="1">
+    <row r="28" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>GM</v>
@@ -8467,7 +8622,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="1:29" s="19" customFormat="1">
+    <row r="29" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>GF</v>
@@ -8510,7 +8665,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="1:29" s="19" customFormat="1">
+    <row r="30" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>CSW</v>
@@ -8553,20 +8708,20 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="S31" s="6"/>
     </row>
-    <row r="32" spans="1:29" s="19" customFormat="1">
+    <row r="32" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="S32" s="6"/>
       <c r="W32" s="7"/>
     </row>
-    <row r="33" spans="1:29" s="19" customFormat="1">
+    <row r="33" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="S33" s="6"/>
       <c r="W33" s="7"/>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>97</v>
       </c>
@@ -8599,7 +8754,7 @@
       </c>
       <c r="AC34" s="19"/>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="C35" s="9">
         <v>2000</v>
@@ -8671,7 +8826,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:29">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -8707,7 +8862,7 @@
       <c r="AB36" s="27"/>
       <c r="AC36" s="27"/>
     </row>
-    <row r="37" spans="1:29">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -8742,7 +8897,7 @@
       <c r="AB37" s="27"/>
       <c r="AC37" s="27"/>
     </row>
-    <row r="38" spans="1:29">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>PWID</v>
@@ -8777,7 +8932,7 @@
       <c r="AB38" s="27"/>
       <c r="AC38" s="27"/>
     </row>
-    <row r="39" spans="1:29">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>GM</v>
@@ -8812,7 +8967,7 @@
       <c r="AB39" s="27"/>
       <c r="AC39" s="27"/>
     </row>
-    <row r="40" spans="1:29">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>GF</v>
@@ -8847,7 +9002,7 @@
       <c r="AB40" s="27"/>
       <c r="AC40" s="27"/>
     </row>
-    <row r="41" spans="1:29">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>CSW</v>
@@ -8882,7 +9037,7 @@
       <c r="AB41" s="27"/>
       <c r="AC41" s="27"/>
     </row>
-    <row r="42" spans="1:29">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="S42" s="6"/>
     </row>
   </sheetData>
@@ -8898,7 +9053,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T33"/>
   <sheetViews>
@@ -8906,13 +9061,13 @@
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="7"/>
-    <col min="20" max="20" width="14.25" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="7"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>41</v>
       </c>
@@ -8935,7 +9090,7 @@
       <c r="S1" s="10"/>
       <c r="T1" s="10"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="C2" s="11">
         <v>2000</v>
@@ -8990,7 +9145,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="5" t="s">
         <v>93</v>
@@ -9016,13 +9171,13 @@
       </c>
       <c r="T3" s="24"/>
     </row>
-    <row r="5" spans="1:20" s="19" customFormat="1">
+    <row r="5" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
     </row>
-    <row r="6" spans="1:20" s="19" customFormat="1">
+    <row r="6" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>42</v>
       </c>
@@ -9045,7 +9200,7 @@
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="C8" s="11">
         <v>2000</v>
@@ -9100,7 +9255,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="5" t="s">
         <v>93</v>
@@ -9150,13 +9305,13 @@
       </c>
       <c r="T9" s="24"/>
     </row>
-    <row r="11" spans="1:20" s="19" customFormat="1">
+    <row r="11" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:20" s="19" customFormat="1">
+    <row r="12" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>43</v>
       </c>
@@ -9179,7 +9334,7 @@
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="C14" s="11">
         <v>2000</v>
@@ -9234,7 +9389,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="5" t="s">
         <v>93</v>
@@ -9260,19 +9415,19 @@
       </c>
       <c r="T15" s="24"/>
     </row>
-    <row r="17" spans="1:20" s="19" customFormat="1">
+    <row r="17" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="1:20" s="19" customFormat="1">
+    <row r="18" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="1:20" s="19" customFormat="1">
+    <row r="19" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>138</v>
       </c>
       <c r="B19" s="7"/>
     </row>
-    <row r="20" spans="1:20" s="19" customFormat="1">
+    <row r="20" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="20">
         <v>2000</v>
@@ -9326,7 +9481,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="19" customFormat="1">
+    <row r="21" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>93</v>
       </c>
@@ -9351,16 +9506,16 @@
       </c>
       <c r="T21" s="24"/>
     </row>
-    <row r="22" spans="1:20" s="19" customFormat="1">
+    <row r="22" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="1:20" s="19" customFormat="1">
+    <row r="23" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="1:20" s="19" customFormat="1">
+    <row r="24" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>33</v>
       </c>
@@ -9383,7 +9538,7 @@
       <c r="S25" s="10"/>
       <c r="T25" s="10"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="C26" s="11">
         <v>2000</v>
@@ -9438,7 +9593,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="5" t="s">
         <v>93</v>
@@ -9464,13 +9619,13 @@
       </c>
       <c r="T27" s="24"/>
     </row>
-    <row r="31" spans="1:20" s="19" customFormat="1">
+    <row r="31" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>115</v>
       </c>
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="1:20" s="19" customFormat="1">
+    <row r="32" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="20">
         <v>2000</v>
@@ -9524,7 +9679,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="2:20" s="19" customFormat="1">
+    <row r="33" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>93</v>
       </c>
@@ -9561,7 +9716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AC49"/>
   <sheetViews>
@@ -9569,14 +9724,14 @@
       <selection activeCell="C5" sqref="C5:R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="7"/>
-    <col min="20" max="20" width="14.25" customWidth="1"/>
-    <col min="23" max="23" width="12.375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="7"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
@@ -9608,7 +9763,7 @@
       </c>
       <c r="AC1" s="19"/>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="C2" s="11">
         <v>2000</v>
@@ -9679,7 +9834,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -9723,7 +9878,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -9769,7 +9924,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -9817,7 +9972,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -9861,7 +10016,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -9905,7 +10060,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -9949,15 +10104,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:29" s="19" customFormat="1">
+    <row r="10" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="W10" s="7"/>
     </row>
-    <row r="11" spans="1:29" s="19" customFormat="1">
+    <row r="11" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="W11" s="7"/>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>44</v>
       </c>
@@ -9989,7 +10144,7 @@
       </c>
       <c r="AC12" s="19"/>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="C13" s="11">
         <v>2000</v>
@@ -10060,7 +10215,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="5" t="s">
         <v>94</v>
@@ -10103,15 +10258,15 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="16" spans="1:29" s="19" customFormat="1">
+    <row r="16" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
       <c r="W16" s="7"/>
     </row>
-    <row r="17" spans="1:29" s="19" customFormat="1">
+    <row r="17" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="W17" s="7"/>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>29</v>
       </c>
@@ -10143,7 +10298,7 @@
       </c>
       <c r="AC18" s="19"/>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="C19" s="11">
         <v>2000</v>
@@ -10214,7 +10369,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="5" t="s">
         <v>93</v>
@@ -10283,15 +10438,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:29" s="19" customFormat="1">
+    <row r="21" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="W21" s="7"/>
     </row>
-    <row r="22" spans="1:29" s="19" customFormat="1">
+    <row r="22" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="W22" s="7"/>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>30</v>
       </c>
@@ -10323,7 +10478,7 @@
       </c>
       <c r="AC24" s="19"/>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="C25" s="11">
         <v>2000</v>
@@ -10394,7 +10549,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="5" t="s">
         <v>93</v>
@@ -10464,15 +10619,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:29" s="19" customFormat="1">
+    <row r="28" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="W28" s="7"/>
     </row>
-    <row r="29" spans="1:29" s="19" customFormat="1">
+    <row r="29" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="W29" s="7"/>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>116</v>
       </c>
@@ -10504,7 +10659,7 @@
       </c>
       <c r="AC30" s="19"/>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="C31" s="11">
         <v>2000</v>
@@ -10575,7 +10730,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:29">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="5" t="s">
         <v>93</v>
@@ -10627,19 +10782,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:29" s="19" customFormat="1">
+    <row r="33" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="W33" s="7"/>
     </row>
-    <row r="34" spans="1:29" s="19" customFormat="1">
+    <row r="34" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="W34" s="7"/>
     </row>
-    <row r="35" spans="1:29" s="19" customFormat="1">
+    <row r="35" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="W35" s="7"/>
     </row>
-    <row r="36" spans="1:29" s="19" customFormat="1">
+    <row r="36" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
         <v>35</v>
       </c>
@@ -10652,7 +10807,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:29" s="19" customFormat="1">
+    <row r="37" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="20">
         <v>2000</v>
@@ -10722,7 +10877,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:29" s="19" customFormat="1">
+    <row r="38" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -10755,7 +10910,7 @@
       <c r="AB38" s="27"/>
       <c r="AC38" s="27"/>
     </row>
-    <row r="39" spans="1:29" s="19" customFormat="1">
+    <row r="39" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -10788,7 +10943,7 @@
       <c r="AB39" s="27"/>
       <c r="AC39" s="27"/>
     </row>
-    <row r="40" spans="1:29" s="19" customFormat="1">
+    <row r="40" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>PWID</v>
@@ -10821,7 +10976,7 @@
       <c r="AB40" s="27"/>
       <c r="AC40" s="27"/>
     </row>
-    <row r="41" spans="1:29" s="19" customFormat="1">
+    <row r="41" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>GM</v>
@@ -10854,7 +11009,7 @@
       <c r="AB41" s="27"/>
       <c r="AC41" s="27"/>
     </row>
-    <row r="42" spans="1:29" s="19" customFormat="1">
+    <row r="42" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>GF</v>
@@ -10888,7 +11043,7 @@
       <c r="AB42" s="27"/>
       <c r="AC42" s="27"/>
     </row>
-    <row r="43" spans="1:29" s="19" customFormat="1">
+    <row r="43" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>CSW</v>
@@ -10921,7 +11076,7 @@
       <c r="AB43" s="27"/>
       <c r="AC43" s="27"/>
     </row>
-    <row r="47" spans="1:29" s="19" customFormat="1">
+    <row r="47" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>36</v>
       </c>
@@ -10934,7 +11089,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:29" s="19" customFormat="1">
+    <row r="48" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
       <c r="C48" s="20">
         <v>2000</v>
@@ -11004,7 +11159,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="2:29" s="19" customFormat="1">
+    <row r="49" spans="2:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>93</v>
       </c>
@@ -11059,7 +11214,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AE74"/>
   <sheetViews>
@@ -11067,15 +11222,15 @@
       <selection activeCell="S56" sqref="S56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="7"/>
-    <col min="20" max="20" width="14.375" style="36" customWidth="1"/>
-    <col min="23" max="23" width="11.375" customWidth="1"/>
-    <col min="31" max="31" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="7"/>
+    <col min="20" max="20" width="14.42578125" style="36" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" customWidth="1"/>
+    <col min="31" max="31" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>109</v>
       </c>
@@ -11106,7 +11261,7 @@
       </c>
       <c r="AC1" s="19"/>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
       <c r="C2" s="13">
         <v>2000</v>
@@ -11180,7 +11335,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -11218,7 +11373,7 @@
       <c r="AB3" s="39"/>
       <c r="AC3" s="39"/>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -11256,7 +11411,7 @@
       <c r="AB4" s="39"/>
       <c r="AC4" s="39"/>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -11294,7 +11449,7 @@
       <c r="AB5" s="39"/>
       <c r="AC5" s="39"/>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -11332,7 +11487,7 @@
       <c r="AB6" s="39"/>
       <c r="AC6" s="39"/>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -11370,7 +11525,7 @@
       <c r="AB7" s="39"/>
       <c r="AC7" s="39"/>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -11408,15 +11563,15 @@
       <c r="AB8" s="39"/>
       <c r="AC8" s="39"/>
     </row>
-    <row r="10" spans="1:29" s="19" customFormat="1">
+    <row r="10" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="T10" s="36"/>
     </row>
-    <row r="11" spans="1:29" s="19" customFormat="1">
+    <row r="11" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="T11" s="36"/>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>110</v>
       </c>
@@ -11447,7 +11602,7 @@
       </c>
       <c r="AC12" s="19"/>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="C13" s="13">
         <v>2000</v>
@@ -11521,7 +11676,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -11559,7 +11714,7 @@
       <c r="AB14" s="35"/>
       <c r="AC14" s="35"/>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -11597,7 +11752,7 @@
       <c r="AB15" s="35"/>
       <c r="AC15" s="35"/>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -11635,7 +11790,7 @@
       <c r="AB16" s="35"/>
       <c r="AC16" s="35"/>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -11673,7 +11828,7 @@
       <c r="AB17" s="35"/>
       <c r="AC17" s="35"/>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -11711,7 +11866,7 @@
       <c r="AB18" s="35"/>
       <c r="AC18" s="35"/>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -11749,15 +11904,15 @@
       <c r="AB19" s="35"/>
       <c r="AC19" s="35"/>
     </row>
-    <row r="21" spans="1:29" s="19" customFormat="1">
+    <row r="21" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="T21" s="36"/>
     </row>
-    <row r="22" spans="1:29" s="19" customFormat="1">
+    <row r="22" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="T22" s="36"/>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>111</v>
       </c>
@@ -11788,7 +11943,7 @@
       </c>
       <c r="AC23" s="19"/>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="C24" s="13">
         <v>2000</v>
@@ -11862,7 +12017,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -11900,7 +12055,7 @@
       <c r="AB25" s="35"/>
       <c r="AC25" s="35"/>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -11938,7 +12093,7 @@
       <c r="AB26" s="35"/>
       <c r="AC26" s="35"/>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -11976,7 +12131,7 @@
       <c r="AB27" s="35"/>
       <c r="AC27" s="35"/>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -12014,7 +12169,7 @@
       <c r="AB28" s="35"/>
       <c r="AC28" s="35"/>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -12052,7 +12207,7 @@
       <c r="AB29" s="35"/>
       <c r="AC29" s="35"/>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -12090,15 +12245,15 @@
       <c r="AB30" s="35"/>
       <c r="AC30" s="35"/>
     </row>
-    <row r="32" spans="1:29" s="19" customFormat="1">
+    <row r="32" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="T32" s="36"/>
     </row>
-    <row r="33" spans="1:29" s="19" customFormat="1">
+    <row r="33" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="T33" s="36"/>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>119</v>
       </c>
@@ -12129,7 +12284,7 @@
       </c>
       <c r="AC34" s="19"/>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="C35" s="13">
         <v>2000</v>
@@ -12203,7 +12358,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:29">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -12251,7 +12406,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="37" spans="1:29">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="B37" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -12307,7 +12462,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="38" spans="1:29">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="B38" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -12355,7 +12510,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="39" spans="1:29">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -12403,7 +12558,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="40" spans="1:29">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -12451,7 +12606,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="41" spans="1:29">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -12499,15 +12654,15 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="43" spans="1:29" s="19" customFormat="1">
+    <row r="43" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
       <c r="T43" s="36"/>
     </row>
-    <row r="44" spans="1:29" s="19" customFormat="1">
+    <row r="44" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
       <c r="T44" s="36"/>
     </row>
-    <row r="45" spans="1:29">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>118</v>
       </c>
@@ -12538,7 +12693,7 @@
       </c>
       <c r="AC45" s="19"/>
     </row>
-    <row r="46" spans="1:29">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="C46" s="13">
         <v>2000</v>
@@ -12612,7 +12767,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:29">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -12660,7 +12815,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="48" spans="1:29">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -12716,7 +12871,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
       <c r="B49" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -12764,7 +12919,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="50" spans="1:31">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -12816,7 +12971,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:31">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -12868,7 +13023,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:31">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -12916,15 +13071,15 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="54" spans="1:31" s="19" customFormat="1">
+    <row r="54" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
       <c r="T54" s="36"/>
     </row>
-    <row r="55" spans="1:31" s="19" customFormat="1">
+    <row r="55" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="7"/>
       <c r="T55" s="36"/>
     </row>
-    <row r="56" spans="1:31">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>117</v>
       </c>
@@ -12955,7 +13110,7 @@
       </c>
       <c r="AC56" s="19"/>
     </row>
-    <row r="57" spans="1:31">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="C57" s="13">
         <v>2000</v>
@@ -13029,7 +13184,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="58" spans="1:31">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -13067,7 +13222,7 @@
       <c r="AB58" s="35"/>
       <c r="AC58" s="35"/>
     </row>
-    <row r="59" spans="1:31">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="B59" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -13131,7 +13286,7 @@
         <v>0.19500000000000006</v>
       </c>
     </row>
-    <row r="60" spans="1:31">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -13170,7 +13325,7 @@
       <c r="AC60" s="35"/>
       <c r="AE60" s="58"/>
     </row>
-    <row r="61" spans="1:31">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
       <c r="B61" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -13212,7 +13367,7 @@
         <v>87.674999999999997</v>
       </c>
     </row>
-    <row r="62" spans="1:31">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -13250,7 +13405,7 @@
       <c r="AB62" s="35"/>
       <c r="AC62" s="35"/>
     </row>
-    <row r="63" spans="1:31">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -13306,15 +13461,15 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="65" spans="1:29" s="19" customFormat="1">
+    <row r="65" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="7"/>
       <c r="T65" s="36"/>
     </row>
-    <row r="66" spans="1:29" s="19" customFormat="1">
+    <row r="66" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="7"/>
       <c r="T66" s="36"/>
     </row>
-    <row r="67" spans="1:29">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>45</v>
       </c>
@@ -13345,7 +13500,7 @@
       </c>
       <c r="AC67" s="19"/>
     </row>
-    <row r="68" spans="1:29">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="C68" s="13">
         <v>2000</v>
@@ -13419,7 +13574,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="69" spans="1:29">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -13457,7 +13612,7 @@
       <c r="AB69" s="35"/>
       <c r="AC69" s="35"/>
     </row>
-    <row r="70" spans="1:29">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -13495,7 +13650,7 @@
       <c r="AB70" s="35"/>
       <c r="AC70" s="35"/>
     </row>
-    <row r="71" spans="1:29">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -13533,7 +13688,7 @@
       <c r="AB71" s="35"/>
       <c r="AC71" s="35"/>
     </row>
-    <row r="72" spans="1:29">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -13571,7 +13726,7 @@
       <c r="AB72" s="35"/>
       <c r="AC72" s="35"/>
     </row>
-    <row r="73" spans="1:29">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
       <c r="B73" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -13609,7 +13764,7 @@
       <c r="AB73" s="35"/>
       <c r="AC73" s="35"/>
     </row>
-    <row r="74" spans="1:29">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="B74" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -13660,7 +13815,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AC20"/>
   <sheetViews>
@@ -13668,17 +13823,17 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.375" style="36" customWidth="1"/>
-    <col min="21" max="21" width="8.625" style="36"/>
-    <col min="22" max="22" width="9.125" style="36" customWidth="1"/>
-    <col min="23" max="23" width="11.75" style="7" customWidth="1"/>
-    <col min="24" max="29" width="8.625" style="36"/>
+    <col min="2" max="2" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" style="36" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" style="36"/>
+    <col min="22" max="22" width="9.140625" style="36" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" style="7" customWidth="1"/>
+    <col min="24" max="29" width="8.5703125" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>120</v>
       </c>
@@ -13706,7 +13861,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="C2" s="15">
         <v>2000</v>
@@ -13780,7 +13935,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -13818,7 +13973,7 @@
       <c r="AB3" s="35"/>
       <c r="AC3" s="35"/>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -13856,7 +14011,7 @@
       <c r="AB4" s="35"/>
       <c r="AC4" s="35"/>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -13894,7 +14049,7 @@
       <c r="AB5" s="35"/>
       <c r="AC5" s="35"/>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -13932,7 +14087,7 @@
       <c r="AB6" s="35"/>
       <c r="AC6" s="35"/>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -13970,7 +14125,7 @@
       <c r="AB7" s="35"/>
       <c r="AC7" s="35"/>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -14008,7 +14163,7 @@
       <c r="AB8" s="35"/>
       <c r="AC8" s="35"/>
     </row>
-    <row r="10" spans="1:29" s="19" customFormat="1">
+    <row r="10" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="T10" s="36"/>
       <c r="U10" s="36"/>
@@ -14021,7 +14176,7 @@
       <c r="AB10" s="36"/>
       <c r="AC10" s="36"/>
     </row>
-    <row r="11" spans="1:29" s="19" customFormat="1">
+    <row r="11" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="T11" s="36"/>
       <c r="U11" s="36"/>
@@ -14034,7 +14189,7 @@
       <c r="AB11" s="36"/>
       <c r="AC11" s="36"/>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
@@ -14063,7 +14218,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="C13" s="15">
         <v>2000</v>
@@ -14134,7 +14289,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="56" t="s">
         <v>16</v>
@@ -14187,7 +14342,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:29" s="19" customFormat="1">
+    <row r="16" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
       <c r="T16" s="36"/>
       <c r="U16" s="36"/>
@@ -14200,7 +14355,7 @@
       <c r="AB16" s="36"/>
       <c r="AC16" s="36"/>
     </row>
-    <row r="17" spans="1:29" s="19" customFormat="1">
+    <row r="17" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="T17" s="36"/>
       <c r="U17" s="36"/>
@@ -14213,7 +14368,7 @@
       <c r="AB17" s="36"/>
       <c r="AC17" s="36"/>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>46</v>
       </c>
@@ -14241,7 +14396,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="C19" s="15">
         <v>2000</v>
@@ -14315,7 +14470,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="56" t="s">
         <v>16</v>
@@ -14379,7 +14534,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z41"/>
   <sheetViews>
@@ -14387,12 +14542,12 @@
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="15" width="6.625" customWidth="1"/>
+    <col min="1" max="15" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" customHeight="1">
+    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>131</v>
       </c>
@@ -14421,7 +14576,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="43"/>
       <c r="C2" s="5" t="str">
@@ -14467,7 +14622,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -14500,7 +14655,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -14531,7 +14686,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -14566,7 +14721,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -14600,7 +14755,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -14631,7 +14786,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -14666,7 +14821,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -14694,9 +14849,9 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" s="19" customFormat="1"/>
-    <row r="11" spans="1:26" s="19" customFormat="1"/>
-    <row r="12" spans="1:26">
+    <row r="10" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>129</v>
       </c>
@@ -14726,7 +14881,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="43"/>
       <c r="C13" s="5" t="str">
@@ -14772,7 +14927,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -14805,7 +14960,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -14836,7 +14991,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -14871,7 +15026,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -14906,7 +15061,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -14937,7 +15092,7 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -14954,7 +15109,7 @@
       </c>
       <c r="H19" s="42"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -14964,7 +15119,7 @@
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
     </row>
-    <row r="21" spans="1:26" s="19" customFormat="1">
+    <row r="21" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -14992,8 +15147,8 @@
       <c r="Y21" s="17"/>
       <c r="Z21" s="17"/>
     </row>
-    <row r="22" spans="1:26" s="19" customFormat="1"/>
-    <row r="23" spans="1:26">
+    <row r="22" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>130</v>
       </c>
@@ -15005,7 +15160,7 @@
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="43"/>
       <c r="C24" s="5" t="str">
@@ -15033,7 +15188,7 @@
         <v>CSW</v>
       </c>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -15046,7 +15201,7 @@
       <c r="G25" s="42"/>
       <c r="H25" s="42"/>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
       <c r="B26" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -15059,7 +15214,7 @@
       <c r="G26" s="42"/>
       <c r="H26" s="42"/>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -15072,7 +15227,7 @@
       <c r="G27" s="42"/>
       <c r="H27" s="42"/>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -15085,7 +15240,7 @@
       <c r="G28" s="42"/>
       <c r="H28" s="42"/>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -15098,7 +15253,7 @@
       <c r="G29" s="42"/>
       <c r="H29" s="42"/>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="16"/>
       <c r="B30" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -15113,7 +15268,7 @@
       <c r="G30" s="42"/>
       <c r="H30" s="42"/>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -15123,7 +15278,7 @@
       <c r="G31" s="17"/>
       <c r="H31" s="17"/>
     </row>
-    <row r="32" spans="1:26" s="19" customFormat="1">
+    <row r="32" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -15151,8 +15306,8 @@
       <c r="Y32" s="17"/>
       <c r="Z32" s="17"/>
     </row>
-    <row r="33" spans="1:8" s="19" customFormat="1"/>
-    <row r="34" spans="1:8">
+    <row r="33" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>132</v>
       </c>
@@ -15164,7 +15319,7 @@
       <c r="G34" s="17"/>
       <c r="H34" s="17"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
       <c r="B35" s="43"/>
       <c r="C35" s="5" t="str">
@@ -15192,7 +15347,7 @@
         <v>CSW</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="5" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -15205,7 +15360,7 @@
       <c r="G36" s="42"/>
       <c r="H36" s="42"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="5" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -15218,7 +15373,7 @@
       <c r="G37" s="42"/>
       <c r="H37" s="42"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="5" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -15233,7 +15388,7 @@
       <c r="G38" s="42"/>
       <c r="H38" s="42"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="5" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -15246,7 +15401,7 @@
       <c r="G39" s="42"/>
       <c r="H39" s="42"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="5" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -15259,7 +15414,7 @@
       <c r="G40" s="42"/>
       <c r="H40" s="42"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="5" t="str">
         <f>'Populations &amp; programs'!$C$8</f>

</xml_diff>

<commit_message>
slight change to spreadsheet, not sure what
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="10"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -3225,8 +3225,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8134,8 +8134,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC10" sqref="AC10"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10138,8 +10138,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS71"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U55" sqref="U55"/>
+    <sheetView tabSelected="1" topLeftCell="R17" workbookViewId="0">
+      <selection activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13269,8 +13269,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS85"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AE10" sqref="AE10"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="W80" sqref="W80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17287,7 +17287,9 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
fixed bug with how programs are read in
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="5"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="164">
   <si>
     <t>Men who have sex with men</t>
   </si>
@@ -55,11 +55,11 @@
   </si>
   <si>
     <t>PMTCT</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Prevention of mother-to-child transmission</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -74,11 +74,11 @@
       </rPr>
       <t>C</t>
     </r>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Average</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Prevalence of any discharging STIs</t>
@@ -548,10 +548,17 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -705,795 +712,799 @@
   </borders>
   <cellStyleXfs count="663">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="655"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="655" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="655"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="655" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="655"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="655" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="655"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="655" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="11" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="11" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="10" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="655" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="655" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2919,7 +2930,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
@@ -3210,7 +3221,7 @@
       <c r="H19" s="24"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -3791,7 +3802,7 @@
       <c r="E69" s="22"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -4073,7 +4084,7 @@
       <c r="E28" s="22"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -5279,7 +5290,7 @@
       <c r="T57" s="29"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -5424,7 +5435,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
       <c r="H4" s="27">
-        <f t="shared" ref="F4:Q4" si="0">550000*H3</f>
+        <f t="shared" ref="H4:Q4" si="0">550000*H3</f>
         <v>77000.000000000015</v>
       </c>
       <c r="I4" s="27">
@@ -5968,7 +5979,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="598"/>
   <extLst>
@@ -7456,7 +7467,7 @@
       <c r="U53" s="26"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -8119,7 +8130,7 @@
       <c r="T33" s="22"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -8134,8 +8145,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AO3" sqref="AO3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8330,26 +8341,66 @@
       <c r="T3" s="25">
         <v>0.01</v>
       </c>
-      <c r="W3" s="40"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
-      <c r="AC3" s="40"/>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AI3" s="40"/>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AM3" s="25"/>
-      <c r="AO3" s="40"/>
-      <c r="AP3" s="25"/>
-      <c r="AQ3" s="25"/>
-      <c r="AR3" s="25"/>
-      <c r="AS3" s="25"/>
+      <c r="W3" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="X3" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="Y3" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="Z3" s="25">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="25">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD3" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="AE3" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="AF3" s="25">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="25">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ3" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="AK3" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="AL3" s="25">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="25">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP3" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="AQ3" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="AR3" s="25">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
@@ -10122,7 +10173,7 @@
       <c r="S42" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -10138,7 +10189,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R17" workbookViewId="0">
+    <sheetView topLeftCell="R17" workbookViewId="0">
       <selection activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
@@ -13253,7 +13304,7 @@
       <c r="AS71" s="25"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -17271,7 +17322,7 @@
       <c r="AS85" s="30"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -18335,7 +18386,7 @@
       <c r="AS20" s="30"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
@@ -19241,7 +19292,7 @@
       <c r="H41" s="36"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
fixed condom efficacy bug in model.py
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Disutilities &amp; costs" sheetId="14" r:id="rId12"/>
     <sheet name="Macroeconomics" sheetId="18" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -491,9 +491,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
@@ -658,7 +658,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -1306,7 +1306,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
@@ -1361,10 +1361,10 @@
     <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="662" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="662" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="662" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1421,7 +1421,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2417,7 +2417,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -3089,8 +3089,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14538,8 +14538,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
resolved conflicts in example.xlsx
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="4"/>
@@ -21,7 +21,7 @@
     <sheet name="Disutilities &amp; costs" sheetId="14" r:id="rId12"/>
     <sheet name="Macroeconomics" sheetId="18" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -545,8 +545,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -628,6 +628,7 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -724,7 +725,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
@@ -1372,7 +1373,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="56">
@@ -1494,7 +1495,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -8145,9 +8146,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AO3" sqref="AO3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
trying to resolve example.xlsx merge issue
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="4"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -2482,9 +2482,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8146,7 +8144,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
changing data in example.xlsx
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="164">
   <si>
     <t>Men who have sex with men</t>
   </si>
@@ -2482,7 +2482,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8144,7 +8144,9 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8338,66 +8340,26 @@
       <c r="T3" s="25">
         <v>0.01</v>
       </c>
-      <c r="W3" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="X3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="Y3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="Z3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="55" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="AE3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="AF3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="AK3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="AL3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="AQ3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="AR3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="25">
-        <v>0</v>
-      </c>
+      <c r="W3" s="55"/>
+      <c r="X3" s="25"/>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AA3" s="25"/>
+      <c r="AC3" s="55"/>
+      <c r="AD3" s="25"/>
+      <c r="AE3" s="25"/>
+      <c r="AF3" s="25"/>
+      <c r="AG3" s="25"/>
+      <c r="AI3" s="55"/>
+      <c r="AJ3" s="25"/>
+      <c r="AK3" s="25"/>
+      <c r="AL3" s="25"/>
+      <c r="AM3" s="25"/>
+      <c r="AO3" s="55"/>
+      <c r="AP3" s="25"/>
+      <c r="AQ3" s="25"/>
+      <c r="AR3" s="25"/>
+      <c r="AS3" s="25"/>
     </row>
     <row r="4" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">

</xml_diff>

<commit_message>
slight revisions to spreadsheet prior to sending it to david
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="5"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -1345,7 +1345,7 @@
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1472,6 +1472,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -3750,7 +3753,9 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W41" sqref="W41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4032,7 +4037,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5239,7 +5244,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5487,8 +5492,8 @@
       <c r="J9" s="25"/>
       <c r="K9" s="22"/>
       <c r="L9" s="25"/>
-      <c r="M9" s="25">
-        <v>0.3</v>
+      <c r="M9" s="55">
+        <v>1922</v>
       </c>
       <c r="N9" s="23"/>
       <c r="O9" s="25"/>
@@ -5520,7 +5525,7 @@
       <c r="K10" s="25"/>
       <c r="L10" s="22"/>
       <c r="M10" s="43">
-        <v>300000</v>
+        <v>3483</v>
       </c>
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
@@ -5618,8 +5623,8 @@
       <c r="J15" s="25"/>
       <c r="K15" s="22"/>
       <c r="L15" s="25"/>
-      <c r="M15" s="22">
-        <v>2343</v>
+      <c r="M15" s="25">
+        <v>0.2</v>
       </c>
       <c r="N15" s="23"/>
       <c r="O15" s="25"/>
@@ -5650,7 +5655,7 @@
       <c r="K16" s="25"/>
       <c r="L16" s="22"/>
       <c r="M16" s="43">
-        <v>1034</v>
+        <v>130000</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -5680,10 +5685,10 @@
       <c r="J18" s="25"/>
       <c r="K18" s="22"/>
       <c r="L18" s="25"/>
-      <c r="M18" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="N18" s="23"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="22">
+        <v>2343</v>
+      </c>
       <c r="O18" s="25"/>
       <c r="P18" s="22"/>
       <c r="Q18" s="25"/>
@@ -5711,10 +5716,10 @@
       <c r="J19" s="22"/>
       <c r="K19" s="25"/>
       <c r="L19" s="22"/>
-      <c r="M19" s="43">
-        <v>130000</v>
-      </c>
-      <c r="N19" s="23"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43">
+        <v>1034</v>
+      </c>
       <c r="O19" s="23"/>
       <c r="P19" s="22"/>
       <c r="Q19" s="25"/>
@@ -5742,10 +5747,10 @@
       <c r="J21" s="25"/>
       <c r="K21" s="22"/>
       <c r="L21" s="25"/>
-      <c r="M21" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="N21" s="23"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="55">
+        <v>153</v>
+      </c>
       <c r="O21" s="25"/>
       <c r="P21" s="22"/>
       <c r="Q21" s="25"/>
@@ -5773,10 +5778,10 @@
       <c r="J22" s="22"/>
       <c r="K22" s="25"/>
       <c r="L22" s="22"/>
-      <c r="M22" s="43">
-        <v>400000</v>
-      </c>
-      <c r="N22" s="23"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="55">
+        <v>5340</v>
+      </c>
       <c r="O22" s="23"/>
       <c r="P22" s="22"/>
       <c r="Q22" s="25"/>
@@ -7955,7 +7960,7 @@
   <dimension ref="A1:AS42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W25" sqref="W25:AA30"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9878,8 +9883,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14:AA14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed some bugs with updating population sizes
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="40" windowWidth="19420" windowHeight="10960" tabRatio="863" activeTab="4"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Disutilities &amp; costs" sheetId="14" r:id="rId12"/>
     <sheet name="Macroeconomics" sheetId="18" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -543,12 +543,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -724,7 +724,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
@@ -1372,7 +1372,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="56">
@@ -1494,7 +1494,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -2477,7 +2477,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L22"/>
   <sheetViews>
@@ -2485,26 +2485,26 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="20"/>
+    <col min="1" max="1" width="9.140625" style="20"/>
     <col min="2" max="2" width="5" style="20" customWidth="1"/>
-    <col min="3" max="3" width="13.875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="20" customWidth="1"/>
     <col min="4" max="4" width="18" style="20" customWidth="1"/>
-    <col min="5" max="5" width="55.375" style="20" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="20" customWidth="1"/>
-    <col min="7" max="8" width="9.125" style="20"/>
-    <col min="9" max="10" width="14.25" style="20" customWidth="1"/>
-    <col min="11" max="11" width="12.125" style="20" customWidth="1"/>
-    <col min="12" max="16384" width="9.125" style="20"/>
+    <col min="5" max="5" width="55.42578125" style="20" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="20" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="20"/>
+    <col min="9" max="10" width="14.28515625" style="20" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="20" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2" s="21" t="s">
         <v>92</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="21">
         <v>1</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="21">
         <v>2</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="21">
         <v>3</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="21">
         <v>4</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="21">
         <v>5</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="21">
         <v>6</v>
       </c>
@@ -2746,22 +2746,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="21"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="21"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="21"/>
       <c r="C13" s="21" t="s">
         <v>92</v>
@@ -2776,7 +2776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="21">
         <v>1</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="21">
         <v>2</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="21">
         <v>3</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="21">
         <v>4</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="21">
         <v>5</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="21">
         <v>6</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="21">
         <v>7</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="21">
         <v>8</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="21">
         <v>9</v>
       </c>
@@ -2941,7 +2941,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z19"/>
   <sheetViews>
@@ -2949,12 +2949,12 @@
       <selection activeCell="B14" sqref="B14:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>72</v>
       </c>
@@ -2966,7 +2966,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:26" s="6" customFormat="1">
+    <row r="2" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="4" t="str">
@@ -2994,7 +2994,7 @@
         <v>CSW</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -3006,7 +3006,7 @@
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -3018,7 +3018,7 @@
       <c r="G4" s="24"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -3030,7 +3030,7 @@
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -3042,7 +3042,7 @@
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -3054,7 +3054,7 @@
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -3066,7 +3066,7 @@
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
     </row>
-    <row r="9" spans="1:26" s="18" customFormat="1">
+    <row r="9" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="37"/>
       <c r="C9" s="16"/>
@@ -3094,10 +3094,10 @@
       <c r="Y9" s="16"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" s="18" customFormat="1">
+    <row r="10" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="37"/>
       <c r="C11" s="2"/>
@@ -3107,7 +3107,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>129</v>
       </c>
@@ -3119,7 +3119,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:26" s="6" customFormat="1">
+    <row r="13" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="4" t="str">
@@ -3147,7 +3147,7 @@
         <v>CSW</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -3159,7 +3159,7 @@
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -3171,7 +3171,7 @@
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -3183,7 +3183,7 @@
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -3195,7 +3195,7 @@
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -3207,7 +3207,7 @@
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -3231,7 +3231,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H69"/>
   <sheetViews>
@@ -3239,19 +3239,19 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="18"/>
-    <col min="2" max="2" width="33.25" style="18" customWidth="1"/>
-    <col min="3" max="16384" width="9.125" style="18"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="33.28515625" style="18" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="6" customFormat="1">
+    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>20</v>
       </c>
@@ -3272,7 +3272,7 @@
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -3282,7 +3282,7 @@
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
         <v>22</v>
       </c>
@@ -3292,7 +3292,7 @@
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
         <v>23</v>
       </c>
@@ -3302,7 +3302,7 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
         <v>19</v>
       </c>
@@ -3312,7 +3312,7 @@
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
         <v>157</v>
       </c>
@@ -3322,7 +3322,7 @@
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>158</v>
       </c>
@@ -3332,7 +3332,7 @@
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -3342,12 +3342,12 @@
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="6" customFormat="1">
+    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="4" t="s">
         <v>24</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
         <v>27</v>
       </c>
@@ -3368,7 +3368,7 @@
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="19" t="s">
         <v>139</v>
       </c>
@@ -3378,7 +3378,7 @@
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
         <v>130</v>
       </c>
@@ -3388,7 +3388,7 @@
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
         <v>131</v>
       </c>
@@ -3398,7 +3398,7 @@
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
         <v>141</v>
       </c>
@@ -3408,7 +3408,7 @@
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -3418,13 +3418,13 @@
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>156</v>
       </c>
       <c r="B23" s="19"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>24</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
         <v>132</v>
       </c>
@@ -3445,7 +3445,7 @@
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
         <v>130</v>
       </c>
@@ -3455,7 +3455,7 @@
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
         <v>133</v>
       </c>
@@ -3465,7 +3465,7 @@
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="19" t="s">
         <v>142</v>
       </c>
@@ -3475,7 +3475,7 @@
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -3485,12 +3485,12 @@
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" s="4" t="s">
         <v>24</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="19" t="s">
         <v>134</v>
       </c>
@@ -3511,7 +3511,7 @@
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" s="19" t="s">
         <v>135</v>
       </c>
@@ -3521,7 +3521,7 @@
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="19" t="s">
         <v>136</v>
       </c>
@@ -3531,10 +3531,10 @@
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="19"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -3544,12 +3544,12 @@
       <c r="G39" s="16"/>
       <c r="H39" s="16"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="4" t="s">
         <v>24</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" s="19" t="s">
         <v>137</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="19" t="s">
         <v>138</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -3598,12 +3598,12 @@
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C48" s="4" t="s">
         <v>24</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
         <v>27</v>
       </c>
@@ -3624,7 +3624,7 @@
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B50" s="19" t="s">
         <v>139</v>
       </c>
@@ -3634,7 +3634,7 @@
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>140</v>
       </c>
@@ -3644,7 +3644,7 @@
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="19" t="s">
         <v>131</v>
       </c>
@@ -3654,7 +3654,7 @@
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>141</v>
       </c>
@@ -3664,7 +3664,7 @@
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" s="19" t="s">
         <v>28</v>
       </c>
@@ -3674,7 +3674,7 @@
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
         <v>39</v>
       </c>
@@ -3684,7 +3684,7 @@
       <c r="D55" s="22"/>
       <c r="E55" s="22"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="16"/>
       <c r="B58" s="16"/>
       <c r="C58" s="16"/>
@@ -3694,12 +3694,12 @@
       <c r="G58" s="16"/>
       <c r="H58" s="16"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C60" s="4" t="s">
         <v>24</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" s="19" t="s">
         <v>120</v>
       </c>
@@ -3720,7 +3720,7 @@
       <c r="D61" s="22"/>
       <c r="E61" s="22"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" s="19" t="s">
         <v>29</v>
       </c>
@@ -3730,7 +3730,7 @@
       <c r="D62" s="22"/>
       <c r="E62" s="22"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B63" s="19" t="s">
         <v>40</v>
       </c>
@@ -3740,7 +3740,7 @@
       <c r="D63" s="22"/>
       <c r="E63" s="22"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" s="19" t="s">
         <v>30</v>
       </c>
@@ -3750,7 +3750,7 @@
       <c r="D64" s="22"/>
       <c r="E64" s="22"/>
     </row>
-    <row r="65" spans="2:5">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="19" t="s">
         <v>121</v>
       </c>
@@ -3760,7 +3760,7 @@
       <c r="D65" s="22"/>
       <c r="E65" s="22"/>
     </row>
-    <row r="66" spans="2:5">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="19" t="s">
         <v>31</v>
       </c>
@@ -3770,7 +3770,7 @@
       <c r="D66" s="22"/>
       <c r="E66" s="22"/>
     </row>
-    <row r="67" spans="2:5">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="19" t="s">
         <v>122</v>
       </c>
@@ -3780,7 +3780,7 @@
       <c r="D67" s="22"/>
       <c r="E67" s="22"/>
     </row>
-    <row r="68" spans="2:5">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="19" t="s">
         <v>4</v>
       </c>
@@ -3790,7 +3790,7 @@
       <c r="D68" s="22"/>
       <c r="E68" s="22"/>
     </row>
-    <row r="69" spans="2:5">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="19" t="s">
         <v>5</v>
       </c>
@@ -3812,18 +3812,18 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>163</v>
       </c>
@@ -3832,7 +3832,7 @@
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="4" t="s">
@@ -3845,7 +3845,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="18" customFormat="1">
+    <row r="3" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>162</v>
       </c>
@@ -3855,7 +3855,7 @@
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
         <v>143</v>
@@ -3866,7 +3866,7 @@
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="19" t="s">
         <v>144</v>
@@ -3877,7 +3877,7 @@
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="19" t="s">
         <v>145</v>
@@ -3888,7 +3888,7 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="19" t="s">
         <v>146</v>
@@ -3899,7 +3899,7 @@
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="s">
         <v>43</v>
@@ -3910,15 +3910,15 @@
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
     </row>
-    <row r="10" spans="1:8" s="18" customFormat="1"/>
-    <row r="11" spans="1:8" s="18" customFormat="1">
+    <row r="10" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -3928,7 +3928,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>161</v>
       </c>
@@ -3937,7 +3937,7 @@
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="4" t="s">
@@ -3950,7 +3950,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
         <v>27</v>
@@ -3961,7 +3961,7 @@
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="19" t="s">
         <v>139</v>
@@ -3972,7 +3972,7 @@
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
         <v>140</v>
@@ -3983,7 +3983,7 @@
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="19" t="s">
         <v>131</v>
@@ -3994,7 +3994,7 @@
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="19" t="s">
         <v>141</v>
@@ -4005,7 +4005,7 @@
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>160</v>
       </c>
@@ -4014,7 +4014,7 @@
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="4" t="s">
@@ -4027,7 +4027,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="19" t="s">
         <v>27</v>
@@ -4038,7 +4038,7 @@
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="19" t="s">
         <v>139</v>
@@ -4049,7 +4049,7 @@
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="19" t="s">
         <v>140</v>
@@ -4060,7 +4060,7 @@
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="19" t="s">
         <v>131</v>
@@ -4071,7 +4071,7 @@
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="19" t="s">
         <v>141</v>
@@ -4094,21 +4094,21 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T57"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="3" max="4" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="3" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>148</v>
       </c>
@@ -4130,7 +4130,7 @@
       <c r="R1" s="18"/>
       <c r="S1" s="18"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="C2" s="19">
         <v>2015</v>
@@ -4185,7 +4185,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
         <v>34</v>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="T3" s="29"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>149</v>
       </c>
@@ -4280,7 +4280,7 @@
       <c r="R7" s="18"/>
       <c r="S7" s="18"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="C8" s="19">
         <v>2015</v>
@@ -4335,7 +4335,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="4" t="s">
         <v>34</v>
@@ -4408,7 +4408,7 @@
       </c>
       <c r="T9" s="29"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>74</v>
       </c>
@@ -4430,7 +4430,7 @@
       <c r="R13" s="18"/>
       <c r="S13" s="18"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="C14" s="19">
         <v>2015</v>
@@ -4485,7 +4485,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
         <v>34</v>
@@ -4558,14 +4558,14 @@
       </c>
       <c r="T15" s="29"/>
     </row>
-    <row r="19" spans="1:20" s="18" customFormat="1">
+    <row r="19" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>81</v>
       </c>
       <c r="B19" s="6"/>
       <c r="T19" s="6"/>
     </row>
-    <row r="20" spans="1:20" s="18" customFormat="1">
+    <row r="20" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="19">
         <v>2015</v>
@@ -4619,7 +4619,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="18" customFormat="1">
+    <row r="21" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>34</v>
       </c>
@@ -4644,26 +4644,26 @@
       </c>
       <c r="T21" s="29"/>
     </row>
-    <row r="22" spans="1:20" s="18" customFormat="1">
+    <row r="22" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="T22" s="6"/>
     </row>
-    <row r="23" spans="1:20" s="18" customFormat="1">
+    <row r="23" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="T23" s="6"/>
     </row>
-    <row r="24" spans="1:20" s="18" customFormat="1">
+    <row r="24" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="T24" s="6"/>
     </row>
-    <row r="25" spans="1:20" s="18" customFormat="1">
+    <row r="25" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>75</v>
       </c>
       <c r="B25" s="6"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="1:20" s="18" customFormat="1">
+    <row r="26" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="C26" s="19">
         <v>2015</v>
@@ -4717,7 +4717,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="18" customFormat="1">
+    <row r="27" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>34</v>
       </c>
@@ -4790,14 +4790,14 @@
       </c>
       <c r="T27" s="29"/>
     </row>
-    <row r="31" spans="1:20" s="18" customFormat="1">
+    <row r="31" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>76</v>
       </c>
       <c r="B31" s="6"/>
       <c r="T31" s="6"/>
     </row>
-    <row r="32" spans="1:20" s="18" customFormat="1">
+    <row r="32" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="C32" s="19">
         <v>2015</v>
@@ -4851,7 +4851,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="18" customFormat="1">
+    <row r="33" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>34</v>
       </c>
@@ -4908,26 +4908,26 @@
       </c>
       <c r="T33" s="29"/>
     </row>
-    <row r="34" spans="1:20" s="18" customFormat="1">
+    <row r="34" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="T34" s="6"/>
     </row>
-    <row r="35" spans="1:20" s="18" customFormat="1">
+    <row r="35" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="T35" s="6"/>
     </row>
-    <row r="36" spans="1:20" s="18" customFormat="1">
+    <row r="36" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="T36" s="6"/>
     </row>
-    <row r="37" spans="1:20" s="18" customFormat="1">
+    <row r="37" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>77</v>
       </c>
       <c r="B37" s="6"/>
       <c r="T37" s="6"/>
     </row>
-    <row r="38" spans="1:20" s="18" customFormat="1">
+    <row r="38" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="19">
         <v>2015</v>
@@ -4981,7 +4981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="18" customFormat="1">
+    <row r="39" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>34</v>
       </c>
@@ -5006,26 +5006,26 @@
       </c>
       <c r="T39" s="29"/>
     </row>
-    <row r="40" spans="1:20" s="18" customFormat="1">
+    <row r="40" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="T40" s="6"/>
     </row>
-    <row r="41" spans="1:20" s="18" customFormat="1">
+    <row r="41" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="T41" s="6"/>
     </row>
-    <row r="42" spans="1:20" s="18" customFormat="1">
+    <row r="42" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="T42" s="6"/>
     </row>
-    <row r="43" spans="1:20" s="18" customFormat="1">
+    <row r="43" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>78</v>
       </c>
       <c r="B43" s="6"/>
       <c r="T43" s="6"/>
     </row>
-    <row r="44" spans="1:20" s="18" customFormat="1">
+    <row r="44" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="C44" s="19">
         <v>2015</v>
@@ -5079,7 +5079,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:20" s="18" customFormat="1">
+    <row r="45" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>34</v>
       </c>
@@ -5104,14 +5104,14 @@
       </c>
       <c r="T45" s="29"/>
     </row>
-    <row r="49" spans="1:20" s="18" customFormat="1">
+    <row r="49" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>79</v>
       </c>
       <c r="B49" s="6"/>
       <c r="T49" s="6"/>
     </row>
-    <row r="50" spans="1:20" s="18" customFormat="1">
+    <row r="50" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="C50" s="19">
         <v>2015</v>
@@ -5165,7 +5165,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:20" s="18" customFormat="1">
+    <row r="51" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>34</v>
       </c>
@@ -5190,26 +5190,26 @@
       </c>
       <c r="T51" s="29"/>
     </row>
-    <row r="52" spans="1:20" s="18" customFormat="1">
+    <row r="52" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="T52" s="6"/>
     </row>
-    <row r="53" spans="1:20" s="18" customFormat="1">
+    <row r="53" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="T53" s="6"/>
     </row>
-    <row r="54" spans="1:20" s="18" customFormat="1">
+    <row r="54" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="T54" s="6"/>
     </row>
-    <row r="55" spans="1:20" s="18" customFormat="1">
+    <row r="55" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
         <v>80</v>
       </c>
       <c r="B55" s="6"/>
       <c r="T55" s="6"/>
     </row>
-    <row r="56" spans="1:20" s="18" customFormat="1">
+    <row r="56" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="C56" s="19">
         <v>2015</v>
@@ -5263,7 +5263,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:20" s="18" customFormat="1">
+    <row r="57" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
         <v>34</v>
       </c>
@@ -5300,7 +5300,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:V28"/>
   <sheetViews>
@@ -5308,21 +5308,21 @@
       <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.125" style="18"/>
+    <col min="1" max="2" width="9.140625" style="18"/>
     <col min="3" max="3" width="11" style="18" customWidth="1"/>
-    <col min="4" max="20" width="9.125" style="18"/>
-    <col min="21" max="21" width="15.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.125" style="18"/>
+    <col min="4" max="20" width="9.140625" style="18"/>
+    <col min="21" max="21" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D2" s="19">
         <v>2000</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$D$14</f>
         <v>NSP</v>
@@ -5418,7 +5418,7 @@
       </c>
       <c r="U3" s="25"/>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$D$14</f>
         <v>NSP</v>
@@ -5468,10 +5468,10 @@
       </c>
       <c r="U4" s="39"/>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$D$15</f>
         <v>OST</v>
@@ -5502,7 +5502,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$D$15</f>
         <v>OST</v>
@@ -5533,10 +5533,10 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="str">
         <f>'Populations &amp; programs'!$D$16</f>
         <v>MSM programs</v>
@@ -5567,7 +5567,7 @@
       </c>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="4" t="str">
         <f>'Populations &amp; programs'!$D$16</f>
@@ -5599,11 +5599,11 @@
       </c>
       <c r="U10" s="39"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="4" t="str">
         <f>'Populations &amp; programs'!$D$17</f>
@@ -5636,7 +5636,7 @@
       <c r="U12" s="25"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="str">
         <f>'Populations &amp; programs'!$D$17</f>
         <v>FSW programs</v>
@@ -5667,7 +5667,7 @@
       </c>
       <c r="U13" s="39"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$D$18</f>
         <v>ART</v>
@@ -5698,7 +5698,7 @@
       </c>
       <c r="U15" s="25"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$D$18</f>
         <v>ART</v>
@@ -5729,7 +5729,7 @@
       </c>
       <c r="U16" s="39"/>
     </row>
-    <row r="18" spans="2:21">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$D$19</f>
         <v>HTC</v>
@@ -5760,7 +5760,7 @@
       </c>
       <c r="U18" s="25"/>
     </row>
-    <row r="19" spans="2:21">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$D$19</f>
         <v>HTC</v>
@@ -5791,7 +5791,7 @@
       </c>
       <c r="U19" s="39"/>
     </row>
-    <row r="21" spans="2:21">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="str">
         <f>'Populations &amp; programs'!$D$20</f>
         <v>SBCC</v>
@@ -5822,7 +5822,7 @@
       </c>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="2:21">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="str">
         <f>'Populations &amp; programs'!$D$20</f>
         <v>SBCC</v>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="U22" s="39"/>
     </row>
-    <row r="24" spans="2:21">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="str">
         <f>'Populations &amp; programs'!$D$21</f>
         <v>STI programs</v>
@@ -5884,7 +5884,7 @@
       </c>
       <c r="U24" s="25"/>
     </row>
-    <row r="25" spans="2:21">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="str">
         <f>'Populations &amp; programs'!$D$21</f>
         <v>STI programs</v>
@@ -5915,7 +5915,7 @@
       </c>
       <c r="U25" s="39"/>
     </row>
-    <row r="27" spans="2:21">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="str">
         <f>'Populations &amp; programs'!$D$22</f>
         <v>PMTCT</v>
@@ -5946,7 +5946,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="2:21">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="str">
         <f>'Populations &amp; programs'!$D$22</f>
         <v>PMTCT</v>
@@ -5989,7 +5989,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U53"/>
   <sheetViews>
@@ -5997,22 +5997,22 @@
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.125" style="18"/>
-    <col min="4" max="4" width="9.375" style="18" customWidth="1"/>
-    <col min="5" max="20" width="9.125" style="18"/>
-    <col min="21" max="21" width="15.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.875" style="18" customWidth="1"/>
-    <col min="23" max="16384" width="9.125" style="18"/>
+    <col min="1" max="3" width="9.140625" style="18"/>
+    <col min="4" max="4" width="9.42578125" style="18" customWidth="1"/>
+    <col min="5" max="20" width="9.140625" style="18"/>
+    <col min="21" max="21" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" style="18" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D2" s="19">
         <v>2000</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -6096,7 +6096,7 @@
         <v>37500</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -6127,7 +6127,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -6158,12 +6158,12 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="U6" s="28"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -6192,7 +6192,7 @@
       </c>
       <c r="U7" s="27"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -6223,7 +6223,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -6252,7 +6252,7 @@
       </c>
       <c r="U9" s="27"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="28"/>
@@ -6273,7 +6273,7 @@
       <c r="S10" s="28"/>
       <c r="U10" s="28"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -6312,7 +6312,7 @@
       </c>
       <c r="U11" s="27"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -6351,7 +6351,7 @@
       </c>
       <c r="U12" s="27"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -6390,7 +6390,7 @@
       </c>
       <c r="U13" s="27"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="28"/>
@@ -6411,7 +6411,7 @@
       <c r="S14" s="28"/>
       <c r="U14" s="28"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -6440,7 +6440,7 @@
       </c>
       <c r="U15" s="27"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -6501,7 +6501,7 @@
       </c>
       <c r="U16" s="27"/>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -6530,7 +6530,7 @@
       </c>
       <c r="U17" s="27"/>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="28"/>
@@ -6551,7 +6551,7 @@
       <c r="S18" s="28"/>
       <c r="U18" s="28"/>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -6580,7 +6580,7 @@
       </c>
       <c r="U19" s="27"/>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -6641,7 +6641,7 @@
       </c>
       <c r="U20" s="27"/>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -6670,7 +6670,7 @@
       </c>
       <c r="U21" s="27"/>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="28"/>
@@ -6691,7 +6691,7 @@
       <c r="S22" s="28"/>
       <c r="U22" s="28"/>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -6720,7 +6720,7 @@
       </c>
       <c r="U23" s="27"/>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -6781,7 +6781,7 @@
       </c>
       <c r="U24" s="27"/>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -6810,12 +6810,12 @@
       </c>
       <c r="U25" s="27"/>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D30" s="19">
         <v>2000</v>
       </c>
@@ -6868,7 +6868,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -6899,7 +6899,7 @@
       </c>
       <c r="U31" s="26"/>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -6930,7 +6930,7 @@
       </c>
       <c r="U32" s="26"/>
     </row>
-    <row r="33" spans="2:21">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -6961,11 +6961,11 @@
       </c>
       <c r="U33" s="26"/>
     </row>
-    <row r="34" spans="2:21">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
     </row>
-    <row r="35" spans="2:21">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -7000,7 +7000,7 @@
       </c>
       <c r="U35" s="26"/>
     </row>
-    <row r="36" spans="2:21">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -7035,7 +7035,7 @@
       </c>
       <c r="U36" s="26"/>
     </row>
-    <row r="37" spans="2:21">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -7070,11 +7070,11 @@
       </c>
       <c r="U37" s="26"/>
     </row>
-    <row r="38" spans="2:21">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
     </row>
-    <row r="39" spans="2:21">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -7109,7 +7109,7 @@
       </c>
       <c r="U39" s="26"/>
     </row>
-    <row r="40" spans="2:21">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -7144,7 +7144,7 @@
       </c>
       <c r="U40" s="26"/>
     </row>
-    <row r="41" spans="2:21">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -7179,11 +7179,11 @@
       </c>
       <c r="U41" s="26"/>
     </row>
-    <row r="42" spans="2:21">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
     </row>
-    <row r="43" spans="2:21">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -7212,7 +7212,7 @@
       </c>
       <c r="U43" s="26"/>
     </row>
-    <row r="44" spans="2:21">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -7243,7 +7243,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="45" spans="2:21">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -7272,11 +7272,11 @@
       </c>
       <c r="U45" s="26"/>
     </row>
-    <row r="46" spans="2:21">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
     </row>
-    <row r="47" spans="2:21">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -7305,7 +7305,7 @@
       </c>
       <c r="U47" s="26"/>
     </row>
-    <row r="48" spans="2:21">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -7342,7 +7342,7 @@
       </c>
       <c r="U48" s="26"/>
     </row>
-    <row r="49" spans="2:21">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -7371,11 +7371,11 @@
       </c>
       <c r="U49" s="26"/>
     </row>
-    <row r="50" spans="2:21">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
     </row>
-    <row r="51" spans="2:21">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -7404,7 +7404,7 @@
       </c>
       <c r="U51" s="26"/>
     </row>
-    <row r="52" spans="2:21">
+    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -7435,7 +7435,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="53" spans="2:21">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -7476,7 +7476,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T33"/>
   <sheetViews>
@@ -7484,13 +7484,13 @@
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="20" max="20" width="14.25" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>124</v>
       </c>
@@ -7513,7 +7513,7 @@
       <c r="S1" s="9"/>
       <c r="T1" s="9"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="C2" s="10">
         <v>2000</v>
@@ -7568,7 +7568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="4" t="s">
         <v>34</v>
@@ -7594,13 +7594,13 @@
       </c>
       <c r="T3" s="22"/>
     </row>
-    <row r="5" spans="1:20" s="18" customFormat="1">
+    <row r="5" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:20" s="18" customFormat="1">
+    <row r="6" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>125</v>
       </c>
@@ -7623,7 +7623,7 @@
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="C8" s="10">
         <v>2000</v>
@@ -7678,7 +7678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
         <v>34</v>
@@ -7728,13 +7728,13 @@
       </c>
       <c r="T9" s="22"/>
     </row>
-    <row r="11" spans="1:20" s="18" customFormat="1">
+    <row r="11" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:20" s="18" customFormat="1">
+    <row r="12" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>126</v>
       </c>
@@ -7757,7 +7757,7 @@
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="C14" s="10">
         <v>2000</v>
@@ -7812,7 +7812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="4" t="s">
         <v>34</v>
@@ -7838,19 +7838,19 @@
       </c>
       <c r="T15" s="22"/>
     </row>
-    <row r="17" spans="1:20" s="18" customFormat="1">
+    <row r="17" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:20" s="18" customFormat="1">
+    <row r="18" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:20" s="18" customFormat="1">
+    <row r="19" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>84</v>
       </c>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:20" s="18" customFormat="1">
+    <row r="20" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="19">
         <v>2000</v>
@@ -7904,7 +7904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="18" customFormat="1">
+    <row r="21" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>34</v>
       </c>
@@ -7929,16 +7929,16 @@
       </c>
       <c r="T21" s="22"/>
     </row>
-    <row r="22" spans="1:20" s="18" customFormat="1">
+    <row r="22" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:20" s="18" customFormat="1">
+    <row r="23" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:20" s="18" customFormat="1">
+    <row r="24" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>116</v>
       </c>
@@ -7961,7 +7961,7 @@
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="C26" s="10">
         <v>2000</v>
@@ -8016,7 +8016,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="4" t="s">
         <v>34</v>
@@ -8042,13 +8042,13 @@
       </c>
       <c r="T27" s="22"/>
     </row>
-    <row r="31" spans="1:20" s="18" customFormat="1">
+    <row r="31" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>151</v>
       </c>
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="1:20" s="18" customFormat="1">
+    <row r="32" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="C32" s="19">
         <v>2000</v>
@@ -8102,7 +8102,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="2:20" s="18" customFormat="1">
+    <row r="33" spans="2:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>34</v>
       </c>
@@ -8139,7 +8139,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS42"/>
   <sheetViews>
@@ -8147,24 +8147,24 @@
       <selection activeCell="AP23" sqref="AP23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="21" max="21" width="9.125" customWidth="1"/>
-    <col min="22" max="22" width="8.875" customWidth="1"/>
-    <col min="23" max="23" width="10.375" style="6" customWidth="1"/>
-    <col min="28" max="28" width="8.875" style="18" customWidth="1"/>
-    <col min="29" max="29" width="10.375" style="6" customWidth="1"/>
-    <col min="30" max="33" width="8.625" style="18"/>
-    <col min="34" max="34" width="8.875" style="18" customWidth="1"/>
-    <col min="35" max="35" width="10.375" style="6" customWidth="1"/>
-    <col min="36" max="39" width="8.625" style="18"/>
-    <col min="40" max="40" width="8.875" style="18" customWidth="1"/>
-    <col min="41" max="41" width="10.375" style="6" customWidth="1"/>
-    <col min="42" max="45" width="8.625" style="18"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="21" max="21" width="9.140625" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" style="6" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" style="18" customWidth="1"/>
+    <col min="29" max="29" width="10.42578125" style="6" customWidth="1"/>
+    <col min="30" max="33" width="8.5703125" style="18"/>
+    <col min="34" max="34" width="8.85546875" style="18" customWidth="1"/>
+    <col min="35" max="35" width="10.42578125" style="6" customWidth="1"/>
+    <col min="36" max="39" width="8.5703125" style="18"/>
+    <col min="40" max="40" width="8.85546875" style="18" customWidth="1"/>
+    <col min="41" max="41" width="10.42578125" style="6" customWidth="1"/>
+    <col min="42" max="45" width="8.5703125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="18" customFormat="1">
+    <row r="1" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>123</v>
       </c>
@@ -8198,7 +8198,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="18" customFormat="1">
+    <row r="2" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="19">
         <v>2000</v>
@@ -8312,7 +8312,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:45" s="18" customFormat="1">
+    <row r="3" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -8360,7 +8360,7 @@
       <c r="AR3" s="25"/>
       <c r="AS3" s="25"/>
     </row>
-    <row r="4" spans="1:45" s="18" customFormat="1">
+    <row r="4" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -8408,7 +8408,7 @@
       <c r="AR4" s="25"/>
       <c r="AS4" s="25"/>
     </row>
-    <row r="5" spans="1:45" s="18" customFormat="1">
+    <row r="5" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -8456,7 +8456,7 @@
       <c r="AR5" s="25"/>
       <c r="AS5" s="25"/>
     </row>
-    <row r="6" spans="1:45" s="18" customFormat="1">
+    <row r="6" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -8504,7 +8504,7 @@
       <c r="AR6" s="25"/>
       <c r="AS6" s="25"/>
     </row>
-    <row r="7" spans="1:45" s="18" customFormat="1">
+    <row r="7" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -8552,7 +8552,7 @@
       <c r="AR7" s="25"/>
       <c r="AS7" s="25"/>
     </row>
-    <row r="8" spans="1:45" s="18" customFormat="1">
+    <row r="8" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -8600,28 +8600,28 @@
       <c r="AR8" s="25"/>
       <c r="AS8" s="25"/>
     </row>
-    <row r="9" spans="1:45" s="18" customFormat="1">
+    <row r="9" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="W9" s="6"/>
       <c r="AC9" s="6"/>
       <c r="AI9" s="6"/>
       <c r="AO9" s="6"/>
     </row>
-    <row r="10" spans="1:45" s="18" customFormat="1">
+    <row r="10" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="W10" s="6"/>
       <c r="AC10" s="6"/>
       <c r="AI10" s="6"/>
       <c r="AO10" s="6"/>
     </row>
-    <row r="11" spans="1:45" s="18" customFormat="1">
+    <row r="11" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="W11" s="6"/>
       <c r="AC11" s="6"/>
       <c r="AI11" s="6"/>
       <c r="AO11" s="6"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>150</v>
       </c>
@@ -8669,7 +8669,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="C13" s="8">
         <v>2000</v>
@@ -8784,7 +8784,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -8843,7 +8843,7 @@
       <c r="AR14" s="25"/>
       <c r="AS14" s="25"/>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -8902,7 +8902,7 @@
       <c r="AR15" s="25"/>
       <c r="AS15" s="25"/>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -8961,7 +8961,7 @@
       <c r="AR16" s="25"/>
       <c r="AS16" s="25"/>
     </row>
-    <row r="17" spans="1:45">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -9020,7 +9020,7 @@
       <c r="AR17" s="25"/>
       <c r="AS17" s="25"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -9079,7 +9079,7 @@
       <c r="AR18" s="25"/>
       <c r="AS18" s="25"/>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
@@ -9138,28 +9138,28 @@
       <c r="AR19" s="25"/>
       <c r="AS19" s="25"/>
     </row>
-    <row r="20" spans="1:45" s="18" customFormat="1">
+    <row r="20" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="W20" s="6"/>
       <c r="AC20" s="6"/>
       <c r="AI20" s="6"/>
       <c r="AO20" s="6"/>
     </row>
-    <row r="21" spans="1:45" s="18" customFormat="1">
+    <row r="21" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="W21" s="6"/>
       <c r="AC21" s="6"/>
       <c r="AI21" s="6"/>
       <c r="AO21" s="6"/>
     </row>
-    <row r="22" spans="1:45" s="18" customFormat="1">
+    <row r="22" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="W22" s="6"/>
       <c r="AC22" s="6"/>
       <c r="AI22" s="6"/>
       <c r="AO22" s="6"/>
     </row>
-    <row r="23" spans="1:45" s="18" customFormat="1">
+    <row r="23" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>71</v>
       </c>
@@ -9193,7 +9193,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:45" s="18" customFormat="1">
+    <row r="24" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="19">
         <v>2000</v>
@@ -9307,7 +9307,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:45" s="18" customFormat="1">
+    <row r="25" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -9365,7 +9365,7 @@
       <c r="AR25" s="25"/>
       <c r="AS25" s="25"/>
     </row>
-    <row r="26" spans="1:45" s="18" customFormat="1">
+    <row r="26" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -9423,7 +9423,7 @@
       <c r="AR26" s="25"/>
       <c r="AS26" s="25"/>
     </row>
-    <row r="27" spans="1:45" s="18" customFormat="1">
+    <row r="27" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -9481,7 +9481,7 @@
       <c r="AR27" s="25"/>
       <c r="AS27" s="25"/>
     </row>
-    <row r="28" spans="1:45" s="18" customFormat="1">
+    <row r="28" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -9539,7 +9539,7 @@
       <c r="AR28" s="25"/>
       <c r="AS28" s="25"/>
     </row>
-    <row r="29" spans="1:45" s="18" customFormat="1">
+    <row r="29" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -9597,7 +9597,7 @@
       <c r="AR29" s="25"/>
       <c r="AS29" s="25"/>
     </row>
-    <row r="30" spans="1:45" s="18" customFormat="1">
+    <row r="30" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -9655,10 +9655,10 @@
       <c r="AR30" s="25"/>
       <c r="AS30" s="25"/>
     </row>
-    <row r="31" spans="1:45">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
       <c r="S31" s="5"/>
     </row>
-    <row r="32" spans="1:45" s="18" customFormat="1">
+    <row r="32" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="S32" s="5"/>
       <c r="W32" s="6"/>
@@ -9666,7 +9666,7 @@
       <c r="AI32" s="6"/>
       <c r="AO32" s="6"/>
     </row>
-    <row r="33" spans="1:45" s="18" customFormat="1">
+    <row r="33" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="S33" s="5"/>
       <c r="W33" s="6"/>
@@ -9674,7 +9674,7 @@
       <c r="AI33" s="6"/>
       <c r="AO33" s="6"/>
     </row>
-    <row r="34" spans="1:45">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>38</v>
       </c>
@@ -9723,7 +9723,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:45">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="C35" s="8">
         <v>2000</v>
@@ -9838,7 +9838,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:45">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -9887,7 +9887,7 @@
       <c r="AR36" s="25"/>
       <c r="AS36" s="25"/>
     </row>
-    <row r="37" spans="1:45">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -9935,7 +9935,7 @@
       <c r="AR37" s="25"/>
       <c r="AS37" s="25"/>
     </row>
-    <row r="38" spans="1:45">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -9983,7 +9983,7 @@
       <c r="AR38" s="25"/>
       <c r="AS38" s="25"/>
     </row>
-    <row r="39" spans="1:45">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -10031,7 +10031,7 @@
       <c r="AR39" s="25"/>
       <c r="AS39" s="25"/>
     </row>
-    <row r="40" spans="1:45">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -10079,7 +10079,7 @@
       <c r="AR40" s="25"/>
       <c r="AS40" s="25"/>
     </row>
-    <row r="41" spans="1:45">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -10127,7 +10127,7 @@
       <c r="AR41" s="25"/>
       <c r="AS41" s="25"/>
     </row>
-    <row r="42" spans="1:45">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="S42" s="5"/>
     </row>
   </sheetData>
@@ -10142,7 +10142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS71"/>
   <sheetViews>
@@ -10150,20 +10150,20 @@
       <selection activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="20" max="20" width="14.25" customWidth="1"/>
-    <col min="23" max="23" width="12.375" style="6" customWidth="1"/>
-    <col min="29" max="29" width="12.375" style="6" customWidth="1"/>
-    <col min="30" max="33" width="8.625" style="18"/>
-    <col min="35" max="35" width="12.375" style="6" customWidth="1"/>
-    <col min="36" max="39" width="8.625" style="18"/>
-    <col min="41" max="41" width="12.375" style="6" customWidth="1"/>
-    <col min="42" max="45" width="8.625" style="18"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" style="6" customWidth="1"/>
+    <col min="29" max="29" width="12.42578125" style="6" customWidth="1"/>
+    <col min="30" max="33" width="8.5703125" style="18"/>
+    <col min="35" max="35" width="12.42578125" style="6" customWidth="1"/>
+    <col min="36" max="39" width="8.5703125" style="18"/>
+    <col min="41" max="41" width="12.42578125" style="6" customWidth="1"/>
+    <col min="42" max="45" width="8.5703125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>117</v>
       </c>
@@ -10212,7 +10212,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="C2" s="10">
         <v>2000</v>
@@ -10327,7 +10327,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -10386,7 +10386,7 @@
       <c r="AR3" s="25"/>
       <c r="AS3" s="25"/>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -10447,7 +10447,7 @@
       <c r="AR4" s="25"/>
       <c r="AS4" s="25"/>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -10510,7 +10510,7 @@
       <c r="AR5" s="25"/>
       <c r="AS5" s="25"/>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -10569,7 +10569,7 @@
       <c r="AR6" s="25"/>
       <c r="AS6" s="25"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -10628,7 +10628,7 @@
       <c r="AR7" s="25"/>
       <c r="AS7" s="25"/>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
@@ -10687,21 +10687,21 @@
       <c r="AR8" s="25"/>
       <c r="AS8" s="25"/>
     </row>
-    <row r="10" spans="1:45" s="18" customFormat="1">
+    <row r="10" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="W10" s="6"/>
       <c r="AC10" s="6"/>
       <c r="AI10" s="6"/>
       <c r="AO10" s="6"/>
     </row>
-    <row r="11" spans="1:45" s="18" customFormat="1">
+    <row r="11" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="W11" s="6"/>
       <c r="AC11" s="6"/>
       <c r="AI11" s="6"/>
       <c r="AO11" s="6"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>127</v>
       </c>
@@ -10750,7 +10750,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="C13" s="10">
         <v>2000</v>
@@ -10865,7 +10865,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="4" t="s">
         <v>35</v>
@@ -10923,21 +10923,21 @@
       <c r="AR14" s="25"/>
       <c r="AS14" s="25"/>
     </row>
-    <row r="16" spans="1:45" s="18" customFormat="1">
+    <row r="16" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="W16" s="6"/>
       <c r="AC16" s="6"/>
       <c r="AI16" s="6"/>
       <c r="AO16" s="6"/>
     </row>
-    <row r="17" spans="1:45" s="18" customFormat="1">
+    <row r="17" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="W17" s="6"/>
       <c r="AC17" s="6"/>
       <c r="AI17" s="6"/>
       <c r="AO17" s="6"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>82</v>
       </c>
@@ -10986,7 +10986,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="C19" s="10">
         <v>2000</v>
@@ -11101,7 +11101,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:45">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="4" t="s">
         <v>34</v>
@@ -11185,21 +11185,21 @@
       <c r="AR20" s="39"/>
       <c r="AS20" s="39"/>
     </row>
-    <row r="21" spans="1:45" s="18" customFormat="1">
+    <row r="21" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="W21" s="6"/>
       <c r="AC21" s="6"/>
       <c r="AI21" s="6"/>
       <c r="AO21" s="6"/>
     </row>
-    <row r="22" spans="1:45" s="18" customFormat="1">
+    <row r="22" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="W22" s="6"/>
       <c r="AC22" s="6"/>
       <c r="AI22" s="6"/>
       <c r="AO22" s="6"/>
     </row>
-    <row r="24" spans="1:45">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>115</v>
       </c>
@@ -11248,7 +11248,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:45">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="C25" s="10">
         <v>2000</v>
@@ -11363,7 +11363,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:45">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="4" t="s">
         <v>34</v>
@@ -11447,28 +11447,28 @@
       <c r="AR26" s="39"/>
       <c r="AS26" s="39"/>
     </row>
-    <row r="27" spans="1:45" s="18" customFormat="1">
+    <row r="27" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="W27" s="6"/>
       <c r="AC27" s="6"/>
       <c r="AI27" s="6"/>
       <c r="AO27" s="6"/>
     </row>
-    <row r="28" spans="1:45" s="18" customFormat="1" ht="14.25" customHeight="1">
+    <row r="28" spans="1:45" s="18" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="W28" s="6"/>
       <c r="AC28" s="6"/>
       <c r="AI28" s="6"/>
       <c r="AO28" s="6"/>
     </row>
-    <row r="29" spans="1:45" s="18" customFormat="1">
+    <row r="29" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="W29" s="6"/>
       <c r="AC29" s="6"/>
       <c r="AI29" s="6"/>
       <c r="AO29" s="6"/>
     </row>
-    <row r="30" spans="1:45" s="18" customFormat="1">
+    <row r="30" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>2</v>
       </c>
@@ -11502,7 +11502,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:45" s="18" customFormat="1">
+    <row r="31" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="C31" s="19">
         <v>2000</v>
@@ -11616,7 +11616,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:45" s="18" customFormat="1">
+    <row r="32" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -11664,7 +11664,7 @@
       <c r="AR32" s="25"/>
       <c r="AS32" s="25"/>
     </row>
-    <row r="33" spans="1:45" s="18" customFormat="1">
+    <row r="33" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -11712,7 +11712,7 @@
       <c r="AR33" s="25"/>
       <c r="AS33" s="25"/>
     </row>
-    <row r="34" spans="1:45" s="18" customFormat="1">
+    <row r="34" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -11760,7 +11760,7 @@
       <c r="AR34" s="25"/>
       <c r="AS34" s="25"/>
     </row>
-    <row r="35" spans="1:45" s="18" customFormat="1">
+    <row r="35" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -11808,7 +11808,7 @@
       <c r="AR35" s="25"/>
       <c r="AS35" s="25"/>
     </row>
-    <row r="36" spans="1:45" s="18" customFormat="1">
+    <row r="36" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -11857,7 +11857,7 @@
       <c r="AR36" s="25"/>
       <c r="AS36" s="25"/>
     </row>
-    <row r="37" spans="1:45" s="18" customFormat="1">
+    <row r="37" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -11905,21 +11905,21 @@
       <c r="AR37" s="25"/>
       <c r="AS37" s="25"/>
     </row>
-    <row r="38" spans="1:45" s="18" customFormat="1">
+    <row r="38" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="W38" s="6"/>
       <c r="AC38" s="6"/>
       <c r="AI38" s="6"/>
       <c r="AO38" s="6"/>
     </row>
-    <row r="40" spans="1:45" s="18" customFormat="1">
+    <row r="40" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="W40" s="6"/>
       <c r="AC40" s="6"/>
       <c r="AI40" s="6"/>
       <c r="AO40" s="6"/>
     </row>
-    <row r="41" spans="1:45" s="18" customFormat="1">
+    <row r="41" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>3</v>
       </c>
@@ -11953,7 +11953,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:45" s="18" customFormat="1">
+    <row r="42" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="C42" s="19">
         <v>2000</v>
@@ -12067,7 +12067,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:45" s="18" customFormat="1">
+    <row r="43" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -12115,7 +12115,7 @@
       <c r="AR43" s="25"/>
       <c r="AS43" s="25"/>
     </row>
-    <row r="44" spans="1:45" s="18" customFormat="1">
+    <row r="44" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -12163,7 +12163,7 @@
       <c r="AR44" s="25"/>
       <c r="AS44" s="25"/>
     </row>
-    <row r="45" spans="1:45" s="18" customFormat="1">
+    <row r="45" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -12211,7 +12211,7 @@
       <c r="AR45" s="25"/>
       <c r="AS45" s="25"/>
     </row>
-    <row r="46" spans="1:45" s="18" customFormat="1">
+    <row r="46" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -12259,7 +12259,7 @@
       <c r="AR46" s="25"/>
       <c r="AS46" s="25"/>
     </row>
-    <row r="47" spans="1:45" s="18" customFormat="1">
+    <row r="47" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -12308,7 +12308,7 @@
       <c r="AR47" s="25"/>
       <c r="AS47" s="25"/>
     </row>
-    <row r="48" spans="1:45" s="18" customFormat="1">
+    <row r="48" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -12356,28 +12356,28 @@
       <c r="AR48" s="25"/>
       <c r="AS48" s="25"/>
     </row>
-    <row r="49" spans="1:45" s="18" customFormat="1">
+    <row r="49" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="W49" s="6"/>
       <c r="AC49" s="6"/>
       <c r="AI49" s="6"/>
       <c r="AO49" s="6"/>
     </row>
-    <row r="50" spans="1:45" s="18" customFormat="1">
+    <row r="50" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="W50" s="6"/>
       <c r="AC50" s="6"/>
       <c r="AI50" s="6"/>
       <c r="AO50" s="6"/>
     </row>
-    <row r="51" spans="1:45" s="18" customFormat="1">
+    <row r="51" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="W51" s="6"/>
       <c r="AC51" s="6"/>
       <c r="AI51" s="6"/>
       <c r="AO51" s="6"/>
     </row>
-    <row r="52" spans="1:45">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>0</v>
       </c>
@@ -12426,7 +12426,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:45">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="C53" s="10">
         <v>2000</v>
@@ -12541,7 +12541,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:45">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="4" t="s">
         <v>34</v>
@@ -12607,28 +12607,28 @@
       <c r="AR54" s="25"/>
       <c r="AS54" s="25"/>
     </row>
-    <row r="55" spans="1:45" s="18" customFormat="1">
+    <row r="55" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="W55" s="6"/>
       <c r="AC55" s="6"/>
       <c r="AI55" s="6"/>
       <c r="AO55" s="6"/>
     </row>
-    <row r="56" spans="1:45" s="18" customFormat="1">
+    <row r="56" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="W56" s="6"/>
       <c r="AC56" s="6"/>
       <c r="AI56" s="6"/>
       <c r="AO56" s="6"/>
     </row>
-    <row r="57" spans="1:45" s="18" customFormat="1">
+    <row r="57" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="W57" s="6"/>
       <c r="AC57" s="6"/>
       <c r="AI57" s="6"/>
       <c r="AO57" s="6"/>
     </row>
-    <row r="58" spans="1:45" s="18" customFormat="1">
+    <row r="58" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>118</v>
       </c>
@@ -12662,7 +12662,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:45" s="18" customFormat="1">
+    <row r="59" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="C59" s="19">
         <v>2000</v>
@@ -12776,7 +12776,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:45" s="18" customFormat="1">
+    <row r="60" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -12824,7 +12824,7 @@
       <c r="AR60" s="25"/>
       <c r="AS60" s="25"/>
     </row>
-    <row r="61" spans="1:45" s="18" customFormat="1">
+    <row r="61" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -12872,7 +12872,7 @@
       <c r="AR61" s="25"/>
       <c r="AS61" s="25"/>
     </row>
-    <row r="62" spans="1:45" s="18" customFormat="1">
+    <row r="62" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -12920,7 +12920,7 @@
       <c r="AR62" s="25"/>
       <c r="AS62" s="25"/>
     </row>
-    <row r="63" spans="1:45" s="18" customFormat="1">
+    <row r="63" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -12968,7 +12968,7 @@
       <c r="AR63" s="25"/>
       <c r="AS63" s="25"/>
     </row>
-    <row r="64" spans="1:45" s="18" customFormat="1">
+    <row r="64" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -13017,7 +13017,7 @@
       <c r="AR64" s="25"/>
       <c r="AS64" s="25"/>
     </row>
-    <row r="65" spans="1:45" s="18" customFormat="1">
+    <row r="65" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -13065,7 +13065,7 @@
       <c r="AR65" s="25"/>
       <c r="AS65" s="25"/>
     </row>
-    <row r="69" spans="1:45" s="18" customFormat="1">
+    <row r="69" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
         <v>119</v>
       </c>
@@ -13099,7 +13099,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:45" s="18" customFormat="1">
+    <row r="70" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="C70" s="19">
         <v>2000</v>
@@ -13213,7 +13213,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:45" s="18" customFormat="1">
+    <row r="71" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
         <v>34</v>
       </c>
@@ -13272,7 +13272,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS85"/>
   <sheetViews>
@@ -13280,20 +13280,20 @@
       <selection activeCell="W80" sqref="W80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="20" max="20" width="14.375" style="31" customWidth="1"/>
-    <col min="23" max="23" width="11.375" customWidth="1"/>
-    <col min="29" max="29" width="11.375" style="18" customWidth="1"/>
-    <col min="30" max="33" width="8.625" style="18"/>
-    <col min="35" max="35" width="11.375" style="18" customWidth="1"/>
-    <col min="36" max="39" width="8.625" style="18"/>
-    <col min="41" max="41" width="11.375" style="18" customWidth="1"/>
-    <col min="42" max="45" width="8.625" style="18"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="20" max="20" width="14.42578125" style="31" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" customWidth="1"/>
+    <col min="29" max="29" width="11.42578125" style="18" customWidth="1"/>
+    <col min="30" max="33" width="8.5703125" style="18"/>
+    <col min="35" max="35" width="11.42578125" style="18" customWidth="1"/>
+    <col min="36" max="39" width="8.5703125" style="18"/>
+    <col min="41" max="41" width="11.42578125" style="18" customWidth="1"/>
+    <col min="42" max="45" width="8.5703125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>50</v>
       </c>
@@ -13341,7 +13341,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="C2" s="12">
         <v>2000</v>
@@ -13458,7 +13458,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -13509,7 +13509,7 @@
       <c r="AR3" s="34"/>
       <c r="AS3" s="34"/>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -13560,7 +13560,7 @@
       <c r="AR4" s="34"/>
       <c r="AS4" s="34"/>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -13611,7 +13611,7 @@
       <c r="AR5" s="34"/>
       <c r="AS5" s="34"/>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -13662,7 +13662,7 @@
       <c r="AR6" s="34"/>
       <c r="AS6" s="34"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -13713,7 +13713,7 @@
       <c r="AR7" s="34"/>
       <c r="AS7" s="34"/>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
@@ -13764,15 +13764,15 @@
       <c r="AR8" s="34"/>
       <c r="AS8" s="34"/>
     </row>
-    <row r="10" spans="1:45" s="18" customFormat="1">
+    <row r="10" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="T10" s="31"/>
     </row>
-    <row r="11" spans="1:45" s="18" customFormat="1">
+    <row r="11" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="T11" s="31"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>51</v>
       </c>
@@ -13820,7 +13820,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="C13" s="12">
         <v>2000</v>
@@ -13937,7 +13937,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -13988,7 +13988,7 @@
       <c r="AR14" s="30"/>
       <c r="AS14" s="30"/>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -14039,7 +14039,7 @@
       <c r="AR15" s="30"/>
       <c r="AS15" s="30"/>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -14090,7 +14090,7 @@
       <c r="AR16" s="30"/>
       <c r="AS16" s="30"/>
     </row>
-    <row r="17" spans="1:45">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -14141,7 +14141,7 @@
       <c r="AR17" s="30"/>
       <c r="AS17" s="30"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -14192,7 +14192,7 @@
       <c r="AR18" s="30"/>
       <c r="AS18" s="30"/>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
@@ -14243,15 +14243,15 @@
       <c r="AR19" s="30"/>
       <c r="AS19" s="30"/>
     </row>
-    <row r="21" spans="1:45" s="18" customFormat="1">
+    <row r="21" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="T21" s="31"/>
     </row>
-    <row r="22" spans="1:45" s="18" customFormat="1">
+    <row r="22" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="T22" s="31"/>
     </row>
-    <row r="23" spans="1:45">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>147</v>
       </c>
@@ -14299,7 +14299,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:45">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="C24" s="12">
         <v>2000</v>
@@ -14416,7 +14416,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:45">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -14467,7 +14467,7 @@
       <c r="AR25" s="30"/>
       <c r="AS25" s="30"/>
     </row>
-    <row r="26" spans="1:45">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -14518,7 +14518,7 @@
       <c r="AR26" s="30"/>
       <c r="AS26" s="30"/>
     </row>
-    <row r="27" spans="1:45">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -14569,7 +14569,7 @@
       <c r="AR27" s="30"/>
       <c r="AS27" s="30"/>
     </row>
-    <row r="28" spans="1:45">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -14620,7 +14620,7 @@
       <c r="AR28" s="30"/>
       <c r="AS28" s="30"/>
     </row>
-    <row r="29" spans="1:45">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -14671,7 +14671,7 @@
       <c r="AR29" s="30"/>
       <c r="AS29" s="30"/>
     </row>
-    <row r="30" spans="1:45">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
@@ -14722,15 +14722,15 @@
       <c r="AR30" s="30"/>
       <c r="AS30" s="30"/>
     </row>
-    <row r="32" spans="1:45" s="18" customFormat="1">
+    <row r="32" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="T32" s="31"/>
     </row>
-    <row r="33" spans="1:45" s="18" customFormat="1">
+    <row r="33" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="T33" s="31"/>
     </row>
-    <row r="34" spans="1:45">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>154</v>
       </c>
@@ -14778,7 +14778,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:45">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="C35" s="12">
         <v>2000</v>
@@ -14895,7 +14895,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:45">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -14956,7 +14956,7 @@
       <c r="AR36" s="30"/>
       <c r="AS36" s="30"/>
     </row>
-    <row r="37" spans="1:45">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -15025,7 +15025,7 @@
       <c r="AR37" s="30"/>
       <c r="AS37" s="30"/>
     </row>
-    <row r="38" spans="1:45">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -15086,7 +15086,7 @@
       <c r="AR38" s="30"/>
       <c r="AS38" s="30"/>
     </row>
-    <row r="39" spans="1:45">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -15147,7 +15147,7 @@
       <c r="AR39" s="30"/>
       <c r="AS39" s="30"/>
     </row>
-    <row r="40" spans="1:45">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -15208,7 +15208,7 @@
       <c r="AR40" s="30"/>
       <c r="AS40" s="30"/>
     </row>
-    <row r="41" spans="1:45">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
@@ -15269,15 +15269,15 @@
       <c r="AR41" s="30"/>
       <c r="AS41" s="30"/>
     </row>
-    <row r="43" spans="1:45" s="18" customFormat="1">
+    <row r="43" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="T43" s="31"/>
     </row>
-    <row r="44" spans="1:45" s="18" customFormat="1">
+    <row r="44" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="T44" s="31"/>
     </row>
-    <row r="45" spans="1:45">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>153</v>
       </c>
@@ -15325,7 +15325,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:45">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="C46" s="12">
         <v>2000</v>
@@ -15442,7 +15442,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:45">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -15503,7 +15503,7 @@
       <c r="AR47" s="30"/>
       <c r="AS47" s="30"/>
     </row>
-    <row r="48" spans="1:45">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -15572,7 +15572,7 @@
       <c r="AR48" s="30"/>
       <c r="AS48" s="30"/>
     </row>
-    <row r="49" spans="1:45">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -15633,7 +15633,7 @@
       <c r="AR49" s="30"/>
       <c r="AS49" s="30"/>
     </row>
-    <row r="50" spans="1:45">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -15698,7 +15698,7 @@
       <c r="AR50" s="30"/>
       <c r="AS50" s="30"/>
     </row>
-    <row r="51" spans="1:45">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -15763,7 +15763,7 @@
       <c r="AR51" s="30"/>
       <c r="AS51" s="30"/>
     </row>
-    <row r="52" spans="1:45">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
@@ -15824,15 +15824,15 @@
       <c r="AR52" s="30"/>
       <c r="AS52" s="30"/>
     </row>
-    <row r="54" spans="1:45" s="18" customFormat="1">
+    <row r="54" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="T54" s="31"/>
     </row>
-    <row r="55" spans="1:45" s="18" customFormat="1">
+    <row r="55" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="T55" s="31"/>
     </row>
-    <row r="56" spans="1:45">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>152</v>
       </c>
@@ -15880,7 +15880,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:45">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="C57" s="12">
         <v>2000</v>
@@ -15997,7 +15997,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:45">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -16048,7 +16048,7 @@
       <c r="AR58" s="30"/>
       <c r="AS58" s="30"/>
     </row>
-    <row r="59" spans="1:45">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -16117,7 +16117,7 @@
       <c r="AR59" s="30"/>
       <c r="AS59" s="30"/>
     </row>
-    <row r="60" spans="1:45">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -16168,7 +16168,7 @@
       <c r="AR60" s="30"/>
       <c r="AS60" s="30"/>
     </row>
-    <row r="61" spans="1:45">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -16219,7 +16219,7 @@
       <c r="AR61" s="30"/>
       <c r="AS61" s="30"/>
     </row>
-    <row r="62" spans="1:45">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -16270,7 +16270,7 @@
       <c r="AR62" s="30"/>
       <c r="AS62" s="30"/>
     </row>
-    <row r="63" spans="1:45">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
@@ -16339,15 +16339,15 @@
       <c r="AR63" s="30"/>
       <c r="AS63" s="30"/>
     </row>
-    <row r="65" spans="1:45" s="18" customFormat="1">
+    <row r="65" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="T65" s="31"/>
     </row>
-    <row r="66" spans="1:45" s="18" customFormat="1">
+    <row r="66" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="T66" s="31"/>
     </row>
-    <row r="67" spans="1:45">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>128</v>
       </c>
@@ -16395,7 +16395,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:45">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="C68" s="12">
         <v>2000</v>
@@ -16512,7 +16512,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:45">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -16563,7 +16563,7 @@
       <c r="AR69" s="30"/>
       <c r="AS69" s="30"/>
     </row>
-    <row r="70" spans="1:45">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -16614,7 +16614,7 @@
       <c r="AR70" s="30"/>
       <c r="AS70" s="30"/>
     </row>
-    <row r="71" spans="1:45">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -16665,7 +16665,7 @@
       <c r="AR71" s="30"/>
       <c r="AS71" s="30"/>
     </row>
-    <row r="72" spans="1:45">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -16716,7 +16716,7 @@
       <c r="AR72" s="30"/>
       <c r="AS72" s="30"/>
     </row>
-    <row r="73" spans="1:45">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -16767,7 +16767,7 @@
       <c r="AR73" s="30"/>
       <c r="AS73" s="30"/>
     </row>
-    <row r="74" spans="1:45">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
@@ -16818,19 +16818,19 @@
       <c r="AR74" s="30"/>
       <c r="AS74" s="30"/>
     </row>
-    <row r="75" spans="1:45" s="18" customFormat="1">
+    <row r="75" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="T75" s="31"/>
     </row>
-    <row r="76" spans="1:45" s="18" customFormat="1">
+    <row r="76" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
       <c r="T76" s="31"/>
     </row>
-    <row r="77" spans="1:45" s="18" customFormat="1">
+    <row r="77" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="T77" s="31"/>
     </row>
-    <row r="78" spans="1:45" s="18" customFormat="1">
+    <row r="78" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>1</v>
       </c>
@@ -16861,7 +16861,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:45" s="18" customFormat="1">
+    <row r="79" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="C79" s="19">
         <v>2000</v>
@@ -16977,7 +16977,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="1:45" s="18" customFormat="1">
+    <row r="80" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
         <v>MSM</v>
@@ -17027,7 +17027,7 @@
       <c r="AR80" s="30"/>
       <c r="AS80" s="30"/>
     </row>
-    <row r="81" spans="2:45" s="18" customFormat="1">
+    <row r="81" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
         <v>FSW</v>
@@ -17077,7 +17077,7 @@
       <c r="AR81" s="30"/>
       <c r="AS81" s="30"/>
     </row>
-    <row r="82" spans="2:45" s="18" customFormat="1">
+    <row r="82" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
         <v>Male PWID</v>
@@ -17127,7 +17127,7 @@
       <c r="AR82" s="30"/>
       <c r="AS82" s="30"/>
     </row>
-    <row r="83" spans="2:45" s="18" customFormat="1">
+    <row r="83" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
         <v>Other males</v>
@@ -17177,7 +17177,7 @@
       <c r="AR83" s="30"/>
       <c r="AS83" s="30"/>
     </row>
-    <row r="84" spans="2:45" s="18" customFormat="1">
+    <row r="84" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
         <v>Other females</v>
@@ -17227,7 +17227,7 @@
       <c r="AR84" s="30"/>
       <c r="AS84" s="30"/>
     </row>
-    <row r="85" spans="2:45" s="18" customFormat="1">
+    <row r="85" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
         <v>Clients</v>
@@ -17289,7 +17289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS20"/>
   <sheetViews>
@@ -17297,23 +17297,23 @@
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.375" style="31" customWidth="1"/>
-    <col min="21" max="21" width="8.625" style="31"/>
-    <col min="22" max="22" width="9.125" style="31" customWidth="1"/>
-    <col min="23" max="23" width="11.75" style="6" customWidth="1"/>
-    <col min="24" max="27" width="8.625" style="31"/>
-    <col min="29" max="29" width="11.75" style="6" customWidth="1"/>
-    <col min="30" max="33" width="8.625" style="31"/>
-    <col min="35" max="35" width="11.75" style="6" customWidth="1"/>
-    <col min="36" max="39" width="8.625" style="31"/>
-    <col min="41" max="41" width="11.75" style="6" customWidth="1"/>
-    <col min="42" max="45" width="8.625" style="31"/>
+    <col min="2" max="2" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" style="31" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" style="31"/>
+    <col min="22" max="22" width="9.140625" style="31" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" style="6" customWidth="1"/>
+    <col min="24" max="27" width="8.5703125" style="31"/>
+    <col min="29" max="29" width="11.7109375" style="6" customWidth="1"/>
+    <col min="30" max="33" width="8.5703125" style="31"/>
+    <col min="35" max="35" width="11.7109375" style="6" customWidth="1"/>
+    <col min="36" max="39" width="8.5703125" style="31"/>
+    <col min="41" max="41" width="11.7109375" style="6" customWidth="1"/>
+    <col min="42" max="45" width="8.5703125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>155</v>
       </c>
@@ -17359,7 +17359,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="C2" s="14">
         <v>2000</v>
@@ -17476,7 +17476,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -17527,7 +17527,7 @@
       <c r="AR3" s="30"/>
       <c r="AS3" s="30"/>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -17578,7 +17578,7 @@
       <c r="AR4" s="30"/>
       <c r="AS4" s="30"/>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -17629,7 +17629,7 @@
       <c r="AR5" s="30"/>
       <c r="AS5" s="30"/>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -17680,7 +17680,7 @@
       <c r="AR6" s="30"/>
       <c r="AS6" s="30"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -17731,7 +17731,7 @@
       <c r="AR7" s="30"/>
       <c r="AS7" s="30"/>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
@@ -17782,7 +17782,7 @@
       <c r="AR8" s="30"/>
       <c r="AS8" s="30"/>
     </row>
-    <row r="10" spans="1:45" s="18" customFormat="1">
+    <row r="10" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="T10" s="31"/>
       <c r="U10" s="31"/>
@@ -17808,7 +17808,7 @@
       <c r="AR10" s="31"/>
       <c r="AS10" s="31"/>
     </row>
-    <row r="11" spans="1:45" s="18" customFormat="1">
+    <row r="11" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="T11" s="31"/>
       <c r="U11" s="31"/>
@@ -17834,7 +17834,7 @@
       <c r="AR11" s="31"/>
       <c r="AS11" s="31"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>73</v>
       </c>
@@ -17880,7 +17880,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="C13" s="14">
         <v>2000</v>
@@ -17995,7 +17995,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="48" t="s">
         <v>70</v>
@@ -18061,7 +18061,7 @@
       <c r="AR14" s="30"/>
       <c r="AS14" s="30"/>
     </row>
-    <row r="16" spans="1:45" s="18" customFormat="1">
+    <row r="16" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="T16" s="31"/>
       <c r="U16" s="31"/>
@@ -18087,7 +18087,7 @@
       <c r="AR16" s="31"/>
       <c r="AS16" s="31"/>
     </row>
-    <row r="17" spans="1:45" s="18" customFormat="1">
+    <row r="17" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="T17" s="31"/>
       <c r="U17" s="31"/>
@@ -18113,7 +18113,7 @@
       <c r="AR17" s="31"/>
       <c r="AS17" s="31"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>114</v>
       </c>
@@ -18159,7 +18159,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="C19" s="14">
         <v>2000</v>
@@ -18276,7 +18276,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:45">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="48" t="s">
         <v>70</v>
@@ -18352,7 +18352,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z41"/>
   <sheetViews>
@@ -18360,12 +18360,12 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="15" width="6.625" customWidth="1"/>
+    <col min="1" max="15" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" customHeight="1">
+    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>54</v>
       </c>
@@ -18394,7 +18394,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="37"/>
       <c r="C2" s="4" t="str">
@@ -18440,7 +18440,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -18473,7 +18473,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -18504,7 +18504,7 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -18539,7 +18539,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -18573,7 +18573,7 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -18604,7 +18604,7 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
@@ -18639,7 +18639,7 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -18667,9 +18667,9 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:26" s="18" customFormat="1"/>
-    <row r="11" spans="1:26" s="18" customFormat="1"/>
-    <row r="12" spans="1:26">
+    <row r="10" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>52</v>
       </c>
@@ -18699,7 +18699,7 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="37"/>
       <c r="C13" s="4" t="str">
@@ -18745,7 +18745,7 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -18778,7 +18778,7 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -18809,7 +18809,7 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -18844,7 +18844,7 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -18879,7 +18879,7 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -18910,7 +18910,7 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
@@ -18927,7 +18927,7 @@
       </c>
       <c r="H19" s="36"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -18937,7 +18937,7 @@
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="1:26" s="18" customFormat="1">
+    <row r="21" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -18965,8 +18965,8 @@
       <c r="Y21" s="16"/>
       <c r="Z21" s="16"/>
     </row>
-    <row r="22" spans="1:26" s="18" customFormat="1"/>
-    <row r="23" spans="1:26">
+    <row r="22" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>53</v>
       </c>
@@ -18978,7 +18978,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="37"/>
       <c r="C24" s="4" t="str">
@@ -19006,7 +19006,7 @@
         <v>CSW</v>
       </c>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -19019,7 +19019,7 @@
       <c r="G25" s="36"/>
       <c r="H25" s="36"/>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -19032,7 +19032,7 @@
       <c r="G26" s="36"/>
       <c r="H26" s="36"/>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -19045,7 +19045,7 @@
       <c r="G27" s="36"/>
       <c r="H27" s="36"/>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -19058,7 +19058,7 @@
       <c r="G28" s="36"/>
       <c r="H28" s="36"/>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -19071,7 +19071,7 @@
       <c r="G29" s="36"/>
       <c r="H29" s="36"/>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>
@@ -19086,7 +19086,7 @@
       <c r="G30" s="36"/>
       <c r="H30" s="36"/>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -19096,7 +19096,7 @@
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
     </row>
-    <row r="32" spans="1:26" s="18" customFormat="1">
+    <row r="32" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -19124,8 +19124,8 @@
       <c r="Y32" s="16"/>
       <c r="Z32" s="16"/>
     </row>
-    <row r="33" spans="1:8" s="18" customFormat="1"/>
-    <row r="34" spans="1:8">
+    <row r="33" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>55</v>
       </c>
@@ -19137,7 +19137,7 @@
       <c r="G34" s="16"/>
       <c r="H34" s="16"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="37"/>
       <c r="C35" s="4" t="str">
@@ -19165,7 +19165,7 @@
         <v>CSW</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$D$3</f>
@@ -19178,7 +19178,7 @@
       <c r="G36" s="36"/>
       <c r="H36" s="36"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$D$4</f>
@@ -19191,7 +19191,7 @@
       <c r="G37" s="36"/>
       <c r="H37" s="36"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="4" t="str">
         <f>'Populations &amp; programs'!$D$5</f>
@@ -19206,7 +19206,7 @@
       <c r="G38" s="36"/>
       <c r="H38" s="36"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="4" t="str">
         <f>'Populations &amp; programs'!$D$6</f>
@@ -19219,7 +19219,7 @@
       <c r="G39" s="36"/>
       <c r="H39" s="36"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="4" t="str">
         <f>'Populations &amp; programs'!$D$7</f>
@@ -19232,7 +19232,7 @@
       <c r="G40" s="36"/>
       <c r="H40" s="36"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="4" t="str">
         <f>'Populations &amp; programs'!$D$8</f>

</xml_diff>

<commit_message>
updated spreadsheet with davids version; updated profile.py
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="12"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Disutilities &amp; costs" sheetId="14" r:id="rId12"/>
     <sheet name="Macroeconomics" sheetId="18" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="156">
   <si>
     <t>Men who have sex with men</t>
   </si>
@@ -52,11 +52,11 @@
   </si>
   <si>
     <t>Prevention of mother-to-child transmission</t>
-    <phoneticPr fontId="12" type="noConversion"/>
+    <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
     <t>Average</t>
-    <phoneticPr fontId="12" type="noConversion"/>
+    <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
     <t>Prevalence of any discharging STIs</t>
@@ -507,14 +507,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -682,799 +691,813 @@
   </borders>
   <cellStyleXfs count="663">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="655"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="655" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="655"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="655" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="655"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="655" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="655"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="655" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="11" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="11" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="2" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="10" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="1" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="655" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="655" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="167" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2451,9 +2474,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2866,7 +2887,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
@@ -2883,7 +2904,7 @@
   <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="F3" sqref="F3:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3105,7 +3126,9 @@
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
+      <c r="G15" s="24">
+        <v>10</v>
+      </c>
       <c r="H15" s="24"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -3116,7 +3139,9 @@
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
+      <c r="F16" s="24">
+        <v>15</v>
+      </c>
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
     </row>
@@ -3130,7 +3155,9 @@
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
       <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
+      <c r="H17" s="24">
+        <v>40</v>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="str">
@@ -3152,12 +3179,14 @@
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
+      <c r="F19" s="24">
+        <v>10</v>
+      </c>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -3738,7 +3767,7 @@
       <c r="E69" s="22"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -4022,7 +4051,7 @@
       <c r="E28" s="22"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -4037,7 +4066,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5228,7 +5257,7 @@
       <c r="T57" s="29"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -5244,14 +5273,20 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="18"/>
     <col min="3" max="3" width="11" style="18" customWidth="1"/>
-    <col min="4" max="20" width="9.140625" style="18"/>
+    <col min="4" max="6" width="9.140625" style="18"/>
+    <col min="7" max="8" width="10.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="18"/>
+    <col min="11" max="15" width="10.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="9.140625" style="18"/>
     <col min="21" max="21" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="9.140625" style="18"/>
   </cols>
@@ -5365,43 +5400,36 @@
       <c r="C4" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="27">
-        <f>550000*E3</f>
-        <v>11000</v>
-      </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27">
-        <f t="shared" ref="H4:Q4" si="0">550000*H3</f>
-        <v>77000.000000000015</v>
-      </c>
-      <c r="I4" s="27">
-        <f t="shared" si="0"/>
-        <v>93500</v>
-      </c>
-      <c r="J4" s="27">
-        <f t="shared" si="0"/>
-        <v>27500</v>
-      </c>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27">
-        <f t="shared" si="0"/>
-        <v>110000</v>
-      </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27">
-        <f t="shared" si="0"/>
-        <v>214500</v>
-      </c>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27">
-        <f t="shared" si="0"/>
-        <v>154000.00000000003</v>
-      </c>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56">
+        <v>12000</v>
+      </c>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56">
+        <v>75000</v>
+      </c>
+      <c r="I4" s="56">
+        <v>100000</v>
+      </c>
+      <c r="J4" s="56">
+        <v>36000</v>
+      </c>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56">
+        <v>112000</v>
+      </c>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56">
+        <v>210000</v>
+      </c>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="56">
+        <v>161000</v>
+      </c>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
       <c r="T4" s="5" t="s">
         <v>81</v>
       </c>
@@ -5422,24 +5450,32 @@
       <c r="E6" s="25"/>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
-      <c r="H6" s="25"/>
+      <c r="H6" s="25">
+        <v>0.15</v>
+      </c>
       <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="22"/>
+      <c r="J6" s="25">
+        <v>0.18</v>
+      </c>
+      <c r="K6" s="25">
+        <v>0.2</v>
+      </c>
       <c r="L6" s="25"/>
       <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
+      <c r="N6" s="25">
+        <v>0.28000000000000003</v>
+      </c>
       <c r="O6" s="25"/>
       <c r="P6" s="22"/>
-      <c r="Q6" s="25"/>
+      <c r="Q6" s="25">
+        <v>0.33</v>
+      </c>
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
       <c r="T6" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="U6" s="25">
-        <v>0.2</v>
-      </c>
+      <c r="U6" s="25"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
@@ -5449,28 +5485,34 @@
       <c r="C7" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56">
+        <v>25000</v>
+      </c>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56">
+        <v>31000</v>
+      </c>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56">
+        <v>52000</v>
+      </c>
+      <c r="O7" s="56"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56">
+        <v>100000</v>
+      </c>
+      <c r="R7" s="56"/>
+      <c r="S7" s="56"/>
       <c r="T7" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="U7" s="52">
-        <v>25000</v>
-      </c>
+      <c r="U7" s="52"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
@@ -5497,7 +5539,9 @@
       </c>
       <c r="N9" s="23"/>
       <c r="O9" s="25"/>
-      <c r="P9" s="22"/>
+      <c r="P9" s="55">
+        <v>2315</v>
+      </c>
       <c r="Q9" s="25"/>
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
@@ -5515,24 +5559,26 @@
       <c r="C10" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="43">
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56">
         <v>3483</v>
       </c>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56">
+        <v>4467</v>
+      </c>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="56"/>
+      <c r="S10" s="56"/>
       <c r="T10" s="5" t="s">
         <v>81</v>
       </c>
@@ -5561,12 +5607,16 @@
       <c r="K12" s="22"/>
       <c r="L12" s="25"/>
       <c r="M12" s="25">
-        <v>0.6</v>
+        <v>0.16</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="25"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="25"/>
+      <c r="P12" s="25">
+        <v>0.32</v>
+      </c>
+      <c r="Q12" s="25">
+        <v>0.35</v>
+      </c>
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
       <c r="T12" s="5" t="s">
@@ -5583,24 +5633,28 @@
       <c r="C13" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="43">
-        <v>400000</v>
-      </c>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="56">
+        <v>40000</v>
+      </c>
+      <c r="N13" s="56"/>
+      <c r="O13" s="56"/>
+      <c r="P13" s="56">
+        <v>85000</v>
+      </c>
+      <c r="Q13" s="56">
+        <v>100000</v>
+      </c>
+      <c r="R13" s="56"/>
+      <c r="S13" s="56"/>
       <c r="T13" s="5" t="s">
         <v>81</v>
       </c>
@@ -5627,9 +5681,15 @@
         <v>0.2</v>
       </c>
       <c r="N15" s="23"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="25"/>
+      <c r="O15" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="P15" s="25">
+        <v>0.75</v>
+      </c>
+      <c r="Q15" s="25">
+        <v>0.8</v>
+      </c>
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
       <c r="T15" s="5" t="s">
@@ -5645,24 +5705,30 @@
       <c r="C16" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="43">
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56">
         <v>130000</v>
       </c>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56">
+        <v>210000</v>
+      </c>
+      <c r="P16" s="56">
+        <v>300000</v>
+      </c>
+      <c r="Q16" s="56">
+        <v>340000</v>
+      </c>
+      <c r="R16" s="56"/>
+      <c r="S16" s="56"/>
       <c r="T16" s="5" t="s">
         <v>81</v>
       </c>
@@ -5679,19 +5745,39 @@
       <c r="D18" s="22"/>
       <c r="E18" s="25"/>
       <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
+      <c r="G18" s="22">
+        <v>2343</v>
+      </c>
+      <c r="H18" s="22">
+        <v>2547</v>
+      </c>
+      <c r="I18" s="22">
+        <v>2763</v>
+      </c>
+      <c r="J18" s="22">
+        <v>2997</v>
+      </c>
+      <c r="K18" s="22">
+        <v>3220</v>
+      </c>
+      <c r="L18" s="22">
+        <v>3441</v>
+      </c>
+      <c r="M18" s="22">
+        <v>3660</v>
+      </c>
       <c r="N18" s="22">
-        <v>2343</v>
-      </c>
-      <c r="O18" s="25"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="25"/>
+        <v>3866</v>
+      </c>
+      <c r="O18" s="22">
+        <v>4071</v>
+      </c>
+      <c r="P18" s="22">
+        <v>4290</v>
+      </c>
+      <c r="Q18" s="22">
+        <v>4491</v>
+      </c>
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
       <c r="T18" s="5" t="s">
@@ -5707,24 +5793,44 @@
       <c r="C19" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43">
-        <v>1034</v>
-      </c>
-      <c r="O19" s="23"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56">
+        <v>827591</v>
+      </c>
+      <c r="H19" s="56">
+        <v>878339</v>
+      </c>
+      <c r="I19" s="56">
+        <v>931131</v>
+      </c>
+      <c r="J19" s="56">
+        <v>979989</v>
+      </c>
+      <c r="K19" s="56">
+        <v>1025140</v>
+      </c>
+      <c r="L19" s="56">
+        <v>1209617</v>
+      </c>
+      <c r="M19" s="56">
+        <v>1163420</v>
+      </c>
+      <c r="N19" s="56">
+        <v>1262842</v>
+      </c>
+      <c r="O19" s="56">
+        <v>1311927</v>
+      </c>
+      <c r="P19" s="56">
+        <v>14475730</v>
+      </c>
+      <c r="Q19" s="56">
+        <v>1451467</v>
+      </c>
+      <c r="R19" s="56"/>
+      <c r="S19" s="56"/>
       <c r="T19" s="5" t="s">
         <v>81</v>
       </c>
@@ -5745,14 +5851,18 @@
       <c r="H21" s="25"/>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
-      <c r="K21" s="22"/>
+      <c r="K21" s="22">
+        <v>123</v>
+      </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
       <c r="N21" s="55">
         <v>153</v>
       </c>
       <c r="O21" s="25"/>
-      <c r="P21" s="22"/>
+      <c r="P21" s="22">
+        <v>208</v>
+      </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="22"/>
       <c r="S21" s="22"/>
@@ -5769,33 +5879,37 @@
       <c r="C22" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="55">
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="56">
+        <v>4010</v>
+      </c>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56">
         <v>5340</v>
       </c>
-      <c r="O22" s="23"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="25"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="22"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56">
+        <v>6840</v>
+      </c>
+      <c r="Q22" s="56"/>
+      <c r="R22" s="56"/>
+      <c r="S22" s="56"/>
       <c r="T22" s="5" t="s">
         <v>81</v>
       </c>
       <c r="U22" s="39"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="598"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="598" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5810,7 +5924,7 @@
   <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6006,7 +6120,9 @@
       <c r="T7" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="U7" s="27"/>
+      <c r="U7" s="27">
+        <v>24000</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="str">
@@ -6066,7 +6182,9 @@
       <c r="T9" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="U9" s="27"/>
+      <c r="U9" s="27">
+        <v>12000</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
@@ -7281,7 +7399,7 @@
       <c r="U53" s="26"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -7294,10 +7412,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:T33"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7925,17 +8043,39 @@
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
+      <c r="F33" s="22">
+        <v>42</v>
+      </c>
+      <c r="G33" s="22">
+        <v>65</v>
+      </c>
+      <c r="H33" s="22">
+        <v>120</v>
+      </c>
+      <c r="I33" s="22">
+        <v>370</v>
+      </c>
+      <c r="J33" s="22">
+        <v>580</v>
+      </c>
+      <c r="K33" s="22">
+        <v>810</v>
+      </c>
+      <c r="L33" s="22">
+        <v>810</v>
+      </c>
+      <c r="M33" s="22">
+        <v>781</v>
+      </c>
+      <c r="N33" s="22">
+        <v>410</v>
+      </c>
+      <c r="O33" s="22">
+        <v>341</v>
+      </c>
+      <c r="P33" s="22">
+        <v>365</v>
+      </c>
       <c r="Q33" s="22"/>
       <c r="R33" s="22"/>
       <c r="S33" s="5" t="s">
@@ -7943,8 +8083,22 @@
       </c>
       <c r="T33" s="22"/>
     </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -7960,7 +8114,7 @@
   <dimension ref="A1:AS42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8155,66 +8309,26 @@
       <c r="T3" s="25">
         <v>0.01</v>
       </c>
-      <c r="W3" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="X3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="Y3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="Z3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="53" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="AE3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="AF3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="AK3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="AL3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="AP3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="AQ3" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="AR3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="25">
-        <v>0</v>
-      </c>
+      <c r="W3" s="53"/>
+      <c r="X3" s="25"/>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AA3" s="25"/>
+      <c r="AC3" s="53"/>
+      <c r="AD3" s="25"/>
+      <c r="AE3" s="25"/>
+      <c r="AF3" s="25"/>
+      <c r="AG3" s="25"/>
+      <c r="AI3" s="53"/>
+      <c r="AJ3" s="25"/>
+      <c r="AK3" s="25"/>
+      <c r="AL3" s="25"/>
+      <c r="AM3" s="25"/>
+      <c r="AO3" s="53"/>
+      <c r="AP3" s="25"/>
+      <c r="AQ3" s="25"/>
+      <c r="AR3" s="25"/>
+      <c r="AS3" s="25"/>
     </row>
     <row r="4" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
@@ -8291,11 +8405,21 @@
       <c r="T5" s="25">
         <v>0.03</v>
       </c>
-      <c r="W5" s="40"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25"/>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="25"/>
+      <c r="W5" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="X5" s="25">
+        <v>0.03</v>
+      </c>
+      <c r="Y5" s="25">
+        <v>0.03</v>
+      </c>
+      <c r="Z5" s="59">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AA5" s="59">
+        <v>2.8000000000000001E-2</v>
+      </c>
       <c r="AC5" s="40"/>
       <c r="AD5" s="25"/>
       <c r="AE5" s="25"/>
@@ -8655,24 +8779,36 @@
       <c r="I14" s="22"/>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
+      <c r="L14" s="26">
+        <v>4.4999999999999998E-2</v>
+      </c>
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
+      <c r="O14" s="25">
+        <v>0.08</v>
+      </c>
       <c r="P14" s="22"/>
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T14" s="25">
-        <v>0</v>
-      </c>
-      <c r="W14" s="40"/>
-      <c r="X14" s="46"/>
-      <c r="Y14" s="25"/>
-      <c r="Z14" s="25"/>
-      <c r="AA14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="W14" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="X14" s="59">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y14" s="59">
+        <v>0.1</v>
+      </c>
+      <c r="Z14" s="59">
+        <v>0.03</v>
+      </c>
+      <c r="AA14" s="59">
+        <v>0.04</v>
+      </c>
       <c r="AC14" s="40"/>
       <c r="AD14" s="46"/>
       <c r="AE14" s="25"/>
@@ -8704,24 +8840,36 @@
       <c r="I15" s="22"/>
       <c r="J15" s="22"/>
       <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
+      <c r="L15" s="25">
+        <v>0.03</v>
+      </c>
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
+      <c r="O15" s="26">
+        <v>5.5E-2</v>
+      </c>
       <c r="P15" s="22"/>
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T15" s="25">
-        <v>0</v>
-      </c>
-      <c r="W15" s="40"/>
-      <c r="X15" s="25"/>
-      <c r="Y15" s="25"/>
-      <c r="Z15" s="25"/>
-      <c r="AA15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="W15" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="X15" s="59">
+        <v>0.03</v>
+      </c>
+      <c r="Y15" s="59">
+        <v>0.06</v>
+      </c>
+      <c r="Z15" s="59">
+        <v>0.01</v>
+      </c>
+      <c r="AA15" s="59">
+        <v>0.03</v>
+      </c>
       <c r="AC15" s="40"/>
       <c r="AD15" s="25"/>
       <c r="AE15" s="25"/>
@@ -8753,24 +8901,36 @@
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
+      <c r="L16" s="25">
+        <v>0.04</v>
+      </c>
       <c r="M16" s="22"/>
       <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
+      <c r="O16" s="26">
+        <v>3.6999999999999998E-2</v>
+      </c>
       <c r="P16" s="22"/>
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T16" s="25">
-        <v>0</v>
-      </c>
-      <c r="W16" s="40"/>
-      <c r="X16" s="25"/>
-      <c r="Y16" s="25"/>
-      <c r="Z16" s="25"/>
-      <c r="AA16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="W16" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="X16" s="59">
+        <v>0.03</v>
+      </c>
+      <c r="Y16" s="59">
+        <v>0.05</v>
+      </c>
+      <c r="Z16" s="59">
+        <v>0.02</v>
+      </c>
+      <c r="AA16" s="59">
+        <v>0.03</v>
+      </c>
       <c r="AC16" s="40"/>
       <c r="AD16" s="25"/>
       <c r="AE16" s="25"/>
@@ -8802,24 +8962,36 @@
       <c r="I17" s="22"/>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
+      <c r="L17" s="26">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="M17" s="22"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
+      <c r="O17" s="26">
+        <v>2.5000000000000001E-2</v>
+      </c>
       <c r="P17" s="22"/>
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T17" s="25">
-        <v>0</v>
-      </c>
-      <c r="W17" s="40"/>
-      <c r="X17" s="25"/>
-      <c r="Y17" s="25"/>
-      <c r="Z17" s="25"/>
-      <c r="AA17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="W17" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="X17" s="59">
+        <v>0.01</v>
+      </c>
+      <c r="Y17" s="59">
+        <v>0.03</v>
+      </c>
+      <c r="Z17" s="59">
+        <v>0.01</v>
+      </c>
+      <c r="AA17" s="59">
+        <v>0.02</v>
+      </c>
       <c r="AC17" s="40"/>
       <c r="AD17" s="25"/>
       <c r="AE17" s="25"/>
@@ -8851,24 +9023,36 @@
       <c r="I18" s="22"/>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
+      <c r="L18" s="25">
+        <v>0.01</v>
+      </c>
       <c r="M18" s="22"/>
       <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
+      <c r="O18" s="26">
+        <v>1.7000000000000001E-2</v>
+      </c>
       <c r="P18" s="22"/>
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T18" s="25">
-        <v>0</v>
-      </c>
-      <c r="W18" s="40"/>
-      <c r="X18" s="25"/>
-      <c r="Y18" s="25"/>
-      <c r="Z18" s="25"/>
-      <c r="AA18" s="25"/>
+      <c r="T18" s="25"/>
+      <c r="W18" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="X18" s="59">
+        <v>0.01</v>
+      </c>
+      <c r="Y18" s="59">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Z18" s="59">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AA18" s="59">
+        <v>0.02</v>
+      </c>
       <c r="AC18" s="40"/>
       <c r="AD18" s="25"/>
       <c r="AE18" s="25"/>
@@ -8900,29 +9084,51 @@
       <c r="I19" s="22"/>
       <c r="J19" s="22"/>
       <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
+      <c r="L19" s="26">
+        <v>2.5000000000000001E-2</v>
+      </c>
       <c r="M19" s="22"/>
       <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
+      <c r="O19" s="26">
+        <v>3.5000000000000003E-2</v>
+      </c>
       <c r="P19" s="22"/>
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T19" s="25">
-        <v>0</v>
-      </c>
-      <c r="W19" s="40"/>
-      <c r="X19" s="25"/>
-      <c r="Y19" s="25"/>
-      <c r="Z19" s="25"/>
-      <c r="AA19" s="25"/>
-      <c r="AC19" s="40"/>
-      <c r="AD19" s="25"/>
-      <c r="AE19" s="25"/>
-      <c r="AF19" s="25"/>
-      <c r="AG19" s="25"/>
+      <c r="T19" s="25"/>
+      <c r="W19" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="X19" s="59">
+        <v>0.02</v>
+      </c>
+      <c r="Y19" s="59">
+        <v>0.04</v>
+      </c>
+      <c r="Z19" s="59">
+        <v>0.02</v>
+      </c>
+      <c r="AA19" s="59">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AC19" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD19" s="59">
+        <v>0.02</v>
+      </c>
+      <c r="AE19" s="59">
+        <v>0.04</v>
+      </c>
+      <c r="AF19" s="59">
+        <v>0.02</v>
+      </c>
+      <c r="AG19" s="59">
+        <v>3.5000000000000003E-2</v>
+      </c>
       <c r="AI19" s="40"/>
       <c r="AJ19" s="25"/>
       <c r="AK19" s="25"/>
@@ -9117,24 +9323,36 @@
       <c r="I25" s="22"/>
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
+      <c r="L25" s="25">
+        <v>0.05</v>
+      </c>
       <c r="M25" s="22"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
+      <c r="O25" s="25">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="P25" s="22"/>
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T25" s="25">
-        <v>0</v>
-      </c>
-      <c r="W25" s="40"/>
-      <c r="X25" s="46"/>
-      <c r="Y25" s="25"/>
-      <c r="Z25" s="25"/>
-      <c r="AA25" s="25"/>
+      <c r="T25" s="25"/>
+      <c r="W25" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="X25" s="46">
+        <v>0.05</v>
+      </c>
+      <c r="Y25" s="25">
+        <v>0.09</v>
+      </c>
+      <c r="Z25" s="25">
+        <v>0.03</v>
+      </c>
+      <c r="AA25" s="25">
+        <v>0.04</v>
+      </c>
       <c r="AC25" s="40"/>
       <c r="AD25" s="46"/>
       <c r="AE25" s="25"/>
@@ -9165,24 +9383,36 @@
       <c r="I26" s="22"/>
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
+      <c r="L26" s="25">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="M26" s="22"/>
       <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
+      <c r="O26" s="25">
+        <v>0.05</v>
+      </c>
       <c r="P26" s="22"/>
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T26" s="25">
-        <v>0</v>
-      </c>
-      <c r="W26" s="40"/>
-      <c r="X26" s="25"/>
-      <c r="Y26" s="25"/>
-      <c r="Z26" s="25"/>
-      <c r="AA26" s="25"/>
+      <c r="T26" s="25"/>
+      <c r="W26" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="X26" s="59">
+        <v>0.05</v>
+      </c>
+      <c r="Y26" s="59">
+        <v>0.08</v>
+      </c>
+      <c r="Z26" s="59">
+        <v>0.02</v>
+      </c>
+      <c r="AA26" s="59">
+        <v>0.03</v>
+      </c>
       <c r="AC26" s="40"/>
       <c r="AD26" s="25"/>
       <c r="AE26" s="25"/>
@@ -9213,24 +9443,36 @@
       <c r="I27" s="22"/>
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
+      <c r="L27" s="26">
+        <v>2.1000000000000001E-2</v>
+      </c>
       <c r="M27" s="22"/>
       <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
+      <c r="O27" s="26">
+        <v>1.6E-2</v>
+      </c>
       <c r="P27" s="22"/>
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T27" s="25">
-        <v>0</v>
-      </c>
-      <c r="W27" s="40"/>
-      <c r="X27" s="25"/>
-      <c r="Y27" s="25"/>
-      <c r="Z27" s="25"/>
-      <c r="AA27" s="25"/>
+      <c r="T27" s="25"/>
+      <c r="W27" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="X27" s="59">
+        <v>0.02</v>
+      </c>
+      <c r="Y27" s="59">
+        <v>0.03</v>
+      </c>
+      <c r="Z27" s="59">
+        <v>0.01</v>
+      </c>
+      <c r="AA27" s="59">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="AC27" s="40"/>
       <c r="AD27" s="25"/>
       <c r="AE27" s="25"/>
@@ -9261,24 +9503,36 @@
       <c r="I28" s="22"/>
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
+      <c r="L28" s="26">
+        <v>2.5999999999999999E-2</v>
+      </c>
       <c r="M28" s="22"/>
       <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
+      <c r="O28" s="26">
+        <v>3.1E-2</v>
+      </c>
       <c r="P28" s="22"/>
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
       <c r="S28" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T28" s="25">
-        <v>0</v>
-      </c>
-      <c r="W28" s="40"/>
-      <c r="X28" s="25"/>
-      <c r="Y28" s="25"/>
-      <c r="Z28" s="25"/>
-      <c r="AA28" s="25"/>
+      <c r="T28" s="25"/>
+      <c r="W28" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="X28" s="59">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Y28" s="59">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="Z28" s="59">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AA28" s="59">
+        <v>2.5000000000000001E-2</v>
+      </c>
       <c r="AC28" s="40"/>
       <c r="AD28" s="25"/>
       <c r="AE28" s="25"/>
@@ -9309,24 +9563,36 @@
       <c r="I29" s="22"/>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
+      <c r="L29" s="25">
+        <v>0.02</v>
+      </c>
       <c r="M29" s="22"/>
       <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
+      <c r="O29" s="25">
+        <v>0.04</v>
+      </c>
       <c r="P29" s="22"/>
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
       <c r="S29" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T29" s="25">
-        <v>0</v>
-      </c>
-      <c r="W29" s="40"/>
-      <c r="X29" s="25"/>
-      <c r="Y29" s="25"/>
-      <c r="Z29" s="25"/>
-      <c r="AA29" s="25"/>
+      <c r="T29" s="25"/>
+      <c r="W29" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="X29" s="59">
+        <v>0.04</v>
+      </c>
+      <c r="Y29" s="59">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="Z29" s="59">
+        <v>0.02</v>
+      </c>
+      <c r="AA29" s="59">
+        <v>0.03</v>
+      </c>
       <c r="AC29" s="40"/>
       <c r="AD29" s="25"/>
       <c r="AE29" s="25"/>
@@ -9357,29 +9623,51 @@
       <c r="I30" s="22"/>
       <c r="J30" s="22"/>
       <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
+      <c r="L30" s="26">
+        <v>3.5000000000000003E-2</v>
+      </c>
       <c r="M30" s="22"/>
       <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
+      <c r="O30" s="26">
+        <v>2.3E-2</v>
+      </c>
       <c r="P30" s="22"/>
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
       <c r="S30" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T30" s="25">
-        <v>0</v>
-      </c>
-      <c r="W30" s="40"/>
-      <c r="X30" s="25"/>
-      <c r="Y30" s="25"/>
-      <c r="Z30" s="25"/>
-      <c r="AA30" s="25"/>
-      <c r="AC30" s="40"/>
-      <c r="AD30" s="25"/>
-      <c r="AE30" s="25"/>
-      <c r="AF30" s="25"/>
-      <c r="AG30" s="25"/>
+      <c r="T30" s="25"/>
+      <c r="W30" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="X30" s="59">
+        <v>0.04</v>
+      </c>
+      <c r="Y30" s="59">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="Z30" s="59">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AA30" s="59">
+        <v>0.04</v>
+      </c>
+      <c r="AC30" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD30" s="59">
+        <v>0.04</v>
+      </c>
+      <c r="AE30" s="59">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AF30" s="59">
+        <v>0.02</v>
+      </c>
+      <c r="AG30" s="59">
+        <v>0.03</v>
+      </c>
       <c r="AI30" s="40"/>
       <c r="AJ30" s="25"/>
       <c r="AK30" s="25"/>
@@ -9600,7 +9888,7 @@
         <v>81</v>
       </c>
       <c r="T36" s="25">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="W36" s="29"/>
       <c r="X36" s="25"/>
@@ -9648,7 +9936,7 @@
         <v>81</v>
       </c>
       <c r="T37" s="25">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="W37" s="29"/>
       <c r="X37" s="25"/>
@@ -9696,7 +9984,7 @@
         <v>81</v>
       </c>
       <c r="T38" s="25">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="W38" s="29"/>
       <c r="X38" s="25"/>
@@ -9744,7 +10032,7 @@
         <v>81</v>
       </c>
       <c r="T39" s="25">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="W39" s="29"/>
       <c r="X39" s="25"/>
@@ -9792,7 +10080,7 @@
         <v>81</v>
       </c>
       <c r="T40" s="25">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="W40" s="29"/>
       <c r="X40" s="25"/>
@@ -9840,7 +10128,7 @@
         <v>81</v>
       </c>
       <c r="T41" s="25">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="W41" s="29"/>
       <c r="X41" s="25"/>
@@ -9867,7 +10155,7 @@
       <c r="S42" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -9884,7 +10172,7 @@
   <dimension ref="A1:AS71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10090,13 +10378,13 @@
         <v>81</v>
       </c>
       <c r="T3" s="25">
-        <v>0.03</v>
+        <v>0.15</v>
       </c>
       <c r="W3" s="40" t="s">
         <v>52</v>
       </c>
       <c r="X3" s="25">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Y3" s="25">
         <v>0.3</v>
@@ -10216,16 +10504,36 @@
         <v>81</v>
       </c>
       <c r="T5" s="22"/>
-      <c r="W5" s="40"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25"/>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="25"/>
-      <c r="AC5" s="40"/>
-      <c r="AD5" s="25"/>
-      <c r="AE5" s="25"/>
-      <c r="AF5" s="25"/>
-      <c r="AG5" s="25"/>
+      <c r="W5" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="X5" s="25">
+        <v>0.3</v>
+      </c>
+      <c r="Y5" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="Z5" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="AA5" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="AC5" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD5" s="25">
+        <v>0.3</v>
+      </c>
+      <c r="AE5" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="AF5" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="AG5" s="25">
+        <v>0.5</v>
+      </c>
       <c r="AI5" s="40"/>
       <c r="AJ5" s="25"/>
       <c r="AK5" s="25"/>
@@ -10263,13 +10571,23 @@
         <v>81</v>
       </c>
       <c r="T6" s="25">
-        <v>0.01</v>
-      </c>
-      <c r="W6" s="40"/>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="25"/>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="25"/>
+        <v>0.02</v>
+      </c>
+      <c r="W6" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="X6" s="25">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y6" s="25">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Z6" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="AA6" s="25">
+        <v>0.1</v>
+      </c>
       <c r="AC6" s="40"/>
       <c r="AD6" s="25"/>
       <c r="AE6" s="25"/>
@@ -10312,13 +10630,23 @@
         <v>81</v>
       </c>
       <c r="T7" s="25">
-        <v>0.01</v>
-      </c>
-      <c r="W7" s="40"/>
-      <c r="X7" s="25"/>
-      <c r="Y7" s="25"/>
-      <c r="Z7" s="25"/>
-      <c r="AA7" s="25"/>
+        <v>0.03</v>
+      </c>
+      <c r="W7" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="X7" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="Y7" s="25">
+        <v>0.04</v>
+      </c>
+      <c r="Z7" s="25">
+        <v>0.08</v>
+      </c>
+      <c r="AA7" s="25">
+        <v>0.14000000000000001</v>
+      </c>
       <c r="AC7" s="40"/>
       <c r="AD7" s="25"/>
       <c r="AE7" s="25"/>
@@ -10363,16 +10691,36 @@
       <c r="T8" s="25">
         <v>0.05</v>
       </c>
-      <c r="W8" s="45"/>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="25"/>
-      <c r="Z8" s="25"/>
-      <c r="AA8" s="25"/>
-      <c r="AC8" s="45"/>
-      <c r="AD8" s="25"/>
-      <c r="AE8" s="25"/>
-      <c r="AF8" s="25"/>
-      <c r="AG8" s="25"/>
+      <c r="W8" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="X8" s="25">
+        <v>0.03</v>
+      </c>
+      <c r="Y8" s="25">
+        <v>0.06</v>
+      </c>
+      <c r="Z8" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="AA8" s="25">
+        <v>0.15</v>
+      </c>
+      <c r="AC8" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD8" s="25">
+        <v>0.03</v>
+      </c>
+      <c r="AE8" s="25">
+        <v>0.06</v>
+      </c>
+      <c r="AF8" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="AG8" s="25">
+        <v>0.08</v>
+      </c>
       <c r="AI8" s="45"/>
       <c r="AJ8" s="25"/>
       <c r="AK8" s="25"/>
@@ -10589,11 +10937,21 @@
       <c r="T14" s="25">
         <v>0.5</v>
       </c>
-      <c r="W14" s="40"/>
-      <c r="X14" s="25"/>
-      <c r="Y14" s="25"/>
-      <c r="Z14" s="25"/>
-      <c r="AA14" s="25"/>
+      <c r="W14" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="X14" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="Y14" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="Z14" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="AA14" s="25">
+        <v>0.75</v>
+      </c>
       <c r="AC14" s="40"/>
       <c r="AD14" s="25"/>
       <c r="AE14" s="25"/>
@@ -11327,14 +11685,24 @@
       <c r="S32" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T32" s="24">
+      <c r="T32" s="39">
+        <v>0.02</v>
+      </c>
+      <c r="W32" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="X32" s="25">
         <v>0</v>
       </c>
-      <c r="W32" s="40"/>
-      <c r="X32" s="25"/>
-      <c r="Y32" s="25"/>
-      <c r="Z32" s="25"/>
-      <c r="AA32" s="25"/>
+      <c r="Y32" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="Z32" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="AA32" s="25">
+        <v>0.4</v>
+      </c>
       <c r="AC32" s="40"/>
       <c r="AD32" s="25"/>
       <c r="AE32" s="25"/>
@@ -11375,14 +11743,24 @@
       <c r="S33" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T33" s="24">
-        <v>0</v>
-      </c>
-      <c r="W33" s="40"/>
-      <c r="X33" s="25"/>
-      <c r="Y33" s="25"/>
-      <c r="Z33" s="25"/>
-      <c r="AA33" s="25"/>
+      <c r="T33" s="39">
+        <v>0.08</v>
+      </c>
+      <c r="W33" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="X33" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="Y33" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="Z33" s="25">
+        <v>0.3</v>
+      </c>
+      <c r="AA33" s="25">
+        <v>0.5</v>
+      </c>
       <c r="AC33" s="40"/>
       <c r="AD33" s="25"/>
       <c r="AE33" s="25"/>
@@ -11423,10 +11801,10 @@
       <c r="S34" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T34" s="24">
+      <c r="T34" s="39">
         <v>0</v>
       </c>
-      <c r="W34" s="40"/>
+      <c r="W34" s="57"/>
       <c r="X34" s="25"/>
       <c r="Y34" s="25"/>
       <c r="Z34" s="25"/>
@@ -11471,7 +11849,7 @@
       <c r="S35" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T35" s="24">
+      <c r="T35" s="39">
         <v>0</v>
       </c>
       <c r="W35" s="40"/>
@@ -11519,7 +11897,7 @@
       <c r="S36" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T36" s="24">
+      <c r="T36" s="39">
         <f>2/50</f>
         <v>0.04</v>
       </c>
@@ -11568,8 +11946,8 @@
       <c r="S37" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T37" s="24">
-        <v>0</v>
+      <c r="T37" s="39">
+        <v>0.01</v>
       </c>
       <c r="W37" s="40"/>
       <c r="X37" s="25"/>
@@ -12948,7 +13326,7 @@
       <c r="AS71" s="25"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -12965,7 +13343,7 @@
   <dimension ref="A1:AS85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14941,11 +15319,21 @@
       <c r="AA41" s="30">
         <v>0.12</v>
       </c>
-      <c r="AC41" s="40"/>
-      <c r="AD41" s="30"/>
-      <c r="AE41" s="30"/>
-      <c r="AF41" s="30"/>
-      <c r="AG41" s="30"/>
+      <c r="AC41" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD41" s="30">
+        <v>0.05</v>
+      </c>
+      <c r="AE41" s="30">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AF41" s="30">
+        <v>0.08</v>
+      </c>
+      <c r="AG41" s="30">
+        <v>0.12</v>
+      </c>
       <c r="AI41" s="40"/>
       <c r="AJ41" s="30"/>
       <c r="AK41" s="30"/>
@@ -15496,11 +15884,21 @@
       <c r="AA52" s="30">
         <v>0.7</v>
       </c>
-      <c r="AC52" s="40"/>
-      <c r="AD52" s="30"/>
-      <c r="AE52" s="30"/>
-      <c r="AF52" s="30"/>
-      <c r="AG52" s="30"/>
+      <c r="AC52" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD52" s="30">
+        <v>0.4</v>
+      </c>
+      <c r="AE52" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="AF52" s="30">
+        <v>0.65</v>
+      </c>
+      <c r="AG52" s="30">
+        <v>0.75</v>
+      </c>
       <c r="AI52" s="40"/>
       <c r="AJ52" s="30"/>
       <c r="AK52" s="30"/>
@@ -16966,7 +17364,7 @@
       <c r="AS85" s="30"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -16983,7 +17381,7 @@
   <dimension ref="A1:AS20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17196,15 +17594,15 @@
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
       <c r="W3" s="29"/>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="30"/>
-      <c r="Z3" s="30"/>
-      <c r="AA3" s="30"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="29"/>
       <c r="AC3" s="29"/>
-      <c r="AD3" s="30"/>
-      <c r="AE3" s="30"/>
-      <c r="AF3" s="30"/>
-      <c r="AG3" s="30"/>
+      <c r="AD3" s="29"/>
+      <c r="AE3" s="29"/>
+      <c r="AF3" s="29"/>
+      <c r="AG3" s="29"/>
       <c r="AI3" s="29"/>
       <c r="AJ3" s="30"/>
       <c r="AK3" s="30"/>
@@ -17247,15 +17645,15 @@
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="29"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
+      <c r="X4" s="29"/>
+      <c r="Y4" s="29"/>
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="29"/>
       <c r="AC4" s="29"/>
-      <c r="AD4" s="30"/>
-      <c r="AE4" s="30"/>
-      <c r="AF4" s="30"/>
-      <c r="AG4" s="30"/>
+      <c r="AD4" s="29"/>
+      <c r="AE4" s="29"/>
+      <c r="AF4" s="29"/>
+      <c r="AG4" s="29"/>
       <c r="AI4" s="29"/>
       <c r="AJ4" s="30"/>
       <c r="AK4" s="30"/>
@@ -17297,16 +17695,26 @@
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="30"/>
-      <c r="Y5" s="30"/>
-      <c r="Z5" s="30"/>
-      <c r="AA5" s="30"/>
+      <c r="W5" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="X5" s="29">
+        <v>300</v>
+      </c>
+      <c r="Y5" s="29">
+        <v>450</v>
+      </c>
+      <c r="Z5" s="29">
+        <v>50</v>
+      </c>
+      <c r="AA5" s="29">
+        <v>120</v>
+      </c>
       <c r="AC5" s="29"/>
-      <c r="AD5" s="30"/>
-      <c r="AE5" s="30"/>
-      <c r="AF5" s="30"/>
-      <c r="AG5" s="30"/>
+      <c r="AD5" s="29"/>
+      <c r="AE5" s="29"/>
+      <c r="AF5" s="29"/>
+      <c r="AG5" s="29"/>
       <c r="AI5" s="29"/>
       <c r="AJ5" s="30"/>
       <c r="AK5" s="30"/>
@@ -17349,15 +17757,15 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="29"/>
-      <c r="X6" s="30"/>
-      <c r="Y6" s="30"/>
-      <c r="Z6" s="30"/>
-      <c r="AA6" s="30"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="29"/>
       <c r="AC6" s="29"/>
-      <c r="AD6" s="30"/>
-      <c r="AE6" s="30"/>
-      <c r="AF6" s="30"/>
-      <c r="AG6" s="30"/>
+      <c r="AD6" s="29"/>
+      <c r="AE6" s="29"/>
+      <c r="AF6" s="29"/>
+      <c r="AG6" s="29"/>
       <c r="AI6" s="29"/>
       <c r="AJ6" s="30"/>
       <c r="AK6" s="30"/>
@@ -17400,15 +17808,15 @@
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="29"/>
-      <c r="X7" s="30"/>
-      <c r="Y7" s="30"/>
-      <c r="Z7" s="30"/>
-      <c r="AA7" s="30"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="29"/>
       <c r="AC7" s="29"/>
-      <c r="AD7" s="30"/>
-      <c r="AE7" s="30"/>
-      <c r="AF7" s="30"/>
-      <c r="AG7" s="30"/>
+      <c r="AD7" s="29"/>
+      <c r="AE7" s="29"/>
+      <c r="AF7" s="29"/>
+      <c r="AG7" s="29"/>
       <c r="AI7" s="29"/>
       <c r="AJ7" s="30"/>
       <c r="AK7" s="30"/>
@@ -17451,15 +17859,15 @@
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="29"/>
-      <c r="X8" s="30"/>
-      <c r="Y8" s="30"/>
-      <c r="Z8" s="30"/>
-      <c r="AA8" s="30"/>
+      <c r="X8" s="29"/>
+      <c r="Y8" s="29"/>
+      <c r="Z8" s="29"/>
+      <c r="AA8" s="29"/>
       <c r="AC8" s="29"/>
-      <c r="AD8" s="30"/>
-      <c r="AE8" s="30"/>
-      <c r="AF8" s="30"/>
-      <c r="AG8" s="30"/>
+      <c r="AD8" s="29"/>
+      <c r="AE8" s="29"/>
+      <c r="AF8" s="29"/>
+      <c r="AG8" s="29"/>
       <c r="AI8" s="29"/>
       <c r="AJ8" s="30"/>
       <c r="AK8" s="30"/>
@@ -18030,7 +18438,7 @@
       <c r="AS20" s="30"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
@@ -18936,7 +19344,7 @@
       <c r="H41" s="36"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
working on equilibration etc.
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Disutilities &amp; costs" sheetId="14" r:id="rId12"/>
     <sheet name="Macroeconomics" sheetId="18" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -508,10 +508,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -703,7 +703,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
@@ -1351,7 +1351,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="60">
@@ -1473,7 +1473,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1486,7 +1486,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1497,7 +1497,7 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2474,7 +2474,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3201,7 +3201,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -4066,7 +4066,9 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5273,7 +5275,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5797,37 +5799,37 @@
       <c r="E19" s="56"/>
       <c r="F19" s="56"/>
       <c r="G19" s="56">
-        <v>827591</v>
+        <v>353.21852326077681</v>
       </c>
       <c r="H19" s="56">
-        <v>878339</v>
+        <v>344.85237534354144</v>
       </c>
       <c r="I19" s="56">
-        <v>931131</v>
+        <v>337</v>
       </c>
       <c r="J19" s="56">
-        <v>979989</v>
+        <v>326.98998998998997</v>
       </c>
       <c r="K19" s="56">
-        <v>1025140</v>
+        <v>318.36645962732922</v>
       </c>
       <c r="L19" s="56">
-        <v>1209617</v>
+        <v>351.53065969195001</v>
       </c>
       <c r="M19" s="56">
-        <v>1163420</v>
+        <v>317.87431693989072</v>
       </c>
       <c r="N19" s="56">
-        <v>1262842</v>
+        <v>326.65338851526127</v>
       </c>
       <c r="O19" s="56">
-        <v>1311927</v>
+        <v>322.26160648489315</v>
       </c>
       <c r="P19" s="56">
-        <v>14475730</v>
+        <v>343.99300699300699</v>
       </c>
       <c r="Q19" s="56">
-        <v>1451467</v>
+        <v>323.19461144511246</v>
       </c>
       <c r="R19" s="56"/>
       <c r="S19" s="56"/>
@@ -5924,7 +5926,7 @@
   <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13342,8 +13344,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13550,7 +13552,7 @@
         <v>81</v>
       </c>
       <c r="T3" s="33">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="U3" s="31"/>
       <c r="V3" s="31"/>
@@ -14029,7 +14031,7 @@
         <v>81</v>
       </c>
       <c r="T14" s="29">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
@@ -17381,7 +17383,7 @@
   <dimension ref="A1:AS20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18099,21 +18101,21 @@
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="25">
-        <v>0.3</v>
+        <v>0.06</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="25">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="25">
-        <v>0.2</v>
+        <v>0.04</v>
       </c>
       <c r="I14" s="22"/>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
       <c r="L14" s="25">
-        <v>0.2</v>
+        <v>0.04</v>
       </c>
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>

</xml_diff>

<commit_message>
working on equilibration still
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="6"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -3201,8 +3201,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3531,13 +3531,13 @@
         <v>42</v>
       </c>
       <c r="C42" s="25">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D42" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="E42" s="25">
         <v>0.15</v>
-      </c>
-      <c r="E42" s="25">
-        <v>0.25</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -13344,7 +13344,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed so test_optima runs
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="8"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -217,11 +217,11 @@
   </si>
   <si>
     <t>Prevention of mother-to-child transmission</t>
-    <phoneticPr fontId="12" type="noConversion"/>
+    <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
     <t>Average</t>
-    <phoneticPr fontId="12" type="noConversion"/>
+    <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
     <t>Prevalence of any discharging STIs</t>
@@ -496,10 +496,17 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -667,800 +674,807 @@
   </borders>
   <cellStyleXfs count="663">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="655"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="655" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="655"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="655" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="655"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="655" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="655"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="655" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="11" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="11" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="2" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="10" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="1" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="655" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="655" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="663">
@@ -2436,7 +2450,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2805,7 +2819,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -3096,7 +3110,7 @@
       <c r="H19" s="24"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -3677,7 +3691,7 @@
       <c r="E69" s="22"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -3961,7 +3975,7 @@
       <c r="E28" s="22"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -5167,7 +5181,7 @@
       <c r="T57" s="29"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -5732,7 +5746,7 @@
       <c r="U22" s="39"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -7219,7 +7233,7 @@
       <c r="U53" s="26"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -7882,7 +7896,7 @@
       <c r="T33" s="22"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -7897,7 +7911,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9763,7 +9777,7 @@
       <c r="S42" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -9778,8 +9792,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS71"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9987,8 +10001,8 @@
       <c r="T3" s="25">
         <v>0.03</v>
       </c>
-      <c r="W3" s="40" t="s">
-        <v>26</v>
+      <c r="W3" s="50" t="s">
+        <v>96</v>
       </c>
       <c r="X3" s="25">
         <v>0</v>
@@ -10048,8 +10062,8 @@
         <v>134</v>
       </c>
       <c r="T4" s="25"/>
-      <c r="W4" s="40" t="s">
-        <v>27</v>
+      <c r="W4" s="56" t="s">
+        <v>88</v>
       </c>
       <c r="X4" s="25">
         <v>0.5</v>
@@ -12843,7 +12857,7 @@
       <c r="AS71" s="25"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -12858,8 +12872,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="W64" sqref="W64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14507,8 +14521,8 @@
       </c>
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
-      <c r="W36" s="40" t="s">
-        <v>26</v>
+      <c r="W36" s="56" t="s">
+        <v>96</v>
       </c>
       <c r="X36" s="30">
         <v>0.2</v>
@@ -14576,8 +14590,8 @@
       <c r="T37" s="30"/>
       <c r="U37" s="6"/>
       <c r="V37" s="6"/>
-      <c r="W37" s="40" t="s">
-        <v>27</v>
+      <c r="W37" s="56" t="s">
+        <v>88</v>
       </c>
       <c r="X37" s="30">
         <v>0.2</v>
@@ -14820,8 +14834,8 @@
       </c>
       <c r="U41" s="6"/>
       <c r="V41" s="6"/>
-      <c r="W41" s="40" t="s">
-        <v>27</v>
+      <c r="W41" s="56" t="s">
+        <v>88</v>
       </c>
       <c r="X41" s="30">
         <v>0.05</v>
@@ -15054,8 +15068,8 @@
       </c>
       <c r="U47" s="6"/>
       <c r="V47" s="6"/>
-      <c r="W47" s="40" t="s">
-        <v>26</v>
+      <c r="W47" s="56" t="s">
+        <v>96</v>
       </c>
       <c r="X47" s="30">
         <v>0.3</v>
@@ -15123,8 +15137,8 @@
       <c r="T48" s="30"/>
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
-      <c r="W48" s="40" t="s">
-        <v>27</v>
+      <c r="W48" s="56" t="s">
+        <v>88</v>
       </c>
       <c r="X48" s="30">
         <v>0.6</v>
@@ -15184,7 +15198,7 @@
       </c>
       <c r="U49" s="6"/>
       <c r="V49" s="6"/>
-      <c r="W49" s="40" t="s">
+      <c r="W49" s="56" t="s">
         <v>93</v>
       </c>
       <c r="X49" s="30">
@@ -15375,8 +15389,8 @@
       </c>
       <c r="U52" s="6"/>
       <c r="V52" s="6"/>
-      <c r="W52" s="40" t="s">
-        <v>27</v>
+      <c r="W52" s="56" t="s">
+        <v>88</v>
       </c>
       <c r="X52" s="30">
         <v>0.4</v>
@@ -15668,8 +15682,8 @@
       <c r="T59" s="40"/>
       <c r="U59" s="6"/>
       <c r="V59" s="6"/>
-      <c r="W59" s="42" t="s">
-        <v>27</v>
+      <c r="W59" s="57" t="s">
+        <v>88</v>
       </c>
       <c r="X59" s="30">
         <v>0.7</v>
@@ -15890,8 +15904,8 @@
       <c r="T63" s="41"/>
       <c r="U63" s="6"/>
       <c r="V63" s="6"/>
-      <c r="W63" s="42" t="s">
-        <v>27</v>
+      <c r="W63" s="57" t="s">
+        <v>88</v>
       </c>
       <c r="X63" s="30">
         <v>0.7</v>
@@ -16860,7 +16874,7 @@
       <c r="AS85" s="30"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -17924,7 +17938,7 @@
       <c r="AS20" s="30"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -17940,9 +17954,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18832,7 +18844,7 @@
       <c r="H41" s="36"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
still troubleshooting optimization, also made other bugfixes
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="40" windowWidth="19420" windowHeight="10960" tabRatio="863" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Disutilities &amp; costs" sheetId="14" r:id="rId12"/>
     <sheet name="Macroeconomics" sheetId="18" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="130000"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -496,12 +496,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -2451,7 +2451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K20"/>
   <sheetViews>
@@ -2459,25 +2459,25 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="20"/>
+    <col min="1" max="1" width="9.140625" style="20"/>
     <col min="2" max="2" width="5" style="20" customWidth="1"/>
     <col min="3" max="3" width="18" style="20" customWidth="1"/>
-    <col min="4" max="4" width="55.375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="10.125" style="20" customWidth="1"/>
-    <col min="6" max="7" width="9.125" style="20"/>
-    <col min="8" max="9" width="14.25" style="20" customWidth="1"/>
-    <col min="10" max="10" width="12.125" style="20" customWidth="1"/>
-    <col min="11" max="16384" width="9.125" style="20"/>
+    <col min="4" max="4" width="55.42578125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="20" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="20"/>
+    <col min="8" max="9" width="14.28515625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="20" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" s="21" t="s">
         <v>12</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="21">
         <v>1</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="21">
         <v>2</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="21">
         <v>3</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="21">
         <v>4</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="21">
         <v>5</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="21">
         <v>6</v>
       </c>
@@ -2698,22 +2698,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="21"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="21"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="21"/>
       <c r="C13" s="21" t="s">
         <v>12</v>
@@ -2725,7 +2725,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="21">
         <v>1</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="21">
         <v>2</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="21">
         <v>3</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="21">
         <v>4</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="21">
         <v>5</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="21">
         <v>6</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="21">
         <v>7</v>
       </c>
@@ -2835,7 +2835,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z19"/>
   <sheetViews>
@@ -2843,13 +2843,13 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="3" max="8" width="17.625" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="3" max="8" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
@@ -2861,7 +2861,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:26" s="6" customFormat="1">
+    <row r="2" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="4" t="str">
@@ -2889,7 +2889,7 @@
         <v>Clients</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -2901,7 +2901,7 @@
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -2913,7 +2913,7 @@
       <c r="G4" s="24"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -2925,7 +2925,7 @@
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -2937,7 +2937,7 @@
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -2949,7 +2949,7 @@
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -2961,7 +2961,7 @@
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
     </row>
-    <row r="9" spans="1:26" s="18" customFormat="1">
+    <row r="9" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="37"/>
       <c r="C9" s="16"/>
@@ -2989,10 +2989,10 @@
       <c r="Y9" s="16"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" s="18" customFormat="1">
+    <row r="10" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="37"/>
       <c r="C11" s="2"/>
@@ -3002,7 +3002,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>103</v>
       </c>
@@ -3014,7 +3014,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:26" s="6" customFormat="1">
+    <row r="13" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="4" t="str">
@@ -3042,7 +3042,7 @@
         <v>Clients</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -3054,7 +3054,7 @@
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -3066,7 +3066,7 @@
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -3078,7 +3078,7 @@
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -3090,7 +3090,7 @@
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -3102,7 +3102,7 @@
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -3115,7 +3115,6 @@
       <c r="H19" s="24"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3127,7 +3126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H69"/>
   <sheetViews>
@@ -3135,19 +3134,19 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="18"/>
-    <col min="2" max="2" width="33.25" style="18" customWidth="1"/>
-    <col min="3" max="16384" width="9.125" style="18"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="33.28515625" style="18" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="6" customFormat="1">
+    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
@@ -3158,7 +3157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>91</v>
       </c>
@@ -3168,7 +3167,7 @@
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
         <v>92</v>
       </c>
@@ -3178,7 +3177,7 @@
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
         <v>93</v>
       </c>
@@ -3188,7 +3187,7 @@
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
         <v>94</v>
       </c>
@@ -3198,7 +3197,7 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
         <v>90</v>
       </c>
@@ -3208,7 +3207,7 @@
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
         <v>131</v>
       </c>
@@ -3218,7 +3217,7 @@
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>132</v>
       </c>
@@ -3228,7 +3227,7 @@
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -3238,12 +3237,12 @@
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="6" customFormat="1">
+    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="4" t="s">
         <v>0</v>
       </c>
@@ -3254,7 +3253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
         <v>3</v>
       </c>
@@ -3264,7 +3263,7 @@
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="19" t="s">
         <v>113</v>
       </c>
@@ -3274,7 +3273,7 @@
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
         <v>104</v>
       </c>
@@ -3284,7 +3283,7 @@
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
         <v>105</v>
       </c>
@@ -3294,7 +3293,7 @@
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
         <v>115</v>
       </c>
@@ -3304,7 +3303,7 @@
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -3314,13 +3313,13 @@
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>130</v>
       </c>
       <c r="B23" s="19"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>0</v>
       </c>
@@ -3331,7 +3330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
         <v>106</v>
       </c>
@@ -3341,7 +3340,7 @@
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
         <v>104</v>
       </c>
@@ -3351,7 +3350,7 @@
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
         <v>107</v>
       </c>
@@ -3361,7 +3360,7 @@
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="19" t="s">
         <v>116</v>
       </c>
@@ -3371,7 +3370,7 @@
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -3381,12 +3380,12 @@
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" s="4" t="s">
         <v>0</v>
       </c>
@@ -3397,7 +3396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="19" t="s">
         <v>108</v>
       </c>
@@ -3407,7 +3406,7 @@
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" s="19" t="s">
         <v>109</v>
       </c>
@@ -3417,7 +3416,7 @@
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="19" t="s">
         <v>110</v>
       </c>
@@ -3427,10 +3426,10 @@
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="19"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -3440,12 +3439,12 @@
       <c r="G39" s="16"/>
       <c r="H39" s="16"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="4" t="s">
         <v>0</v>
       </c>
@@ -3456,7 +3455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" s="19" t="s">
         <v>111</v>
       </c>
@@ -3470,7 +3469,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="19" t="s">
         <v>112</v>
       </c>
@@ -3484,7 +3483,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -3494,12 +3493,12 @@
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C48" s="4" t="s">
         <v>0</v>
       </c>
@@ -3510,7 +3509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
         <v>3</v>
       </c>
@@ -3520,7 +3519,7 @@
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B50" s="19" t="s">
         <v>113</v>
       </c>
@@ -3530,7 +3529,7 @@
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>114</v>
       </c>
@@ -3540,7 +3539,7 @@
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="19" t="s">
         <v>105</v>
       </c>
@@ -3550,7 +3549,7 @@
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>115</v>
       </c>
@@ -3560,7 +3559,7 @@
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" s="19" t="s">
         <v>4</v>
       </c>
@@ -3570,7 +3569,7 @@
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
         <v>15</v>
       </c>
@@ -3580,7 +3579,7 @@
       <c r="D55" s="22"/>
       <c r="E55" s="22"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="16"/>
       <c r="B58" s="16"/>
       <c r="C58" s="16"/>
@@ -3590,12 +3589,12 @@
       <c r="G58" s="16"/>
       <c r="H58" s="16"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C60" s="4" t="s">
         <v>0</v>
       </c>
@@ -3606,7 +3605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" s="19" t="s">
         <v>58</v>
       </c>
@@ -3616,7 +3615,7 @@
       <c r="D61" s="22"/>
       <c r="E61" s="22"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" s="19" t="s">
         <v>5</v>
       </c>
@@ -3626,7 +3625,7 @@
       <c r="D62" s="22"/>
       <c r="E62" s="22"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B63" s="19" t="s">
         <v>16</v>
       </c>
@@ -3636,7 +3635,7 @@
       <c r="D63" s="22"/>
       <c r="E63" s="22"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" s="19" t="s">
         <v>6</v>
       </c>
@@ -3646,7 +3645,7 @@
       <c r="D64" s="22"/>
       <c r="E64" s="22"/>
     </row>
-    <row r="65" spans="2:5">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="19" t="s">
         <v>95</v>
       </c>
@@ -3656,7 +3655,7 @@
       <c r="D65" s="22"/>
       <c r="E65" s="22"/>
     </row>
-    <row r="66" spans="2:5">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="19" t="s">
         <v>7</v>
       </c>
@@ -3666,7 +3665,7 @@
       <c r="D66" s="22"/>
       <c r="E66" s="22"/>
     </row>
-    <row r="67" spans="2:5">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="19" t="s">
         <v>96</v>
       </c>
@@ -3676,7 +3675,7 @@
       <c r="D67" s="22"/>
       <c r="E67" s="22"/>
     </row>
-    <row r="68" spans="2:5">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="19" t="s">
         <v>84</v>
       </c>
@@ -3686,7 +3685,7 @@
       <c r="D68" s="22"/>
       <c r="E68" s="22"/>
     </row>
-    <row r="69" spans="2:5">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="19" t="s">
         <v>85</v>
       </c>
@@ -3697,7 +3696,6 @@
       <c r="E69" s="22"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3709,20 +3707,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W41" sqref="W41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>137</v>
       </c>
@@ -3731,7 +3729,7 @@
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="4" t="s">
@@ -3744,7 +3742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="18" customFormat="1">
+    <row r="3" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>136</v>
       </c>
@@ -3754,7 +3752,7 @@
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
         <v>117</v>
@@ -3765,7 +3763,7 @@
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="19" t="s">
         <v>118</v>
@@ -3776,7 +3774,7 @@
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="19" t="s">
         <v>119</v>
@@ -3787,7 +3785,7 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="19" t="s">
         <v>120</v>
@@ -3798,7 +3796,7 @@
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="s">
         <v>19</v>
@@ -3809,15 +3807,15 @@
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
     </row>
-    <row r="10" spans="1:8" s="18" customFormat="1"/>
-    <row r="11" spans="1:8" s="18" customFormat="1">
+    <row r="10" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -3827,7 +3825,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>135</v>
       </c>
@@ -3836,7 +3834,7 @@
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="4" t="s">
@@ -3849,7 +3847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
         <v>3</v>
@@ -3860,7 +3858,7 @@
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="19" t="s">
         <v>113</v>
@@ -3871,7 +3869,7 @@
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
         <v>114</v>
@@ -3882,7 +3880,7 @@
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="19" t="s">
         <v>105</v>
@@ -3893,7 +3891,7 @@
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="19" t="s">
         <v>115</v>
@@ -3904,7 +3902,7 @@
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>134</v>
       </c>
@@ -3913,7 +3911,7 @@
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="4" t="s">
@@ -3926,7 +3924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="19" t="s">
         <v>3</v>
@@ -3937,52 +3935,51 @@
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="19" t="s">
         <v>113</v>
       </c>
       <c r="C25" s="22">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="19" t="s">
         <v>114</v>
       </c>
       <c r="C26" s="22">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="19" t="s">
         <v>105</v>
       </c>
       <c r="C27" s="22">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="19" t="s">
         <v>115</v>
       </c>
       <c r="C28" s="22">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3994,21 +3991,21 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T57"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="3" max="4" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="3" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>29</v>
       </c>
@@ -4030,7 +4027,7 @@
       <c r="R1" s="18"/>
       <c r="S1" s="18"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="C2" s="19">
         <v>2015</v>
@@ -4085,7 +4082,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -4158,7 +4155,7 @@
       </c>
       <c r="T3" s="29"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>30</v>
       </c>
@@ -4180,7 +4177,7 @@
       <c r="R7" s="18"/>
       <c r="S7" s="18"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="C8" s="19">
         <v>2015</v>
@@ -4235,7 +4232,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="4" t="s">
         <v>10</v>
@@ -4308,7 +4305,7 @@
       </c>
       <c r="T9" s="29"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>44</v>
       </c>
@@ -4330,7 +4327,7 @@
       <c r="R13" s="18"/>
       <c r="S13" s="18"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="C14" s="19">
         <v>2015</v>
@@ -4385,7 +4382,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
         <v>10</v>
@@ -4458,14 +4455,14 @@
       </c>
       <c r="T15" s="29"/>
     </row>
-    <row r="19" spans="1:20" s="18" customFormat="1">
+    <row r="19" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>51</v>
       </c>
       <c r="B19" s="6"/>
       <c r="T19" s="6"/>
     </row>
-    <row r="20" spans="1:20" s="18" customFormat="1">
+    <row r="20" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="19">
         <v>2015</v>
@@ -4519,7 +4516,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="18" customFormat="1">
+    <row r="21" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
@@ -4544,26 +4541,26 @@
       </c>
       <c r="T21" s="29"/>
     </row>
-    <row r="22" spans="1:20" s="18" customFormat="1">
+    <row r="22" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="T22" s="6"/>
     </row>
-    <row r="23" spans="1:20" s="18" customFormat="1">
+    <row r="23" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="T23" s="6"/>
     </row>
-    <row r="24" spans="1:20" s="18" customFormat="1">
+    <row r="24" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="T24" s="6"/>
     </row>
-    <row r="25" spans="1:20" s="18" customFormat="1">
+    <row r="25" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>45</v>
       </c>
       <c r="B25" s="6"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="1:20" s="18" customFormat="1">
+    <row r="26" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="C26" s="19">
         <v>2015</v>
@@ -4617,7 +4614,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="18" customFormat="1">
+    <row r="27" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>10</v>
       </c>
@@ -4690,14 +4687,14 @@
       </c>
       <c r="T27" s="29"/>
     </row>
-    <row r="31" spans="1:20" s="18" customFormat="1">
+    <row r="31" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>46</v>
       </c>
       <c r="B31" s="6"/>
       <c r="T31" s="6"/>
     </row>
-    <row r="32" spans="1:20" s="18" customFormat="1">
+    <row r="32" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="C32" s="19">
         <v>2015</v>
@@ -4751,7 +4748,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="18" customFormat="1">
+    <row r="33" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>10</v>
       </c>
@@ -4808,26 +4805,26 @@
       </c>
       <c r="T33" s="29"/>
     </row>
-    <row r="34" spans="1:20" s="18" customFormat="1">
+    <row r="34" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="T34" s="6"/>
     </row>
-    <row r="35" spans="1:20" s="18" customFormat="1">
+    <row r="35" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="T35" s="6"/>
     </row>
-    <row r="36" spans="1:20" s="18" customFormat="1">
+    <row r="36" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="T36" s="6"/>
     </row>
-    <row r="37" spans="1:20" s="18" customFormat="1">
+    <row r="37" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>47</v>
       </c>
       <c r="B37" s="6"/>
       <c r="T37" s="6"/>
     </row>
-    <row r="38" spans="1:20" s="18" customFormat="1">
+    <row r="38" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="19">
         <v>2015</v>
@@ -4881,7 +4878,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="18" customFormat="1">
+    <row r="39" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>10</v>
       </c>
@@ -4906,26 +4903,26 @@
       </c>
       <c r="T39" s="29"/>
     </row>
-    <row r="40" spans="1:20" s="18" customFormat="1">
+    <row r="40" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="T40" s="6"/>
     </row>
-    <row r="41" spans="1:20" s="18" customFormat="1">
+    <row r="41" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="T41" s="6"/>
     </row>
-    <row r="42" spans="1:20" s="18" customFormat="1">
+    <row r="42" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="T42" s="6"/>
     </row>
-    <row r="43" spans="1:20" s="18" customFormat="1">
+    <row r="43" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="6"/>
       <c r="T43" s="6"/>
     </row>
-    <row r="44" spans="1:20" s="18" customFormat="1">
+    <row r="44" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="C44" s="19">
         <v>2015</v>
@@ -4979,7 +4976,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:20" s="18" customFormat="1">
+    <row r="45" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>10</v>
       </c>
@@ -5004,14 +5001,14 @@
       </c>
       <c r="T45" s="29"/>
     </row>
-    <row r="49" spans="1:20" s="18" customFormat="1">
+    <row r="49" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B49" s="6"/>
       <c r="T49" s="6"/>
     </row>
-    <row r="50" spans="1:20" s="18" customFormat="1">
+    <row r="50" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="C50" s="19">
         <v>2015</v>
@@ -5065,7 +5062,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:20" s="18" customFormat="1">
+    <row r="51" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>10</v>
       </c>
@@ -5090,26 +5087,26 @@
       </c>
       <c r="T51" s="29"/>
     </row>
-    <row r="52" spans="1:20" s="18" customFormat="1">
+    <row r="52" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="T52" s="6"/>
     </row>
-    <row r="53" spans="1:20" s="18" customFormat="1">
+    <row r="53" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="T53" s="6"/>
     </row>
-    <row r="54" spans="1:20" s="18" customFormat="1">
+    <row r="54" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="T54" s="6"/>
     </row>
-    <row r="55" spans="1:20" s="18" customFormat="1">
+    <row r="55" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
         <v>50</v>
       </c>
       <c r="B55" s="6"/>
       <c r="T55" s="6"/>
     </row>
-    <row r="56" spans="1:20" s="18" customFormat="1">
+    <row r="56" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="C56" s="19">
         <v>2015</v>
@@ -5163,7 +5160,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:20" s="18" customFormat="1">
+    <row r="57" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
         <v>10</v>
       </c>
@@ -5189,7 +5186,6 @@
       <c r="T57" s="29"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -5201,7 +5197,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:V22"/>
   <sheetViews>
@@ -5209,21 +5205,21 @@
       <selection activeCell="M12" sqref="M12:M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.125" style="18"/>
+    <col min="1" max="2" width="9.140625" style="18"/>
     <col min="3" max="3" width="11" style="18" customWidth="1"/>
-    <col min="4" max="20" width="9.125" style="18"/>
-    <col min="21" max="21" width="15.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.125" style="18"/>
+    <col min="4" max="20" width="9.140625" style="18"/>
+    <col min="21" max="21" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D2" s="19">
         <v>2000</v>
       </c>
@@ -5276,7 +5272,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$14</f>
         <v>SBCC</v>
@@ -5319,7 +5315,7 @@
       </c>
       <c r="U3" s="25"/>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$14</f>
         <v>SBCC</v>
@@ -5369,10 +5365,10 @@
       </c>
       <c r="U4" s="39"/>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$15</f>
         <v>NSP</v>
@@ -5403,7 +5399,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$15</f>
         <v>NSP</v>
@@ -5434,10 +5430,10 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="str">
         <f>'Populations &amp; programs'!$C$16</f>
         <v>OST</v>
@@ -5468,7 +5464,7 @@
       </c>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="4" t="str">
         <f>'Populations &amp; programs'!$C$16</f>
@@ -5500,11 +5496,11 @@
       </c>
       <c r="U10" s="39"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="4" t="str">
         <f>'Populations &amp; programs'!$C$17</f>
@@ -5537,7 +5533,7 @@
       <c r="U12" s="25"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="str">
         <f>'Populations &amp; programs'!$C$17</f>
         <v>MSM programs</v>
@@ -5568,7 +5564,7 @@
       </c>
       <c r="U13" s="39"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$C$18</f>
         <v>FSW programs</v>
@@ -5599,7 +5595,7 @@
       </c>
       <c r="U15" s="25"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$C$18</f>
         <v>FSW programs</v>
@@ -5630,7 +5626,7 @@
       </c>
       <c r="U16" s="39"/>
     </row>
-    <row r="18" spans="2:21">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$C$19</f>
         <v>ART</v>
@@ -5661,7 +5657,7 @@
       </c>
       <c r="U18" s="25"/>
     </row>
-    <row r="19" spans="2:21">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$C$19</f>
         <v>ART</v>
@@ -5692,7 +5688,7 @@
       </c>
       <c r="U19" s="39"/>
     </row>
-    <row r="21" spans="2:21">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="str">
         <f>'Populations &amp; programs'!$C$20</f>
         <v>PMTCT</v>
@@ -5723,7 +5719,7 @@
       </c>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="2:21">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="str">
         <f>'Populations &amp; programs'!$C$20</f>
         <v>PMTCT</v>
@@ -5766,7 +5762,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U53"/>
   <sheetViews>
@@ -5774,22 +5770,22 @@
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.125" style="18"/>
-    <col min="4" max="4" width="9.375" style="18" customWidth="1"/>
-    <col min="5" max="20" width="9.125" style="18"/>
-    <col min="21" max="21" width="15.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.875" style="18" customWidth="1"/>
-    <col min="23" max="16384" width="9.125" style="18"/>
+    <col min="1" max="3" width="9.140625" style="18"/>
+    <col min="4" max="4" width="9.42578125" style="18" customWidth="1"/>
+    <col min="5" max="20" width="9.140625" style="18"/>
+    <col min="21" max="21" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" style="18" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D2" s="19">
         <v>2000</v>
       </c>
@@ -5842,7 +5838,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -5873,7 +5869,7 @@
         <v>37500</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -5904,7 +5900,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -5935,12 +5931,12 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="U6" s="28"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -5969,7 +5965,7 @@
       </c>
       <c r="U7" s="27"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -6000,7 +5996,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -6029,7 +6025,7 @@
       </c>
       <c r="U9" s="27"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="28"/>
@@ -6050,7 +6046,7 @@
       <c r="S10" s="28"/>
       <c r="U10" s="28"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -6089,7 +6085,7 @@
       </c>
       <c r="U11" s="27"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -6128,7 +6124,7 @@
       </c>
       <c r="U12" s="27"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -6167,7 +6163,7 @@
       </c>
       <c r="U13" s="27"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="28"/>
@@ -6188,7 +6184,7 @@
       <c r="S14" s="28"/>
       <c r="U14" s="28"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -6217,7 +6213,7 @@
       </c>
       <c r="U15" s="27"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -6278,7 +6274,7 @@
       </c>
       <c r="U16" s="27"/>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -6307,7 +6303,7 @@
       </c>
       <c r="U17" s="27"/>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="28"/>
@@ -6328,7 +6324,7 @@
       <c r="S18" s="28"/>
       <c r="U18" s="28"/>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -6357,7 +6353,7 @@
       </c>
       <c r="U19" s="27"/>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -6418,7 +6414,7 @@
       </c>
       <c r="U20" s="27"/>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -6447,7 +6443,7 @@
       </c>
       <c r="U21" s="27"/>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="28"/>
@@ -6468,7 +6464,7 @@
       <c r="S22" s="28"/>
       <c r="U22" s="28"/>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -6497,7 +6493,7 @@
       </c>
       <c r="U23" s="27"/>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -6558,7 +6554,7 @@
       </c>
       <c r="U24" s="27"/>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -6587,12 +6583,12 @@
       </c>
       <c r="U25" s="27"/>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D30" s="19">
         <v>2000</v>
       </c>
@@ -6645,7 +6641,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -6676,7 +6672,7 @@
       </c>
       <c r="U31" s="26"/>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -6707,7 +6703,7 @@
       </c>
       <c r="U32" s="26"/>
     </row>
-    <row r="33" spans="2:21">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -6738,11 +6734,11 @@
       </c>
       <c r="U33" s="26"/>
     </row>
-    <row r="34" spans="2:21">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
     </row>
-    <row r="35" spans="2:21">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -6777,7 +6773,7 @@
       </c>
       <c r="U35" s="26"/>
     </row>
-    <row r="36" spans="2:21">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -6812,7 +6808,7 @@
       </c>
       <c r="U36" s="26"/>
     </row>
-    <row r="37" spans="2:21">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -6847,11 +6843,11 @@
       </c>
       <c r="U37" s="26"/>
     </row>
-    <row r="38" spans="2:21">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
     </row>
-    <row r="39" spans="2:21">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -6886,7 +6882,7 @@
       </c>
       <c r="U39" s="26"/>
     </row>
-    <row r="40" spans="2:21">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -6921,7 +6917,7 @@
       </c>
       <c r="U40" s="26"/>
     </row>
-    <row r="41" spans="2:21">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -6956,11 +6952,11 @@
       </c>
       <c r="U41" s="26"/>
     </row>
-    <row r="42" spans="2:21">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
     </row>
-    <row r="43" spans="2:21">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -6989,7 +6985,7 @@
       </c>
       <c r="U43" s="26"/>
     </row>
-    <row r="44" spans="2:21">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -7020,7 +7016,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="45" spans="2:21">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -7049,11 +7045,11 @@
       </c>
       <c r="U45" s="26"/>
     </row>
-    <row r="46" spans="2:21">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
     </row>
-    <row r="47" spans="2:21">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -7082,7 +7078,7 @@
       </c>
       <c r="U47" s="26"/>
     </row>
-    <row r="48" spans="2:21">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -7119,7 +7115,7 @@
       </c>
       <c r="U48" s="26"/>
     </row>
-    <row r="49" spans="2:21">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -7148,11 +7144,11 @@
       </c>
       <c r="U49" s="26"/>
     </row>
-    <row r="50" spans="2:21">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
     </row>
-    <row r="51" spans="2:21">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -7181,7 +7177,7 @@
       </c>
       <c r="U51" s="26"/>
     </row>
-    <row r="52" spans="2:21">
+    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -7212,7 +7208,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="53" spans="2:21">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -7253,7 +7249,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T33"/>
   <sheetViews>
@@ -7261,13 +7257,13 @@
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="20" max="20" width="14.25" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>98</v>
       </c>
@@ -7290,7 +7286,7 @@
       <c r="S1" s="9"/>
       <c r="T1" s="9"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="C2" s="10">
         <v>2000</v>
@@ -7345,7 +7341,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -7371,13 +7367,13 @@
       </c>
       <c r="T3" s="22"/>
     </row>
-    <row r="5" spans="1:20" s="18" customFormat="1">
+    <row r="5" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:20" s="18" customFormat="1">
+    <row r="6" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>99</v>
       </c>
@@ -7400,7 +7396,7 @@
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="C8" s="10">
         <v>2000</v>
@@ -7455,7 +7451,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
         <v>10</v>
@@ -7505,13 +7501,13 @@
       </c>
       <c r="T9" s="22"/>
     </row>
-    <row r="11" spans="1:20" s="18" customFormat="1">
+    <row r="11" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:20" s="18" customFormat="1">
+    <row r="12" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>100</v>
       </c>
@@ -7534,7 +7530,7 @@
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="C14" s="10">
         <v>2000</v>
@@ -7589,7 +7585,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="4" t="s">
         <v>10</v>
@@ -7615,19 +7611,19 @@
       </c>
       <c r="T15" s="22"/>
     </row>
-    <row r="17" spans="1:20" s="18" customFormat="1">
+    <row r="17" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:20" s="18" customFormat="1">
+    <row r="18" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:20" s="18" customFormat="1">
+    <row r="19" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>147</v>
       </c>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:20" s="18" customFormat="1">
+    <row r="20" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="19">
         <v>2000</v>
@@ -7681,7 +7677,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="18" customFormat="1">
+    <row r="21" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
@@ -7706,16 +7702,16 @@
       </c>
       <c r="T21" s="22"/>
     </row>
-    <row r="22" spans="1:20" s="18" customFormat="1">
+    <row r="22" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:20" s="18" customFormat="1">
+    <row r="23" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:20" s="18" customFormat="1">
+    <row r="24" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>54</v>
       </c>
@@ -7738,7 +7734,7 @@
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="C26" s="10">
         <v>2000</v>
@@ -7793,7 +7789,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="4" t="s">
         <v>10</v>
@@ -7819,13 +7815,13 @@
       </c>
       <c r="T27" s="22"/>
     </row>
-    <row r="31" spans="1:20" s="18" customFormat="1">
+    <row r="31" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="1:20" s="18" customFormat="1">
+    <row r="32" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="C32" s="19">
         <v>2000</v>
@@ -7879,7 +7875,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="2:20" s="18" customFormat="1">
+    <row r="33" spans="2:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>10</v>
       </c>
@@ -7905,7 +7901,6 @@
       <c r="T33" s="22"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -7917,30 +7912,30 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS42"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="21" max="21" width="9.125" customWidth="1"/>
-    <col min="22" max="22" width="8.875" customWidth="1"/>
-    <col min="23" max="23" width="10.375" style="6" customWidth="1"/>
-    <col min="28" max="28" width="8.875" style="18" customWidth="1"/>
-    <col min="29" max="29" width="10.375" style="6" customWidth="1"/>
-    <col min="30" max="33" width="8.625" style="18"/>
-    <col min="34" max="34" width="8.875" style="18" customWidth="1"/>
-    <col min="35" max="35" width="10.375" style="6" customWidth="1"/>
-    <col min="36" max="39" width="8.625" style="18"/>
-    <col min="40" max="40" width="8.875" style="18" customWidth="1"/>
-    <col min="41" max="41" width="10.375" style="6" customWidth="1"/>
-    <col min="42" max="45" width="8.625" style="18"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="21" max="21" width="9.140625" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" style="6" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" style="18" customWidth="1"/>
+    <col min="29" max="29" width="10.42578125" style="6" customWidth="1"/>
+    <col min="30" max="33" width="8.5703125" style="18"/>
+    <col min="34" max="34" width="8.85546875" style="18" customWidth="1"/>
+    <col min="35" max="35" width="10.42578125" style="6" customWidth="1"/>
+    <col min="36" max="39" width="8.5703125" style="18"/>
+    <col min="40" max="40" width="8.85546875" style="18" customWidth="1"/>
+    <col min="41" max="41" width="10.42578125" style="6" customWidth="1"/>
+    <col min="42" max="45" width="8.5703125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="18" customFormat="1">
+    <row r="1" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>97</v>
       </c>
@@ -7974,7 +7969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="18" customFormat="1">
+    <row r="2" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="19">
         <v>2000</v>
@@ -8088,7 +8083,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:45" s="18" customFormat="1">
+    <row r="3" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -8136,7 +8131,7 @@
       <c r="AR3" s="25"/>
       <c r="AS3" s="25"/>
     </row>
-    <row r="4" spans="1:45" s="18" customFormat="1">
+    <row r="4" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -8184,7 +8179,7 @@
       <c r="AR4" s="25"/>
       <c r="AS4" s="25"/>
     </row>
-    <row r="5" spans="1:45" s="18" customFormat="1">
+    <row r="5" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -8232,7 +8227,7 @@
       <c r="AR5" s="25"/>
       <c r="AS5" s="25"/>
     </row>
-    <row r="6" spans="1:45" s="18" customFormat="1">
+    <row r="6" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -8280,7 +8275,7 @@
       <c r="AR6" s="25"/>
       <c r="AS6" s="25"/>
     </row>
-    <row r="7" spans="1:45" s="18" customFormat="1">
+    <row r="7" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -8328,7 +8323,7 @@
       <c r="AR7" s="25"/>
       <c r="AS7" s="25"/>
     </row>
-    <row r="8" spans="1:45" s="18" customFormat="1">
+    <row r="8" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -8376,28 +8371,28 @@
       <c r="AR8" s="25"/>
       <c r="AS8" s="25"/>
     </row>
-    <row r="9" spans="1:45" s="18" customFormat="1">
+    <row r="9" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="W9" s="6"/>
       <c r="AC9" s="6"/>
       <c r="AI9" s="6"/>
       <c r="AO9" s="6"/>
     </row>
-    <row r="10" spans="1:45" s="18" customFormat="1">
+    <row r="10" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="W10" s="6"/>
       <c r="AC10" s="6"/>
       <c r="AI10" s="6"/>
       <c r="AO10" s="6"/>
     </row>
-    <row r="11" spans="1:45" s="18" customFormat="1">
+    <row r="11" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="W11" s="6"/>
       <c r="AC11" s="6"/>
       <c r="AI11" s="6"/>
       <c r="AO11" s="6"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>31</v>
       </c>
@@ -8445,7 +8440,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="C13" s="8">
         <v>2000</v>
@@ -8560,7 +8555,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -8609,7 +8604,7 @@
       <c r="AR14" s="25"/>
       <c r="AS14" s="25"/>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -8658,7 +8653,7 @@
       <c r="AR15" s="25"/>
       <c r="AS15" s="25"/>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -8707,7 +8702,7 @@
       <c r="AR16" s="25"/>
       <c r="AS16" s="25"/>
     </row>
-    <row r="17" spans="1:45">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -8756,7 +8751,7 @@
       <c r="AR17" s="25"/>
       <c r="AS17" s="25"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -8805,7 +8800,7 @@
       <c r="AR18" s="25"/>
       <c r="AS18" s="25"/>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -8854,28 +8849,28 @@
       <c r="AR19" s="25"/>
       <c r="AS19" s="25"/>
     </row>
-    <row r="20" spans="1:45" s="18" customFormat="1">
+    <row r="20" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="W20" s="6"/>
       <c r="AC20" s="6"/>
       <c r="AI20" s="6"/>
       <c r="AO20" s="6"/>
     </row>
-    <row r="21" spans="1:45" s="18" customFormat="1">
+    <row r="21" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="W21" s="6"/>
       <c r="AC21" s="6"/>
       <c r="AI21" s="6"/>
       <c r="AO21" s="6"/>
     </row>
-    <row r="22" spans="1:45" s="18" customFormat="1">
+    <row r="22" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="W22" s="6"/>
       <c r="AC22" s="6"/>
       <c r="AI22" s="6"/>
       <c r="AO22" s="6"/>
     </row>
-    <row r="23" spans="1:45" s="18" customFormat="1">
+    <row r="23" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>42</v>
       </c>
@@ -8909,7 +8904,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:45" s="18" customFormat="1">
+    <row r="24" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="19">
         <v>2000</v>
@@ -9023,7 +9018,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:45" s="18" customFormat="1">
+    <row r="25" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -9071,7 +9066,7 @@
       <c r="AR25" s="25"/>
       <c r="AS25" s="25"/>
     </row>
-    <row r="26" spans="1:45" s="18" customFormat="1">
+    <row r="26" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -9119,7 +9114,7 @@
       <c r="AR26" s="25"/>
       <c r="AS26" s="25"/>
     </row>
-    <row r="27" spans="1:45" s="18" customFormat="1">
+    <row r="27" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -9167,7 +9162,7 @@
       <c r="AR27" s="25"/>
       <c r="AS27" s="25"/>
     </row>
-    <row r="28" spans="1:45" s="18" customFormat="1">
+    <row r="28" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -9215,7 +9210,7 @@
       <c r="AR28" s="25"/>
       <c r="AS28" s="25"/>
     </row>
-    <row r="29" spans="1:45" s="18" customFormat="1">
+    <row r="29" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -9263,7 +9258,7 @@
       <c r="AR29" s="25"/>
       <c r="AS29" s="25"/>
     </row>
-    <row r="30" spans="1:45" s="18" customFormat="1">
+    <row r="30" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -9311,10 +9306,10 @@
       <c r="AR30" s="25"/>
       <c r="AS30" s="25"/>
     </row>
-    <row r="31" spans="1:45">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
       <c r="S31" s="5"/>
     </row>
-    <row r="32" spans="1:45" s="18" customFormat="1">
+    <row r="32" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="S32" s="5"/>
       <c r="W32" s="6"/>
@@ -9322,7 +9317,7 @@
       <c r="AI32" s="6"/>
       <c r="AO32" s="6"/>
     </row>
-    <row r="33" spans="1:45" s="18" customFormat="1">
+    <row r="33" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="S33" s="5"/>
       <c r="W33" s="6"/>
@@ -9330,7 +9325,7 @@
       <c r="AI33" s="6"/>
       <c r="AO33" s="6"/>
     </row>
-    <row r="34" spans="1:45">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>14</v>
       </c>
@@ -9379,7 +9374,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:45">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="C35" s="8">
         <v>2000</v>
@@ -9494,7 +9489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:45">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -9543,7 +9538,7 @@
       <c r="AR36" s="25"/>
       <c r="AS36" s="25"/>
     </row>
-    <row r="37" spans="1:45">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -9591,7 +9586,7 @@
       <c r="AR37" s="25"/>
       <c r="AS37" s="25"/>
     </row>
-    <row r="38" spans="1:45">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -9639,7 +9634,7 @@
       <c r="AR38" s="25"/>
       <c r="AS38" s="25"/>
     </row>
-    <row r="39" spans="1:45">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -9687,7 +9682,7 @@
       <c r="AR39" s="25"/>
       <c r="AS39" s="25"/>
     </row>
-    <row r="40" spans="1:45">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -9735,7 +9730,7 @@
       <c r="AR40" s="25"/>
       <c r="AS40" s="25"/>
     </row>
-    <row r="41" spans="1:45">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -9783,11 +9778,10 @@
       <c r="AR41" s="25"/>
       <c r="AS41" s="25"/>
     </row>
-    <row r="42" spans="1:45">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="S42" s="5"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -9799,28 +9793,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="20" max="20" width="14.25" customWidth="1"/>
-    <col min="23" max="23" width="12.375" style="6" customWidth="1"/>
-    <col min="29" max="29" width="12.375" style="6" customWidth="1"/>
-    <col min="30" max="33" width="8.625" style="18"/>
-    <col min="35" max="35" width="12.375" style="6" customWidth="1"/>
-    <col min="36" max="39" width="8.625" style="18"/>
-    <col min="41" max="41" width="12.375" style="6" customWidth="1"/>
-    <col min="42" max="45" width="8.625" style="18"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" style="6" customWidth="1"/>
+    <col min="29" max="29" width="12.42578125" style="6" customWidth="1"/>
+    <col min="30" max="33" width="8.5703125" style="18"/>
+    <col min="35" max="35" width="12.42578125" style="6" customWidth="1"/>
+    <col min="36" max="39" width="8.5703125" style="18"/>
+    <col min="41" max="41" width="12.42578125" style="6" customWidth="1"/>
+    <col min="42" max="45" width="8.5703125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>55</v>
       </c>
@@ -9869,7 +9863,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="C2" s="10">
         <v>2000</v>
@@ -9984,7 +9978,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -10016,7 +10010,7 @@
         <v>74</v>
       </c>
       <c r="X3" s="25">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="Y3" s="25">
         <v>0.3</v>
@@ -10043,7 +10037,7 @@
       <c r="AR3" s="25"/>
       <c r="AS3" s="25"/>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -10104,7 +10098,7 @@
       <c r="AR4" s="25"/>
       <c r="AS4" s="25"/>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -10157,7 +10151,7 @@
       <c r="AR5" s="25"/>
       <c r="AS5" s="25"/>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -10206,7 +10200,7 @@
       <c r="AR6" s="25"/>
       <c r="AS6" s="25"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -10255,7 +10249,7 @@
       <c r="AR7" s="25"/>
       <c r="AS7" s="25"/>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -10304,21 +10298,21 @@
       <c r="AR8" s="25"/>
       <c r="AS8" s="25"/>
     </row>
-    <row r="10" spans="1:45" s="18" customFormat="1">
+    <row r="10" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="W10" s="6"/>
       <c r="AC10" s="6"/>
       <c r="AI10" s="6"/>
       <c r="AO10" s="6"/>
     </row>
-    <row r="11" spans="1:45" s="18" customFormat="1">
+    <row r="11" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="W11" s="6"/>
       <c r="AC11" s="6"/>
       <c r="AI11" s="6"/>
       <c r="AO11" s="6"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>101</v>
       </c>
@@ -10367,7 +10361,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="C13" s="10">
         <v>2000</v>
@@ -10482,7 +10476,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="4" t="s">
         <v>11</v>
@@ -10530,21 +10524,21 @@
       <c r="AR14" s="25"/>
       <c r="AS14" s="25"/>
     </row>
-    <row r="16" spans="1:45" s="18" customFormat="1">
+    <row r="16" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="W16" s="6"/>
       <c r="AC16" s="6"/>
       <c r="AI16" s="6"/>
       <c r="AO16" s="6"/>
     </row>
-    <row r="17" spans="1:45" s="18" customFormat="1">
+    <row r="17" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="W17" s="6"/>
       <c r="AC17" s="6"/>
       <c r="AI17" s="6"/>
       <c r="AO17" s="6"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>52</v>
       </c>
@@ -10593,7 +10587,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="C19" s="10">
         <v>2000</v>
@@ -10708,7 +10702,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:45">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="4" t="s">
         <v>10</v>
@@ -10792,21 +10786,21 @@
       <c r="AR20" s="39"/>
       <c r="AS20" s="39"/>
     </row>
-    <row r="21" spans="1:45" s="18" customFormat="1">
+    <row r="21" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="W21" s="6"/>
       <c r="AC21" s="6"/>
       <c r="AI21" s="6"/>
       <c r="AO21" s="6"/>
     </row>
-    <row r="22" spans="1:45" s="18" customFormat="1">
+    <row r="22" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="W22" s="6"/>
       <c r="AC22" s="6"/>
       <c r="AI22" s="6"/>
       <c r="AO22" s="6"/>
     </row>
-    <row r="24" spans="1:45">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>53</v>
       </c>
@@ -10855,7 +10849,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:45">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="C25" s="10">
         <v>2000</v>
@@ -10970,7 +10964,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:45">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="4" t="s">
         <v>10</v>
@@ -11054,28 +11048,28 @@
       <c r="AR26" s="39"/>
       <c r="AS26" s="39"/>
     </row>
-    <row r="27" spans="1:45" s="18" customFormat="1">
+    <row r="27" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="W27" s="6"/>
       <c r="AC27" s="6"/>
       <c r="AI27" s="6"/>
       <c r="AO27" s="6"/>
     </row>
-    <row r="28" spans="1:45" s="18" customFormat="1" ht="14.25" customHeight="1">
+    <row r="28" spans="1:45" s="18" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="W28" s="6"/>
       <c r="AC28" s="6"/>
       <c r="AI28" s="6"/>
       <c r="AO28" s="6"/>
     </row>
-    <row r="29" spans="1:45" s="18" customFormat="1">
+    <row r="29" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="W29" s="6"/>
       <c r="AC29" s="6"/>
       <c r="AI29" s="6"/>
       <c r="AO29" s="6"/>
     </row>
-    <row r="30" spans="1:45" s="18" customFormat="1">
+    <row r="30" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>82</v>
       </c>
@@ -11109,7 +11103,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:45" s="18" customFormat="1">
+    <row r="31" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="C31" s="19">
         <v>2000</v>
@@ -11223,7 +11217,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:45" s="18" customFormat="1">
+    <row r="32" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -11271,7 +11265,7 @@
       <c r="AR32" s="25"/>
       <c r="AS32" s="25"/>
     </row>
-    <row r="33" spans="1:45" s="18" customFormat="1">
+    <row r="33" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -11319,7 +11313,7 @@
       <c r="AR33" s="25"/>
       <c r="AS33" s="25"/>
     </row>
-    <row r="34" spans="1:45" s="18" customFormat="1">
+    <row r="34" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -11367,7 +11361,7 @@
       <c r="AR34" s="25"/>
       <c r="AS34" s="25"/>
     </row>
-    <row r="35" spans="1:45" s="18" customFormat="1">
+    <row r="35" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -11415,7 +11409,7 @@
       <c r="AR35" s="25"/>
       <c r="AS35" s="25"/>
     </row>
-    <row r="36" spans="1:45" s="18" customFormat="1">
+    <row r="36" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -11464,7 +11458,7 @@
       <c r="AR36" s="25"/>
       <c r="AS36" s="25"/>
     </row>
-    <row r="37" spans="1:45" s="18" customFormat="1">
+    <row r="37" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -11512,21 +11506,21 @@
       <c r="AR37" s="25"/>
       <c r="AS37" s="25"/>
     </row>
-    <row r="38" spans="1:45" s="18" customFormat="1">
+    <row r="38" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="W38" s="6"/>
       <c r="AC38" s="6"/>
       <c r="AI38" s="6"/>
       <c r="AO38" s="6"/>
     </row>
-    <row r="40" spans="1:45" s="18" customFormat="1">
+    <row r="40" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="W40" s="6"/>
       <c r="AC40" s="6"/>
       <c r="AI40" s="6"/>
       <c r="AO40" s="6"/>
     </row>
-    <row r="41" spans="1:45" s="18" customFormat="1">
+    <row r="41" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>83</v>
       </c>
@@ -11560,7 +11554,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:45" s="18" customFormat="1">
+    <row r="42" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="C42" s="19">
         <v>2000</v>
@@ -11674,7 +11668,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:45" s="18" customFormat="1">
+    <row r="43" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -11722,7 +11716,7 @@
       <c r="AR43" s="25"/>
       <c r="AS43" s="25"/>
     </row>
-    <row r="44" spans="1:45" s="18" customFormat="1">
+    <row r="44" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -11770,7 +11764,7 @@
       <c r="AR44" s="25"/>
       <c r="AS44" s="25"/>
     </row>
-    <row r="45" spans="1:45" s="18" customFormat="1">
+    <row r="45" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -11818,7 +11812,7 @@
       <c r="AR45" s="25"/>
       <c r="AS45" s="25"/>
     </row>
-    <row r="46" spans="1:45" s="18" customFormat="1">
+    <row r="46" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -11866,7 +11860,7 @@
       <c r="AR46" s="25"/>
       <c r="AS46" s="25"/>
     </row>
-    <row r="47" spans="1:45" s="18" customFormat="1">
+    <row r="47" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -11915,7 +11909,7 @@
       <c r="AR47" s="25"/>
       <c r="AS47" s="25"/>
     </row>
-    <row r="48" spans="1:45" s="18" customFormat="1">
+    <row r="48" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -11963,28 +11957,28 @@
       <c r="AR48" s="25"/>
       <c r="AS48" s="25"/>
     </row>
-    <row r="49" spans="1:45" s="18" customFormat="1">
+    <row r="49" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="W49" s="6"/>
       <c r="AC49" s="6"/>
       <c r="AI49" s="6"/>
       <c r="AO49" s="6"/>
     </row>
-    <row r="50" spans="1:45" s="18" customFormat="1">
+    <row r="50" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="W50" s="6"/>
       <c r="AC50" s="6"/>
       <c r="AI50" s="6"/>
       <c r="AO50" s="6"/>
     </row>
-    <row r="51" spans="1:45" s="18" customFormat="1">
+    <row r="51" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="W51" s="6"/>
       <c r="AC51" s="6"/>
       <c r="AI51" s="6"/>
       <c r="AO51" s="6"/>
     </row>
-    <row r="52" spans="1:45">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>80</v>
       </c>
@@ -12033,7 +12027,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:45">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="C53" s="10">
         <v>2000</v>
@@ -12148,7 +12142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:45">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="4" t="s">
         <v>10</v>
@@ -12214,28 +12208,28 @@
       <c r="AR54" s="25"/>
       <c r="AS54" s="25"/>
     </row>
-    <row r="55" spans="1:45" s="18" customFormat="1">
+    <row r="55" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="W55" s="6"/>
       <c r="AC55" s="6"/>
       <c r="AI55" s="6"/>
       <c r="AO55" s="6"/>
     </row>
-    <row r="56" spans="1:45" s="18" customFormat="1">
+    <row r="56" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="W56" s="6"/>
       <c r="AC56" s="6"/>
       <c r="AI56" s="6"/>
       <c r="AO56" s="6"/>
     </row>
-    <row r="57" spans="1:45" s="18" customFormat="1">
+    <row r="57" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="W57" s="6"/>
       <c r="AC57" s="6"/>
       <c r="AI57" s="6"/>
       <c r="AO57" s="6"/>
     </row>
-    <row r="58" spans="1:45" s="18" customFormat="1">
+    <row r="58" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>56</v>
       </c>
@@ -12269,7 +12263,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:45" s="18" customFormat="1">
+    <row r="59" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="C59" s="19">
         <v>2000</v>
@@ -12383,7 +12377,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:45" s="18" customFormat="1">
+    <row r="60" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -12431,7 +12425,7 @@
       <c r="AR60" s="25"/>
       <c r="AS60" s="25"/>
     </row>
-    <row r="61" spans="1:45" s="18" customFormat="1">
+    <row r="61" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -12479,7 +12473,7 @@
       <c r="AR61" s="25"/>
       <c r="AS61" s="25"/>
     </row>
-    <row r="62" spans="1:45" s="18" customFormat="1">
+    <row r="62" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -12527,7 +12521,7 @@
       <c r="AR62" s="25"/>
       <c r="AS62" s="25"/>
     </row>
-    <row r="63" spans="1:45" s="18" customFormat="1">
+    <row r="63" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -12575,7 +12569,7 @@
       <c r="AR63" s="25"/>
       <c r="AS63" s="25"/>
     </row>
-    <row r="64" spans="1:45" s="18" customFormat="1">
+    <row r="64" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -12624,7 +12618,7 @@
       <c r="AR64" s="25"/>
       <c r="AS64" s="25"/>
     </row>
-    <row r="65" spans="1:45" s="18" customFormat="1">
+    <row r="65" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -12672,7 +12666,7 @@
       <c r="AR65" s="25"/>
       <c r="AS65" s="25"/>
     </row>
-    <row r="69" spans="1:45" s="18" customFormat="1">
+    <row r="69" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
         <v>57</v>
       </c>
@@ -12706,7 +12700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:45" s="18" customFormat="1">
+    <row r="70" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="C70" s="19">
         <v>2000</v>
@@ -12820,7 +12814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:45" s="18" customFormat="1">
+    <row r="71" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
         <v>10</v>
       </c>
@@ -12868,7 +12862,6 @@
       <c r="AS71" s="25"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -12880,7 +12873,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS85"/>
   <sheetViews>
@@ -12888,20 +12881,20 @@
       <selection activeCell="W64" sqref="W64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="20" max="20" width="14.375" style="31" customWidth="1"/>
-    <col min="23" max="23" width="11.375" customWidth="1"/>
-    <col min="29" max="29" width="11.375" style="18" customWidth="1"/>
-    <col min="30" max="33" width="8.625" style="18"/>
-    <col min="35" max="35" width="11.375" style="18" customWidth="1"/>
-    <col min="36" max="39" width="8.625" style="18"/>
-    <col min="41" max="41" width="11.375" style="18" customWidth="1"/>
-    <col min="42" max="45" width="8.625" style="18"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="20" max="20" width="14.42578125" style="31" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" customWidth="1"/>
+    <col min="29" max="29" width="11.42578125" style="18" customWidth="1"/>
+    <col min="30" max="33" width="8.5703125" style="18"/>
+    <col min="35" max="35" width="11.42578125" style="18" customWidth="1"/>
+    <col min="36" max="39" width="8.5703125" style="18"/>
+    <col min="41" max="41" width="11.42578125" style="18" customWidth="1"/>
+    <col min="42" max="45" width="8.5703125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>26</v>
       </c>
@@ -12949,7 +12942,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="C2" s="12">
         <v>2000</v>
@@ -13066,7 +13059,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -13117,7 +13110,7 @@
       <c r="AR3" s="34"/>
       <c r="AS3" s="34"/>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -13168,7 +13161,7 @@
       <c r="AR4" s="34"/>
       <c r="AS4" s="34"/>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -13219,7 +13212,7 @@
       <c r="AR5" s="34"/>
       <c r="AS5" s="34"/>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -13270,7 +13263,7 @@
       <c r="AR6" s="34"/>
       <c r="AS6" s="34"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -13321,7 +13314,7 @@
       <c r="AR7" s="34"/>
       <c r="AS7" s="34"/>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -13372,15 +13365,15 @@
       <c r="AR8" s="34"/>
       <c r="AS8" s="34"/>
     </row>
-    <row r="10" spans="1:45" s="18" customFormat="1">
+    <row r="10" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="T10" s="31"/>
     </row>
-    <row r="11" spans="1:45" s="18" customFormat="1">
+    <row r="11" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="T11" s="31"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>27</v>
       </c>
@@ -13428,7 +13421,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="C13" s="12">
         <v>2000</v>
@@ -13545,7 +13538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -13596,7 +13589,7 @@
       <c r="AR14" s="30"/>
       <c r="AS14" s="30"/>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -13647,7 +13640,7 @@
       <c r="AR15" s="30"/>
       <c r="AS15" s="30"/>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -13698,7 +13691,7 @@
       <c r="AR16" s="30"/>
       <c r="AS16" s="30"/>
     </row>
-    <row r="17" spans="1:45">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -13749,7 +13742,7 @@
       <c r="AR17" s="30"/>
       <c r="AS17" s="30"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -13800,7 +13793,7 @@
       <c r="AR18" s="30"/>
       <c r="AS18" s="30"/>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -13851,15 +13844,15 @@
       <c r="AR19" s="30"/>
       <c r="AS19" s="30"/>
     </row>
-    <row r="21" spans="1:45" s="18" customFormat="1">
+    <row r="21" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="T21" s="31"/>
     </row>
-    <row r="22" spans="1:45" s="18" customFormat="1">
+    <row r="22" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="T22" s="31"/>
     </row>
-    <row r="23" spans="1:45">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>28</v>
       </c>
@@ -13907,7 +13900,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:45">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="C24" s="12">
         <v>2000</v>
@@ -14024,7 +14017,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:45">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -14075,7 +14068,7 @@
       <c r="AR25" s="30"/>
       <c r="AS25" s="30"/>
     </row>
-    <row r="26" spans="1:45">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -14126,7 +14119,7 @@
       <c r="AR26" s="30"/>
       <c r="AS26" s="30"/>
     </row>
-    <row r="27" spans="1:45">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -14177,7 +14170,7 @@
       <c r="AR27" s="30"/>
       <c r="AS27" s="30"/>
     </row>
-    <row r="28" spans="1:45">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -14228,7 +14221,7 @@
       <c r="AR28" s="30"/>
       <c r="AS28" s="30"/>
     </row>
-    <row r="29" spans="1:45">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -14279,7 +14272,7 @@
       <c r="AR29" s="30"/>
       <c r="AS29" s="30"/>
     </row>
-    <row r="30" spans="1:45">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -14330,15 +14323,15 @@
       <c r="AR30" s="30"/>
       <c r="AS30" s="30"/>
     </row>
-    <row r="32" spans="1:45" s="18" customFormat="1">
+    <row r="32" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="T32" s="31"/>
     </row>
-    <row r="33" spans="1:45" s="18" customFormat="1">
+    <row r="33" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="T33" s="31"/>
     </row>
-    <row r="34" spans="1:45">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>128</v>
       </c>
@@ -14386,7 +14379,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:45">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="C35" s="12">
         <v>2000</v>
@@ -14503,7 +14496,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:45">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -14564,7 +14557,7 @@
       <c r="AR36" s="30"/>
       <c r="AS36" s="30"/>
     </row>
-    <row r="37" spans="1:45">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -14633,7 +14626,7 @@
       <c r="AR37" s="30"/>
       <c r="AS37" s="30"/>
     </row>
-    <row r="38" spans="1:45">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -14694,7 +14687,7 @@
       <c r="AR38" s="30"/>
       <c r="AS38" s="30"/>
     </row>
-    <row r="39" spans="1:45">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -14755,7 +14748,7 @@
       <c r="AR39" s="30"/>
       <c r="AS39" s="30"/>
     </row>
-    <row r="40" spans="1:45">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -14816,7 +14809,7 @@
       <c r="AR40" s="30"/>
       <c r="AS40" s="30"/>
     </row>
-    <row r="41" spans="1:45">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -14877,15 +14870,15 @@
       <c r="AR41" s="30"/>
       <c r="AS41" s="30"/>
     </row>
-    <row r="43" spans="1:45" s="18" customFormat="1">
+    <row r="43" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="T43" s="31"/>
     </row>
-    <row r="44" spans="1:45" s="18" customFormat="1">
+    <row r="44" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="T44" s="31"/>
     </row>
-    <row r="45" spans="1:45">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>127</v>
       </c>
@@ -14933,7 +14926,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:45">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="C46" s="12">
         <v>2000</v>
@@ -15050,7 +15043,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:45">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -15111,7 +15104,7 @@
       <c r="AR47" s="30"/>
       <c r="AS47" s="30"/>
     </row>
-    <row r="48" spans="1:45">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -15180,7 +15173,7 @@
       <c r="AR48" s="30"/>
       <c r="AS48" s="30"/>
     </row>
-    <row r="49" spans="1:45">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -15241,7 +15234,7 @@
       <c r="AR49" s="30"/>
       <c r="AS49" s="30"/>
     </row>
-    <row r="50" spans="1:45">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -15306,7 +15299,7 @@
       <c r="AR50" s="30"/>
       <c r="AS50" s="30"/>
     </row>
-    <row r="51" spans="1:45">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -15371,7 +15364,7 @@
       <c r="AR51" s="30"/>
       <c r="AS51" s="30"/>
     </row>
-    <row r="52" spans="1:45">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -15432,15 +15425,15 @@
       <c r="AR52" s="30"/>
       <c r="AS52" s="30"/>
     </row>
-    <row r="54" spans="1:45" s="18" customFormat="1">
+    <row r="54" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="T54" s="31"/>
     </row>
-    <row r="55" spans="1:45" s="18" customFormat="1">
+    <row r="55" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="T55" s="31"/>
     </row>
-    <row r="56" spans="1:45">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>33</v>
       </c>
@@ -15488,7 +15481,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:45">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="C57" s="12">
         <v>2000</v>
@@ -15605,7 +15598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:45">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -15656,7 +15649,7 @@
       <c r="AR58" s="30"/>
       <c r="AS58" s="30"/>
     </row>
-    <row r="59" spans="1:45">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -15725,7 +15718,7 @@
       <c r="AR59" s="30"/>
       <c r="AS59" s="30"/>
     </row>
-    <row r="60" spans="1:45">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -15776,7 +15769,7 @@
       <c r="AR60" s="30"/>
       <c r="AS60" s="30"/>
     </row>
-    <row r="61" spans="1:45">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -15827,7 +15820,7 @@
       <c r="AR61" s="30"/>
       <c r="AS61" s="30"/>
     </row>
-    <row r="62" spans="1:45">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -15878,7 +15871,7 @@
       <c r="AR62" s="30"/>
       <c r="AS62" s="30"/>
     </row>
-    <row r="63" spans="1:45">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -15947,15 +15940,15 @@
       <c r="AR63" s="30"/>
       <c r="AS63" s="30"/>
     </row>
-    <row r="65" spans="1:45" s="18" customFormat="1">
+    <row r="65" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="T65" s="31"/>
     </row>
-    <row r="66" spans="1:45" s="18" customFormat="1">
+    <row r="66" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="T66" s="31"/>
     </row>
-    <row r="67" spans="1:45">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>102</v>
       </c>
@@ -16003,7 +15996,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:45">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="C68" s="12">
         <v>2000</v>
@@ -16120,7 +16113,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:45">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -16171,7 +16164,7 @@
       <c r="AR69" s="30"/>
       <c r="AS69" s="30"/>
     </row>
-    <row r="70" spans="1:45">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -16222,7 +16215,7 @@
       <c r="AR70" s="30"/>
       <c r="AS70" s="30"/>
     </row>
-    <row r="71" spans="1:45">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -16273,7 +16266,7 @@
       <c r="AR71" s="30"/>
       <c r="AS71" s="30"/>
     </row>
-    <row r="72" spans="1:45">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -16324,7 +16317,7 @@
       <c r="AR72" s="30"/>
       <c r="AS72" s="30"/>
     </row>
-    <row r="73" spans="1:45">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -16375,7 +16368,7 @@
       <c r="AR73" s="30"/>
       <c r="AS73" s="30"/>
     </row>
-    <row r="74" spans="1:45">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -16426,19 +16419,19 @@
       <c r="AR74" s="30"/>
       <c r="AS74" s="30"/>
     </row>
-    <row r="75" spans="1:45" s="18" customFormat="1">
+    <row r="75" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="T75" s="31"/>
     </row>
-    <row r="76" spans="1:45" s="18" customFormat="1">
+    <row r="76" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
       <c r="T76" s="31"/>
     </row>
-    <row r="77" spans="1:45" s="18" customFormat="1">
+    <row r="77" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="T77" s="31"/>
     </row>
-    <row r="78" spans="1:45" s="18" customFormat="1">
+    <row r="78" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>81</v>
       </c>
@@ -16469,7 +16462,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:45" s="18" customFormat="1">
+    <row r="79" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="C79" s="19">
         <v>2000</v>
@@ -16585,7 +16578,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:45" s="18" customFormat="1">
+    <row r="80" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -16635,7 +16628,7 @@
       <c r="AR80" s="30"/>
       <c r="AS80" s="30"/>
     </row>
-    <row r="81" spans="2:45" s="18" customFormat="1">
+    <row r="81" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -16685,7 +16678,7 @@
       <c r="AR81" s="30"/>
       <c r="AS81" s="30"/>
     </row>
-    <row r="82" spans="2:45" s="18" customFormat="1">
+    <row r="82" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -16735,7 +16728,7 @@
       <c r="AR82" s="30"/>
       <c r="AS82" s="30"/>
     </row>
-    <row r="83" spans="2:45" s="18" customFormat="1">
+    <row r="83" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -16785,7 +16778,7 @@
       <c r="AR83" s="30"/>
       <c r="AS83" s="30"/>
     </row>
-    <row r="84" spans="2:45" s="18" customFormat="1">
+    <row r="84" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -16835,7 +16828,7 @@
       <c r="AR84" s="30"/>
       <c r="AS84" s="30"/>
     </row>
-    <row r="85" spans="2:45" s="18" customFormat="1">
+    <row r="85" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -16886,7 +16879,6 @@
       <c r="AS85" s="30"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -16898,31 +16890,31 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.375" style="31" customWidth="1"/>
-    <col min="21" max="21" width="8.625" style="31"/>
-    <col min="22" max="22" width="9.125" style="31" customWidth="1"/>
-    <col min="23" max="23" width="11.75" style="6" customWidth="1"/>
-    <col min="24" max="27" width="8.625" style="31"/>
-    <col min="29" max="29" width="11.75" style="6" customWidth="1"/>
-    <col min="30" max="33" width="8.625" style="31"/>
-    <col min="35" max="35" width="11.75" style="6" customWidth="1"/>
-    <col min="36" max="39" width="8.625" style="31"/>
-    <col min="41" max="41" width="11.75" style="6" customWidth="1"/>
-    <col min="42" max="45" width="8.625" style="31"/>
+    <col min="2" max="2" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" style="31" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" style="31"/>
+    <col min="22" max="22" width="9.140625" style="31" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" style="6" customWidth="1"/>
+    <col min="24" max="27" width="8.5703125" style="31"/>
+    <col min="29" max="29" width="11.7109375" style="6" customWidth="1"/>
+    <col min="30" max="33" width="8.5703125" style="31"/>
+    <col min="35" max="35" width="11.7109375" style="6" customWidth="1"/>
+    <col min="36" max="39" width="8.5703125" style="31"/>
+    <col min="41" max="41" width="11.7109375" style="6" customWidth="1"/>
+    <col min="42" max="45" width="8.5703125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>129</v>
       </c>
@@ -16968,7 +16960,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="C2" s="14">
         <v>2000</v>
@@ -17085,7 +17077,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -17136,7 +17128,7 @@
       <c r="AR3" s="30"/>
       <c r="AS3" s="30"/>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -17187,7 +17179,7 @@
       <c r="AR4" s="30"/>
       <c r="AS4" s="30"/>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -17238,7 +17230,7 @@
       <c r="AR5" s="30"/>
       <c r="AS5" s="30"/>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -17289,7 +17281,7 @@
       <c r="AR6" s="30"/>
       <c r="AS6" s="30"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -17340,7 +17332,7 @@
       <c r="AR7" s="30"/>
       <c r="AS7" s="30"/>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -17391,7 +17383,7 @@
       <c r="AR8" s="30"/>
       <c r="AS8" s="30"/>
     </row>
-    <row r="10" spans="1:45" s="18" customFormat="1">
+    <row r="10" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="T10" s="31"/>
       <c r="U10" s="31"/>
@@ -17417,7 +17409,7 @@
       <c r="AR10" s="31"/>
       <c r="AS10" s="31"/>
     </row>
-    <row r="11" spans="1:45" s="18" customFormat="1">
+    <row r="11" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="T11" s="31"/>
       <c r="U11" s="31"/>
@@ -17443,7 +17435,7 @@
       <c r="AR11" s="31"/>
       <c r="AS11" s="31"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -17489,7 +17481,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="C13" s="14">
         <v>2000</v>
@@ -17604,7 +17596,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="48" t="s">
         <v>35</v>
@@ -17670,7 +17662,7 @@
       <c r="AR14" s="30"/>
       <c r="AS14" s="30"/>
     </row>
-    <row r="16" spans="1:45" s="18" customFormat="1">
+    <row r="16" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="T16" s="31"/>
       <c r="U16" s="31"/>
@@ -17696,7 +17688,7 @@
       <c r="AR16" s="31"/>
       <c r="AS16" s="31"/>
     </row>
-    <row r="17" spans="1:45" s="18" customFormat="1">
+    <row r="17" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="T17" s="31"/>
       <c r="U17" s="31"/>
@@ -17722,7 +17714,7 @@
       <c r="AR17" s="31"/>
       <c r="AS17" s="31"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>79</v>
       </c>
@@ -17768,7 +17760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="C19" s="14">
         <v>2000</v>
@@ -17885,7 +17877,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:45">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="48" t="s">
         <v>41</v>
@@ -17950,7 +17942,6 @@
       <c r="AS20" s="30"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -17962,20 +17953,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.625" customWidth="1"/>
-    <col min="3" max="8" width="13.625" customWidth="1"/>
-    <col min="9" max="15" width="6.625" customWidth="1"/>
+    <col min="1" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="15" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" customHeight="1">
+    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>140</v>
       </c>
@@ -18004,7 +17995,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="37"/>
       <c r="C2" s="4" t="str">
@@ -18050,7 +18041,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -18083,7 +18074,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -18114,7 +18105,7 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -18149,7 +18140,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -18183,7 +18174,7 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -18214,7 +18205,7 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -18249,7 +18240,7 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -18277,9 +18268,9 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:26" s="18" customFormat="1"/>
-    <row r="11" spans="1:26" s="18" customFormat="1"/>
-    <row r="12" spans="1:26">
+    <row r="10" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>138</v>
       </c>
@@ -18309,7 +18300,7 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="37"/>
       <c r="C13" s="4" t="str">
@@ -18355,7 +18346,7 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -18388,7 +18379,7 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -18419,7 +18410,7 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -18454,7 +18445,7 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -18489,7 +18480,7 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -18520,7 +18511,7 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -18537,7 +18528,7 @@
       </c>
       <c r="H19" s="36"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -18547,7 +18538,7 @@
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="1:26" s="18" customFormat="1">
+    <row r="21" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -18575,8 +18566,8 @@
       <c r="Y21" s="16"/>
       <c r="Z21" s="16"/>
     </row>
-    <row r="22" spans="1:26" s="18" customFormat="1"/>
-    <row r="23" spans="1:26">
+    <row r="22" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>139</v>
       </c>
@@ -18588,7 +18579,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="37"/>
       <c r="C24" s="4" t="str">
@@ -18616,7 +18607,7 @@
         <v>Clients</v>
       </c>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -18629,7 +18620,7 @@
       <c r="G25" s="36"/>
       <c r="H25" s="36"/>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -18642,7 +18633,7 @@
       <c r="G26" s="36"/>
       <c r="H26" s="36"/>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -18655,7 +18646,7 @@
       <c r="G27" s="36"/>
       <c r="H27" s="36"/>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -18668,7 +18659,7 @@
       <c r="G28" s="36"/>
       <c r="H28" s="36"/>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -18681,7 +18672,7 @@
       <c r="G29" s="36"/>
       <c r="H29" s="36"/>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -18696,7 +18687,7 @@
       <c r="G30" s="36"/>
       <c r="H30" s="36"/>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -18706,7 +18697,7 @@
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
     </row>
-    <row r="32" spans="1:26" s="18" customFormat="1">
+    <row r="32" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -18734,8 +18725,8 @@
       <c r="Y32" s="16"/>
       <c r="Z32" s="16"/>
     </row>
-    <row r="33" spans="1:8" s="18" customFormat="1"/>
-    <row r="34" spans="1:8">
+    <row r="33" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>141</v>
       </c>
@@ -18747,7 +18738,7 @@
       <c r="G34" s="16"/>
       <c r="H34" s="16"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="37"/>
       <c r="C35" s="4" t="str">
@@ -18775,7 +18766,7 @@
         <v>Clients</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -18788,7 +18779,7 @@
       <c r="G36" s="36"/>
       <c r="H36" s="36"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -18801,7 +18792,7 @@
       <c r="G37" s="36"/>
       <c r="H37" s="36"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -18816,7 +18807,7 @@
       <c r="G38" s="36"/>
       <c r="H38" s="36"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -18829,7 +18820,7 @@
       <c r="G39" s="36"/>
       <c r="H39" s="36"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -18842,7 +18833,7 @@
       <c r="G40" s="36"/>
       <c r="H40" s="36"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -18856,7 +18847,6 @@
       <c r="H41" s="36"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
improve(spreadsheet): updated example data provided by cliff
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="40" windowWidth="19420" windowHeight="10960" tabRatio="863" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Disutilities &amp; costs" sheetId="14" r:id="rId12"/>
     <sheet name="Macroeconomics" sheetId="18" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="130000"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -496,12 +496,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -2451,7 +2451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K20"/>
   <sheetViews>
@@ -2459,25 +2459,25 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="20"/>
+    <col min="1" max="1" width="9.140625" style="20"/>
     <col min="2" max="2" width="5" style="20" customWidth="1"/>
     <col min="3" max="3" width="18" style="20" customWidth="1"/>
-    <col min="4" max="4" width="55.375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="10.125" style="20" customWidth="1"/>
-    <col min="6" max="7" width="9.125" style="20"/>
-    <col min="8" max="9" width="14.25" style="20" customWidth="1"/>
-    <col min="10" max="10" width="12.125" style="20" customWidth="1"/>
-    <col min="11" max="16384" width="9.125" style="20"/>
+    <col min="4" max="4" width="55.42578125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="20" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="20"/>
+    <col min="8" max="9" width="14.28515625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="20" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" s="21" t="s">
         <v>12</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="21">
         <v>1</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="21">
         <v>2</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="21">
         <v>3</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="21">
         <v>4</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="21">
         <v>5</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="21">
         <v>6</v>
       </c>
@@ -2698,22 +2698,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="21"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="21"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="21"/>
       <c r="C13" s="21" t="s">
         <v>12</v>
@@ -2725,7 +2725,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="21">
         <v>1</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="21">
         <v>2</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="21">
         <v>3</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="21">
         <v>4</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="21">
         <v>5</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="21">
         <v>6</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="21">
         <v>7</v>
       </c>
@@ -2835,7 +2835,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z19"/>
   <sheetViews>
@@ -2843,13 +2843,13 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="3" max="8" width="17.625" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="3" max="8" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
@@ -2861,7 +2861,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:26" s="6" customFormat="1">
+    <row r="2" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="4" t="str">
@@ -2889,7 +2889,7 @@
         <v>Clients</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -2901,7 +2901,7 @@
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -2913,7 +2913,7 @@
       <c r="G4" s="24"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -2925,7 +2925,7 @@
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -2937,7 +2937,7 @@
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -2949,7 +2949,7 @@
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -2961,7 +2961,7 @@
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
     </row>
-    <row r="9" spans="1:26" s="18" customFormat="1">
+    <row r="9" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="37"/>
       <c r="C9" s="16"/>
@@ -2989,10 +2989,10 @@
       <c r="Y9" s="16"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" s="18" customFormat="1">
+    <row r="10" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="37"/>
       <c r="C11" s="2"/>
@@ -3002,7 +3002,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>103</v>
       </c>
@@ -3014,7 +3014,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:26" s="6" customFormat="1">
+    <row r="13" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="37"/>
       <c r="C13" s="4" t="str">
@@ -3042,7 +3042,7 @@
         <v>Clients</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -3054,7 +3054,7 @@
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -3066,7 +3066,7 @@
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -3078,7 +3078,7 @@
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -3090,7 +3090,7 @@
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -3102,7 +3102,7 @@
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -3115,7 +3115,6 @@
       <c r="H19" s="24"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3127,7 +3126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H69"/>
   <sheetViews>
@@ -3135,19 +3134,19 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="18"/>
-    <col min="2" max="2" width="33.25" style="18" customWidth="1"/>
-    <col min="3" max="16384" width="9.125" style="18"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="33.28515625" style="18" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="6" customFormat="1">
+    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
@@ -3158,7 +3157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>91</v>
       </c>
@@ -3168,7 +3167,7 @@
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
         <v>92</v>
       </c>
@@ -3178,7 +3177,7 @@
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
         <v>93</v>
       </c>
@@ -3188,7 +3187,7 @@
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
         <v>94</v>
       </c>
@@ -3198,7 +3197,7 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
         <v>90</v>
       </c>
@@ -3208,7 +3207,7 @@
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
         <v>131</v>
       </c>
@@ -3218,7 +3217,7 @@
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>132</v>
       </c>
@@ -3228,7 +3227,7 @@
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -3238,12 +3237,12 @@
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="6" customFormat="1">
+    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="4" t="s">
         <v>0</v>
       </c>
@@ -3254,7 +3253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
         <v>3</v>
       </c>
@@ -3264,7 +3263,7 @@
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="19" t="s">
         <v>113</v>
       </c>
@@ -3274,7 +3273,7 @@
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
         <v>104</v>
       </c>
@@ -3284,7 +3283,7 @@
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
         <v>105</v>
       </c>
@@ -3294,7 +3293,7 @@
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
         <v>115</v>
       </c>
@@ -3304,7 +3303,7 @@
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -3314,13 +3313,13 @@
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>130</v>
       </c>
       <c r="B23" s="19"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>0</v>
       </c>
@@ -3331,7 +3330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
         <v>106</v>
       </c>
@@ -3341,7 +3340,7 @@
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
         <v>104</v>
       </c>
@@ -3351,7 +3350,7 @@
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
         <v>107</v>
       </c>
@@ -3361,7 +3360,7 @@
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="19" t="s">
         <v>116</v>
       </c>
@@ -3371,7 +3370,7 @@
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -3381,12 +3380,12 @@
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" s="4" t="s">
         <v>0</v>
       </c>
@@ -3397,7 +3396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="19" t="s">
         <v>108</v>
       </c>
@@ -3407,7 +3406,7 @@
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" s="19" t="s">
         <v>109</v>
       </c>
@@ -3417,7 +3416,7 @@
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="19" t="s">
         <v>110</v>
       </c>
@@ -3427,10 +3426,10 @@
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="19"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -3440,12 +3439,12 @@
       <c r="G39" s="16"/>
       <c r="H39" s="16"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="4" t="s">
         <v>0</v>
       </c>
@@ -3456,7 +3455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" s="19" t="s">
         <v>111</v>
       </c>
@@ -3470,7 +3469,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="19" t="s">
         <v>112</v>
       </c>
@@ -3484,7 +3483,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -3494,12 +3493,12 @@
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C48" s="4" t="s">
         <v>0</v>
       </c>
@@ -3510,7 +3509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
         <v>3</v>
       </c>
@@ -3520,7 +3519,7 @@
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B50" s="19" t="s">
         <v>113</v>
       </c>
@@ -3530,7 +3529,7 @@
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>114</v>
       </c>
@@ -3540,7 +3539,7 @@
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="19" t="s">
         <v>105</v>
       </c>
@@ -3550,7 +3549,7 @@
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>115</v>
       </c>
@@ -3560,7 +3559,7 @@
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" s="19" t="s">
         <v>4</v>
       </c>
@@ -3570,7 +3569,7 @@
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
         <v>15</v>
       </c>
@@ -3580,7 +3579,7 @@
       <c r="D55" s="22"/>
       <c r="E55" s="22"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="16"/>
       <c r="B58" s="16"/>
       <c r="C58" s="16"/>
@@ -3590,12 +3589,12 @@
       <c r="G58" s="16"/>
       <c r="H58" s="16"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C60" s="4" t="s">
         <v>0</v>
       </c>
@@ -3606,7 +3605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" s="19" t="s">
         <v>58</v>
       </c>
@@ -3616,7 +3615,7 @@
       <c r="D61" s="22"/>
       <c r="E61" s="22"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" s="19" t="s">
         <v>5</v>
       </c>
@@ -3626,7 +3625,7 @@
       <c r="D62" s="22"/>
       <c r="E62" s="22"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B63" s="19" t="s">
         <v>16</v>
       </c>
@@ -3636,7 +3635,7 @@
       <c r="D63" s="22"/>
       <c r="E63" s="22"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" s="19" t="s">
         <v>6</v>
       </c>
@@ -3646,7 +3645,7 @@
       <c r="D64" s="22"/>
       <c r="E64" s="22"/>
     </row>
-    <row r="65" spans="2:5">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="19" t="s">
         <v>95</v>
       </c>
@@ -3656,7 +3655,7 @@
       <c r="D65" s="22"/>
       <c r="E65" s="22"/>
     </row>
-    <row r="66" spans="2:5">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="19" t="s">
         <v>7</v>
       </c>
@@ -3666,7 +3665,7 @@
       <c r="D66" s="22"/>
       <c r="E66" s="22"/>
     </row>
-    <row r="67" spans="2:5">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="19" t="s">
         <v>96</v>
       </c>
@@ -3676,7 +3675,7 @@
       <c r="D67" s="22"/>
       <c r="E67" s="22"/>
     </row>
-    <row r="68" spans="2:5">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="19" t="s">
         <v>84</v>
       </c>
@@ -3686,7 +3685,7 @@
       <c r="D68" s="22"/>
       <c r="E68" s="22"/>
     </row>
-    <row r="69" spans="2:5">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="19" t="s">
         <v>85</v>
       </c>
@@ -3697,7 +3696,6 @@
       <c r="E69" s="22"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3709,20 +3707,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W41" sqref="W41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>137</v>
       </c>
@@ -3731,7 +3729,7 @@
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="4" t="s">
@@ -3744,7 +3742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="18" customFormat="1">
+    <row r="3" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>136</v>
       </c>
@@ -3754,7 +3752,7 @@
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
         <v>117</v>
@@ -3765,7 +3763,7 @@
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="19" t="s">
         <v>118</v>
@@ -3776,7 +3774,7 @@
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="19" t="s">
         <v>119</v>
@@ -3787,7 +3785,7 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="19" t="s">
         <v>120</v>
@@ -3798,7 +3796,7 @@
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="s">
         <v>19</v>
@@ -3809,15 +3807,15 @@
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
     </row>
-    <row r="10" spans="1:8" s="18" customFormat="1"/>
-    <row r="11" spans="1:8" s="18" customFormat="1">
+    <row r="10" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -3827,7 +3825,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>135</v>
       </c>
@@ -3836,7 +3834,7 @@
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="4" t="s">
@@ -3849,7 +3847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
         <v>3</v>
@@ -3860,7 +3858,7 @@
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="19" t="s">
         <v>113</v>
@@ -3871,7 +3869,7 @@
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
         <v>114</v>
@@ -3882,7 +3880,7 @@
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="19" t="s">
         <v>105</v>
@@ -3893,7 +3891,7 @@
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="19" t="s">
         <v>115</v>
@@ -3904,7 +3902,7 @@
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>134</v>
       </c>
@@ -3913,7 +3911,7 @@
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="4" t="s">
@@ -3926,7 +3924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="19" t="s">
         <v>3</v>
@@ -3937,52 +3935,51 @@
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="19" t="s">
         <v>113</v>
       </c>
       <c r="C25" s="22">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="19" t="s">
         <v>114</v>
       </c>
       <c r="C26" s="22">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="19" t="s">
         <v>105</v>
       </c>
       <c r="C27" s="22">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="19" t="s">
         <v>115</v>
       </c>
       <c r="C28" s="22">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3994,21 +3991,21 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T57"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="3" max="4" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="3" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>29</v>
       </c>
@@ -4030,7 +4027,7 @@
       <c r="R1" s="18"/>
       <c r="S1" s="18"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="C2" s="19">
         <v>2015</v>
@@ -4085,7 +4082,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -4158,7 +4155,7 @@
       </c>
       <c r="T3" s="29"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>30</v>
       </c>
@@ -4180,7 +4177,7 @@
       <c r="R7" s="18"/>
       <c r="S7" s="18"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="C8" s="19">
         <v>2015</v>
@@ -4235,7 +4232,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="4" t="s">
         <v>10</v>
@@ -4308,7 +4305,7 @@
       </c>
       <c r="T9" s="29"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>44</v>
       </c>
@@ -4330,7 +4327,7 @@
       <c r="R13" s="18"/>
       <c r="S13" s="18"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="C14" s="19">
         <v>2015</v>
@@ -4385,7 +4382,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
         <v>10</v>
@@ -4458,14 +4455,14 @@
       </c>
       <c r="T15" s="29"/>
     </row>
-    <row r="19" spans="1:20" s="18" customFormat="1">
+    <row r="19" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>51</v>
       </c>
       <c r="B19" s="6"/>
       <c r="T19" s="6"/>
     </row>
-    <row r="20" spans="1:20" s="18" customFormat="1">
+    <row r="20" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="19">
         <v>2015</v>
@@ -4519,7 +4516,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="18" customFormat="1">
+    <row r="21" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
@@ -4544,26 +4541,26 @@
       </c>
       <c r="T21" s="29"/>
     </row>
-    <row r="22" spans="1:20" s="18" customFormat="1">
+    <row r="22" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="T22" s="6"/>
     </row>
-    <row r="23" spans="1:20" s="18" customFormat="1">
+    <row r="23" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="T23" s="6"/>
     </row>
-    <row r="24" spans="1:20" s="18" customFormat="1">
+    <row r="24" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="T24" s="6"/>
     </row>
-    <row r="25" spans="1:20" s="18" customFormat="1">
+    <row r="25" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>45</v>
       </c>
       <c r="B25" s="6"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="1:20" s="18" customFormat="1">
+    <row r="26" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="C26" s="19">
         <v>2015</v>
@@ -4617,7 +4614,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="18" customFormat="1">
+    <row r="27" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>10</v>
       </c>
@@ -4690,14 +4687,14 @@
       </c>
       <c r="T27" s="29"/>
     </row>
-    <row r="31" spans="1:20" s="18" customFormat="1">
+    <row r="31" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>46</v>
       </c>
       <c r="B31" s="6"/>
       <c r="T31" s="6"/>
     </row>
-    <row r="32" spans="1:20" s="18" customFormat="1">
+    <row r="32" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="C32" s="19">
         <v>2015</v>
@@ -4751,7 +4748,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="18" customFormat="1">
+    <row r="33" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>10</v>
       </c>
@@ -4808,26 +4805,26 @@
       </c>
       <c r="T33" s="29"/>
     </row>
-    <row r="34" spans="1:20" s="18" customFormat="1">
+    <row r="34" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="T34" s="6"/>
     </row>
-    <row r="35" spans="1:20" s="18" customFormat="1">
+    <row r="35" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="T35" s="6"/>
     </row>
-    <row r="36" spans="1:20" s="18" customFormat="1">
+    <row r="36" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="T36" s="6"/>
     </row>
-    <row r="37" spans="1:20" s="18" customFormat="1">
+    <row r="37" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>47</v>
       </c>
       <c r="B37" s="6"/>
       <c r="T37" s="6"/>
     </row>
-    <row r="38" spans="1:20" s="18" customFormat="1">
+    <row r="38" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="19">
         <v>2015</v>
@@ -4881,7 +4878,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="18" customFormat="1">
+    <row r="39" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>10</v>
       </c>
@@ -4906,26 +4903,26 @@
       </c>
       <c r="T39" s="29"/>
     </row>
-    <row r="40" spans="1:20" s="18" customFormat="1">
+    <row r="40" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="T40" s="6"/>
     </row>
-    <row r="41" spans="1:20" s="18" customFormat="1">
+    <row r="41" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="T41" s="6"/>
     </row>
-    <row r="42" spans="1:20" s="18" customFormat="1">
+    <row r="42" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="T42" s="6"/>
     </row>
-    <row r="43" spans="1:20" s="18" customFormat="1">
+    <row r="43" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="6"/>
       <c r="T43" s="6"/>
     </row>
-    <row r="44" spans="1:20" s="18" customFormat="1">
+    <row r="44" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="C44" s="19">
         <v>2015</v>
@@ -4979,7 +4976,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:20" s="18" customFormat="1">
+    <row r="45" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>10</v>
       </c>
@@ -5004,14 +5001,14 @@
       </c>
       <c r="T45" s="29"/>
     </row>
-    <row r="49" spans="1:20" s="18" customFormat="1">
+    <row r="49" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B49" s="6"/>
       <c r="T49" s="6"/>
     </row>
-    <row r="50" spans="1:20" s="18" customFormat="1">
+    <row r="50" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="C50" s="19">
         <v>2015</v>
@@ -5065,7 +5062,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:20" s="18" customFormat="1">
+    <row r="51" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>10</v>
       </c>
@@ -5090,26 +5087,26 @@
       </c>
       <c r="T51" s="29"/>
     </row>
-    <row r="52" spans="1:20" s="18" customFormat="1">
+    <row r="52" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="T52" s="6"/>
     </row>
-    <row r="53" spans="1:20" s="18" customFormat="1">
+    <row r="53" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="T53" s="6"/>
     </row>
-    <row r="54" spans="1:20" s="18" customFormat="1">
+    <row r="54" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="T54" s="6"/>
     </row>
-    <row r="55" spans="1:20" s="18" customFormat="1">
+    <row r="55" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
         <v>50</v>
       </c>
       <c r="B55" s="6"/>
       <c r="T55" s="6"/>
     </row>
-    <row r="56" spans="1:20" s="18" customFormat="1">
+    <row r="56" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="C56" s="19">
         <v>2015</v>
@@ -5163,7 +5160,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:20" s="18" customFormat="1">
+    <row r="57" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
         <v>10</v>
       </c>
@@ -5189,7 +5186,6 @@
       <c r="T57" s="29"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -5201,7 +5197,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:V22"/>
   <sheetViews>
@@ -5209,21 +5205,21 @@
       <selection activeCell="M12" sqref="M12:M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.125" style="18"/>
+    <col min="1" max="2" width="9.140625" style="18"/>
     <col min="3" max="3" width="11" style="18" customWidth="1"/>
-    <col min="4" max="20" width="9.125" style="18"/>
-    <col min="21" max="21" width="15.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.125" style="18"/>
+    <col min="4" max="20" width="9.140625" style="18"/>
+    <col min="21" max="21" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D2" s="19">
         <v>2000</v>
       </c>
@@ -5276,7 +5272,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$14</f>
         <v>SBCC</v>
@@ -5319,7 +5315,7 @@
       </c>
       <c r="U3" s="25"/>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$14</f>
         <v>SBCC</v>
@@ -5369,10 +5365,10 @@
       </c>
       <c r="U4" s="39"/>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$15</f>
         <v>NSP</v>
@@ -5403,7 +5399,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$15</f>
         <v>NSP</v>
@@ -5434,10 +5430,10 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="str">
         <f>'Populations &amp; programs'!$C$16</f>
         <v>OST</v>
@@ -5468,7 +5464,7 @@
       </c>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="4" t="str">
         <f>'Populations &amp; programs'!$C$16</f>
@@ -5500,11 +5496,11 @@
       </c>
       <c r="U10" s="39"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="4" t="str">
         <f>'Populations &amp; programs'!$C$17</f>
@@ -5537,7 +5533,7 @@
       <c r="U12" s="25"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="str">
         <f>'Populations &amp; programs'!$C$17</f>
         <v>MSM programs</v>
@@ -5568,7 +5564,7 @@
       </c>
       <c r="U13" s="39"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$C$18</f>
         <v>FSW programs</v>
@@ -5599,7 +5595,7 @@
       </c>
       <c r="U15" s="25"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$C$18</f>
         <v>FSW programs</v>
@@ -5630,7 +5626,7 @@
       </c>
       <c r="U16" s="39"/>
     </row>
-    <row r="18" spans="2:21">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$C$19</f>
         <v>ART</v>
@@ -5661,7 +5657,7 @@
       </c>
       <c r="U18" s="25"/>
     </row>
-    <row r="19" spans="2:21">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$C$19</f>
         <v>ART</v>
@@ -5692,7 +5688,7 @@
       </c>
       <c r="U19" s="39"/>
     </row>
-    <row r="21" spans="2:21">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="str">
         <f>'Populations &amp; programs'!$C$20</f>
         <v>PMTCT</v>
@@ -5723,7 +5719,7 @@
       </c>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="2:21">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="str">
         <f>'Populations &amp; programs'!$C$20</f>
         <v>PMTCT</v>
@@ -5766,7 +5762,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U53"/>
   <sheetViews>
@@ -5774,22 +5770,22 @@
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.125" style="18"/>
-    <col min="4" max="4" width="9.375" style="18" customWidth="1"/>
-    <col min="5" max="20" width="9.125" style="18"/>
-    <col min="21" max="21" width="15.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.875" style="18" customWidth="1"/>
-    <col min="23" max="16384" width="9.125" style="18"/>
+    <col min="1" max="3" width="9.140625" style="18"/>
+    <col min="4" max="4" width="9.42578125" style="18" customWidth="1"/>
+    <col min="5" max="20" width="9.140625" style="18"/>
+    <col min="21" max="21" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" style="18" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D2" s="19">
         <v>2000</v>
       </c>
@@ -5842,7 +5838,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -5873,7 +5869,7 @@
         <v>37500</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -5904,7 +5900,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -5935,12 +5931,12 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="U6" s="28"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -5969,7 +5965,7 @@
       </c>
       <c r="U7" s="27"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -6000,7 +5996,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -6029,7 +6025,7 @@
       </c>
       <c r="U9" s="27"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="28"/>
@@ -6050,7 +6046,7 @@
       <c r="S10" s="28"/>
       <c r="U10" s="28"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -6089,7 +6085,7 @@
       </c>
       <c r="U11" s="27"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -6128,7 +6124,7 @@
       </c>
       <c r="U12" s="27"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -6167,7 +6163,7 @@
       </c>
       <c r="U13" s="27"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="28"/>
@@ -6188,7 +6184,7 @@
       <c r="S14" s="28"/>
       <c r="U14" s="28"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -6217,7 +6213,7 @@
       </c>
       <c r="U15" s="27"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -6278,7 +6274,7 @@
       </c>
       <c r="U16" s="27"/>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -6307,7 +6303,7 @@
       </c>
       <c r="U17" s="27"/>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="28"/>
@@ -6328,7 +6324,7 @@
       <c r="S18" s="28"/>
       <c r="U18" s="28"/>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -6357,7 +6353,7 @@
       </c>
       <c r="U19" s="27"/>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -6418,7 +6414,7 @@
       </c>
       <c r="U20" s="27"/>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -6447,7 +6443,7 @@
       </c>
       <c r="U21" s="27"/>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="28"/>
@@ -6468,7 +6464,7 @@
       <c r="S22" s="28"/>
       <c r="U22" s="28"/>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -6497,7 +6493,7 @@
       </c>
       <c r="U23" s="27"/>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -6558,7 +6554,7 @@
       </c>
       <c r="U24" s="27"/>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -6587,12 +6583,12 @@
       </c>
       <c r="U25" s="27"/>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D30" s="19">
         <v>2000</v>
       </c>
@@ -6645,7 +6641,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -6676,7 +6672,7 @@
       </c>
       <c r="U31" s="26"/>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -6707,7 +6703,7 @@
       </c>
       <c r="U32" s="26"/>
     </row>
-    <row r="33" spans="2:21">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -6738,11 +6734,11 @@
       </c>
       <c r="U33" s="26"/>
     </row>
-    <row r="34" spans="2:21">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
     </row>
-    <row r="35" spans="2:21">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -6777,7 +6773,7 @@
       </c>
       <c r="U35" s="26"/>
     </row>
-    <row r="36" spans="2:21">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -6812,7 +6808,7 @@
       </c>
       <c r="U36" s="26"/>
     </row>
-    <row r="37" spans="2:21">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -6847,11 +6843,11 @@
       </c>
       <c r="U37" s="26"/>
     </row>
-    <row r="38" spans="2:21">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
     </row>
-    <row r="39" spans="2:21">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -6886,7 +6882,7 @@
       </c>
       <c r="U39" s="26"/>
     </row>
-    <row r="40" spans="2:21">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -6921,7 +6917,7 @@
       </c>
       <c r="U40" s="26"/>
     </row>
-    <row r="41" spans="2:21">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -6956,11 +6952,11 @@
       </c>
       <c r="U41" s="26"/>
     </row>
-    <row r="42" spans="2:21">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
     </row>
-    <row r="43" spans="2:21">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -6989,7 +6985,7 @@
       </c>
       <c r="U43" s="26"/>
     </row>
-    <row r="44" spans="2:21">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -7020,7 +7016,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="45" spans="2:21">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -7049,11 +7045,11 @@
       </c>
       <c r="U45" s="26"/>
     </row>
-    <row r="46" spans="2:21">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
     </row>
-    <row r="47" spans="2:21">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -7082,7 +7078,7 @@
       </c>
       <c r="U47" s="26"/>
     </row>
-    <row r="48" spans="2:21">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -7119,7 +7115,7 @@
       </c>
       <c r="U48" s="26"/>
     </row>
-    <row r="49" spans="2:21">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -7148,11 +7144,11 @@
       </c>
       <c r="U49" s="26"/>
     </row>
-    <row r="50" spans="2:21">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
     </row>
-    <row r="51" spans="2:21">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -7181,7 +7177,7 @@
       </c>
       <c r="U51" s="26"/>
     </row>
-    <row r="52" spans="2:21">
+    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -7212,7 +7208,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="53" spans="2:21">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -7253,7 +7249,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T33"/>
   <sheetViews>
@@ -7261,13 +7257,13 @@
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="20" max="20" width="14.25" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>98</v>
       </c>
@@ -7290,7 +7286,7 @@
       <c r="S1" s="9"/>
       <c r="T1" s="9"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="C2" s="10">
         <v>2000</v>
@@ -7345,7 +7341,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -7371,13 +7367,13 @@
       </c>
       <c r="T3" s="22"/>
     </row>
-    <row r="5" spans="1:20" s="18" customFormat="1">
+    <row r="5" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:20" s="18" customFormat="1">
+    <row r="6" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>99</v>
       </c>
@@ -7400,7 +7396,7 @@
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="C8" s="10">
         <v>2000</v>
@@ -7455,7 +7451,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
         <v>10</v>
@@ -7505,13 +7501,13 @@
       </c>
       <c r="T9" s="22"/>
     </row>
-    <row r="11" spans="1:20" s="18" customFormat="1">
+    <row r="11" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:20" s="18" customFormat="1">
+    <row r="12" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>100</v>
       </c>
@@ -7534,7 +7530,7 @@
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="C14" s="10">
         <v>2000</v>
@@ -7589,7 +7585,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="4" t="s">
         <v>10</v>
@@ -7615,19 +7611,19 @@
       </c>
       <c r="T15" s="22"/>
     </row>
-    <row r="17" spans="1:20" s="18" customFormat="1">
+    <row r="17" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:20" s="18" customFormat="1">
+    <row r="18" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:20" s="18" customFormat="1">
+    <row r="19" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>147</v>
       </c>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:20" s="18" customFormat="1">
+    <row r="20" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="19">
         <v>2000</v>
@@ -7681,7 +7677,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="18" customFormat="1">
+    <row r="21" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
@@ -7706,16 +7702,16 @@
       </c>
       <c r="T21" s="22"/>
     </row>
-    <row r="22" spans="1:20" s="18" customFormat="1">
+    <row r="22" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:20" s="18" customFormat="1">
+    <row r="23" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:20" s="18" customFormat="1">
+    <row r="24" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>54</v>
       </c>
@@ -7738,7 +7734,7 @@
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="C26" s="10">
         <v>2000</v>
@@ -7793,7 +7789,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="4" t="s">
         <v>10</v>
@@ -7819,13 +7815,13 @@
       </c>
       <c r="T27" s="22"/>
     </row>
-    <row r="31" spans="1:20" s="18" customFormat="1">
+    <row r="31" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="1:20" s="18" customFormat="1">
+    <row r="32" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="C32" s="19">
         <v>2000</v>
@@ -7879,7 +7875,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="2:20" s="18" customFormat="1">
+    <row r="33" spans="2:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>10</v>
       </c>
@@ -7905,7 +7901,6 @@
       <c r="T33" s="22"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -7917,30 +7912,30 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS42"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="21" max="21" width="9.125" customWidth="1"/>
-    <col min="22" max="22" width="8.875" customWidth="1"/>
-    <col min="23" max="23" width="10.375" style="6" customWidth="1"/>
-    <col min="28" max="28" width="8.875" style="18" customWidth="1"/>
-    <col min="29" max="29" width="10.375" style="6" customWidth="1"/>
-    <col min="30" max="33" width="8.625" style="18"/>
-    <col min="34" max="34" width="8.875" style="18" customWidth="1"/>
-    <col min="35" max="35" width="10.375" style="6" customWidth="1"/>
-    <col min="36" max="39" width="8.625" style="18"/>
-    <col min="40" max="40" width="8.875" style="18" customWidth="1"/>
-    <col min="41" max="41" width="10.375" style="6" customWidth="1"/>
-    <col min="42" max="45" width="8.625" style="18"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="21" max="21" width="9.140625" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" style="6" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" style="18" customWidth="1"/>
+    <col min="29" max="29" width="10.42578125" style="6" customWidth="1"/>
+    <col min="30" max="33" width="8.5703125" style="18"/>
+    <col min="34" max="34" width="8.85546875" style="18" customWidth="1"/>
+    <col min="35" max="35" width="10.42578125" style="6" customWidth="1"/>
+    <col min="36" max="39" width="8.5703125" style="18"/>
+    <col min="40" max="40" width="8.85546875" style="18" customWidth="1"/>
+    <col min="41" max="41" width="10.42578125" style="6" customWidth="1"/>
+    <col min="42" max="45" width="8.5703125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="18" customFormat="1">
+    <row r="1" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>97</v>
       </c>
@@ -7974,7 +7969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="18" customFormat="1">
+    <row r="2" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="19">
         <v>2000</v>
@@ -8088,7 +8083,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:45" s="18" customFormat="1">
+    <row r="3" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -8136,7 +8131,7 @@
       <c r="AR3" s="25"/>
       <c r="AS3" s="25"/>
     </row>
-    <row r="4" spans="1:45" s="18" customFormat="1">
+    <row r="4" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -8184,7 +8179,7 @@
       <c r="AR4" s="25"/>
       <c r="AS4" s="25"/>
     </row>
-    <row r="5" spans="1:45" s="18" customFormat="1">
+    <row r="5" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -8232,7 +8227,7 @@
       <c r="AR5" s="25"/>
       <c r="AS5" s="25"/>
     </row>
-    <row r="6" spans="1:45" s="18" customFormat="1">
+    <row r="6" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -8280,7 +8275,7 @@
       <c r="AR6" s="25"/>
       <c r="AS6" s="25"/>
     </row>
-    <row r="7" spans="1:45" s="18" customFormat="1">
+    <row r="7" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -8328,7 +8323,7 @@
       <c r="AR7" s="25"/>
       <c r="AS7" s="25"/>
     </row>
-    <row r="8" spans="1:45" s="18" customFormat="1">
+    <row r="8" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -8376,28 +8371,28 @@
       <c r="AR8" s="25"/>
       <c r="AS8" s="25"/>
     </row>
-    <row r="9" spans="1:45" s="18" customFormat="1">
+    <row r="9" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="W9" s="6"/>
       <c r="AC9" s="6"/>
       <c r="AI9" s="6"/>
       <c r="AO9" s="6"/>
     </row>
-    <row r="10" spans="1:45" s="18" customFormat="1">
+    <row r="10" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="W10" s="6"/>
       <c r="AC10" s="6"/>
       <c r="AI10" s="6"/>
       <c r="AO10" s="6"/>
     </row>
-    <row r="11" spans="1:45" s="18" customFormat="1">
+    <row r="11" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="W11" s="6"/>
       <c r="AC11" s="6"/>
       <c r="AI11" s="6"/>
       <c r="AO11" s="6"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>31</v>
       </c>
@@ -8445,7 +8440,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="C13" s="8">
         <v>2000</v>
@@ -8560,7 +8555,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -8609,7 +8604,7 @@
       <c r="AR14" s="25"/>
       <c r="AS14" s="25"/>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -8658,7 +8653,7 @@
       <c r="AR15" s="25"/>
       <c r="AS15" s="25"/>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -8707,7 +8702,7 @@
       <c r="AR16" s="25"/>
       <c r="AS16" s="25"/>
     </row>
-    <row r="17" spans="1:45">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -8756,7 +8751,7 @@
       <c r="AR17" s="25"/>
       <c r="AS17" s="25"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -8805,7 +8800,7 @@
       <c r="AR18" s="25"/>
       <c r="AS18" s="25"/>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -8854,28 +8849,28 @@
       <c r="AR19" s="25"/>
       <c r="AS19" s="25"/>
     </row>
-    <row r="20" spans="1:45" s="18" customFormat="1">
+    <row r="20" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="W20" s="6"/>
       <c r="AC20" s="6"/>
       <c r="AI20" s="6"/>
       <c r="AO20" s="6"/>
     </row>
-    <row r="21" spans="1:45" s="18" customFormat="1">
+    <row r="21" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="W21" s="6"/>
       <c r="AC21" s="6"/>
       <c r="AI21" s="6"/>
       <c r="AO21" s="6"/>
     </row>
-    <row r="22" spans="1:45" s="18" customFormat="1">
+    <row r="22" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="W22" s="6"/>
       <c r="AC22" s="6"/>
       <c r="AI22" s="6"/>
       <c r="AO22" s="6"/>
     </row>
-    <row r="23" spans="1:45" s="18" customFormat="1">
+    <row r="23" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>42</v>
       </c>
@@ -8909,7 +8904,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:45" s="18" customFormat="1">
+    <row r="24" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="19">
         <v>2000</v>
@@ -9023,7 +9018,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:45" s="18" customFormat="1">
+    <row r="25" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -9071,7 +9066,7 @@
       <c r="AR25" s="25"/>
       <c r="AS25" s="25"/>
     </row>
-    <row r="26" spans="1:45" s="18" customFormat="1">
+    <row r="26" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -9119,7 +9114,7 @@
       <c r="AR26" s="25"/>
       <c r="AS26" s="25"/>
     </row>
-    <row r="27" spans="1:45" s="18" customFormat="1">
+    <row r="27" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -9167,7 +9162,7 @@
       <c r="AR27" s="25"/>
       <c r="AS27" s="25"/>
     </row>
-    <row r="28" spans="1:45" s="18" customFormat="1">
+    <row r="28" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -9215,7 +9210,7 @@
       <c r="AR28" s="25"/>
       <c r="AS28" s="25"/>
     </row>
-    <row r="29" spans="1:45" s="18" customFormat="1">
+    <row r="29" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -9263,7 +9258,7 @@
       <c r="AR29" s="25"/>
       <c r="AS29" s="25"/>
     </row>
-    <row r="30" spans="1:45" s="18" customFormat="1">
+    <row r="30" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -9311,10 +9306,10 @@
       <c r="AR30" s="25"/>
       <c r="AS30" s="25"/>
     </row>
-    <row r="31" spans="1:45">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
       <c r="S31" s="5"/>
     </row>
-    <row r="32" spans="1:45" s="18" customFormat="1">
+    <row r="32" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="S32" s="5"/>
       <c r="W32" s="6"/>
@@ -9322,7 +9317,7 @@
       <c r="AI32" s="6"/>
       <c r="AO32" s="6"/>
     </row>
-    <row r="33" spans="1:45" s="18" customFormat="1">
+    <row r="33" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="S33" s="5"/>
       <c r="W33" s="6"/>
@@ -9330,7 +9325,7 @@
       <c r="AI33" s="6"/>
       <c r="AO33" s="6"/>
     </row>
-    <row r="34" spans="1:45">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>14</v>
       </c>
@@ -9379,7 +9374,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:45">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="C35" s="8">
         <v>2000</v>
@@ -9494,7 +9489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:45">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -9543,7 +9538,7 @@
       <c r="AR36" s="25"/>
       <c r="AS36" s="25"/>
     </row>
-    <row r="37" spans="1:45">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -9591,7 +9586,7 @@
       <c r="AR37" s="25"/>
       <c r="AS37" s="25"/>
     </row>
-    <row r="38" spans="1:45">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -9639,7 +9634,7 @@
       <c r="AR38" s="25"/>
       <c r="AS38" s="25"/>
     </row>
-    <row r="39" spans="1:45">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -9687,7 +9682,7 @@
       <c r="AR39" s="25"/>
       <c r="AS39" s="25"/>
     </row>
-    <row r="40" spans="1:45">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -9735,7 +9730,7 @@
       <c r="AR40" s="25"/>
       <c r="AS40" s="25"/>
     </row>
-    <row r="41" spans="1:45">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -9783,11 +9778,10 @@
       <c r="AR41" s="25"/>
       <c r="AS41" s="25"/>
     </row>
-    <row r="42" spans="1:45">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="S42" s="5"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -9799,28 +9793,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="20" max="20" width="14.25" customWidth="1"/>
-    <col min="23" max="23" width="12.375" style="6" customWidth="1"/>
-    <col min="29" max="29" width="12.375" style="6" customWidth="1"/>
-    <col min="30" max="33" width="8.625" style="18"/>
-    <col min="35" max="35" width="12.375" style="6" customWidth="1"/>
-    <col min="36" max="39" width="8.625" style="18"/>
-    <col min="41" max="41" width="12.375" style="6" customWidth="1"/>
-    <col min="42" max="45" width="8.625" style="18"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" style="6" customWidth="1"/>
+    <col min="29" max="29" width="12.42578125" style="6" customWidth="1"/>
+    <col min="30" max="33" width="8.5703125" style="18"/>
+    <col min="35" max="35" width="12.42578125" style="6" customWidth="1"/>
+    <col min="36" max="39" width="8.5703125" style="18"/>
+    <col min="41" max="41" width="12.42578125" style="6" customWidth="1"/>
+    <col min="42" max="45" width="8.5703125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>55</v>
       </c>
@@ -9869,7 +9863,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="C2" s="10">
         <v>2000</v>
@@ -9984,7 +9978,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -10016,7 +10010,7 @@
         <v>74</v>
       </c>
       <c r="X3" s="25">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="Y3" s="25">
         <v>0.3</v>
@@ -10043,7 +10037,7 @@
       <c r="AR3" s="25"/>
       <c r="AS3" s="25"/>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -10104,7 +10098,7 @@
       <c r="AR4" s="25"/>
       <c r="AS4" s="25"/>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -10157,7 +10151,7 @@
       <c r="AR5" s="25"/>
       <c r="AS5" s="25"/>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -10206,7 +10200,7 @@
       <c r="AR6" s="25"/>
       <c r="AS6" s="25"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -10255,7 +10249,7 @@
       <c r="AR7" s="25"/>
       <c r="AS7" s="25"/>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -10304,21 +10298,21 @@
       <c r="AR8" s="25"/>
       <c r="AS8" s="25"/>
     </row>
-    <row r="10" spans="1:45" s="18" customFormat="1">
+    <row r="10" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="W10" s="6"/>
       <c r="AC10" s="6"/>
       <c r="AI10" s="6"/>
       <c r="AO10" s="6"/>
     </row>
-    <row r="11" spans="1:45" s="18" customFormat="1">
+    <row r="11" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="W11" s="6"/>
       <c r="AC11" s="6"/>
       <c r="AI11" s="6"/>
       <c r="AO11" s="6"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>101</v>
       </c>
@@ -10367,7 +10361,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="C13" s="10">
         <v>2000</v>
@@ -10482,7 +10476,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="4" t="s">
         <v>11</v>
@@ -10530,21 +10524,21 @@
       <c r="AR14" s="25"/>
       <c r="AS14" s="25"/>
     </row>
-    <row r="16" spans="1:45" s="18" customFormat="1">
+    <row r="16" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="W16" s="6"/>
       <c r="AC16" s="6"/>
       <c r="AI16" s="6"/>
       <c r="AO16" s="6"/>
     </row>
-    <row r="17" spans="1:45" s="18" customFormat="1">
+    <row r="17" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="W17" s="6"/>
       <c r="AC17" s="6"/>
       <c r="AI17" s="6"/>
       <c r="AO17" s="6"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>52</v>
       </c>
@@ -10593,7 +10587,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="C19" s="10">
         <v>2000</v>
@@ -10708,7 +10702,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:45">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="4" t="s">
         <v>10</v>
@@ -10792,21 +10786,21 @@
       <c r="AR20" s="39"/>
       <c r="AS20" s="39"/>
     </row>
-    <row r="21" spans="1:45" s="18" customFormat="1">
+    <row r="21" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="W21" s="6"/>
       <c r="AC21" s="6"/>
       <c r="AI21" s="6"/>
       <c r="AO21" s="6"/>
     </row>
-    <row r="22" spans="1:45" s="18" customFormat="1">
+    <row r="22" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="W22" s="6"/>
       <c r="AC22" s="6"/>
       <c r="AI22" s="6"/>
       <c r="AO22" s="6"/>
     </row>
-    <row r="24" spans="1:45">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>53</v>
       </c>
@@ -10855,7 +10849,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:45">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="C25" s="10">
         <v>2000</v>
@@ -10970,7 +10964,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:45">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="4" t="s">
         <v>10</v>
@@ -11054,28 +11048,28 @@
       <c r="AR26" s="39"/>
       <c r="AS26" s="39"/>
     </row>
-    <row r="27" spans="1:45" s="18" customFormat="1">
+    <row r="27" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="W27" s="6"/>
       <c r="AC27" s="6"/>
       <c r="AI27" s="6"/>
       <c r="AO27" s="6"/>
     </row>
-    <row r="28" spans="1:45" s="18" customFormat="1" ht="14.25" customHeight="1">
+    <row r="28" spans="1:45" s="18" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="W28" s="6"/>
       <c r="AC28" s="6"/>
       <c r="AI28" s="6"/>
       <c r="AO28" s="6"/>
     </row>
-    <row r="29" spans="1:45" s="18" customFormat="1">
+    <row r="29" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="W29" s="6"/>
       <c r="AC29" s="6"/>
       <c r="AI29" s="6"/>
       <c r="AO29" s="6"/>
     </row>
-    <row r="30" spans="1:45" s="18" customFormat="1">
+    <row r="30" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>82</v>
       </c>
@@ -11109,7 +11103,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:45" s="18" customFormat="1">
+    <row r="31" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="C31" s="19">
         <v>2000</v>
@@ -11223,7 +11217,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:45" s="18" customFormat="1">
+    <row r="32" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -11271,7 +11265,7 @@
       <c r="AR32" s="25"/>
       <c r="AS32" s="25"/>
     </row>
-    <row r="33" spans="1:45" s="18" customFormat="1">
+    <row r="33" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -11319,7 +11313,7 @@
       <c r="AR33" s="25"/>
       <c r="AS33" s="25"/>
     </row>
-    <row r="34" spans="1:45" s="18" customFormat="1">
+    <row r="34" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -11367,7 +11361,7 @@
       <c r="AR34" s="25"/>
       <c r="AS34" s="25"/>
     </row>
-    <row r="35" spans="1:45" s="18" customFormat="1">
+    <row r="35" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -11415,7 +11409,7 @@
       <c r="AR35" s="25"/>
       <c r="AS35" s="25"/>
     </row>
-    <row r="36" spans="1:45" s="18" customFormat="1">
+    <row r="36" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -11464,7 +11458,7 @@
       <c r="AR36" s="25"/>
       <c r="AS36" s="25"/>
     </row>
-    <row r="37" spans="1:45" s="18" customFormat="1">
+    <row r="37" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -11512,21 +11506,21 @@
       <c r="AR37" s="25"/>
       <c r="AS37" s="25"/>
     </row>
-    <row r="38" spans="1:45" s="18" customFormat="1">
+    <row r="38" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="W38" s="6"/>
       <c r="AC38" s="6"/>
       <c r="AI38" s="6"/>
       <c r="AO38" s="6"/>
     </row>
-    <row r="40" spans="1:45" s="18" customFormat="1">
+    <row r="40" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="W40" s="6"/>
       <c r="AC40" s="6"/>
       <c r="AI40" s="6"/>
       <c r="AO40" s="6"/>
     </row>
-    <row r="41" spans="1:45" s="18" customFormat="1">
+    <row r="41" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>83</v>
       </c>
@@ -11560,7 +11554,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:45" s="18" customFormat="1">
+    <row r="42" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="C42" s="19">
         <v>2000</v>
@@ -11674,7 +11668,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:45" s="18" customFormat="1">
+    <row r="43" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -11722,7 +11716,7 @@
       <c r="AR43" s="25"/>
       <c r="AS43" s="25"/>
     </row>
-    <row r="44" spans="1:45" s="18" customFormat="1">
+    <row r="44" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -11770,7 +11764,7 @@
       <c r="AR44" s="25"/>
       <c r="AS44" s="25"/>
     </row>
-    <row r="45" spans="1:45" s="18" customFormat="1">
+    <row r="45" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -11818,7 +11812,7 @@
       <c r="AR45" s="25"/>
       <c r="AS45" s="25"/>
     </row>
-    <row r="46" spans="1:45" s="18" customFormat="1">
+    <row r="46" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -11866,7 +11860,7 @@
       <c r="AR46" s="25"/>
       <c r="AS46" s="25"/>
     </row>
-    <row r="47" spans="1:45" s="18" customFormat="1">
+    <row r="47" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -11915,7 +11909,7 @@
       <c r="AR47" s="25"/>
       <c r="AS47" s="25"/>
     </row>
-    <row r="48" spans="1:45" s="18" customFormat="1">
+    <row r="48" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -11963,28 +11957,28 @@
       <c r="AR48" s="25"/>
       <c r="AS48" s="25"/>
     </row>
-    <row r="49" spans="1:45" s="18" customFormat="1">
+    <row r="49" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="W49" s="6"/>
       <c r="AC49" s="6"/>
       <c r="AI49" s="6"/>
       <c r="AO49" s="6"/>
     </row>
-    <row r="50" spans="1:45" s="18" customFormat="1">
+    <row r="50" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="W50" s="6"/>
       <c r="AC50" s="6"/>
       <c r="AI50" s="6"/>
       <c r="AO50" s="6"/>
     </row>
-    <row r="51" spans="1:45" s="18" customFormat="1">
+    <row r="51" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="W51" s="6"/>
       <c r="AC51" s="6"/>
       <c r="AI51" s="6"/>
       <c r="AO51" s="6"/>
     </row>
-    <row r="52" spans="1:45">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>80</v>
       </c>
@@ -12033,7 +12027,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:45">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="C53" s="10">
         <v>2000</v>
@@ -12148,7 +12142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:45">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="4" t="s">
         <v>10</v>
@@ -12214,28 +12208,28 @@
       <c r="AR54" s="25"/>
       <c r="AS54" s="25"/>
     </row>
-    <row r="55" spans="1:45" s="18" customFormat="1">
+    <row r="55" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="W55" s="6"/>
       <c r="AC55" s="6"/>
       <c r="AI55" s="6"/>
       <c r="AO55" s="6"/>
     </row>
-    <row r="56" spans="1:45" s="18" customFormat="1">
+    <row r="56" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="W56" s="6"/>
       <c r="AC56" s="6"/>
       <c r="AI56" s="6"/>
       <c r="AO56" s="6"/>
     </row>
-    <row r="57" spans="1:45" s="18" customFormat="1">
+    <row r="57" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="W57" s="6"/>
       <c r="AC57" s="6"/>
       <c r="AI57" s="6"/>
       <c r="AO57" s="6"/>
     </row>
-    <row r="58" spans="1:45" s="18" customFormat="1">
+    <row r="58" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>56</v>
       </c>
@@ -12269,7 +12263,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:45" s="18" customFormat="1">
+    <row r="59" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="C59" s="19">
         <v>2000</v>
@@ -12383,7 +12377,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:45" s="18" customFormat="1">
+    <row r="60" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -12431,7 +12425,7 @@
       <c r="AR60" s="25"/>
       <c r="AS60" s="25"/>
     </row>
-    <row r="61" spans="1:45" s="18" customFormat="1">
+    <row r="61" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -12479,7 +12473,7 @@
       <c r="AR61" s="25"/>
       <c r="AS61" s="25"/>
     </row>
-    <row r="62" spans="1:45" s="18" customFormat="1">
+    <row r="62" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -12527,7 +12521,7 @@
       <c r="AR62" s="25"/>
       <c r="AS62" s="25"/>
     </row>
-    <row r="63" spans="1:45" s="18" customFormat="1">
+    <row r="63" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -12575,7 +12569,7 @@
       <c r="AR63" s="25"/>
       <c r="AS63" s="25"/>
     </row>
-    <row r="64" spans="1:45" s="18" customFormat="1">
+    <row r="64" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -12624,7 +12618,7 @@
       <c r="AR64" s="25"/>
       <c r="AS64" s="25"/>
     </row>
-    <row r="65" spans="1:45" s="18" customFormat="1">
+    <row r="65" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -12672,7 +12666,7 @@
       <c r="AR65" s="25"/>
       <c r="AS65" s="25"/>
     </row>
-    <row r="69" spans="1:45" s="18" customFormat="1">
+    <row r="69" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
         <v>57</v>
       </c>
@@ -12706,7 +12700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:45" s="18" customFormat="1">
+    <row r="70" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="C70" s="19">
         <v>2000</v>
@@ -12820,7 +12814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:45" s="18" customFormat="1">
+    <row r="71" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
         <v>10</v>
       </c>
@@ -12868,7 +12862,6 @@
       <c r="AS71" s="25"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -12880,7 +12873,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS85"/>
   <sheetViews>
@@ -12888,20 +12881,20 @@
       <selection activeCell="W64" sqref="W64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.625" style="6"/>
-    <col min="20" max="20" width="14.375" style="31" customWidth="1"/>
-    <col min="23" max="23" width="11.375" customWidth="1"/>
-    <col min="29" max="29" width="11.375" style="18" customWidth="1"/>
-    <col min="30" max="33" width="8.625" style="18"/>
-    <col min="35" max="35" width="11.375" style="18" customWidth="1"/>
-    <col min="36" max="39" width="8.625" style="18"/>
-    <col min="41" max="41" width="11.375" style="18" customWidth="1"/>
-    <col min="42" max="45" width="8.625" style="18"/>
+    <col min="2" max="2" width="8.5703125" style="6"/>
+    <col min="20" max="20" width="14.42578125" style="31" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" customWidth="1"/>
+    <col min="29" max="29" width="11.42578125" style="18" customWidth="1"/>
+    <col min="30" max="33" width="8.5703125" style="18"/>
+    <col min="35" max="35" width="11.42578125" style="18" customWidth="1"/>
+    <col min="36" max="39" width="8.5703125" style="18"/>
+    <col min="41" max="41" width="11.42578125" style="18" customWidth="1"/>
+    <col min="42" max="45" width="8.5703125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>26</v>
       </c>
@@ -12949,7 +12942,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="C2" s="12">
         <v>2000</v>
@@ -13066,7 +13059,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -13117,7 +13110,7 @@
       <c r="AR3" s="34"/>
       <c r="AS3" s="34"/>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -13168,7 +13161,7 @@
       <c r="AR4" s="34"/>
       <c r="AS4" s="34"/>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -13219,7 +13212,7 @@
       <c r="AR5" s="34"/>
       <c r="AS5" s="34"/>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -13270,7 +13263,7 @@
       <c r="AR6" s="34"/>
       <c r="AS6" s="34"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -13321,7 +13314,7 @@
       <c r="AR7" s="34"/>
       <c r="AS7" s="34"/>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -13372,15 +13365,15 @@
       <c r="AR8" s="34"/>
       <c r="AS8" s="34"/>
     </row>
-    <row r="10" spans="1:45" s="18" customFormat="1">
+    <row r="10" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="T10" s="31"/>
     </row>
-    <row r="11" spans="1:45" s="18" customFormat="1">
+    <row r="11" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="T11" s="31"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>27</v>
       </c>
@@ -13428,7 +13421,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="C13" s="12">
         <v>2000</v>
@@ -13545,7 +13538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -13596,7 +13589,7 @@
       <c r="AR14" s="30"/>
       <c r="AS14" s="30"/>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -13647,7 +13640,7 @@
       <c r="AR15" s="30"/>
       <c r="AS15" s="30"/>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -13698,7 +13691,7 @@
       <c r="AR16" s="30"/>
       <c r="AS16" s="30"/>
     </row>
-    <row r="17" spans="1:45">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -13749,7 +13742,7 @@
       <c r="AR17" s="30"/>
       <c r="AS17" s="30"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -13800,7 +13793,7 @@
       <c r="AR18" s="30"/>
       <c r="AS18" s="30"/>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -13851,15 +13844,15 @@
       <c r="AR19" s="30"/>
       <c r="AS19" s="30"/>
     </row>
-    <row r="21" spans="1:45" s="18" customFormat="1">
+    <row r="21" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="T21" s="31"/>
     </row>
-    <row r="22" spans="1:45" s="18" customFormat="1">
+    <row r="22" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="T22" s="31"/>
     </row>
-    <row r="23" spans="1:45">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>28</v>
       </c>
@@ -13907,7 +13900,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:45">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="C24" s="12">
         <v>2000</v>
@@ -14024,7 +14017,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:45">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -14075,7 +14068,7 @@
       <c r="AR25" s="30"/>
       <c r="AS25" s="30"/>
     </row>
-    <row r="26" spans="1:45">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -14126,7 +14119,7 @@
       <c r="AR26" s="30"/>
       <c r="AS26" s="30"/>
     </row>
-    <row r="27" spans="1:45">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -14177,7 +14170,7 @@
       <c r="AR27" s="30"/>
       <c r="AS27" s="30"/>
     </row>
-    <row r="28" spans="1:45">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -14228,7 +14221,7 @@
       <c r="AR28" s="30"/>
       <c r="AS28" s="30"/>
     </row>
-    <row r="29" spans="1:45">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -14279,7 +14272,7 @@
       <c r="AR29" s="30"/>
       <c r="AS29" s="30"/>
     </row>
-    <row r="30" spans="1:45">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -14330,15 +14323,15 @@
       <c r="AR30" s="30"/>
       <c r="AS30" s="30"/>
     </row>
-    <row r="32" spans="1:45" s="18" customFormat="1">
+    <row r="32" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="T32" s="31"/>
     </row>
-    <row r="33" spans="1:45" s="18" customFormat="1">
+    <row r="33" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="T33" s="31"/>
     </row>
-    <row r="34" spans="1:45">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>128</v>
       </c>
@@ -14386,7 +14379,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:45">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="C35" s="12">
         <v>2000</v>
@@ -14503,7 +14496,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:45">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -14564,7 +14557,7 @@
       <c r="AR36" s="30"/>
       <c r="AS36" s="30"/>
     </row>
-    <row r="37" spans="1:45">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -14633,7 +14626,7 @@
       <c r="AR37" s="30"/>
       <c r="AS37" s="30"/>
     </row>
-    <row r="38" spans="1:45">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -14694,7 +14687,7 @@
       <c r="AR38" s="30"/>
       <c r="AS38" s="30"/>
     </row>
-    <row r="39" spans="1:45">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -14755,7 +14748,7 @@
       <c r="AR39" s="30"/>
       <c r="AS39" s="30"/>
     </row>
-    <row r="40" spans="1:45">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -14816,7 +14809,7 @@
       <c r="AR40" s="30"/>
       <c r="AS40" s="30"/>
     </row>
-    <row r="41" spans="1:45">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -14877,15 +14870,15 @@
       <c r="AR41" s="30"/>
       <c r="AS41" s="30"/>
     </row>
-    <row r="43" spans="1:45" s="18" customFormat="1">
+    <row r="43" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="T43" s="31"/>
     </row>
-    <row r="44" spans="1:45" s="18" customFormat="1">
+    <row r="44" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="T44" s="31"/>
     </row>
-    <row r="45" spans="1:45">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>127</v>
       </c>
@@ -14933,7 +14926,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:45">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="C46" s="12">
         <v>2000</v>
@@ -15050,7 +15043,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:45">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -15111,7 +15104,7 @@
       <c r="AR47" s="30"/>
       <c r="AS47" s="30"/>
     </row>
-    <row r="48" spans="1:45">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -15180,7 +15173,7 @@
       <c r="AR48" s="30"/>
       <c r="AS48" s="30"/>
     </row>
-    <row r="49" spans="1:45">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -15241,7 +15234,7 @@
       <c r="AR49" s="30"/>
       <c r="AS49" s="30"/>
     </row>
-    <row r="50" spans="1:45">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -15306,7 +15299,7 @@
       <c r="AR50" s="30"/>
       <c r="AS50" s="30"/>
     </row>
-    <row r="51" spans="1:45">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -15371,7 +15364,7 @@
       <c r="AR51" s="30"/>
       <c r="AS51" s="30"/>
     </row>
-    <row r="52" spans="1:45">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -15432,15 +15425,15 @@
       <c r="AR52" s="30"/>
       <c r="AS52" s="30"/>
     </row>
-    <row r="54" spans="1:45" s="18" customFormat="1">
+    <row r="54" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="T54" s="31"/>
     </row>
-    <row r="55" spans="1:45" s="18" customFormat="1">
+    <row r="55" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="T55" s="31"/>
     </row>
-    <row r="56" spans="1:45">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>33</v>
       </c>
@@ -15488,7 +15481,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:45">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="C57" s="12">
         <v>2000</v>
@@ -15605,7 +15598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:45">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -15656,7 +15649,7 @@
       <c r="AR58" s="30"/>
       <c r="AS58" s="30"/>
     </row>
-    <row r="59" spans="1:45">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -15725,7 +15718,7 @@
       <c r="AR59" s="30"/>
       <c r="AS59" s="30"/>
     </row>
-    <row r="60" spans="1:45">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -15776,7 +15769,7 @@
       <c r="AR60" s="30"/>
       <c r="AS60" s="30"/>
     </row>
-    <row r="61" spans="1:45">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -15827,7 +15820,7 @@
       <c r="AR61" s="30"/>
       <c r="AS61" s="30"/>
     </row>
-    <row r="62" spans="1:45">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -15878,7 +15871,7 @@
       <c r="AR62" s="30"/>
       <c r="AS62" s="30"/>
     </row>
-    <row r="63" spans="1:45">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -15947,15 +15940,15 @@
       <c r="AR63" s="30"/>
       <c r="AS63" s="30"/>
     </row>
-    <row r="65" spans="1:45" s="18" customFormat="1">
+    <row r="65" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="T65" s="31"/>
     </row>
-    <row r="66" spans="1:45" s="18" customFormat="1">
+    <row r="66" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="T66" s="31"/>
     </row>
-    <row r="67" spans="1:45">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>102</v>
       </c>
@@ -16003,7 +15996,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:45">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="C68" s="12">
         <v>2000</v>
@@ -16120,7 +16113,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:45">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -16171,7 +16164,7 @@
       <c r="AR69" s="30"/>
       <c r="AS69" s="30"/>
     </row>
-    <row r="70" spans="1:45">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -16222,7 +16215,7 @@
       <c r="AR70" s="30"/>
       <c r="AS70" s="30"/>
     </row>
-    <row r="71" spans="1:45">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -16273,7 +16266,7 @@
       <c r="AR71" s="30"/>
       <c r="AS71" s="30"/>
     </row>
-    <row r="72" spans="1:45">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -16324,7 +16317,7 @@
       <c r="AR72" s="30"/>
       <c r="AS72" s="30"/>
     </row>
-    <row r="73" spans="1:45">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -16375,7 +16368,7 @@
       <c r="AR73" s="30"/>
       <c r="AS73" s="30"/>
     </row>
-    <row r="74" spans="1:45">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -16426,19 +16419,19 @@
       <c r="AR74" s="30"/>
       <c r="AS74" s="30"/>
     </row>
-    <row r="75" spans="1:45" s="18" customFormat="1">
+    <row r="75" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="T75" s="31"/>
     </row>
-    <row r="76" spans="1:45" s="18" customFormat="1">
+    <row r="76" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
       <c r="T76" s="31"/>
     </row>
-    <row r="77" spans="1:45" s="18" customFormat="1">
+    <row r="77" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="T77" s="31"/>
     </row>
-    <row r="78" spans="1:45" s="18" customFormat="1">
+    <row r="78" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>81</v>
       </c>
@@ -16469,7 +16462,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:45" s="18" customFormat="1">
+    <row r="79" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="C79" s="19">
         <v>2000</v>
@@ -16585,7 +16578,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:45" s="18" customFormat="1">
+    <row r="80" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>MSM</v>
@@ -16635,7 +16628,7 @@
       <c r="AR80" s="30"/>
       <c r="AS80" s="30"/>
     </row>
-    <row r="81" spans="2:45" s="18" customFormat="1">
+    <row r="81" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW</v>
@@ -16685,7 +16678,7 @@
       <c r="AR81" s="30"/>
       <c r="AS81" s="30"/>
     </row>
-    <row r="82" spans="2:45" s="18" customFormat="1">
+    <row r="82" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
         <v>Male PWID</v>
@@ -16735,7 +16728,7 @@
       <c r="AR82" s="30"/>
       <c r="AS82" s="30"/>
     </row>
-    <row r="83" spans="2:45" s="18" customFormat="1">
+    <row r="83" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
         <v>Other males</v>
@@ -16785,7 +16778,7 @@
       <c r="AR83" s="30"/>
       <c r="AS83" s="30"/>
     </row>
-    <row r="84" spans="2:45" s="18" customFormat="1">
+    <row r="84" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
         <v>Other females</v>
@@ -16835,7 +16828,7 @@
       <c r="AR84" s="30"/>
       <c r="AS84" s="30"/>
     </row>
-    <row r="85" spans="2:45" s="18" customFormat="1">
+    <row r="85" spans="2:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
         <v>Clients</v>
@@ -16886,7 +16879,6 @@
       <c r="AS85" s="30"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -16898,31 +16890,31 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.375" style="31" customWidth="1"/>
-    <col min="21" max="21" width="8.625" style="31"/>
-    <col min="22" max="22" width="9.125" style="31" customWidth="1"/>
-    <col min="23" max="23" width="11.75" style="6" customWidth="1"/>
-    <col min="24" max="27" width="8.625" style="31"/>
-    <col min="29" max="29" width="11.75" style="6" customWidth="1"/>
-    <col min="30" max="33" width="8.625" style="31"/>
-    <col min="35" max="35" width="11.75" style="6" customWidth="1"/>
-    <col min="36" max="39" width="8.625" style="31"/>
-    <col min="41" max="41" width="11.75" style="6" customWidth="1"/>
-    <col min="42" max="45" width="8.625" style="31"/>
+    <col min="2" max="2" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" style="31" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" style="31"/>
+    <col min="22" max="22" width="9.140625" style="31" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" style="6" customWidth="1"/>
+    <col min="24" max="27" width="8.5703125" style="31"/>
+    <col min="29" max="29" width="11.7109375" style="6" customWidth="1"/>
+    <col min="30" max="33" width="8.5703125" style="31"/>
+    <col min="35" max="35" width="11.7109375" style="6" customWidth="1"/>
+    <col min="36" max="39" width="8.5703125" style="31"/>
+    <col min="41" max="41" width="11.7109375" style="6" customWidth="1"/>
+    <col min="42" max="45" width="8.5703125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>129</v>
       </c>
@@ -16968,7 +16960,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="C2" s="14">
         <v>2000</v>
@@ -17085,7 +17077,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -17136,7 +17128,7 @@
       <c r="AR3" s="30"/>
       <c r="AS3" s="30"/>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -17187,7 +17179,7 @@
       <c r="AR4" s="30"/>
       <c r="AS4" s="30"/>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -17238,7 +17230,7 @@
       <c r="AR5" s="30"/>
       <c r="AS5" s="30"/>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -17289,7 +17281,7 @@
       <c r="AR6" s="30"/>
       <c r="AS6" s="30"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -17340,7 +17332,7 @@
       <c r="AR7" s="30"/>
       <c r="AS7" s="30"/>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -17391,7 +17383,7 @@
       <c r="AR8" s="30"/>
       <c r="AS8" s="30"/>
     </row>
-    <row r="10" spans="1:45" s="18" customFormat="1">
+    <row r="10" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="T10" s="31"/>
       <c r="U10" s="31"/>
@@ -17417,7 +17409,7 @@
       <c r="AR10" s="31"/>
       <c r="AS10" s="31"/>
     </row>
-    <row r="11" spans="1:45" s="18" customFormat="1">
+    <row r="11" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="T11" s="31"/>
       <c r="U11" s="31"/>
@@ -17443,7 +17435,7 @@
       <c r="AR11" s="31"/>
       <c r="AS11" s="31"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -17489,7 +17481,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="C13" s="14">
         <v>2000</v>
@@ -17604,7 +17596,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="48" t="s">
         <v>35</v>
@@ -17670,7 +17662,7 @@
       <c r="AR14" s="30"/>
       <c r="AS14" s="30"/>
     </row>
-    <row r="16" spans="1:45" s="18" customFormat="1">
+    <row r="16" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="T16" s="31"/>
       <c r="U16" s="31"/>
@@ -17696,7 +17688,7 @@
       <c r="AR16" s="31"/>
       <c r="AS16" s="31"/>
     </row>
-    <row r="17" spans="1:45" s="18" customFormat="1">
+    <row r="17" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="T17" s="31"/>
       <c r="U17" s="31"/>
@@ -17722,7 +17714,7 @@
       <c r="AR17" s="31"/>
       <c r="AS17" s="31"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>79</v>
       </c>
@@ -17768,7 +17760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="C19" s="14">
         <v>2000</v>
@@ -17885,7 +17877,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:45">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="48" t="s">
         <v>41</v>
@@ -17950,7 +17942,6 @@
       <c r="AS20" s="30"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -17962,20 +17953,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.625" customWidth="1"/>
-    <col min="3" max="8" width="13.625" customWidth="1"/>
-    <col min="9" max="15" width="6.625" customWidth="1"/>
+    <col min="1" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="15" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" customHeight="1">
+    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>140</v>
       </c>
@@ -18004,7 +17995,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="37"/>
       <c r="C2" s="4" t="str">
@@ -18050,7 +18041,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -18083,7 +18074,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
       <c r="B4" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -18114,7 +18105,7 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -18149,7 +18140,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -18183,7 +18174,7 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -18214,7 +18205,7 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -18249,7 +18240,7 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -18277,9 +18268,9 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:26" s="18" customFormat="1"/>
-    <row r="11" spans="1:26" s="18" customFormat="1"/>
-    <row r="12" spans="1:26">
+    <row r="10" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>138</v>
       </c>
@@ -18309,7 +18300,7 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="37"/>
       <c r="C13" s="4" t="str">
@@ -18355,7 +18346,7 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -18388,7 +18379,7 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -18419,7 +18410,7 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -18454,7 +18445,7 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -18489,7 +18480,7 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -18520,7 +18511,7 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -18537,7 +18528,7 @@
       </c>
       <c r="H19" s="36"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -18547,7 +18538,7 @@
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="1:26" s="18" customFormat="1">
+    <row r="21" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -18575,8 +18566,8 @@
       <c r="Y21" s="16"/>
       <c r="Z21" s="16"/>
     </row>
-    <row r="22" spans="1:26" s="18" customFormat="1"/>
-    <row r="23" spans="1:26">
+    <row r="22" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>139</v>
       </c>
@@ -18588,7 +18579,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="37"/>
       <c r="C24" s="4" t="str">
@@ -18616,7 +18607,7 @@
         <v>Clients</v>
       </c>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -18629,7 +18620,7 @@
       <c r="G25" s="36"/>
       <c r="H25" s="36"/>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -18642,7 +18633,7 @@
       <c r="G26" s="36"/>
       <c r="H26" s="36"/>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -18655,7 +18646,7 @@
       <c r="G27" s="36"/>
       <c r="H27" s="36"/>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -18668,7 +18659,7 @@
       <c r="G28" s="36"/>
       <c r="H28" s="36"/>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -18681,7 +18672,7 @@
       <c r="G29" s="36"/>
       <c r="H29" s="36"/>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -18696,7 +18687,7 @@
       <c r="G30" s="36"/>
       <c r="H30" s="36"/>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -18706,7 +18697,7 @@
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
     </row>
-    <row r="32" spans="1:26" s="18" customFormat="1">
+    <row r="32" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -18734,8 +18725,8 @@
       <c r="Y32" s="16"/>
       <c r="Z32" s="16"/>
     </row>
-    <row r="33" spans="1:8" s="18" customFormat="1"/>
-    <row r="34" spans="1:8">
+    <row r="33" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>141</v>
       </c>
@@ -18747,7 +18738,7 @@
       <c r="G34" s="16"/>
       <c r="H34" s="16"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="37"/>
       <c r="C35" s="4" t="str">
@@ -18775,7 +18766,7 @@
         <v>Clients</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="4" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
@@ -18788,7 +18779,7 @@
       <c r="G36" s="36"/>
       <c r="H36" s="36"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
@@ -18801,7 +18792,7 @@
       <c r="G37" s="36"/>
       <c r="H37" s="36"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="4" t="str">
         <f>'Populations &amp; programs'!$C$5</f>
@@ -18816,7 +18807,7 @@
       <c r="G38" s="36"/>
       <c r="H38" s="36"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="4" t="str">
         <f>'Populations &amp; programs'!$C$6</f>
@@ -18829,7 +18820,7 @@
       <c r="G39" s="36"/>
       <c r="H39" s="36"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="4" t="str">
         <f>'Populations &amp; programs'!$C$7</f>
@@ -18842,7 +18833,7 @@
       <c r="G40" s="36"/>
       <c r="H40" s="36"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="4" t="str">
         <f>'Populations &amp; programs'!$C$8</f>
@@ -18856,7 +18847,6 @@
       <c r="H41" s="36"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
made some programs more effective
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19425" windowHeight="10965" tabRatio="863" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -2456,7 +2456,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3711,7 +3711,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -5201,8 +5201,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12:M13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7916,7 +7916,9 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS42"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9798,7 +9800,7 @@
   <dimension ref="A1:AS71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12877,8 +12879,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS85"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="W64" sqref="W64"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="X53" sqref="X53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15210,7 +15212,7 @@
         <v>0.3</v>
       </c>
       <c r="Y49" s="30">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z49" s="30">
         <v>0.5</v>
@@ -16895,7 +16897,7 @@
   <dimension ref="A1:AS20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17635,16 +17637,16 @@
         <v>123</v>
       </c>
       <c r="X14" s="30">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="Y14" s="30">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="Z14" s="30">
+        <v>0.05</v>
+      </c>
+      <c r="AA14" s="30">
         <v>0.1</v>
-      </c>
-      <c r="AA14" s="30">
-        <v>0.14000000000000001</v>
       </c>
       <c r="AC14" s="40"/>
       <c r="AD14" s="30"/>

</xml_diff>

<commit_message>
set up function to plot scatter data only
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="863"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14200" tabRatio="863" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -21,9 +21,9 @@
     <sheet name="Disutilities &amp; costs" sheetId="14" r:id="rId12"/>
     <sheet name="Macroeconomics" sheetId="18" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="130000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -33,166 +33,73 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="144">
   <si>
-    <t>Percentage of people who used a condom at last act with regular partners</t>
+    <t>Age-related population transitions (average number of years before movement)</t>
   </si>
   <si>
-    <t>Average number of injections per person per year</t>
+    <t>Government expenditure</t>
   </si>
   <si>
-    <t>Disease progression rate (% per year)</t>
+    <t>General government health expenditure</t>
   </si>
   <si>
-    <t>Mother-to-child (breastfeeding)</t>
+    <t>Domestic HIV spending</t>
   </si>
   <si>
-    <t>Mother-to-child (non-breastfeeding)</t>
+    <t>Global Fund HIV commitments</t>
   </si>
   <si>
-    <t>Relative disease-related transmissibility</t>
+    <t>PEPFAR HIV commitments</t>
   </si>
   <si>
-    <t>Social mitigation costs</t>
+    <t>Other international HIV commitments</t>
   </si>
   <si>
-    <t>HIV-related health care costs (excluding treatment)</t>
+    <t>Private HIV spending</t>
   </si>
   <si>
-    <t>Untreated HIV, acute</t>
+    <t>Total domestic and international health expenditure</t>
   </si>
   <si>
-    <t>Disutility weights</t>
+    <t>Number of people on first-line treatment</t>
   </si>
   <si>
-    <t>Interactions between casual partners</t>
+    <t>Number of people on second-line treatment</t>
   </si>
   <si>
-    <t>Interactions between commercial partners</t>
+    <t>Number of AIDS-related deaths</t>
   </si>
   <si>
-    <t>Interactions between regular partners</t>
+    <t>Percentage of population tested for HIV in the last 12 months</t>
   </si>
   <si>
-    <t>Interactions between people who inject drugs</t>
+    <t>Birth rate (births per woman per year)</t>
   </si>
   <si>
-    <t>Interaction-related transmissibility (% per act)</t>
+    <t>Percentage of HIV-positive women who breastfed</t>
   </si>
   <si>
-    <t>Treatment recovery rate (% per year)</t>
+    <t>Condom use</t>
   </si>
   <si>
-    <t>Treatment failure rate (% per year)</t>
+    <t>Heterosexual</t>
   </si>
   <si>
-    <t>Death rate (% mortality per year)</t>
+    <t>Homosexual</t>
   </si>
   <si>
-    <t>Relative transmissibility</t>
+    <t>Sex worker</t>
   </si>
   <si>
-    <t>Modeled estimate of HIV prevalence</t>
+    <t>Client</t>
   </si>
   <si>
-    <t>Male</t>
+    <t>Other males</t>
   </si>
   <si>
-    <t>Female</t>
+    <t>Other females</t>
   </si>
   <si>
-    <t>Injects</t>
-  </si>
-  <si>
-    <t>Men who have sex with men</t>
-  </si>
-  <si>
-    <t>FSW programs</t>
-  </si>
-  <si>
-    <t>Programs for female sex workers and clients</t>
-  </si>
-  <si>
-    <t>Needle-syringe programs</t>
-  </si>
-  <si>
-    <t>Programs for men who have sex with men</t>
-  </si>
-  <si>
-    <t>Social and behavior change communication</t>
-  </si>
-  <si>
-    <t>SBCC</t>
-  </si>
-  <si>
-    <t>Male PWID</t>
-  </si>
-  <si>
-    <t>Males who inject drugs</t>
-  </si>
-  <si>
-    <t>MSM programs</t>
-  </si>
-  <si>
-    <t>Number of people who inject drugs who are on opiate substitution therapy</t>
-  </si>
-  <si>
-    <t>Number of women on PMTCT (Option B/B+)</t>
-  </si>
-  <si>
-    <t>Number of voluntary medical male circumcisions performed</t>
-  </si>
-  <si>
-    <t>Percentage of people covered by pre-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Percentage of people coveraged by post-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Pre-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Post-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Cost &amp; coverage</t>
-  </si>
-  <si>
-    <t>Saturating</t>
-  </si>
-  <si>
-    <t>Assumption</t>
-  </si>
-  <si>
-    <t>Injecting</t>
-  </si>
-  <si>
-    <t>Heterosexual insertive</t>
-  </si>
-  <si>
-    <t>Heterosexual receptive</t>
-  </si>
-  <si>
-    <t>Homosexual insertive</t>
-  </si>
-  <si>
-    <t>Homosexual receptive</t>
-  </si>
-  <si>
-    <t>Opiate substitution therapy</t>
-  </si>
-  <si>
-    <t>ARV treatment</t>
-  </si>
-  <si>
-    <t>Percentage of people who die from non-HIV-related causes per year</t>
-  </si>
-  <si>
-    <t>Number of HIV tests per year</t>
-  </si>
-  <si>
-    <t>Number of HIV diagnoses per year</t>
+    <t>Clients of female sex workers</t>
   </si>
   <si>
     <t>Modeled estimate of new HIV infections per year</t>
@@ -400,84 +307,177 @@
     <t>Prevalence of any discharging STIs</t>
   </si>
   <si>
-    <t>Age-related population transitions (average number of years before movement)</t>
+    <t>Percentage of people who used a condom at last act with regular partners</t>
   </si>
   <si>
-    <t>Government expenditure</t>
+    <t>Average number of injections per person per year</t>
   </si>
   <si>
-    <t>General government health expenditure</t>
+    <t>Disease progression rate (% per year)</t>
   </si>
   <si>
-    <t>Domestic HIV spending</t>
+    <t>Mother-to-child (breastfeeding)</t>
   </si>
   <si>
-    <t>Global Fund HIV commitments</t>
+    <t>Mother-to-child (non-breastfeeding)</t>
   </si>
   <si>
-    <t>PEPFAR HIV commitments</t>
+    <t>Relative disease-related transmissibility</t>
   </si>
   <si>
-    <t>Other international HIV commitments</t>
+    <t>Social mitigation costs</t>
   </si>
   <si>
-    <t>Private HIV spending</t>
+    <t>HIV-related health care costs (excluding treatment)</t>
   </si>
   <si>
-    <t>Total domestic and international health expenditure</t>
+    <t>Untreated HIV, acute</t>
   </si>
   <si>
-    <t>Number of people on first-line treatment</t>
+    <t>Disutility weights</t>
   </si>
   <si>
-    <t>Number of people on second-line treatment</t>
+    <t>Interactions between casual partners</t>
   </si>
   <si>
-    <t>Number of AIDS-related deaths</t>
+    <t>Interactions between commercial partners</t>
   </si>
   <si>
-    <t>Percentage of population tested for HIV in the last 12 months</t>
+    <t>Interactions between regular partners</t>
   </si>
   <si>
-    <t>Birth rate (births per woman per year)</t>
+    <t>Interactions between people who inject drugs</t>
   </si>
   <si>
-    <t>Percentage of HIV-positive women who breastfed</t>
+    <t>Interaction-related transmissibility (% per act)</t>
   </si>
   <si>
-    <t>Condom use</t>
+    <t>Treatment recovery rate (% per year)</t>
   </si>
   <si>
-    <t>Heterosexual</t>
+    <t>Treatment failure rate (% per year)</t>
   </si>
   <si>
-    <t>Homosexual</t>
+    <t>Death rate (% mortality per year)</t>
   </si>
   <si>
-    <t>Sex worker</t>
+    <t>Relative transmissibility</t>
   </si>
   <si>
-    <t>Client</t>
+    <t>Modeled estimate of HIV prevalence</t>
   </si>
   <si>
-    <t>Other males</t>
+    <t>Male</t>
   </si>
   <si>
-    <t>Other females</t>
+    <t>Female</t>
   </si>
   <si>
-    <t>Clients of female sex workers</t>
+    <t>Injects</t>
+  </si>
+  <si>
+    <t>Men who have sex with men</t>
+  </si>
+  <si>
+    <t>FSW programs</t>
+  </si>
+  <si>
+    <t>Programs for female sex workers and clients</t>
+  </si>
+  <si>
+    <t>Needle-syringe programs</t>
+  </si>
+  <si>
+    <t>Programs for men who have sex with men</t>
+  </si>
+  <si>
+    <t>Social and behavior change communication</t>
+  </si>
+  <si>
+    <t>SBCC</t>
+  </si>
+  <si>
+    <t>Male PWID</t>
+  </si>
+  <si>
+    <t>Males who inject drugs</t>
+  </si>
+  <si>
+    <t>MSM programs</t>
+  </si>
+  <si>
+    <t>Number of people who inject drugs who are on opiate substitution therapy</t>
+  </si>
+  <si>
+    <t>Number of women on PMTCT (Option B/B+)</t>
+  </si>
+  <si>
+    <t>Number of voluntary medical male circumcisions performed</t>
+  </si>
+  <si>
+    <t>Percentage of people covered by pre-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Percentage of people coveraged by post-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Pre-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Post-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Cost &amp; coverage</t>
+  </si>
+  <si>
+    <t>Saturating</t>
+  </si>
+  <si>
+    <t>Assumption</t>
+  </si>
+  <si>
+    <t>Injecting</t>
+  </si>
+  <si>
+    <t>Heterosexual insertive</t>
+  </si>
+  <si>
+    <t>Heterosexual receptive</t>
+  </si>
+  <si>
+    <t>Homosexual insertive</t>
+  </si>
+  <si>
+    <t>Homosexual receptive</t>
+  </si>
+  <si>
+    <t>Opiate substitution therapy</t>
+  </si>
+  <si>
+    <t>ARV treatment</t>
+  </si>
+  <si>
+    <t>Percentage of people who die from non-HIV-related causes per year</t>
+  </si>
+  <si>
+    <t>Number of HIV tests per year</t>
+  </si>
+  <si>
+    <t>Number of HIV diagnoses per year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -653,7 +653,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
@@ -1301,7 +1301,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="50">
@@ -1407,7 +1407,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -2083,7 +2083,7 @@
     <cellStyle name="Percent 2 2" xfId="660"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <mruColors>
       <color rgb="FFB9DAED"/>
@@ -2386,58 +2386,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="20"/>
+    <col min="1" max="1" width="9.125" style="20"/>
     <col min="2" max="2" width="5" style="20" customWidth="1"/>
     <col min="3" max="3" width="18" style="20" customWidth="1"/>
-    <col min="4" max="4" width="55.33203125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" style="20" customWidth="1"/>
-    <col min="6" max="7" width="9.1640625" style="20"/>
-    <col min="8" max="9" width="14.1640625" style="20" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" style="20" customWidth="1"/>
-    <col min="11" max="16384" width="9.1640625" style="20"/>
+    <col min="4" max="4" width="55.375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="20" customWidth="1"/>
+    <col min="6" max="7" width="9.125" style="20"/>
+    <col min="8" max="9" width="14.125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="12.125" style="20" customWidth="1"/>
+    <col min="11" max="16384" width="9.125" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="21" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="C2" s="21" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>137</v>
+        <v>16</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>139</v>
+        <v>18</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2445,10 +2446,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="E3" s="41" t="b">
         <v>1</v>
@@ -2477,10 +2478,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="E4" s="41" t="b">
         <v>0</v>
@@ -2509,10 +2510,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="E5" s="41" t="b">
         <v>1</v>
@@ -2541,10 +2542,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>141</v>
+        <v>20</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>141</v>
+        <v>20</v>
       </c>
       <c r="E6" s="41" t="b">
         <v>1</v>
@@ -2573,10 +2574,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>142</v>
+        <v>21</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>142</v>
+        <v>21</v>
       </c>
       <c r="E7" s="41" t="b">
         <v>0</v>
@@ -2605,10 +2606,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
       <c r="E8" s="41" t="b">
         <v>1</v>
@@ -2643,20 +2644,20 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="21" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="B12" s="21"/>
     </row>
     <row r="13" spans="1:11">
       <c r="B13" s="21"/>
       <c r="C13" s="21" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2664,10 +2665,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="E14" s="41" t="b">
         <v>1</v>
@@ -2678,10 +2679,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="D15" s="45" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="E15" s="41" t="b">
         <v>1</v>
@@ -2692,10 +2693,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="E16" s="41" t="b">
         <v>0</v>
@@ -2706,10 +2707,10 @@
         <v>4</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="E17" s="41" t="b">
         <v>1</v>
@@ -2720,10 +2721,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="45" t="s">
-        <v>24</v>
+        <v>114</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="E18" s="41" t="b">
         <v>1</v>
@@ -2734,10 +2735,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="E19" s="41" t="b">
         <v>0</v>
@@ -2748,10 +2749,10 @@
         <v>7</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="E20" s="41" t="b">
         <v>0</v>
@@ -2761,7 +2762,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -2769,22 +2770,23 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" style="6"/>
-    <col min="3" max="8" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="6"/>
+    <col min="3" max="8" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="3" t="s">
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="2"/>
@@ -2937,7 +2939,7 @@
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="17" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="2"/>
@@ -3048,10 +3050,11 @@
       <c r="H19" s="24"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -3059,39 +3062,40 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="18"/>
-    <col min="2" max="2" width="33.1640625" style="18" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" style="18"/>
+    <col min="1" max="1" width="9.125" style="18"/>
+    <col min="2" max="2" width="33.125" style="18" customWidth="1"/>
+    <col min="3" max="16384" width="9.125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="19" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1">
       <c r="C2" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" s="19" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="C3" s="26">
         <v>4.0000000000000002E-4</v>
@@ -3101,7 +3105,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="B4" s="19" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
       <c r="C4" s="26">
         <v>1E-3</v>
@@ -3111,7 +3115,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="B5" s="19" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="C5" s="26">
         <v>5.9999999999999995E-4</v>
@@ -3121,7 +3125,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="B6" s="19" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="C6" s="26">
         <v>5.0000000000000001E-3</v>
@@ -3131,7 +3135,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="B7" s="19" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
       <c r="C7" s="26">
         <v>3.0000000000000001E-3</v>
@@ -3141,7 +3145,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="B8" s="19" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="C8" s="25">
         <v>0.05</v>
@@ -3151,7 +3155,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="B9" s="19" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="C9" s="25">
         <v>0.03</v>
@@ -3171,23 +3175,23 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="19" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1">
       <c r="C14" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" s="19" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="C15" s="22">
         <v>10</v>
@@ -3197,7 +3201,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="B16" s="19" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C16" s="22">
         <v>1</v>
@@ -3207,7 +3211,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="B17" s="19" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C17" s="22">
         <v>1</v>
@@ -3217,7 +3221,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="B18" s="19" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C18" s="22">
         <v>1</v>
@@ -3227,7 +3231,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="B19" s="19" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C19" s="22">
         <v>3.8</v>
@@ -3247,24 +3251,24 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="19" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="B23" s="19"/>
     </row>
     <row r="24" spans="1:8">
       <c r="C24" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="B25" s="19" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C25" s="25">
         <v>1</v>
@@ -3274,7 +3278,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="B26" s="19" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C26" s="25">
         <v>0.25</v>
@@ -3284,7 +3288,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="B27" s="19" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="C27" s="25">
         <v>0.25</v>
@@ -3294,7 +3298,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="B28" s="19" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="C28" s="25">
         <v>0.5</v>
@@ -3314,23 +3318,23 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="19" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="C33" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="B34" s="19" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="C34" s="25">
         <v>0.45</v>
@@ -3340,7 +3344,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="B35" s="19" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C35" s="25">
         <v>0.7</v>
@@ -3350,7 +3354,7 @@
     </row>
     <row r="36" spans="1:8">
       <c r="B36" s="19" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="C36" s="25">
         <v>0.36</v>
@@ -3373,23 +3377,23 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="19" t="s">
-        <v>16</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="C41" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="B42" s="19" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="C42" s="25">
         <v>0.2</v>
@@ -3403,7 +3407,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="B43" s="19" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="C43" s="25">
         <v>0.1</v>
@@ -3427,23 +3431,23 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="19" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="C48" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="B49" s="19" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="C49" s="25">
         <v>0</v>
@@ -3453,7 +3457,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="B50" s="19" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C50" s="26">
         <v>5.0000000000000001E-4</v>
@@ -3463,7 +3467,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="B51" s="19" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="C51" s="26">
         <v>1E-3</v>
@@ -3473,7 +3477,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="B52" s="19" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C52" s="25">
         <v>0.01</v>
@@ -3483,7 +3487,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="B53" s="19" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C53" s="25">
         <v>0.49</v>
@@ -3493,7 +3497,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="B54" s="19" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="C54" s="25">
         <v>0.04</v>
@@ -3503,7 +3507,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="B55" s="19" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="C55" s="22">
         <v>2</v>
@@ -3523,23 +3527,23 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="19" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="C60" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="B61" s="19" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="C61" s="25">
         <v>0.05</v>
@@ -3549,7 +3553,7 @@
     </row>
     <row r="62" spans="1:8">
       <c r="B62" s="19" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="C62" s="25">
         <v>0.3</v>
@@ -3559,7 +3563,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="B63" s="19" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="C63" s="25">
         <v>0.65</v>
@@ -3569,7 +3573,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="B64" s="19" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="C64" s="25">
         <v>3.5</v>
@@ -3579,7 +3583,7 @@
     </row>
     <row r="65" spans="2:5">
       <c r="B65" s="19" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
       <c r="C65" s="25">
         <v>0.05</v>
@@ -3589,7 +3593,7 @@
     </row>
     <row r="66" spans="2:5">
       <c r="B66" s="19" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C66" s="25">
         <v>0.05</v>
@@ -3599,7 +3603,7 @@
     </row>
     <row r="67" spans="2:5">
       <c r="B67" s="19" t="s">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="C67" s="25">
         <v>0.3</v>
@@ -3609,7 +3613,7 @@
     </row>
     <row r="68" spans="2:5">
       <c r="B68" s="19" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="C68" s="25">
         <v>0.5</v>
@@ -3619,7 +3623,7 @@
     </row>
     <row r="69" spans="2:5">
       <c r="B69" s="19" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="C69" s="25">
         <v>0.5</v>
@@ -3628,10 +3632,11 @@
       <c r="E69" s="22"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -3639,21 +3644,22 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="19" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -3664,18 +3670,18 @@
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="18" customFormat="1">
       <c r="B3" s="19" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="C3" s="24">
         <v>0.05</v>
@@ -3686,7 +3692,7 @@
     <row r="4" spans="1:8">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="C4" s="24">
         <v>0.05</v>
@@ -3697,7 +3703,7 @@
     <row r="5" spans="1:8">
       <c r="A5" s="18"/>
       <c r="B5" s="19" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C5" s="24">
         <v>0.1</v>
@@ -3708,7 +3714,7 @@
     <row r="6" spans="1:8">
       <c r="A6" s="18"/>
       <c r="B6" s="19" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C6" s="24">
         <v>0.15</v>
@@ -3719,7 +3725,7 @@
     <row r="7" spans="1:8">
       <c r="A7" s="18"/>
       <c r="B7" s="19" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="C7" s="24">
         <v>0.5</v>
@@ -3730,7 +3736,7 @@
     <row r="8" spans="1:8">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="C8" s="24">
         <v>5.2999999999999999E-2</v>
@@ -3758,7 +3764,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="19" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -3769,19 +3775,19 @@
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="C14" s="22">
         <v>0</v>
@@ -3792,7 +3798,7 @@
     <row r="15" spans="1:8">
       <c r="A15" s="18"/>
       <c r="B15" s="19" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C15" s="22">
         <v>100</v>
@@ -3803,7 +3809,7 @@
     <row r="16" spans="1:8">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="C16" s="22">
         <v>100</v>
@@ -3814,7 +3820,7 @@
     <row r="17" spans="1:5">
       <c r="A17" s="18"/>
       <c r="B17" s="19" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C17" s="22">
         <v>200</v>
@@ -3825,7 +3831,7 @@
     <row r="18" spans="1:5">
       <c r="A18" s="18"/>
       <c r="B18" s="19" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C18" s="22">
         <v>450</v>
@@ -3835,7 +3841,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="19" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -3846,19 +3852,19 @@
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18"/>
       <c r="B24" s="19" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="C24" s="22">
         <v>0</v>
@@ -3869,7 +3875,7 @@
     <row r="25" spans="1:5">
       <c r="A25" s="18"/>
       <c r="B25" s="19" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C25" s="22">
         <v>100</v>
@@ -3880,7 +3886,7 @@
     <row r="26" spans="1:5">
       <c r="A26" s="18"/>
       <c r="B26" s="19" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="C26" s="22">
         <v>100</v>
@@ -3891,7 +3897,7 @@
     <row r="27" spans="1:5">
       <c r="A27" s="18"/>
       <c r="B27" s="19" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C27" s="22">
         <v>1000</v>
@@ -3902,7 +3908,7 @@
     <row r="28" spans="1:5">
       <c r="A28" s="18"/>
       <c r="B28" s="19" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C28" s="22">
         <v>10000</v>
@@ -3911,10 +3917,11 @@
       <c r="E28" s="22"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -3922,29 +3929,30 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AI57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" style="6"/>
-    <col min="3" max="4" width="13.83203125" style="18" customWidth="1"/>
-    <col min="5" max="11" width="8.6640625" style="18"/>
+    <col min="2" max="2" width="8.625" style="6"/>
+    <col min="3" max="4" width="13.875" style="18" customWidth="1"/>
+    <col min="5" max="11" width="8.625" style="18"/>
     <col min="12" max="12" width="12" style="18" customWidth="1"/>
-    <col min="13" max="17" width="8.6640625" style="18"/>
-    <col min="18" max="18" width="12.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="8.625" style="18"/>
+    <col min="18" max="18" width="12.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
       <c r="A1" s="19" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="S1" s="18"/>
       <c r="T1" s="18"/>
@@ -4060,13 +4068,13 @@
       </c>
       <c r="AH2" s="18"/>
       <c r="AI2" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:35">
       <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C3" s="22">
         <f t="shared" ref="C3:R3" si="0">D3/(1.12)</f>
@@ -4192,7 +4200,7 @@
         <v>350405950838.15192</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI3" s="29"/>
     </row>
@@ -4203,7 +4211,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" s="19" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="S7" s="18"/>
       <c r="T7" s="18"/>
@@ -4319,13 +4327,13 @@
       </c>
       <c r="AH8" s="18"/>
       <c r="AI8" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:35">
       <c r="A9" s="18"/>
       <c r="B9" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C9" s="40">
         <v>30000000000</v>
@@ -4451,13 +4459,13 @@
         <v>180000000000</v>
       </c>
       <c r="AH9" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI9" s="29"/>
     </row>
     <row r="13" spans="1:35">
       <c r="A13" s="19" t="s">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
@@ -4573,13 +4581,13 @@
       </c>
       <c r="AH14" s="18"/>
       <c r="AI14" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:35">
       <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C15" s="22">
         <v>10000000000</v>
@@ -4705,13 +4713,13 @@
         <v>43219423751.506668</v>
       </c>
       <c r="AH15" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI15" s="29"/>
     </row>
     <row r="19" spans="1:35" s="18" customFormat="1">
       <c r="A19" s="19" t="s">
-        <v>129</v>
+        <v>8</v>
       </c>
       <c r="B19" s="6"/>
       <c r="AI19" s="6"/>
@@ -4812,12 +4820,12 @@
         <v>2030</v>
       </c>
       <c r="AI20" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:35" s="18" customFormat="1">
       <c r="B21" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -4851,7 +4859,7 @@
       <c r="AF21" s="22"/>
       <c r="AG21" s="22"/>
       <c r="AH21" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI21" s="29"/>
     </row>
@@ -4869,7 +4877,7 @@
     </row>
     <row r="25" spans="1:35" s="18" customFormat="1">
       <c r="A25" s="19" t="s">
-        <v>123</v>
+        <v>2</v>
       </c>
       <c r="B25" s="6"/>
       <c r="AI25" s="6"/>
@@ -4970,12 +4978,12 @@
         <v>2030</v>
       </c>
       <c r="AI26" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:35" s="18" customFormat="1">
       <c r="B27" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C27" s="22">
         <f>12%*C15</f>
@@ -5102,13 +5110,13 @@
         <v>5186330850.1808004</v>
       </c>
       <c r="AH27" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI27" s="29"/>
     </row>
     <row r="31" spans="1:35" s="18" customFormat="1">
       <c r="A31" s="19" t="s">
-        <v>124</v>
+        <v>3</v>
       </c>
       <c r="B31" s="6"/>
       <c r="AI31" s="6"/>
@@ -5209,12 +5217,12 @@
         <v>2030</v>
       </c>
       <c r="AI32" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:35" s="18" customFormat="1">
       <c r="B33" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C33" s="22">
         <v>15000000</v>
@@ -5310,7 +5318,7 @@
         <v>18000000</v>
       </c>
       <c r="AH33" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI33" s="29"/>
     </row>
@@ -5328,7 +5336,7 @@
     </row>
     <row r="37" spans="1:35" s="18" customFormat="1">
       <c r="A37" s="19" t="s">
-        <v>125</v>
+        <v>4</v>
       </c>
       <c r="B37" s="6"/>
       <c r="AI37" s="6"/>
@@ -5429,12 +5437,12 @@
         <v>2030</v>
       </c>
       <c r="AI38" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:35" s="18" customFormat="1">
       <c r="B39" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
@@ -5468,7 +5476,7 @@
       <c r="AF39" s="22"/>
       <c r="AG39" s="22"/>
       <c r="AH39" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI39" s="29"/>
     </row>
@@ -5486,7 +5494,7 @@
     </row>
     <row r="43" spans="1:35" s="18" customFormat="1">
       <c r="A43" s="19" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="B43" s="6"/>
       <c r="AI43" s="6"/>
@@ -5587,12 +5595,12 @@
         <v>2030</v>
       </c>
       <c r="AI44" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:35" s="18" customFormat="1">
       <c r="B45" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
@@ -5626,13 +5634,13 @@
       <c r="AF45" s="22"/>
       <c r="AG45" s="22"/>
       <c r="AH45" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI45" s="29"/>
     </row>
     <row r="49" spans="1:35" s="18" customFormat="1">
       <c r="A49" s="19" t="s">
-        <v>127</v>
+        <v>6</v>
       </c>
       <c r="B49" s="6"/>
       <c r="AI49" s="6"/>
@@ -5733,12 +5741,12 @@
         <v>2030</v>
       </c>
       <c r="AI50" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:35" s="18" customFormat="1">
       <c r="B51" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
@@ -5772,7 +5780,7 @@
       <c r="AF51" s="22"/>
       <c r="AG51" s="22"/>
       <c r="AH51" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI51" s="29"/>
     </row>
@@ -5790,7 +5798,7 @@
     </row>
     <row r="55" spans="1:35" s="18" customFormat="1">
       <c r="A55" s="19" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="B55" s="6"/>
       <c r="AI55" s="6"/>
@@ -5891,12 +5899,12 @@
         <v>2030</v>
       </c>
       <c r="AI56" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:35" s="18" customFormat="1">
       <c r="B57" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C57" s="22"/>
       <c r="D57" s="22"/>
@@ -5930,16 +5938,16 @@
       <c r="AF57" s="22"/>
       <c r="AG57" s="22"/>
       <c r="AH57" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI57" s="29"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -5947,25 +5955,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12:M13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.1640625" style="18"/>
+    <col min="1" max="2" width="9.125" style="18"/>
     <col min="3" max="3" width="11" style="18" customWidth="1"/>
-    <col min="4" max="20" width="9.1640625" style="18"/>
-    <col min="21" max="21" width="15.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.1640625" style="18"/>
+    <col min="4" max="20" width="9.125" style="18"/>
+    <col min="21" max="21" width="15.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="19" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:22">
@@ -6018,7 +6027,7 @@
         <v>2015</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -6027,7 +6036,7 @@
         <v>SBCC</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="25">
@@ -6060,7 +6069,7 @@
       <c r="R3" s="22"/>
       <c r="S3" s="22"/>
       <c r="T3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U3" s="25"/>
     </row>
@@ -6070,7 +6079,7 @@
         <v>SBCC</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="27">
@@ -6110,7 +6119,7 @@
       <c r="R4" s="24"/>
       <c r="S4" s="24"/>
       <c r="T4" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U4" s="37"/>
     </row>
@@ -6123,7 +6132,7 @@
         <v>NSP</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="25"/>
@@ -6142,7 +6151,7 @@
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
       <c r="T6" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U6" s="25">
         <v>0.2</v>
@@ -6154,7 +6163,7 @@
         <v>NSP</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="23"/>
@@ -6173,7 +6182,7 @@
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
       <c r="T7" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U7" s="47">
         <v>25000</v>
@@ -6188,7 +6197,7 @@
         <v>OST</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="25"/>
@@ -6209,7 +6218,7 @@
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
       <c r="T9" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U9" s="25"/>
     </row>
@@ -6220,7 +6229,7 @@
         <v>OST</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="23"/>
@@ -6241,7 +6250,7 @@
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
       <c r="T10" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U10" s="37"/>
     </row>
@@ -6256,7 +6265,7 @@
         <v>MSM programs</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="25"/>
@@ -6277,7 +6286,7 @@
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
       <c r="T12" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U12" s="25"/>
       <c r="V12" s="6"/>
@@ -6288,7 +6297,7 @@
         <v>MSM programs</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="23"/>
@@ -6309,7 +6318,7 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
       <c r="T13" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U13" s="37"/>
     </row>
@@ -6319,7 +6328,7 @@
         <v>FSW programs</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="25"/>
@@ -6340,7 +6349,7 @@
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
       <c r="T15" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U15" s="25"/>
     </row>
@@ -6350,7 +6359,7 @@
         <v>FSW programs</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
@@ -6371,7 +6380,7 @@
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
       <c r="T16" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U16" s="37"/>
     </row>
@@ -6381,7 +6390,7 @@
         <v>ART</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="25"/>
@@ -6402,7 +6411,7 @@
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
       <c r="T18" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U18" s="25"/>
     </row>
@@ -6412,7 +6421,7 @@
         <v>ART</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="23"/>
@@ -6433,7 +6442,7 @@
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
       <c r="T19" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U19" s="37"/>
     </row>
@@ -6443,7 +6452,7 @@
         <v>PMTCT</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="25"/>
@@ -6464,7 +6473,7 @@
       <c r="R21" s="22"/>
       <c r="S21" s="22"/>
       <c r="T21" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U21" s="25"/>
     </row>
@@ -6474,7 +6483,7 @@
         <v>PMTCT</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
@@ -6495,15 +6504,16 @@
       <c r="R22" s="22"/>
       <c r="S22" s="22"/>
       <c r="T22" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U22" s="37"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -6511,26 +6521,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="9.1640625" style="18"/>
-    <col min="4" max="4" width="9.33203125" style="18" customWidth="1"/>
-    <col min="5" max="20" width="9.1640625" style="18"/>
-    <col min="21" max="21" width="15.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.83203125" style="18" customWidth="1"/>
-    <col min="23" max="16384" width="9.1640625" style="18"/>
+    <col min="1" max="3" width="9.125" style="18"/>
+    <col min="4" max="4" width="9.375" style="18" customWidth="1"/>
+    <col min="5" max="20" width="9.125" style="18"/>
+    <col min="21" max="21" width="15.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.875" style="18" customWidth="1"/>
+    <col min="23" max="16384" width="9.125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="19" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -6583,7 +6594,7 @@
         <v>2015</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -6592,7 +6603,7 @@
         <v>MSM</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
@@ -6611,7 +6622,7 @@
       <c r="R3" s="27"/>
       <c r="S3" s="27"/>
       <c r="T3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U3" s="27">
         <v>37500</v>
@@ -6623,7 +6634,7 @@
         <v>MSM</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
@@ -6642,7 +6653,7 @@
       <c r="R4" s="27"/>
       <c r="S4" s="27"/>
       <c r="T4" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U4" s="27">
         <v>21000</v>
@@ -6654,7 +6665,7 @@
         <v>MSM</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
@@ -6673,7 +6684,7 @@
       <c r="R5" s="27"/>
       <c r="S5" s="27"/>
       <c r="T5" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U5" s="27">
         <v>11000</v>
@@ -6690,7 +6701,7 @@
         <v>FSW</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
@@ -6709,7 +6720,7 @@
       <c r="R7" s="27"/>
       <c r="S7" s="27"/>
       <c r="T7" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U7" s="27"/>
     </row>
@@ -6719,7 +6730,7 @@
         <v>FSW</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
@@ -6738,7 +6749,7 @@
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
       <c r="T8" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U8" s="27">
         <v>15000</v>
@@ -6750,7 +6761,7 @@
         <v>FSW</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
@@ -6769,7 +6780,7 @@
       <c r="R9" s="27"/>
       <c r="S9" s="27"/>
       <c r="T9" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U9" s="27"/>
     </row>
@@ -6800,7 +6811,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
@@ -6829,7 +6840,7 @@
       <c r="R11" s="27"/>
       <c r="S11" s="27"/>
       <c r="T11" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U11" s="27"/>
     </row>
@@ -6839,7 +6850,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
@@ -6868,7 +6879,7 @@
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
       <c r="T12" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U12" s="27"/>
     </row>
@@ -6878,7 +6889,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
@@ -6907,7 +6918,7 @@
       <c r="R13" s="27"/>
       <c r="S13" s="27"/>
       <c r="T13" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U13" s="27"/>
     </row>
@@ -6938,7 +6949,7 @@
         <v>Other males</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
@@ -6957,7 +6968,7 @@
       <c r="R15" s="27"/>
       <c r="S15" s="27"/>
       <c r="T15" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U15" s="27"/>
     </row>
@@ -6967,7 +6978,7 @@
         <v>Other males</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D16" s="22">
         <v>4227500</v>
@@ -7018,7 +7029,7 @@
         <v>6118320.6906761518</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U16" s="27"/>
     </row>
@@ -7028,7 +7039,7 @@
         <v>Other males</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
@@ -7047,7 +7058,7 @@
       <c r="R17" s="27"/>
       <c r="S17" s="27"/>
       <c r="T17" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U17" s="27"/>
     </row>
@@ -7078,7 +7089,7 @@
         <v>Other females</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
@@ -7097,7 +7108,7 @@
       <c r="R19" s="27"/>
       <c r="S19" s="27"/>
       <c r="T19" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U19" s="27"/>
     </row>
@@ -7107,7 +7118,7 @@
         <v>Other females</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D20" s="22">
         <v>4759641.7668505535</v>
@@ -7158,7 +7169,7 @@
         <v>7061706.1901886221</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U20" s="27"/>
     </row>
@@ -7168,7 +7179,7 @@
         <v>Other females</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
@@ -7187,7 +7198,7 @@
       <c r="R21" s="27"/>
       <c r="S21" s="27"/>
       <c r="T21" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U21" s="27"/>
     </row>
@@ -7218,7 +7229,7 @@
         <v>Clients</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -7237,7 +7248,7 @@
       <c r="R23" s="27"/>
       <c r="S23" s="27"/>
       <c r="T23" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U23" s="27"/>
     </row>
@@ -7247,7 +7258,7 @@
         <v>Clients</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D24" s="22">
         <v>522500</v>
@@ -7298,7 +7309,7 @@
         <v>756196.93929705245</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U24" s="27"/>
     </row>
@@ -7308,7 +7319,7 @@
         <v>Clients</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -7327,13 +7338,16 @@
       <c r="R25" s="27"/>
       <c r="S25" s="27"/>
       <c r="T25" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U25" s="27"/>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="G27" s="28"/>
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="19" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -7386,7 +7400,7 @@
         <v>2015</v>
       </c>
       <c r="U30" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -7395,7 +7409,7 @@
         <v>MSM</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -7416,7 +7430,7 @@
       <c r="R31" s="22"/>
       <c r="S31" s="22"/>
       <c r="T31" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U31" s="26"/>
     </row>
@@ -7426,7 +7440,7 @@
         <v>MSM</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -7447,7 +7461,7 @@
       <c r="R32" s="22"/>
       <c r="S32" s="22"/>
       <c r="T32" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U32" s="26"/>
     </row>
@@ -7457,7 +7471,7 @@
         <v>MSM</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
@@ -7478,7 +7492,7 @@
       <c r="R33" s="22"/>
       <c r="S33" s="22"/>
       <c r="T33" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U33" s="26"/>
     </row>
@@ -7492,7 +7506,7 @@
         <v>FSW</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
@@ -7517,7 +7531,7 @@
       <c r="R35" s="22"/>
       <c r="S35" s="22"/>
       <c r="T35" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U35" s="26"/>
     </row>
@@ -7527,7 +7541,7 @@
         <v>FSW</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -7552,7 +7566,7 @@
       <c r="R36" s="22"/>
       <c r="S36" s="22"/>
       <c r="T36" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U36" s="26"/>
     </row>
@@ -7562,7 +7576,7 @@
         <v>FSW</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
@@ -7587,7 +7601,7 @@
       <c r="R37" s="22"/>
       <c r="S37" s="22"/>
       <c r="T37" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U37" s="26"/>
     </row>
@@ -7601,7 +7615,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
@@ -7626,7 +7640,7 @@
       <c r="R39" s="22"/>
       <c r="S39" s="22"/>
       <c r="T39" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U39" s="26"/>
     </row>
@@ -7636,7 +7650,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
@@ -7661,7 +7675,7 @@
       <c r="R40" s="22"/>
       <c r="S40" s="22"/>
       <c r="T40" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U40" s="26"/>
     </row>
@@ -7671,7 +7685,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
@@ -7696,7 +7710,7 @@
       <c r="R41" s="22"/>
       <c r="S41" s="22"/>
       <c r="T41" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U41" s="26"/>
     </row>
@@ -7710,7 +7724,7 @@
         <v>Other males</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
@@ -7729,7 +7743,7 @@
       <c r="R43" s="22"/>
       <c r="S43" s="22"/>
       <c r="T43" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U43" s="26"/>
     </row>
@@ -7739,7 +7753,7 @@
         <v>Other males</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
@@ -7758,7 +7772,7 @@
       <c r="R44" s="22"/>
       <c r="S44" s="22"/>
       <c r="T44" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U44" s="26">
         <v>5.0000000000000001E-4</v>
@@ -7770,7 +7784,7 @@
         <v>Other males</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
@@ -7789,7 +7803,7 @@
       <c r="R45" s="22"/>
       <c r="S45" s="22"/>
       <c r="T45" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U45" s="26"/>
     </row>
@@ -7803,7 +7817,7 @@
         <v>Other females</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
@@ -7822,7 +7836,7 @@
       <c r="R47" s="22"/>
       <c r="S47" s="22"/>
       <c r="T47" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U47" s="26"/>
     </row>
@@ -7832,7 +7846,7 @@
         <v>Other females</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
@@ -7859,7 +7873,7 @@
       <c r="R48" s="22"/>
       <c r="S48" s="22"/>
       <c r="T48" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U48" s="26"/>
     </row>
@@ -7869,7 +7883,7 @@
         <v>Other females</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
@@ -7888,7 +7902,7 @@
       <c r="R49" s="22"/>
       <c r="S49" s="22"/>
       <c r="T49" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U49" s="26"/>
     </row>
@@ -7902,7 +7916,7 @@
         <v>Clients</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
@@ -7921,7 +7935,7 @@
       <c r="R51" s="22"/>
       <c r="S51" s="22"/>
       <c r="T51" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U51" s="26"/>
     </row>
@@ -7931,7 +7945,7 @@
         <v>Clients</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
@@ -7950,7 +7964,7 @@
       <c r="R52" s="22"/>
       <c r="S52" s="22"/>
       <c r="T52" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U52" s="26">
         <v>0.01</v>
@@ -7962,7 +7976,7 @@
         <v>Clients</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
@@ -7981,7 +7995,7 @@
       <c r="R53" s="22"/>
       <c r="S53" s="22"/>
       <c r="T53" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U53" s="26"/>
     </row>
@@ -7989,7 +8003,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -7997,22 +8011,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" style="6"/>
-    <col min="20" max="20" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="6"/>
+    <col min="20" max="20" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="10" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -8085,13 +8100,13 @@
       </c>
       <c r="S2" s="9"/>
       <c r="T2" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="9"/>
       <c r="B3" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -8110,7 +8125,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T3" s="22"/>
     </row>
@@ -8122,7 +8137,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="10" t="s">
-        <v>53</v>
+        <v>143</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -8195,13 +8210,13 @@
       </c>
       <c r="S8" s="9"/>
       <c r="T8" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -8244,7 +8259,7 @@
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
       <c r="S9" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T9" s="22"/>
     </row>
@@ -8256,7 +8271,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="10" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -8329,13 +8344,13 @@
       </c>
       <c r="S14" s="9"/>
       <c r="T14" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="9"/>
       <c r="B15" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -8354,7 +8369,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T15" s="22"/>
     </row>
@@ -8366,7 +8381,7 @@
     </row>
     <row r="19" spans="1:20" s="18" customFormat="1">
       <c r="A19" s="19" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="B19" s="6"/>
     </row>
@@ -8421,12 +8436,12 @@
         <v>2015</v>
       </c>
       <c r="T20" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:20" s="18" customFormat="1">
       <c r="B21" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -8445,7 +8460,7 @@
       <c r="Q21" s="22"/>
       <c r="R21" s="22"/>
       <c r="S21" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T21" s="22"/>
     </row>
@@ -8460,7 +8475,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="10" t="s">
-        <v>132</v>
+        <v>11</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -8533,13 +8548,13 @@
       </c>
       <c r="S26" s="9"/>
       <c r="T26" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="9"/>
       <c r="B27" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
@@ -8558,13 +8573,13 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T27" s="22"/>
     </row>
     <row r="31" spans="1:20" s="18" customFormat="1">
       <c r="A31" s="19" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="B31" s="6"/>
     </row>
@@ -8619,12 +8634,12 @@
         <v>2015</v>
       </c>
       <c r="T32" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="2:20" s="18" customFormat="1">
       <c r="B33" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
@@ -8643,7 +8658,7 @@
       <c r="Q33" s="22"/>
       <c r="R33" s="22"/>
       <c r="S33" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T33" s="22"/>
     </row>
@@ -8651,7 +8666,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -8659,21 +8674,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView topLeftCell="J2" workbookViewId="0">
       <selection activeCell="U2" sqref="U1:AZ1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" style="6"/>
+    <col min="2" max="2" width="8.625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="18" customFormat="1">
       <c r="A1" s="19" t="s">
-        <v>51</v>
+        <v>141</v>
       </c>
       <c r="B1" s="6"/>
     </row>
@@ -8728,7 +8744,7 @@
         <v>2015</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="18" customFormat="1">
@@ -8753,7 +8769,7 @@
       <c r="Q3" s="25"/>
       <c r="R3" s="25"/>
       <c r="S3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T3" s="25">
         <v>0.01</v>
@@ -8781,7 +8797,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T4" s="25">
         <v>0.01</v>
@@ -8809,7 +8825,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T5" s="25">
         <v>0.03</v>
@@ -8837,7 +8853,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T6" s="25">
         <v>0.01</v>
@@ -8865,7 +8881,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T7" s="25">
         <v>0.01</v>
@@ -8893,7 +8909,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T8" s="25">
         <v>0.01</v>
@@ -8910,7 +8926,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="8" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -8983,7 +8999,7 @@
       </c>
       <c r="S13" s="7"/>
       <c r="T13" s="8" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -9009,7 +9025,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T14" s="25">
         <v>0</v>
@@ -9038,7 +9054,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T15" s="25">
         <v>0</v>
@@ -9067,7 +9083,7 @@
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T16" s="25">
         <v>0</v>
@@ -9096,7 +9112,7 @@
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T17" s="25">
         <v>0</v>
@@ -9125,7 +9141,7 @@
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T18" s="25">
         <v>0</v>
@@ -9154,7 +9170,7 @@
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T19" s="25">
         <v>0</v>
@@ -9171,7 +9187,7 @@
     </row>
     <row r="23" spans="1:20" s="18" customFormat="1">
       <c r="A23" s="19" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="B23" s="6"/>
     </row>
@@ -9226,7 +9242,7 @@
         <v>2015</v>
       </c>
       <c r="T24" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:20" s="18" customFormat="1">
@@ -9251,7 +9267,7 @@
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T25" s="25">
         <v>0</v>
@@ -9279,7 +9295,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T26" s="25">
         <v>0</v>
@@ -9307,7 +9323,7 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T27" s="25">
         <v>0</v>
@@ -9335,7 +9351,7 @@
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
       <c r="S28" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T28" s="25">
         <v>0</v>
@@ -9363,7 +9379,7 @@
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
       <c r="S29" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T29" s="25">
         <v>0</v>
@@ -9391,7 +9407,7 @@
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
       <c r="S30" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T30" s="25">
         <v>0</v>
@@ -9410,7 +9426,7 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="8" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -9483,7 +9499,7 @@
       </c>
       <c r="S35" s="7"/>
       <c r="T35" s="8" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -9509,7 +9525,7 @@
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
       <c r="S36" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T36" s="25">
         <v>0</v>
@@ -9537,7 +9553,7 @@
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
       <c r="S37" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T37" s="25">
         <v>0</v>
@@ -9565,7 +9581,7 @@
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
       <c r="S38" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T38" s="25">
         <v>0</v>
@@ -9593,7 +9609,7 @@
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
       <c r="S39" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T39" s="25">
         <v>0</v>
@@ -9621,7 +9637,7 @@
       <c r="Q40" s="22"/>
       <c r="R40" s="22"/>
       <c r="S40" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T40" s="25">
         <v>0</v>
@@ -9649,7 +9665,7 @@
       <c r="Q41" s="22"/>
       <c r="R41" s="22"/>
       <c r="S41" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T41" s="25">
         <v>0</v>
@@ -9662,7 +9678,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -9670,22 +9686,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:AW1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" style="6"/>
-    <col min="20" max="20" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="6"/>
+    <col min="20" max="20" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="10" t="s">
-        <v>133</v>
+        <v>12</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -9758,7 +9775,7 @@
       </c>
       <c r="S2" s="9"/>
       <c r="T2" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -9784,7 +9801,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T3" s="25">
         <v>0.03</v>
@@ -9817,7 +9834,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T4" s="25"/>
     </row>
@@ -9850,7 +9867,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T5" s="22"/>
     </row>
@@ -9877,7 +9894,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T6" s="25">
         <v>0.01</v>
@@ -9906,7 +9923,7 @@
       <c r="Q7" s="25"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T7" s="25">
         <v>0.01</v>
@@ -9935,7 +9952,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T8" s="25">
         <v>0.05</v>
@@ -9949,7 +9966,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="10" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -10022,13 +10039,13 @@
       </c>
       <c r="S13" s="9"/>
       <c r="T13" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="9"/>
       <c r="B14" s="4" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -10047,7 +10064,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T14" s="25">
         <v>0.5</v>
@@ -10061,7 +10078,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="10" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -10134,13 +10151,13 @@
       </c>
       <c r="S19" s="9"/>
       <c r="T19" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="9"/>
       <c r="B20" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C20" s="22">
         <v>0</v>
@@ -10187,7 +10204,7 @@
       <c r="Q20" s="22"/>
       <c r="R20" s="22"/>
       <c r="S20" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T20" s="22"/>
     </row>
@@ -10199,7 +10216,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="10" t="s">
-        <v>131</v>
+        <v>10</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -10272,13 +10289,13 @@
       </c>
       <c r="S25" s="9"/>
       <c r="T25" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="9"/>
       <c r="B26" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C26" s="22">
         <v>0</v>
@@ -10325,7 +10342,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T26" s="22"/>
     </row>
@@ -10340,7 +10357,7 @@
     </row>
     <row r="30" spans="1:20" s="18" customFormat="1">
       <c r="A30" s="19" t="s">
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="B30" s="6"/>
     </row>
@@ -10395,7 +10412,7 @@
         <v>2015</v>
       </c>
       <c r="T31" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:20" s="18" customFormat="1">
@@ -10420,7 +10437,7 @@
       <c r="Q32" s="22"/>
       <c r="R32" s="22"/>
       <c r="S32" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T32" s="24">
         <v>0</v>
@@ -10448,7 +10465,7 @@
       <c r="Q33" s="22"/>
       <c r="R33" s="22"/>
       <c r="S33" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T33" s="24">
         <v>0</v>
@@ -10476,7 +10493,7 @@
       <c r="Q34" s="22"/>
       <c r="R34" s="22"/>
       <c r="S34" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T34" s="24">
         <v>0</v>
@@ -10504,7 +10521,7 @@
       <c r="Q35" s="22"/>
       <c r="R35" s="22"/>
       <c r="S35" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T35" s="24">
         <v>0</v>
@@ -10532,7 +10549,7 @@
       <c r="Q36" s="25"/>
       <c r="R36" s="22"/>
       <c r="S36" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T36" s="24">
         <f>2/50</f>
@@ -10561,7 +10578,7 @@
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
       <c r="S37" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T37" s="24">
         <v>0</v>
@@ -10575,7 +10592,7 @@
     </row>
     <row r="41" spans="1:20" s="18" customFormat="1">
       <c r="A41" s="19" t="s">
-        <v>37</v>
+        <v>127</v>
       </c>
       <c r="B41" s="6"/>
     </row>
@@ -10630,7 +10647,7 @@
         <v>2015</v>
       </c>
       <c r="T42" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:20" s="18" customFormat="1">
@@ -10655,7 +10672,7 @@
       <c r="Q43" s="22"/>
       <c r="R43" s="22"/>
       <c r="S43" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T43" s="24">
         <v>0</v>
@@ -10683,7 +10700,7 @@
       <c r="Q44" s="22"/>
       <c r="R44" s="22"/>
       <c r="S44" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T44" s="24">
         <v>0</v>
@@ -10711,7 +10728,7 @@
       <c r="Q45" s="22"/>
       <c r="R45" s="22"/>
       <c r="S45" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T45" s="24">
         <v>0</v>
@@ -10739,7 +10756,7 @@
       <c r="Q46" s="22"/>
       <c r="R46" s="22"/>
       <c r="S46" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T46" s="24">
         <v>0</v>
@@ -10767,7 +10784,7 @@
       <c r="Q47" s="25"/>
       <c r="R47" s="22"/>
       <c r="S47" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T47" s="24">
         <f>2/50</f>
@@ -10796,7 +10813,7 @@
       <c r="Q48" s="22"/>
       <c r="R48" s="22"/>
       <c r="S48" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T48" s="24">
         <v>0</v>
@@ -10813,7 +10830,7 @@
     </row>
     <row r="52" spans="1:20">
       <c r="A52" s="10" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
@@ -10886,13 +10903,13 @@
       </c>
       <c r="S53" s="9"/>
       <c r="T53" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:20">
       <c r="A54" s="9"/>
       <c r="B54" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C54" s="27"/>
       <c r="D54" s="27"/>
@@ -10921,7 +10938,7 @@
       <c r="Q54" s="27"/>
       <c r="R54" s="27"/>
       <c r="S54" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T54" s="22"/>
     </row>
@@ -10936,7 +10953,7 @@
     </row>
     <row r="58" spans="1:20" s="18" customFormat="1">
       <c r="A58" s="19" t="s">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="B58" s="6"/>
     </row>
@@ -10991,7 +11008,7 @@
         <v>2015</v>
       </c>
       <c r="T59" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:20" s="18" customFormat="1">
@@ -11016,7 +11033,7 @@
       <c r="Q60" s="22"/>
       <c r="R60" s="22"/>
       <c r="S60" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T60" s="24">
         <v>0</v>
@@ -11044,7 +11061,7 @@
       <c r="Q61" s="22"/>
       <c r="R61" s="22"/>
       <c r="S61" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T61" s="24">
         <v>0</v>
@@ -11072,7 +11089,7 @@
       <c r="Q62" s="22"/>
       <c r="R62" s="22"/>
       <c r="S62" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T62" s="24">
         <v>0</v>
@@ -11100,7 +11117,7 @@
       <c r="Q63" s="22"/>
       <c r="R63" s="22"/>
       <c r="S63" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T63" s="24">
         <v>0</v>
@@ -11128,7 +11145,7 @@
       <c r="Q64" s="25"/>
       <c r="R64" s="22"/>
       <c r="S64" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T64" s="24">
         <f>2/50</f>
@@ -11157,7 +11174,7 @@
       <c r="Q65" s="22"/>
       <c r="R65" s="22"/>
       <c r="S65" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T65" s="24">
         <v>0</v>
@@ -11165,7 +11182,7 @@
     </row>
     <row r="69" spans="1:20" s="18" customFormat="1">
       <c r="A69" s="19" t="s">
-        <v>135</v>
+        <v>14</v>
       </c>
       <c r="B69" s="6"/>
     </row>
@@ -11220,12 +11237,12 @@
         <v>2015</v>
       </c>
       <c r="T70" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:20" s="18" customFormat="1">
       <c r="B71" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C71" s="22"/>
       <c r="D71" s="22"/>
@@ -11244,7 +11261,7 @@
       <c r="Q71" s="22"/>
       <c r="R71" s="22"/>
       <c r="S71" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T71" s="25">
         <v>0.3</v>
@@ -11254,7 +11271,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -11262,22 +11279,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T85"/>
   <sheetViews>
     <sheetView topLeftCell="J45" workbookViewId="0">
       <selection activeCell="U45" sqref="U1:AX1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" style="6"/>
-    <col min="20" max="20" width="14.33203125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="6"/>
+    <col min="20" max="20" width="14.375" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="12" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -11349,7 +11367,7 @@
       </c>
       <c r="S2" s="11"/>
       <c r="T2" s="32" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -11375,7 +11393,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T3" s="33">
         <v>80</v>
@@ -11404,7 +11422,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T4" s="33">
         <v>80</v>
@@ -11433,7 +11451,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T5" s="33">
         <v>80</v>
@@ -11462,7 +11480,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T6" s="33">
         <v>80</v>
@@ -11491,7 +11509,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T7" s="33">
         <v>80</v>
@@ -11520,7 +11538,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T8" s="33">
         <v>80</v>
@@ -11536,7 +11554,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="12" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -11608,7 +11626,7 @@
       </c>
       <c r="S13" s="11"/>
       <c r="T13" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -11634,7 +11652,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T14" s="29">
         <v>10</v>
@@ -11663,7 +11681,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T15" s="29">
         <v>10</v>
@@ -11692,7 +11710,7 @@
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T16" s="29">
         <v>10</v>
@@ -11721,7 +11739,7 @@
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T17" s="29">
         <v>10</v>
@@ -11750,7 +11768,7 @@
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T18" s="29">
         <v>10</v>
@@ -11779,7 +11797,7 @@
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T19" s="29">
         <v>10</v>
@@ -11795,7 +11813,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="12" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -11867,7 +11885,7 @@
       </c>
       <c r="S24" s="11"/>
       <c r="T24" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -11893,7 +11911,7 @@
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T25" s="29">
         <v>0</v>
@@ -11922,7 +11940,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T26" s="29">
         <v>500</v>
@@ -11951,7 +11969,7 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T27" s="29">
         <v>0</v>
@@ -11980,7 +11998,7 @@
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
       <c r="S28" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T28" s="29">
         <v>0</v>
@@ -12009,7 +12027,7 @@
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
       <c r="S29" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T29" s="29">
         <v>0</v>
@@ -12038,7 +12056,7 @@
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
       <c r="S30" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T30" s="29">
         <v>10</v>
@@ -12054,7 +12072,7 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="12" t="s">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -12126,7 +12144,7 @@
       </c>
       <c r="S35" s="11"/>
       <c r="T35" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -12152,7 +12170,7 @@
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
       <c r="S36" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T36" s="30">
         <v>0.4</v>
@@ -12191,7 +12209,7 @@
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
       <c r="S37" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T37" s="30"/>
     </row>
@@ -12218,7 +12236,7 @@
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
       <c r="S38" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T38" s="30">
         <v>0.05</v>
@@ -12247,7 +12265,7 @@
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
       <c r="S39" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T39" s="30">
         <v>0.05</v>
@@ -12276,7 +12294,7 @@
       <c r="Q40" s="22"/>
       <c r="R40" s="22"/>
       <c r="S40" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T40" s="30">
         <v>0.05</v>
@@ -12305,7 +12323,7 @@
       <c r="Q41" s="22"/>
       <c r="R41" s="22"/>
       <c r="S41" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T41" s="30">
         <v>7.0000000000000007E-2</v>
@@ -12321,7 +12339,7 @@
     </row>
     <row r="45" spans="1:20">
       <c r="A45" s="19" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
@@ -12393,7 +12411,7 @@
       </c>
       <c r="S46" s="11"/>
       <c r="T46" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:20">
@@ -12419,7 +12437,7 @@
       <c r="Q47" s="22"/>
       <c r="R47" s="22"/>
       <c r="S47" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T47" s="30">
         <v>0.6</v>
@@ -12458,7 +12476,7 @@
       <c r="Q48" s="22"/>
       <c r="R48" s="22"/>
       <c r="S48" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T48" s="30"/>
     </row>
@@ -12485,7 +12503,7 @@
       <c r="Q49" s="22"/>
       <c r="R49" s="22"/>
       <c r="S49" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T49" s="30">
         <v>0.5</v>
@@ -12520,7 +12538,7 @@
       <c r="Q50" s="22"/>
       <c r="R50" s="22"/>
       <c r="S50" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T50" s="30"/>
     </row>
@@ -12553,7 +12571,7 @@
       <c r="Q51" s="22"/>
       <c r="R51" s="22"/>
       <c r="S51" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T51" s="30"/>
     </row>
@@ -12580,7 +12598,7 @@
       <c r="Q52" s="22"/>
       <c r="R52" s="22"/>
       <c r="S52" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T52" s="30">
         <v>0.5</v>
@@ -12596,7 +12614,7 @@
     </row>
     <row r="56" spans="1:20">
       <c r="A56" s="19" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
@@ -12668,7 +12686,7 @@
       </c>
       <c r="S57" s="11"/>
       <c r="T57" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:20">
@@ -12694,7 +12712,7 @@
       <c r="Q58" s="22"/>
       <c r="R58" s="22"/>
       <c r="S58" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T58" s="29">
         <v>0</v>
@@ -12733,7 +12751,7 @@
       <c r="Q59" s="22"/>
       <c r="R59" s="22"/>
       <c r="S59" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T59" s="38"/>
     </row>
@@ -12760,7 +12778,7 @@
       <c r="Q60" s="22"/>
       <c r="R60" s="22"/>
       <c r="S60" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T60" s="30">
         <v>0</v>
@@ -12789,7 +12807,7 @@
       <c r="Q61" s="22"/>
       <c r="R61" s="22"/>
       <c r="S61" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T61" s="30">
         <v>0</v>
@@ -12818,7 +12836,7 @@
       <c r="Q62" s="22"/>
       <c r="R62" s="22"/>
       <c r="S62" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T62" s="29">
         <v>0</v>
@@ -12857,7 +12875,7 @@
       <c r="Q63" s="22"/>
       <c r="R63" s="22"/>
       <c r="S63" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T63" s="39"/>
     </row>
@@ -12871,7 +12889,7 @@
     </row>
     <row r="67" spans="1:20">
       <c r="A67" s="12" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
@@ -12943,7 +12961,7 @@
       </c>
       <c r="S68" s="11"/>
       <c r="T68" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:20">
@@ -12969,7 +12987,7 @@
       <c r="Q69" s="22"/>
       <c r="R69" s="22"/>
       <c r="S69" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T69" s="30">
         <v>0.03</v>
@@ -12998,7 +13016,7 @@
       <c r="Q70" s="22"/>
       <c r="R70" s="22"/>
       <c r="S70" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T70" s="29">
         <v>0</v>
@@ -13027,7 +13045,7 @@
       <c r="Q71" s="22"/>
       <c r="R71" s="22"/>
       <c r="S71" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T71" s="30">
         <v>2.5999999999999999E-2</v>
@@ -13056,7 +13074,7 @@
       <c r="Q72" s="22"/>
       <c r="R72" s="22"/>
       <c r="S72" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T72" s="30">
         <v>0.03</v>
@@ -13085,7 +13103,7 @@
       <c r="Q73" s="22"/>
       <c r="R73" s="22"/>
       <c r="S73" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T73" s="30">
         <v>0</v>
@@ -13114,7 +13132,7 @@
       <c r="Q74" s="22"/>
       <c r="R74" s="22"/>
       <c r="S74" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T74" s="30">
         <v>0.03</v>
@@ -13134,7 +13152,7 @@
     </row>
     <row r="78" spans="1:20" s="18" customFormat="1">
       <c r="A78" s="19" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="B78" s="6"/>
       <c r="T78" s="31"/>
@@ -13190,7 +13208,7 @@
         <v>2015</v>
       </c>
       <c r="T79" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:20" s="18" customFormat="1">
@@ -13215,7 +13233,7 @@
       <c r="Q80" s="22"/>
       <c r="R80" s="22"/>
       <c r="S80" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T80" s="30">
         <v>0.03</v>
@@ -13243,7 +13261,7 @@
       <c r="Q81" s="22"/>
       <c r="R81" s="22"/>
       <c r="S81" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T81" s="29">
         <v>0</v>
@@ -13271,7 +13289,7 @@
       <c r="Q82" s="22"/>
       <c r="R82" s="22"/>
       <c r="S82" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T82" s="30">
         <v>2.5999999999999999E-2</v>
@@ -13299,7 +13317,7 @@
       <c r="Q83" s="22"/>
       <c r="R83" s="22"/>
       <c r="S83" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T83" s="30">
         <v>0.03</v>
@@ -13327,7 +13345,7 @@
       <c r="Q84" s="22"/>
       <c r="R84" s="22"/>
       <c r="S84" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T84" s="30">
         <v>0</v>
@@ -13355,17 +13373,18 @@
       <c r="Q85" s="22"/>
       <c r="R85" s="22"/>
       <c r="S85" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T85" s="30">
         <v>0.03</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -13373,22 +13392,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.33203125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.375" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="14" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -13460,7 +13480,7 @@
       </c>
       <c r="S2" s="13"/>
       <c r="T2" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -13486,7 +13506,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T3" s="29">
         <v>0</v>
@@ -13515,7 +13535,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T4" s="29">
         <v>0</v>
@@ -13544,7 +13564,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T5" s="29">
         <v>400</v>
@@ -13573,7 +13593,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T6" s="29">
         <v>0</v>
@@ -13602,7 +13622,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T7" s="29">
         <v>0</v>
@@ -13631,7 +13651,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T8" s="29">
         <v>0</v>
@@ -13647,7 +13667,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="19" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -13719,13 +13739,13 @@
       </c>
       <c r="S13" s="13"/>
       <c r="T13" s="32" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="13"/>
       <c r="B14" s="43" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="25">
@@ -13752,7 +13772,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T14" s="38"/>
     </row>
@@ -13766,7 +13786,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="14" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -13838,13 +13858,13 @@
       </c>
       <c r="S19" s="13"/>
       <c r="T19" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="13"/>
       <c r="B20" s="43" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C20" s="38"/>
       <c r="D20" s="38">
@@ -13869,15 +13889,16 @@
       <c r="Q20" s="38"/>
       <c r="R20" s="38"/>
       <c r="S20" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T20" s="38"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -13885,21 +13906,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="6.6640625" customWidth="1"/>
-    <col min="3" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="1" max="2" width="6.625" customWidth="1"/>
+    <col min="3" max="8" width="13.625" customWidth="1"/>
+    <col min="9" max="15" width="6.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1">
       <c r="A1" s="17" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -14203,7 +14225,7 @@
     <row r="11" spans="1:26" s="18" customFormat="1"/>
     <row r="12" spans="1:26">
       <c r="A12" s="17" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -14500,7 +14522,7 @@
     <row r="22" spans="1:26" s="18" customFormat="1"/>
     <row r="23" spans="1:26">
       <c r="A23" s="17" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -14659,7 +14681,7 @@
     <row r="33" spans="1:8" s="18" customFormat="1"/>
     <row r="34" spans="1:8">
       <c r="A34" s="17" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -14778,10 +14800,11 @@
       <c r="H41" s="34"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
removed any dependency on unit costs from makeccocs.py
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="863"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14200" tabRatio="863" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -21,9 +21,9 @@
     <sheet name="Disutilities &amp; costs" sheetId="14" r:id="rId12"/>
     <sheet name="Macroeconomics" sheetId="18" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="130000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -33,166 +33,73 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="144">
   <si>
-    <t>Percentage of people who used a condom at last act with regular partners</t>
+    <t>Age-related population transitions (average number of years before movement)</t>
   </si>
   <si>
-    <t>Average number of injections per person per year</t>
+    <t>Government expenditure</t>
   </si>
   <si>
-    <t>Disease progression rate (% per year)</t>
+    <t>General government health expenditure</t>
   </si>
   <si>
-    <t>Mother-to-child (breastfeeding)</t>
+    <t>Domestic HIV spending</t>
   </si>
   <si>
-    <t>Mother-to-child (non-breastfeeding)</t>
+    <t>Global Fund HIV commitments</t>
   </si>
   <si>
-    <t>Relative disease-related transmissibility</t>
+    <t>PEPFAR HIV commitments</t>
   </si>
   <si>
-    <t>Social mitigation costs</t>
+    <t>Other international HIV commitments</t>
   </si>
   <si>
-    <t>HIV-related health care costs (excluding treatment)</t>
+    <t>Private HIV spending</t>
   </si>
   <si>
-    <t>Untreated HIV, acute</t>
+    <t>Total domestic and international health expenditure</t>
   </si>
   <si>
-    <t>Disutility weights</t>
+    <t>Number of people on first-line treatment</t>
   </si>
   <si>
-    <t>Interactions between casual partners</t>
+    <t>Number of people on second-line treatment</t>
   </si>
   <si>
-    <t>Interactions between commercial partners</t>
+    <t>Number of AIDS-related deaths</t>
   </si>
   <si>
-    <t>Interactions between regular partners</t>
+    <t>Percentage of population tested for HIV in the last 12 months</t>
   </si>
   <si>
-    <t>Interactions between people who inject drugs</t>
+    <t>Birth rate (births per woman per year)</t>
   </si>
   <si>
-    <t>Interaction-related transmissibility (% per act)</t>
+    <t>Percentage of HIV-positive women who breastfed</t>
   </si>
   <si>
-    <t>Treatment recovery rate (% per year)</t>
+    <t>Condom use</t>
   </si>
   <si>
-    <t>Treatment failure rate (% per year)</t>
+    <t>Heterosexual</t>
   </si>
   <si>
-    <t>Death rate (% mortality per year)</t>
+    <t>Homosexual</t>
   </si>
   <si>
-    <t>Relative transmissibility</t>
+    <t>Sex worker</t>
   </si>
   <si>
-    <t>Modeled estimate of HIV prevalence</t>
+    <t>Client</t>
   </si>
   <si>
-    <t>Male</t>
+    <t>Other males</t>
   </si>
   <si>
-    <t>Female</t>
+    <t>Other females</t>
   </si>
   <si>
-    <t>Injects</t>
-  </si>
-  <si>
-    <t>Men who have sex with men</t>
-  </si>
-  <si>
-    <t>FSW programs</t>
-  </si>
-  <si>
-    <t>Programs for female sex workers and clients</t>
-  </si>
-  <si>
-    <t>Needle-syringe programs</t>
-  </si>
-  <si>
-    <t>Programs for men who have sex with men</t>
-  </si>
-  <si>
-    <t>Social and behavior change communication</t>
-  </si>
-  <si>
-    <t>SBCC</t>
-  </si>
-  <si>
-    <t>Male PWID</t>
-  </si>
-  <si>
-    <t>Males who inject drugs</t>
-  </si>
-  <si>
-    <t>MSM programs</t>
-  </si>
-  <si>
-    <t>Number of people who inject drugs who are on opiate substitution therapy</t>
-  </si>
-  <si>
-    <t>Number of women on PMTCT (Option B/B+)</t>
-  </si>
-  <si>
-    <t>Number of voluntary medical male circumcisions performed</t>
-  </si>
-  <si>
-    <t>Percentage of people covered by pre-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Percentage of people coveraged by post-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Pre-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Post-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Cost &amp; coverage</t>
-  </si>
-  <si>
-    <t>Saturating</t>
-  </si>
-  <si>
-    <t>Assumption</t>
-  </si>
-  <si>
-    <t>Injecting</t>
-  </si>
-  <si>
-    <t>Heterosexual insertive</t>
-  </si>
-  <si>
-    <t>Heterosexual receptive</t>
-  </si>
-  <si>
-    <t>Homosexual insertive</t>
-  </si>
-  <si>
-    <t>Homosexual receptive</t>
-  </si>
-  <si>
-    <t>Opiate substitution therapy</t>
-  </si>
-  <si>
-    <t>ARV treatment</t>
-  </si>
-  <si>
-    <t>Percentage of people who die from non-HIV-related causes per year</t>
-  </si>
-  <si>
-    <t>Number of HIV tests per year</t>
-  </si>
-  <si>
-    <t>Number of HIV diagnoses per year</t>
+    <t>Clients of female sex workers</t>
   </si>
   <si>
     <t>Modeled estimate of new HIV infections per year</t>
@@ -400,84 +307,177 @@
     <t>Prevalence of any discharging STIs</t>
   </si>
   <si>
-    <t>Age-related population transitions (average number of years before movement)</t>
+    <t>Percentage of people who used a condom at last act with regular partners</t>
   </si>
   <si>
-    <t>Government expenditure</t>
+    <t>Average number of injections per person per year</t>
   </si>
   <si>
-    <t>General government health expenditure</t>
+    <t>Disease progression rate (% per year)</t>
   </si>
   <si>
-    <t>Domestic HIV spending</t>
+    <t>Mother-to-child (breastfeeding)</t>
   </si>
   <si>
-    <t>Global Fund HIV commitments</t>
+    <t>Mother-to-child (non-breastfeeding)</t>
   </si>
   <si>
-    <t>PEPFAR HIV commitments</t>
+    <t>Relative disease-related transmissibility</t>
   </si>
   <si>
-    <t>Other international HIV commitments</t>
+    <t>Social mitigation costs</t>
   </si>
   <si>
-    <t>Private HIV spending</t>
+    <t>HIV-related health care costs (excluding treatment)</t>
   </si>
   <si>
-    <t>Total domestic and international health expenditure</t>
+    <t>Untreated HIV, acute</t>
   </si>
   <si>
-    <t>Number of people on first-line treatment</t>
+    <t>Disutility weights</t>
   </si>
   <si>
-    <t>Number of people on second-line treatment</t>
+    <t>Interactions between casual partners</t>
   </si>
   <si>
-    <t>Number of AIDS-related deaths</t>
+    <t>Interactions between commercial partners</t>
   </si>
   <si>
-    <t>Percentage of population tested for HIV in the last 12 months</t>
+    <t>Interactions between regular partners</t>
   </si>
   <si>
-    <t>Birth rate (births per woman per year)</t>
+    <t>Interactions between people who inject drugs</t>
   </si>
   <si>
-    <t>Percentage of HIV-positive women who breastfed</t>
+    <t>Interaction-related transmissibility (% per act)</t>
   </si>
   <si>
-    <t>Condom use</t>
+    <t>Treatment recovery rate (% per year)</t>
   </si>
   <si>
-    <t>Heterosexual</t>
+    <t>Treatment failure rate (% per year)</t>
   </si>
   <si>
-    <t>Homosexual</t>
+    <t>Death rate (% mortality per year)</t>
   </si>
   <si>
-    <t>Sex worker</t>
+    <t>Relative transmissibility</t>
   </si>
   <si>
-    <t>Client</t>
+    <t>Modeled estimate of HIV prevalence</t>
   </si>
   <si>
-    <t>Other males</t>
+    <t>Male</t>
   </si>
   <si>
-    <t>Other females</t>
+    <t>Female</t>
   </si>
   <si>
-    <t>Clients of female sex workers</t>
+    <t>Injects</t>
+  </si>
+  <si>
+    <t>Men who have sex with men</t>
+  </si>
+  <si>
+    <t>FSW programs</t>
+  </si>
+  <si>
+    <t>Programs for female sex workers and clients</t>
+  </si>
+  <si>
+    <t>Needle-syringe programs</t>
+  </si>
+  <si>
+    <t>Programs for men who have sex with men</t>
+  </si>
+  <si>
+    <t>Social and behavior change communication</t>
+  </si>
+  <si>
+    <t>SBCC</t>
+  </si>
+  <si>
+    <t>Male PWID</t>
+  </si>
+  <si>
+    <t>Males who inject drugs</t>
+  </si>
+  <si>
+    <t>MSM programs</t>
+  </si>
+  <si>
+    <t>Number of people who inject drugs who are on opiate substitution therapy</t>
+  </si>
+  <si>
+    <t>Number of women on PMTCT (Option B/B+)</t>
+  </si>
+  <si>
+    <t>Number of voluntary medical male circumcisions performed</t>
+  </si>
+  <si>
+    <t>Percentage of people covered by pre-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Percentage of people coveraged by post-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Pre-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Post-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Cost &amp; coverage</t>
+  </si>
+  <si>
+    <t>Saturating</t>
+  </si>
+  <si>
+    <t>Assumption</t>
+  </si>
+  <si>
+    <t>Injecting</t>
+  </si>
+  <si>
+    <t>Heterosexual insertive</t>
+  </si>
+  <si>
+    <t>Heterosexual receptive</t>
+  </si>
+  <si>
+    <t>Homosexual insertive</t>
+  </si>
+  <si>
+    <t>Homosexual receptive</t>
+  </si>
+  <si>
+    <t>Opiate substitution therapy</t>
+  </si>
+  <si>
+    <t>ARV treatment</t>
+  </si>
+  <si>
+    <t>Percentage of people who die from non-HIV-related causes per year</t>
+  </si>
+  <si>
+    <t>Number of HIV tests per year</t>
+  </si>
+  <si>
+    <t>Number of HIV diagnoses per year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -653,7 +653,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
@@ -1301,7 +1301,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="50">
@@ -1407,7 +1407,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -2083,7 +2083,7 @@
     <cellStyle name="Percent 2 2" xfId="660"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <mruColors>
       <color rgb="FFB9DAED"/>
@@ -2386,58 +2386,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="20"/>
+    <col min="1" max="1" width="9.125" style="20"/>
     <col min="2" max="2" width="5" style="20" customWidth="1"/>
     <col min="3" max="3" width="18" style="20" customWidth="1"/>
-    <col min="4" max="4" width="55.33203125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" style="20" customWidth="1"/>
-    <col min="6" max="7" width="9.1640625" style="20"/>
-    <col min="8" max="9" width="14.1640625" style="20" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" style="20" customWidth="1"/>
-    <col min="11" max="16384" width="9.1640625" style="20"/>
+    <col min="4" max="4" width="55.375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="20" customWidth="1"/>
+    <col min="6" max="7" width="9.125" style="20"/>
+    <col min="8" max="9" width="14.125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="12.125" style="20" customWidth="1"/>
+    <col min="11" max="16384" width="9.125" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="21" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="C2" s="21" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>137</v>
+        <v>16</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>139</v>
+        <v>18</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2445,10 +2446,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="E3" s="41" t="b">
         <v>1</v>
@@ -2477,10 +2478,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="E4" s="41" t="b">
         <v>0</v>
@@ -2509,10 +2510,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="E5" s="41" t="b">
         <v>1</v>
@@ -2541,10 +2542,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>141</v>
+        <v>20</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>141</v>
+        <v>20</v>
       </c>
       <c r="E6" s="41" t="b">
         <v>1</v>
@@ -2573,10 +2574,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>142</v>
+        <v>21</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>142</v>
+        <v>21</v>
       </c>
       <c r="E7" s="41" t="b">
         <v>0</v>
@@ -2605,10 +2606,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
       <c r="E8" s="41" t="b">
         <v>1</v>
@@ -2643,20 +2644,20 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="21" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="B12" s="21"/>
     </row>
     <row r="13" spans="1:11">
       <c r="B13" s="21"/>
       <c r="C13" s="21" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2664,10 +2665,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="E14" s="41" t="b">
         <v>1</v>
@@ -2678,10 +2679,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="D15" s="45" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="E15" s="41" t="b">
         <v>1</v>
@@ -2692,10 +2693,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="E16" s="41" t="b">
         <v>0</v>
@@ -2706,10 +2707,10 @@
         <v>4</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="E17" s="41" t="b">
         <v>1</v>
@@ -2720,10 +2721,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="45" t="s">
-        <v>24</v>
+        <v>114</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="E18" s="41" t="b">
         <v>1</v>
@@ -2734,10 +2735,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="E19" s="41" t="b">
         <v>0</v>
@@ -2748,10 +2749,10 @@
         <v>7</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="E20" s="41" t="b">
         <v>0</v>
@@ -2761,7 +2762,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -2769,22 +2770,23 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" style="6"/>
-    <col min="3" max="8" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="6"/>
+    <col min="3" max="8" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="3" t="s">
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="2"/>
@@ -2937,7 +2939,7 @@
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="17" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="2"/>
@@ -3051,7 +3053,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -3059,39 +3061,40 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="18"/>
-    <col min="2" max="2" width="33.1640625" style="18" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" style="18"/>
+    <col min="1" max="1" width="9.125" style="18"/>
+    <col min="2" max="2" width="33.125" style="18" customWidth="1"/>
+    <col min="3" max="16384" width="9.125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="19" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1">
       <c r="C2" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" s="19" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="C3" s="26">
         <v>4.0000000000000002E-4</v>
@@ -3101,7 +3104,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="B4" s="19" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
       <c r="C4" s="26">
         <v>1E-3</v>
@@ -3111,7 +3114,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="B5" s="19" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="C5" s="26">
         <v>5.9999999999999995E-4</v>
@@ -3121,7 +3124,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="B6" s="19" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="C6" s="26">
         <v>5.0000000000000001E-3</v>
@@ -3131,7 +3134,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="B7" s="19" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
       <c r="C7" s="26">
         <v>3.0000000000000001E-3</v>
@@ -3141,7 +3144,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="B8" s="19" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="C8" s="25">
         <v>0.05</v>
@@ -3151,7 +3154,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="B9" s="19" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="C9" s="25">
         <v>0.03</v>
@@ -3171,23 +3174,23 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="19" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1">
       <c r="C14" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" s="19" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="C15" s="22">
         <v>10</v>
@@ -3197,7 +3200,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="B16" s="19" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C16" s="22">
         <v>1</v>
@@ -3207,7 +3210,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="B17" s="19" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C17" s="22">
         <v>1</v>
@@ -3217,7 +3220,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="B18" s="19" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C18" s="22">
         <v>1</v>
@@ -3227,7 +3230,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="B19" s="19" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C19" s="22">
         <v>3.8</v>
@@ -3247,24 +3250,24 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="19" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="B23" s="19"/>
     </row>
     <row r="24" spans="1:8">
       <c r="C24" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="B25" s="19" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C25" s="25">
         <v>1</v>
@@ -3274,7 +3277,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="B26" s="19" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C26" s="25">
         <v>0.25</v>
@@ -3284,7 +3287,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="B27" s="19" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="C27" s="25">
         <v>0.25</v>
@@ -3294,7 +3297,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="B28" s="19" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="C28" s="25">
         <v>0.5</v>
@@ -3314,23 +3317,23 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="19" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="C33" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="B34" s="19" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="C34" s="25">
         <v>0.45</v>
@@ -3340,7 +3343,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="B35" s="19" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C35" s="25">
         <v>0.7</v>
@@ -3350,7 +3353,7 @@
     </row>
     <row r="36" spans="1:8">
       <c r="B36" s="19" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="C36" s="25">
         <v>0.36</v>
@@ -3373,23 +3376,23 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="19" t="s">
-        <v>16</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="C41" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="B42" s="19" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="C42" s="25">
         <v>0.2</v>
@@ -3403,7 +3406,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="B43" s="19" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="C43" s="25">
         <v>0.1</v>
@@ -3427,23 +3430,23 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="19" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="C48" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="B49" s="19" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="C49" s="25">
         <v>0</v>
@@ -3453,7 +3456,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="B50" s="19" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C50" s="26">
         <v>5.0000000000000001E-4</v>
@@ -3463,7 +3466,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="B51" s="19" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="C51" s="26">
         <v>1E-3</v>
@@ -3473,7 +3476,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="B52" s="19" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C52" s="25">
         <v>0.01</v>
@@ -3483,7 +3486,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="B53" s="19" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C53" s="25">
         <v>0.49</v>
@@ -3493,7 +3496,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="B54" s="19" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="C54" s="25">
         <v>0.04</v>
@@ -3503,7 +3506,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="B55" s="19" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="C55" s="22">
         <v>2</v>
@@ -3523,23 +3526,23 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="19" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="C60" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="B61" s="19" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="C61" s="25">
         <v>0.05</v>
@@ -3549,7 +3552,7 @@
     </row>
     <row r="62" spans="1:8">
       <c r="B62" s="19" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="C62" s="25">
         <v>0.3</v>
@@ -3559,7 +3562,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="B63" s="19" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="C63" s="25">
         <v>0.65</v>
@@ -3569,7 +3572,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="B64" s="19" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="C64" s="25">
         <v>3.5</v>
@@ -3579,7 +3582,7 @@
     </row>
     <row r="65" spans="2:5">
       <c r="B65" s="19" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
       <c r="C65" s="25">
         <v>0.05</v>
@@ -3589,7 +3592,7 @@
     </row>
     <row r="66" spans="2:5">
       <c r="B66" s="19" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C66" s="25">
         <v>0.05</v>
@@ -3599,7 +3602,7 @@
     </row>
     <row r="67" spans="2:5">
       <c r="B67" s="19" t="s">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="C67" s="25">
         <v>0.3</v>
@@ -3609,7 +3612,7 @@
     </row>
     <row r="68" spans="2:5">
       <c r="B68" s="19" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="C68" s="25">
         <v>0.5</v>
@@ -3619,7 +3622,7 @@
     </row>
     <row r="69" spans="2:5">
       <c r="B69" s="19" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="C69" s="25">
         <v>0.5</v>
@@ -3631,7 +3634,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -3639,21 +3642,22 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="19" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -3664,18 +3668,18 @@
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="18" customFormat="1">
       <c r="B3" s="19" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="C3" s="24">
         <v>0.05</v>
@@ -3686,7 +3690,7 @@
     <row r="4" spans="1:8">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="C4" s="24">
         <v>0.05</v>
@@ -3697,7 +3701,7 @@
     <row r="5" spans="1:8">
       <c r="A5" s="18"/>
       <c r="B5" s="19" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C5" s="24">
         <v>0.1</v>
@@ -3708,7 +3712,7 @@
     <row r="6" spans="1:8">
       <c r="A6" s="18"/>
       <c r="B6" s="19" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C6" s="24">
         <v>0.15</v>
@@ -3719,7 +3723,7 @@
     <row r="7" spans="1:8">
       <c r="A7" s="18"/>
       <c r="B7" s="19" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="C7" s="24">
         <v>0.5</v>
@@ -3730,7 +3734,7 @@
     <row r="8" spans="1:8">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="C8" s="24">
         <v>5.2999999999999999E-2</v>
@@ -3758,7 +3762,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="19" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -3769,19 +3773,19 @@
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="C14" s="22">
         <v>0</v>
@@ -3792,7 +3796,7 @@
     <row r="15" spans="1:8">
       <c r="A15" s="18"/>
       <c r="B15" s="19" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C15" s="22">
         <v>100</v>
@@ -3803,7 +3807,7 @@
     <row r="16" spans="1:8">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="C16" s="22">
         <v>100</v>
@@ -3814,7 +3818,7 @@
     <row r="17" spans="1:5">
       <c r="A17" s="18"/>
       <c r="B17" s="19" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C17" s="22">
         <v>200</v>
@@ -3825,7 +3829,7 @@
     <row r="18" spans="1:5">
       <c r="A18" s="18"/>
       <c r="B18" s="19" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C18" s="22">
         <v>450</v>
@@ -3835,7 +3839,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="19" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -3846,19 +3850,19 @@
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18"/>
       <c r="B24" s="19" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="C24" s="22">
         <v>0</v>
@@ -3869,7 +3873,7 @@
     <row r="25" spans="1:5">
       <c r="A25" s="18"/>
       <c r="B25" s="19" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C25" s="22">
         <v>100</v>
@@ -3880,7 +3884,7 @@
     <row r="26" spans="1:5">
       <c r="A26" s="18"/>
       <c r="B26" s="19" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="C26" s="22">
         <v>100</v>
@@ -3891,7 +3895,7 @@
     <row r="27" spans="1:5">
       <c r="A27" s="18"/>
       <c r="B27" s="19" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C27" s="22">
         <v>1000</v>
@@ -3902,7 +3906,7 @@
     <row r="28" spans="1:5">
       <c r="A28" s="18"/>
       <c r="B28" s="19" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C28" s="22">
         <v>10000</v>
@@ -3914,7 +3918,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -3922,29 +3926,30 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AI57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" style="6"/>
-    <col min="3" max="4" width="13.83203125" style="18" customWidth="1"/>
-    <col min="5" max="11" width="8.6640625" style="18"/>
+    <col min="2" max="2" width="8.625" style="6"/>
+    <col min="3" max="4" width="13.875" style="18" customWidth="1"/>
+    <col min="5" max="11" width="8.625" style="18"/>
     <col min="12" max="12" width="12" style="18" customWidth="1"/>
-    <col min="13" max="17" width="8.6640625" style="18"/>
-    <col min="18" max="18" width="12.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="8.625" style="18"/>
+    <col min="18" max="18" width="12.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
       <c r="A1" s="19" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="S1" s="18"/>
       <c r="T1" s="18"/>
@@ -4060,13 +4065,13 @@
       </c>
       <c r="AH2" s="18"/>
       <c r="AI2" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:35">
       <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C3" s="22">
         <f t="shared" ref="C3:R3" si="0">D3/(1.12)</f>
@@ -4192,7 +4197,7 @@
         <v>350405950838.15192</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI3" s="29"/>
     </row>
@@ -4203,7 +4208,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" s="19" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="S7" s="18"/>
       <c r="T7" s="18"/>
@@ -4319,13 +4324,13 @@
       </c>
       <c r="AH8" s="18"/>
       <c r="AI8" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:35">
       <c r="A9" s="18"/>
       <c r="B9" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C9" s="40">
         <v>30000000000</v>
@@ -4451,13 +4456,13 @@
         <v>180000000000</v>
       </c>
       <c r="AH9" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI9" s="29"/>
     </row>
     <row r="13" spans="1:35">
       <c r="A13" s="19" t="s">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
@@ -4573,13 +4578,13 @@
       </c>
       <c r="AH14" s="18"/>
       <c r="AI14" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:35">
       <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C15" s="22">
         <v>10000000000</v>
@@ -4705,13 +4710,13 @@
         <v>43219423751.506668</v>
       </c>
       <c r="AH15" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI15" s="29"/>
     </row>
     <row r="19" spans="1:35" s="18" customFormat="1">
       <c r="A19" s="19" t="s">
-        <v>129</v>
+        <v>8</v>
       </c>
       <c r="B19" s="6"/>
       <c r="AI19" s="6"/>
@@ -4812,12 +4817,12 @@
         <v>2030</v>
       </c>
       <c r="AI20" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:35" s="18" customFormat="1">
       <c r="B21" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -4851,7 +4856,7 @@
       <c r="AF21" s="22"/>
       <c r="AG21" s="22"/>
       <c r="AH21" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI21" s="29"/>
     </row>
@@ -4869,7 +4874,7 @@
     </row>
     <row r="25" spans="1:35" s="18" customFormat="1">
       <c r="A25" s="19" t="s">
-        <v>123</v>
+        <v>2</v>
       </c>
       <c r="B25" s="6"/>
       <c r="AI25" s="6"/>
@@ -4970,12 +4975,12 @@
         <v>2030</v>
       </c>
       <c r="AI26" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:35" s="18" customFormat="1">
       <c r="B27" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C27" s="22">
         <f>12%*C15</f>
@@ -5102,13 +5107,13 @@
         <v>5186330850.1808004</v>
       </c>
       <c r="AH27" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI27" s="29"/>
     </row>
     <row r="31" spans="1:35" s="18" customFormat="1">
       <c r="A31" s="19" t="s">
-        <v>124</v>
+        <v>3</v>
       </c>
       <c r="B31" s="6"/>
       <c r="AI31" s="6"/>
@@ -5209,12 +5214,12 @@
         <v>2030</v>
       </c>
       <c r="AI32" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:35" s="18" customFormat="1">
       <c r="B33" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C33" s="22">
         <v>15000000</v>
@@ -5310,7 +5315,7 @@
         <v>18000000</v>
       </c>
       <c r="AH33" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI33" s="29"/>
     </row>
@@ -5328,7 +5333,7 @@
     </row>
     <row r="37" spans="1:35" s="18" customFormat="1">
       <c r="A37" s="19" t="s">
-        <v>125</v>
+        <v>4</v>
       </c>
       <c r="B37" s="6"/>
       <c r="AI37" s="6"/>
@@ -5429,12 +5434,12 @@
         <v>2030</v>
       </c>
       <c r="AI38" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:35" s="18" customFormat="1">
       <c r="B39" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
@@ -5468,7 +5473,7 @@
       <c r="AF39" s="22"/>
       <c r="AG39" s="22"/>
       <c r="AH39" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI39" s="29"/>
     </row>
@@ -5486,7 +5491,7 @@
     </row>
     <row r="43" spans="1:35" s="18" customFormat="1">
       <c r="A43" s="19" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="B43" s="6"/>
       <c r="AI43" s="6"/>
@@ -5587,12 +5592,12 @@
         <v>2030</v>
       </c>
       <c r="AI44" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:35" s="18" customFormat="1">
       <c r="B45" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
@@ -5626,13 +5631,13 @@
       <c r="AF45" s="22"/>
       <c r="AG45" s="22"/>
       <c r="AH45" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI45" s="29"/>
     </row>
     <row r="49" spans="1:35" s="18" customFormat="1">
       <c r="A49" s="19" t="s">
-        <v>127</v>
+        <v>6</v>
       </c>
       <c r="B49" s="6"/>
       <c r="AI49" s="6"/>
@@ -5733,12 +5738,12 @@
         <v>2030</v>
       </c>
       <c r="AI50" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:35" s="18" customFormat="1">
       <c r="B51" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
@@ -5772,7 +5777,7 @@
       <c r="AF51" s="22"/>
       <c r="AG51" s="22"/>
       <c r="AH51" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI51" s="29"/>
     </row>
@@ -5790,7 +5795,7 @@
     </row>
     <row r="55" spans="1:35" s="18" customFormat="1">
       <c r="A55" s="19" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="B55" s="6"/>
       <c r="AI55" s="6"/>
@@ -5891,12 +5896,12 @@
         <v>2030</v>
       </c>
       <c r="AI56" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:35" s="18" customFormat="1">
       <c r="B57" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C57" s="22"/>
       <c r="D57" s="22"/>
@@ -5930,16 +5935,15 @@
       <c r="AF57" s="22"/>
       <c r="AG57" s="22"/>
       <c r="AH57" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="AI57" s="29"/>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -5947,25 +5951,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12:M13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.1640625" style="18"/>
+    <col min="1" max="2" width="9.125" style="18"/>
     <col min="3" max="3" width="11" style="18" customWidth="1"/>
-    <col min="4" max="20" width="9.1640625" style="18"/>
-    <col min="21" max="21" width="15.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.1640625" style="18"/>
+    <col min="4" max="20" width="9.125" style="18"/>
+    <col min="21" max="21" width="15.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="19" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:22">
@@ -6018,7 +6023,7 @@
         <v>2015</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -6027,7 +6032,7 @@
         <v>SBCC</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="25">
@@ -6060,7 +6065,7 @@
       <c r="R3" s="22"/>
       <c r="S3" s="22"/>
       <c r="T3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U3" s="25"/>
     </row>
@@ -6070,7 +6075,7 @@
         <v>SBCC</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="27">
@@ -6110,7 +6115,7 @@
       <c r="R4" s="24"/>
       <c r="S4" s="24"/>
       <c r="T4" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U4" s="37"/>
     </row>
@@ -6123,7 +6128,7 @@
         <v>NSP</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="25"/>
@@ -6142,7 +6147,7 @@
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
       <c r="T6" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U6" s="25">
         <v>0.2</v>
@@ -6154,7 +6159,7 @@
         <v>NSP</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="23"/>
@@ -6173,7 +6178,7 @@
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
       <c r="T7" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U7" s="47">
         <v>25000</v>
@@ -6188,7 +6193,7 @@
         <v>OST</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="25"/>
@@ -6209,7 +6214,7 @@
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
       <c r="T9" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U9" s="25"/>
     </row>
@@ -6220,7 +6225,7 @@
         <v>OST</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="23"/>
@@ -6232,7 +6237,8 @@
       <c r="K10" s="25"/>
       <c r="L10" s="22"/>
       <c r="M10" s="40">
-        <v>3483</v>
+        <f>3483*M9</f>
+        <v>6694326</v>
       </c>
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
@@ -6241,7 +6247,7 @@
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
       <c r="T10" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U10" s="37"/>
     </row>
@@ -6256,7 +6262,7 @@
         <v>MSM programs</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="25"/>
@@ -6277,7 +6283,7 @@
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
       <c r="T12" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U12" s="25"/>
       <c r="V12" s="6"/>
@@ -6288,7 +6294,7 @@
         <v>MSM programs</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="23"/>
@@ -6309,7 +6315,7 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
       <c r="T13" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U13" s="37"/>
     </row>
@@ -6319,7 +6325,7 @@
         <v>FSW programs</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="25"/>
@@ -6340,7 +6346,7 @@
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
       <c r="T15" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U15" s="25"/>
     </row>
@@ -6350,7 +6356,7 @@
         <v>FSW programs</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
@@ -6371,7 +6377,7 @@
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
       <c r="T16" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U16" s="37"/>
     </row>
@@ -6381,7 +6387,7 @@
         <v>ART</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="25"/>
@@ -6402,7 +6408,7 @@
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
       <c r="T18" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U18" s="25"/>
     </row>
@@ -6412,7 +6418,7 @@
         <v>ART</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="23"/>
@@ -6425,7 +6431,8 @@
       <c r="L19" s="22"/>
       <c r="M19" s="40"/>
       <c r="N19" s="40">
-        <v>1034</v>
+        <f>1034*N18</f>
+        <v>2422662</v>
       </c>
       <c r="O19" s="23"/>
       <c r="P19" s="22"/>
@@ -6433,7 +6440,7 @@
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
       <c r="T19" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U19" s="37"/>
     </row>
@@ -6443,7 +6450,7 @@
         <v>PMTCT</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="25"/>
@@ -6464,7 +6471,7 @@
       <c r="R21" s="22"/>
       <c r="S21" s="22"/>
       <c r="T21" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U21" s="25"/>
     </row>
@@ -6474,7 +6481,7 @@
         <v>PMTCT</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
@@ -6487,7 +6494,8 @@
       <c r="L22" s="22"/>
       <c r="M22" s="40"/>
       <c r="N22" s="49">
-        <v>5340</v>
+        <f>5340*N21</f>
+        <v>817020</v>
       </c>
       <c r="O22" s="23"/>
       <c r="P22" s="22"/>
@@ -6495,7 +6503,7 @@
       <c r="R22" s="22"/>
       <c r="S22" s="22"/>
       <c r="T22" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U22" s="37"/>
     </row>
@@ -6503,7 +6511,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -6511,26 +6519,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView topLeftCell="V1" workbookViewId="0">
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="9.1640625" style="18"/>
-    <col min="4" max="4" width="9.33203125" style="18" customWidth="1"/>
-    <col min="5" max="20" width="9.1640625" style="18"/>
-    <col min="21" max="21" width="15.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.83203125" style="18" customWidth="1"/>
-    <col min="23" max="16384" width="9.1640625" style="18"/>
+    <col min="1" max="3" width="9.125" style="18"/>
+    <col min="4" max="4" width="9.375" style="18" customWidth="1"/>
+    <col min="5" max="20" width="9.125" style="18"/>
+    <col min="21" max="21" width="15.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.875" style="18" customWidth="1"/>
+    <col min="23" max="16384" width="9.125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="19" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -6583,7 +6592,7 @@
         <v>2015</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -6592,7 +6601,7 @@
         <v>MSM</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
@@ -6611,7 +6620,7 @@
       <c r="R3" s="27"/>
       <c r="S3" s="27"/>
       <c r="T3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U3" s="27">
         <v>37500</v>
@@ -6623,7 +6632,7 @@
         <v>MSM</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
@@ -6642,7 +6651,7 @@
       <c r="R4" s="27"/>
       <c r="S4" s="27"/>
       <c r="T4" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U4" s="27">
         <v>21000</v>
@@ -6654,7 +6663,7 @@
         <v>MSM</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
@@ -6673,7 +6682,7 @@
       <c r="R5" s="27"/>
       <c r="S5" s="27"/>
       <c r="T5" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U5" s="27">
         <v>11000</v>
@@ -6690,7 +6699,7 @@
         <v>FSW</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
@@ -6709,7 +6718,7 @@
       <c r="R7" s="27"/>
       <c r="S7" s="27"/>
       <c r="T7" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U7" s="27"/>
     </row>
@@ -6719,7 +6728,7 @@
         <v>FSW</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
@@ -6738,7 +6747,7 @@
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
       <c r="T8" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U8" s="27">
         <v>15000</v>
@@ -6750,7 +6759,7 @@
         <v>FSW</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
@@ -6769,7 +6778,7 @@
       <c r="R9" s="27"/>
       <c r="S9" s="27"/>
       <c r="T9" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U9" s="27"/>
     </row>
@@ -6800,7 +6809,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
@@ -6829,7 +6838,7 @@
       <c r="R11" s="27"/>
       <c r="S11" s="27"/>
       <c r="T11" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U11" s="27"/>
     </row>
@@ -6839,7 +6848,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
@@ -6868,7 +6877,7 @@
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
       <c r="T12" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U12" s="27"/>
     </row>
@@ -6878,7 +6887,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
@@ -6907,7 +6916,7 @@
       <c r="R13" s="27"/>
       <c r="S13" s="27"/>
       <c r="T13" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U13" s="27"/>
     </row>
@@ -6938,7 +6947,7 @@
         <v>Other males</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
@@ -6957,7 +6966,7 @@
       <c r="R15" s="27"/>
       <c r="S15" s="27"/>
       <c r="T15" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U15" s="27"/>
     </row>
@@ -6967,7 +6976,7 @@
         <v>Other males</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D16" s="22">
         <v>4227500</v>
@@ -7018,7 +7027,7 @@
         <v>6118320.6906761518</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U16" s="27"/>
     </row>
@@ -7028,7 +7037,7 @@
         <v>Other males</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
@@ -7047,7 +7056,7 @@
       <c r="R17" s="27"/>
       <c r="S17" s="27"/>
       <c r="T17" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U17" s="27"/>
     </row>
@@ -7078,7 +7087,7 @@
         <v>Other females</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
@@ -7097,7 +7106,7 @@
       <c r="R19" s="27"/>
       <c r="S19" s="27"/>
       <c r="T19" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U19" s="27"/>
     </row>
@@ -7107,7 +7116,7 @@
         <v>Other females</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D20" s="22">
         <v>4759641.7668505535</v>
@@ -7158,7 +7167,7 @@
         <v>7061706.1901886221</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U20" s="27"/>
     </row>
@@ -7168,7 +7177,7 @@
         <v>Other females</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
@@ -7187,7 +7196,7 @@
       <c r="R21" s="27"/>
       <c r="S21" s="27"/>
       <c r="T21" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U21" s="27"/>
     </row>
@@ -7218,7 +7227,7 @@
         <v>Clients</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -7237,7 +7246,7 @@
       <c r="R23" s="27"/>
       <c r="S23" s="27"/>
       <c r="T23" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U23" s="27"/>
     </row>
@@ -7247,7 +7256,7 @@
         <v>Clients</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D24" s="22">
         <v>522500</v>
@@ -7298,7 +7307,7 @@
         <v>756196.93929705245</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U24" s="27"/>
     </row>
@@ -7308,7 +7317,7 @@
         <v>Clients</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -7327,13 +7336,13 @@
       <c r="R25" s="27"/>
       <c r="S25" s="27"/>
       <c r="T25" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U25" s="27"/>
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="19" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -7386,7 +7395,7 @@
         <v>2015</v>
       </c>
       <c r="U30" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -7395,7 +7404,7 @@
         <v>MSM</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -7416,7 +7425,7 @@
       <c r="R31" s="22"/>
       <c r="S31" s="22"/>
       <c r="T31" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U31" s="26"/>
     </row>
@@ -7426,7 +7435,7 @@
         <v>MSM</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -7447,7 +7456,7 @@
       <c r="R32" s="22"/>
       <c r="S32" s="22"/>
       <c r="T32" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U32" s="26"/>
     </row>
@@ -7457,7 +7466,7 @@
         <v>MSM</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
@@ -7478,7 +7487,7 @@
       <c r="R33" s="22"/>
       <c r="S33" s="22"/>
       <c r="T33" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U33" s="26"/>
     </row>
@@ -7492,7 +7501,7 @@
         <v>FSW</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
@@ -7517,7 +7526,7 @@
       <c r="R35" s="22"/>
       <c r="S35" s="22"/>
       <c r="T35" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U35" s="26"/>
     </row>
@@ -7527,7 +7536,7 @@
         <v>FSW</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -7552,7 +7561,7 @@
       <c r="R36" s="22"/>
       <c r="S36" s="22"/>
       <c r="T36" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U36" s="26"/>
     </row>
@@ -7562,7 +7571,7 @@
         <v>FSW</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
@@ -7587,7 +7596,7 @@
       <c r="R37" s="22"/>
       <c r="S37" s="22"/>
       <c r="T37" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U37" s="26"/>
     </row>
@@ -7601,7 +7610,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
@@ -7626,7 +7635,7 @@
       <c r="R39" s="22"/>
       <c r="S39" s="22"/>
       <c r="T39" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U39" s="26"/>
     </row>
@@ -7636,7 +7645,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
@@ -7661,7 +7670,7 @@
       <c r="R40" s="22"/>
       <c r="S40" s="22"/>
       <c r="T40" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U40" s="26"/>
     </row>
@@ -7671,7 +7680,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
@@ -7696,7 +7705,7 @@
       <c r="R41" s="22"/>
       <c r="S41" s="22"/>
       <c r="T41" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U41" s="26"/>
     </row>
@@ -7710,7 +7719,7 @@
         <v>Other males</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
@@ -7729,7 +7738,7 @@
       <c r="R43" s="22"/>
       <c r="S43" s="22"/>
       <c r="T43" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U43" s="26"/>
     </row>
@@ -7739,7 +7748,7 @@
         <v>Other males</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
@@ -7758,7 +7767,7 @@
       <c r="R44" s="22"/>
       <c r="S44" s="22"/>
       <c r="T44" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U44" s="26">
         <v>5.0000000000000001E-4</v>
@@ -7770,7 +7779,7 @@
         <v>Other males</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
@@ -7789,7 +7798,7 @@
       <c r="R45" s="22"/>
       <c r="S45" s="22"/>
       <c r="T45" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U45" s="26"/>
     </row>
@@ -7803,7 +7812,7 @@
         <v>Other females</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
@@ -7822,7 +7831,7 @@
       <c r="R47" s="22"/>
       <c r="S47" s="22"/>
       <c r="T47" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U47" s="26"/>
     </row>
@@ -7832,7 +7841,7 @@
         <v>Other females</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
@@ -7859,7 +7868,7 @@
       <c r="R48" s="22"/>
       <c r="S48" s="22"/>
       <c r="T48" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U48" s="26"/>
     </row>
@@ -7869,7 +7878,7 @@
         <v>Other females</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
@@ -7888,7 +7897,7 @@
       <c r="R49" s="22"/>
       <c r="S49" s="22"/>
       <c r="T49" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U49" s="26"/>
     </row>
@@ -7902,7 +7911,7 @@
         <v>Clients</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
@@ -7921,7 +7930,7 @@
       <c r="R51" s="22"/>
       <c r="S51" s="22"/>
       <c r="T51" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U51" s="26"/>
     </row>
@@ -7931,7 +7940,7 @@
         <v>Clients</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
@@ -7950,7 +7959,7 @@
       <c r="R52" s="22"/>
       <c r="S52" s="22"/>
       <c r="T52" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U52" s="26">
         <v>0.01</v>
@@ -7962,7 +7971,7 @@
         <v>Clients</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
@@ -7981,7 +7990,7 @@
       <c r="R53" s="22"/>
       <c r="S53" s="22"/>
       <c r="T53" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="U53" s="26"/>
     </row>
@@ -7989,7 +7998,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -7997,22 +8006,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" style="6"/>
-    <col min="20" max="20" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="6"/>
+    <col min="20" max="20" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="10" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -8085,13 +8095,13 @@
       </c>
       <c r="S2" s="9"/>
       <c r="T2" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="9"/>
       <c r="B3" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -8110,7 +8120,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T3" s="22"/>
     </row>
@@ -8122,7 +8132,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="10" t="s">
-        <v>53</v>
+        <v>143</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -8195,13 +8205,13 @@
       </c>
       <c r="S8" s="9"/>
       <c r="T8" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -8244,7 +8254,7 @@
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
       <c r="S9" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T9" s="22"/>
     </row>
@@ -8256,7 +8266,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="10" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -8329,13 +8339,13 @@
       </c>
       <c r="S14" s="9"/>
       <c r="T14" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="9"/>
       <c r="B15" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -8354,7 +8364,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T15" s="22"/>
     </row>
@@ -8366,7 +8376,7 @@
     </row>
     <row r="19" spans="1:20" s="18" customFormat="1">
       <c r="A19" s="19" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="B19" s="6"/>
     </row>
@@ -8421,12 +8431,12 @@
         <v>2015</v>
       </c>
       <c r="T20" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:20" s="18" customFormat="1">
       <c r="B21" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -8445,7 +8455,7 @@
       <c r="Q21" s="22"/>
       <c r="R21" s="22"/>
       <c r="S21" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T21" s="22"/>
     </row>
@@ -8460,7 +8470,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="10" t="s">
-        <v>132</v>
+        <v>11</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -8533,13 +8543,13 @@
       </c>
       <c r="S26" s="9"/>
       <c r="T26" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="9"/>
       <c r="B27" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
@@ -8558,13 +8568,13 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T27" s="22"/>
     </row>
     <row r="31" spans="1:20" s="18" customFormat="1">
       <c r="A31" s="19" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="B31" s="6"/>
     </row>
@@ -8619,12 +8629,12 @@
         <v>2015</v>
       </c>
       <c r="T32" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="2:20" s="18" customFormat="1">
       <c r="B33" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
@@ -8643,7 +8653,7 @@
       <c r="Q33" s="22"/>
       <c r="R33" s="22"/>
       <c r="S33" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T33" s="22"/>
     </row>
@@ -8651,7 +8661,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -8659,21 +8669,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView topLeftCell="J2" workbookViewId="0">
       <selection activeCell="U2" sqref="U1:AZ1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" style="6"/>
+    <col min="2" max="2" width="8.625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="18" customFormat="1">
       <c r="A1" s="19" t="s">
-        <v>51</v>
+        <v>141</v>
       </c>
       <c r="B1" s="6"/>
     </row>
@@ -8728,7 +8739,7 @@
         <v>2015</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="18" customFormat="1">
@@ -8753,7 +8764,7 @@
       <c r="Q3" s="25"/>
       <c r="R3" s="25"/>
       <c r="S3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T3" s="25">
         <v>0.01</v>
@@ -8781,7 +8792,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T4" s="25">
         <v>0.01</v>
@@ -8809,7 +8820,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T5" s="25">
         <v>0.03</v>
@@ -8837,7 +8848,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T6" s="25">
         <v>0.01</v>
@@ -8865,7 +8876,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T7" s="25">
         <v>0.01</v>
@@ -8893,7 +8904,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T8" s="25">
         <v>0.01</v>
@@ -8910,7 +8921,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="8" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -8983,7 +8994,7 @@
       </c>
       <c r="S13" s="7"/>
       <c r="T13" s="8" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -9009,7 +9020,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T14" s="25">
         <v>0</v>
@@ -9038,7 +9049,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T15" s="25">
         <v>0</v>
@@ -9067,7 +9078,7 @@
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T16" s="25">
         <v>0</v>
@@ -9096,7 +9107,7 @@
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T17" s="25">
         <v>0</v>
@@ -9125,7 +9136,7 @@
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T18" s="25">
         <v>0</v>
@@ -9154,7 +9165,7 @@
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T19" s="25">
         <v>0</v>
@@ -9171,7 +9182,7 @@
     </row>
     <row r="23" spans="1:20" s="18" customFormat="1">
       <c r="A23" s="19" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="B23" s="6"/>
     </row>
@@ -9226,7 +9237,7 @@
         <v>2015</v>
       </c>
       <c r="T24" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:20" s="18" customFormat="1">
@@ -9251,7 +9262,7 @@
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T25" s="25">
         <v>0</v>
@@ -9279,7 +9290,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T26" s="25">
         <v>0</v>
@@ -9307,7 +9318,7 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T27" s="25">
         <v>0</v>
@@ -9335,7 +9346,7 @@
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
       <c r="S28" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T28" s="25">
         <v>0</v>
@@ -9363,7 +9374,7 @@
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
       <c r="S29" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T29" s="25">
         <v>0</v>
@@ -9391,7 +9402,7 @@
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
       <c r="S30" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T30" s="25">
         <v>0</v>
@@ -9410,7 +9421,7 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="8" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -9483,7 +9494,7 @@
       </c>
       <c r="S35" s="7"/>
       <c r="T35" s="8" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -9509,7 +9520,7 @@
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
       <c r="S36" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T36" s="25">
         <v>0</v>
@@ -9537,7 +9548,7 @@
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
       <c r="S37" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T37" s="25">
         <v>0</v>
@@ -9565,7 +9576,7 @@
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
       <c r="S38" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T38" s="25">
         <v>0</v>
@@ -9593,7 +9604,7 @@
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
       <c r="S39" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T39" s="25">
         <v>0</v>
@@ -9621,7 +9632,7 @@
       <c r="Q40" s="22"/>
       <c r="R40" s="22"/>
       <c r="S40" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T40" s="25">
         <v>0</v>
@@ -9649,7 +9660,7 @@
       <c r="Q41" s="22"/>
       <c r="R41" s="22"/>
       <c r="S41" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T41" s="25">
         <v>0</v>
@@ -9662,7 +9673,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -9670,22 +9681,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T71"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="U1" sqref="U1:AW1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" style="6"/>
-    <col min="20" max="20" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="6"/>
+    <col min="20" max="20" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="10" t="s">
-        <v>133</v>
+        <v>12</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -9758,7 +9770,7 @@
       </c>
       <c r="S2" s="9"/>
       <c r="T2" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -9784,7 +9796,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T3" s="25">
         <v>0.03</v>
@@ -9817,7 +9829,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T4" s="25"/>
     </row>
@@ -9850,7 +9862,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T5" s="22"/>
     </row>
@@ -9877,7 +9889,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T6" s="25">
         <v>0.01</v>
@@ -9906,7 +9918,7 @@
       <c r="Q7" s="25"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T7" s="25">
         <v>0.01</v>
@@ -9935,7 +9947,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T8" s="25">
         <v>0.05</v>
@@ -9949,7 +9961,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="10" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -10022,13 +10034,13 @@
       </c>
       <c r="S13" s="9"/>
       <c r="T13" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="9"/>
       <c r="B14" s="4" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -10047,7 +10059,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T14" s="25">
         <v>0.5</v>
@@ -10061,7 +10073,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="10" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -10134,13 +10146,13 @@
       </c>
       <c r="S19" s="9"/>
       <c r="T19" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="9"/>
       <c r="B20" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C20" s="22">
         <v>0</v>
@@ -10187,7 +10199,7 @@
       <c r="Q20" s="22"/>
       <c r="R20" s="22"/>
       <c r="S20" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T20" s="22"/>
     </row>
@@ -10199,7 +10211,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="10" t="s">
-        <v>131</v>
+        <v>10</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -10272,13 +10284,13 @@
       </c>
       <c r="S25" s="9"/>
       <c r="T25" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="9"/>
       <c r="B26" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C26" s="22">
         <v>0</v>
@@ -10325,7 +10337,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T26" s="22"/>
     </row>
@@ -10340,7 +10352,7 @@
     </row>
     <row r="30" spans="1:20" s="18" customFormat="1">
       <c r="A30" s="19" t="s">
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="B30" s="6"/>
     </row>
@@ -10395,7 +10407,7 @@
         <v>2015</v>
       </c>
       <c r="T31" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:20" s="18" customFormat="1">
@@ -10420,7 +10432,7 @@
       <c r="Q32" s="22"/>
       <c r="R32" s="22"/>
       <c r="S32" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T32" s="24">
         <v>0</v>
@@ -10448,7 +10460,7 @@
       <c r="Q33" s="22"/>
       <c r="R33" s="22"/>
       <c r="S33" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T33" s="24">
         <v>0</v>
@@ -10476,7 +10488,7 @@
       <c r="Q34" s="22"/>
       <c r="R34" s="22"/>
       <c r="S34" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T34" s="24">
         <v>0</v>
@@ -10504,7 +10516,7 @@
       <c r="Q35" s="22"/>
       <c r="R35" s="22"/>
       <c r="S35" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T35" s="24">
         <v>0</v>
@@ -10532,7 +10544,7 @@
       <c r="Q36" s="25"/>
       <c r="R36" s="22"/>
       <c r="S36" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T36" s="24">
         <f>2/50</f>
@@ -10561,7 +10573,7 @@
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
       <c r="S37" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T37" s="24">
         <v>0</v>
@@ -10575,7 +10587,7 @@
     </row>
     <row r="41" spans="1:20" s="18" customFormat="1">
       <c r="A41" s="19" t="s">
-        <v>37</v>
+        <v>127</v>
       </c>
       <c r="B41" s="6"/>
     </row>
@@ -10630,7 +10642,7 @@
         <v>2015</v>
       </c>
       <c r="T42" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:20" s="18" customFormat="1">
@@ -10655,7 +10667,7 @@
       <c r="Q43" s="22"/>
       <c r="R43" s="22"/>
       <c r="S43" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T43" s="24">
         <v>0</v>
@@ -10683,7 +10695,7 @@
       <c r="Q44" s="22"/>
       <c r="R44" s="22"/>
       <c r="S44" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T44" s="24">
         <v>0</v>
@@ -10711,7 +10723,7 @@
       <c r="Q45" s="22"/>
       <c r="R45" s="22"/>
       <c r="S45" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T45" s="24">
         <v>0</v>
@@ -10739,7 +10751,7 @@
       <c r="Q46" s="22"/>
       <c r="R46" s="22"/>
       <c r="S46" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T46" s="24">
         <v>0</v>
@@ -10767,7 +10779,7 @@
       <c r="Q47" s="25"/>
       <c r="R47" s="22"/>
       <c r="S47" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T47" s="24">
         <f>2/50</f>
@@ -10796,7 +10808,7 @@
       <c r="Q48" s="22"/>
       <c r="R48" s="22"/>
       <c r="S48" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T48" s="24">
         <v>0</v>
@@ -10813,7 +10825,7 @@
     </row>
     <row r="52" spans="1:20">
       <c r="A52" s="10" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
@@ -10886,13 +10898,13 @@
       </c>
       <c r="S53" s="9"/>
       <c r="T53" s="10" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:20">
       <c r="A54" s="9"/>
       <c r="B54" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C54" s="27"/>
       <c r="D54" s="27"/>
@@ -10921,7 +10933,7 @@
       <c r="Q54" s="27"/>
       <c r="R54" s="27"/>
       <c r="S54" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T54" s="22"/>
     </row>
@@ -10936,7 +10948,7 @@
     </row>
     <row r="58" spans="1:20" s="18" customFormat="1">
       <c r="A58" s="19" t="s">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="B58" s="6"/>
     </row>
@@ -10991,7 +11003,7 @@
         <v>2015</v>
       </c>
       <c r="T59" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:20" s="18" customFormat="1">
@@ -11016,7 +11028,7 @@
       <c r="Q60" s="22"/>
       <c r="R60" s="22"/>
       <c r="S60" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T60" s="24">
         <v>0</v>
@@ -11044,7 +11056,7 @@
       <c r="Q61" s="22"/>
       <c r="R61" s="22"/>
       <c r="S61" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T61" s="24">
         <v>0</v>
@@ -11072,7 +11084,7 @@
       <c r="Q62" s="22"/>
       <c r="R62" s="22"/>
       <c r="S62" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T62" s="24">
         <v>0</v>
@@ -11100,7 +11112,7 @@
       <c r="Q63" s="22"/>
       <c r="R63" s="22"/>
       <c r="S63" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T63" s="24">
         <v>0</v>
@@ -11128,7 +11140,7 @@
       <c r="Q64" s="25"/>
       <c r="R64" s="22"/>
       <c r="S64" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T64" s="24">
         <f>2/50</f>
@@ -11157,7 +11169,7 @@
       <c r="Q65" s="22"/>
       <c r="R65" s="22"/>
       <c r="S65" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T65" s="24">
         <v>0</v>
@@ -11165,7 +11177,7 @@
     </row>
     <row r="69" spans="1:20" s="18" customFormat="1">
       <c r="A69" s="19" t="s">
-        <v>135</v>
+        <v>14</v>
       </c>
       <c r="B69" s="6"/>
     </row>
@@ -11220,12 +11232,12 @@
         <v>2015</v>
       </c>
       <c r="T70" s="19" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:20" s="18" customFormat="1">
       <c r="B71" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C71" s="22"/>
       <c r="D71" s="22"/>
@@ -11244,7 +11256,7 @@
       <c r="Q71" s="22"/>
       <c r="R71" s="22"/>
       <c r="S71" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T71" s="25">
         <v>0.3</v>
@@ -11254,7 +11266,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -11262,22 +11274,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T85"/>
   <sheetViews>
     <sheetView topLeftCell="J45" workbookViewId="0">
       <selection activeCell="U45" sqref="U1:AX1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" style="6"/>
-    <col min="20" max="20" width="14.33203125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="6"/>
+    <col min="20" max="20" width="14.375" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="12" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -11349,7 +11362,7 @@
       </c>
       <c r="S2" s="11"/>
       <c r="T2" s="32" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -11375,7 +11388,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T3" s="33">
         <v>80</v>
@@ -11404,7 +11417,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T4" s="33">
         <v>80</v>
@@ -11433,7 +11446,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T5" s="33">
         <v>80</v>
@@ -11462,7 +11475,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T6" s="33">
         <v>80</v>
@@ -11491,7 +11504,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T7" s="33">
         <v>80</v>
@@ -11520,7 +11533,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T8" s="33">
         <v>80</v>
@@ -11536,7 +11549,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="12" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -11608,7 +11621,7 @@
       </c>
       <c r="S13" s="11"/>
       <c r="T13" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -11634,7 +11647,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T14" s="29">
         <v>10</v>
@@ -11663,7 +11676,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T15" s="29">
         <v>10</v>
@@ -11692,7 +11705,7 @@
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T16" s="29">
         <v>10</v>
@@ -11721,7 +11734,7 @@
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T17" s="29">
         <v>10</v>
@@ -11750,7 +11763,7 @@
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T18" s="29">
         <v>10</v>
@@ -11779,7 +11792,7 @@
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T19" s="29">
         <v>10</v>
@@ -11795,7 +11808,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="12" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -11867,7 +11880,7 @@
       </c>
       <c r="S24" s="11"/>
       <c r="T24" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -11893,7 +11906,7 @@
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T25" s="29">
         <v>0</v>
@@ -11922,7 +11935,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T26" s="29">
         <v>500</v>
@@ -11951,7 +11964,7 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T27" s="29">
         <v>0</v>
@@ -11980,7 +11993,7 @@
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
       <c r="S28" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T28" s="29">
         <v>0</v>
@@ -12009,7 +12022,7 @@
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
       <c r="S29" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T29" s="29">
         <v>0</v>
@@ -12038,7 +12051,7 @@
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
       <c r="S30" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T30" s="29">
         <v>10</v>
@@ -12054,7 +12067,7 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="12" t="s">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -12126,7 +12139,7 @@
       </c>
       <c r="S35" s="11"/>
       <c r="T35" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -12152,7 +12165,7 @@
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
       <c r="S36" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T36" s="30">
         <v>0.4</v>
@@ -12191,7 +12204,7 @@
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
       <c r="S37" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T37" s="30"/>
     </row>
@@ -12218,7 +12231,7 @@
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
       <c r="S38" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T38" s="30">
         <v>0.05</v>
@@ -12247,7 +12260,7 @@
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
       <c r="S39" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T39" s="30">
         <v>0.05</v>
@@ -12276,7 +12289,7 @@
       <c r="Q40" s="22"/>
       <c r="R40" s="22"/>
       <c r="S40" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T40" s="30">
         <v>0.05</v>
@@ -12305,7 +12318,7 @@
       <c r="Q41" s="22"/>
       <c r="R41" s="22"/>
       <c r="S41" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T41" s="30">
         <v>7.0000000000000007E-2</v>
@@ -12321,7 +12334,7 @@
     </row>
     <row r="45" spans="1:20">
       <c r="A45" s="19" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
@@ -12393,7 +12406,7 @@
       </c>
       <c r="S46" s="11"/>
       <c r="T46" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:20">
@@ -12419,7 +12432,7 @@
       <c r="Q47" s="22"/>
       <c r="R47" s="22"/>
       <c r="S47" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T47" s="30">
         <v>0.6</v>
@@ -12458,7 +12471,7 @@
       <c r="Q48" s="22"/>
       <c r="R48" s="22"/>
       <c r="S48" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T48" s="30"/>
     </row>
@@ -12485,7 +12498,7 @@
       <c r="Q49" s="22"/>
       <c r="R49" s="22"/>
       <c r="S49" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T49" s="30">
         <v>0.5</v>
@@ -12520,7 +12533,7 @@
       <c r="Q50" s="22"/>
       <c r="R50" s="22"/>
       <c r="S50" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T50" s="30"/>
     </row>
@@ -12553,7 +12566,7 @@
       <c r="Q51" s="22"/>
       <c r="R51" s="22"/>
       <c r="S51" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T51" s="30"/>
     </row>
@@ -12580,7 +12593,7 @@
       <c r="Q52" s="22"/>
       <c r="R52" s="22"/>
       <c r="S52" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T52" s="30">
         <v>0.5</v>
@@ -12596,7 +12609,7 @@
     </row>
     <row r="56" spans="1:20">
       <c r="A56" s="19" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
@@ -12668,7 +12681,7 @@
       </c>
       <c r="S57" s="11"/>
       <c r="T57" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:20">
@@ -12694,7 +12707,7 @@
       <c r="Q58" s="22"/>
       <c r="R58" s="22"/>
       <c r="S58" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T58" s="29">
         <v>0</v>
@@ -12733,7 +12746,7 @@
       <c r="Q59" s="22"/>
       <c r="R59" s="22"/>
       <c r="S59" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T59" s="38"/>
     </row>
@@ -12760,7 +12773,7 @@
       <c r="Q60" s="22"/>
       <c r="R60" s="22"/>
       <c r="S60" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T60" s="30">
         <v>0</v>
@@ -12789,7 +12802,7 @@
       <c r="Q61" s="22"/>
       <c r="R61" s="22"/>
       <c r="S61" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T61" s="30">
         <v>0</v>
@@ -12818,7 +12831,7 @@
       <c r="Q62" s="22"/>
       <c r="R62" s="22"/>
       <c r="S62" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T62" s="29">
         <v>0</v>
@@ -12857,7 +12870,7 @@
       <c r="Q63" s="22"/>
       <c r="R63" s="22"/>
       <c r="S63" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T63" s="39"/>
     </row>
@@ -12871,7 +12884,7 @@
     </row>
     <row r="67" spans="1:20">
       <c r="A67" s="12" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
@@ -12943,7 +12956,7 @@
       </c>
       <c r="S68" s="11"/>
       <c r="T68" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:20">
@@ -12969,7 +12982,7 @@
       <c r="Q69" s="22"/>
       <c r="R69" s="22"/>
       <c r="S69" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T69" s="30">
         <v>0.03</v>
@@ -12998,7 +13011,7 @@
       <c r="Q70" s="22"/>
       <c r="R70" s="22"/>
       <c r="S70" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T70" s="29">
         <v>0</v>
@@ -13027,7 +13040,7 @@
       <c r="Q71" s="22"/>
       <c r="R71" s="22"/>
       <c r="S71" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T71" s="30">
         <v>2.5999999999999999E-2</v>
@@ -13056,7 +13069,7 @@
       <c r="Q72" s="22"/>
       <c r="R72" s="22"/>
       <c r="S72" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T72" s="30">
         <v>0.03</v>
@@ -13085,7 +13098,7 @@
       <c r="Q73" s="22"/>
       <c r="R73" s="22"/>
       <c r="S73" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T73" s="30">
         <v>0</v>
@@ -13114,7 +13127,7 @@
       <c r="Q74" s="22"/>
       <c r="R74" s="22"/>
       <c r="S74" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T74" s="30">
         <v>0.03</v>
@@ -13134,7 +13147,7 @@
     </row>
     <row r="78" spans="1:20" s="18" customFormat="1">
       <c r="A78" s="19" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="B78" s="6"/>
       <c r="T78" s="31"/>
@@ -13190,7 +13203,7 @@
         <v>2015</v>
       </c>
       <c r="T79" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:20" s="18" customFormat="1">
@@ -13215,7 +13228,7 @@
       <c r="Q80" s="22"/>
       <c r="R80" s="22"/>
       <c r="S80" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T80" s="30">
         <v>0.03</v>
@@ -13243,7 +13256,7 @@
       <c r="Q81" s="22"/>
       <c r="R81" s="22"/>
       <c r="S81" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T81" s="29">
         <v>0</v>
@@ -13271,7 +13284,7 @@
       <c r="Q82" s="22"/>
       <c r="R82" s="22"/>
       <c r="S82" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T82" s="30">
         <v>2.5999999999999999E-2</v>
@@ -13299,7 +13312,7 @@
       <c r="Q83" s="22"/>
       <c r="R83" s="22"/>
       <c r="S83" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T83" s="30">
         <v>0.03</v>
@@ -13327,7 +13340,7 @@
       <c r="Q84" s="22"/>
       <c r="R84" s="22"/>
       <c r="S84" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T84" s="30">
         <v>0</v>
@@ -13355,7 +13368,7 @@
       <c r="Q85" s="22"/>
       <c r="R85" s="22"/>
       <c r="S85" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T85" s="30">
         <v>0.03</v>
@@ -13365,7 +13378,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -13373,22 +13386,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.33203125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.375" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="14" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -13460,7 +13474,7 @@
       </c>
       <c r="S2" s="13"/>
       <c r="T2" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -13486,7 +13500,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T3" s="29">
         <v>0</v>
@@ -13515,7 +13529,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T4" s="29">
         <v>0</v>
@@ -13544,7 +13558,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T5" s="29">
         <v>400</v>
@@ -13573,7 +13587,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T6" s="29">
         <v>0</v>
@@ -13602,7 +13616,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T7" s="29">
         <v>0</v>
@@ -13631,7 +13645,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T8" s="29">
         <v>0</v>
@@ -13647,7 +13661,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="19" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -13719,13 +13733,13 @@
       </c>
       <c r="S13" s="13"/>
       <c r="T13" s="32" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="13"/>
       <c r="B14" s="43" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="25">
@@ -13752,7 +13766,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T14" s="38"/>
     </row>
@@ -13766,7 +13780,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="14" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -13838,13 +13852,13 @@
       </c>
       <c r="S19" s="13"/>
       <c r="T19" s="4" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="13"/>
       <c r="B20" s="43" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C20" s="38"/>
       <c r="D20" s="38">
@@ -13869,7 +13883,7 @@
       <c r="Q20" s="38"/>
       <c r="R20" s="38"/>
       <c r="S20" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="T20" s="38"/>
     </row>
@@ -13877,7 +13891,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -13885,21 +13899,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="6.6640625" customWidth="1"/>
-    <col min="3" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="1" max="2" width="6.625" customWidth="1"/>
+    <col min="3" max="8" width="13.625" customWidth="1"/>
+    <col min="9" max="15" width="6.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1">
       <c r="A1" s="17" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -14203,7 +14218,7 @@
     <row r="11" spans="1:26" s="18" customFormat="1"/>
     <row r="12" spans="1:26">
       <c r="A12" s="17" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -14500,7 +14515,7 @@
     <row r="22" spans="1:26" s="18" customFormat="1"/>
     <row r="23" spans="1:26">
       <c r="A23" s="17" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -14659,7 +14674,7 @@
     <row r="33" spans="1:8" s="18" customFormat="1"/>
     <row r="34" spans="1:8">
       <c r="A34" s="17" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -14781,7 +14796,7 @@
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
converting coverage from number to percentage where necessary, part 2
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14200" tabRatio="863" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14200" tabRatio="863" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -32,6 +32,235 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="144">
+  <si>
+    <t>Number of people who inject drugs who are on opiate substitution therapy</t>
+  </si>
+  <si>
+    <t>Number of women on PMTCT (Option B/B+)</t>
+  </si>
+  <si>
+    <t>Number of voluntary medical male circumcisions performed</t>
+  </si>
+  <si>
+    <t>Percentage of people covered by pre-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Percentage of people coveraged by post-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Pre-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Post-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Cost &amp; coverage</t>
+  </si>
+  <si>
+    <t>Saturating</t>
+  </si>
+  <si>
+    <t>Assumption</t>
+  </si>
+  <si>
+    <t>Injecting</t>
+  </si>
+  <si>
+    <t>Heterosexual insertive</t>
+  </si>
+  <si>
+    <t>Heterosexual receptive</t>
+  </si>
+  <si>
+    <t>Homosexual insertive</t>
+  </si>
+  <si>
+    <t>Homosexual receptive</t>
+  </si>
+  <si>
+    <t>Opiate substitution therapy</t>
+  </si>
+  <si>
+    <t>ARV treatment</t>
+  </si>
+  <si>
+    <t>Percentage of people who die from non-HIV-related causes per year</t>
+  </si>
+  <si>
+    <t>Number of HIV tests per year</t>
+  </si>
+  <si>
+    <t>Number of HIV diagnoses per year</t>
+  </si>
+  <si>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t>Treated HIV</t>
+  </si>
+  <si>
+    <t>Populations</t>
+  </si>
+  <si>
+    <t>HIV prevalence</t>
+  </si>
+  <si>
+    <t>Number of acts with regular partners per person per year</t>
+  </si>
+  <si>
+    <t>Number of acts with casual partners per person per year</t>
+  </si>
+  <si>
+    <t>Number of acts with commercial partners per person per year</t>
+  </si>
+  <si>
+    <t>Gross domestic product</t>
+  </si>
+  <si>
+    <t>Government revenue</t>
+  </si>
+  <si>
+    <t>Prevalence of any ulcerative STIs</t>
+  </si>
+  <si>
+    <t>Number of people initiating ART each year</t>
+  </si>
+  <si>
+    <t>Percentage of people who used a condom at last act with commercial partners</t>
+  </si>
+  <si>
+    <t>Percentage of people who receptively shared a needle at last injection</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Female sex workers</t>
+  </si>
+  <si>
+    <t>Clients</t>
+  </si>
+  <si>
+    <t>Opiate substition therapy</t>
+  </si>
+  <si>
+    <t>Antiretroviral therapy</t>
+  </si>
+  <si>
+    <t>Prevention of mother-to-child transmission</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prevalence of any discharging STIs</t>
+  </si>
+  <si>
+    <t>Percentage of people who used a condom at last act with regular partners</t>
+  </si>
+  <si>
+    <t>Average number of injections per person per year</t>
+  </si>
+  <si>
+    <t>Disease progression rate (% per year)</t>
+  </si>
+  <si>
+    <t>Mother-to-child (breastfeeding)</t>
+  </si>
+  <si>
+    <t>Mother-to-child (non-breastfeeding)</t>
+  </si>
+  <si>
+    <t>Relative disease-related transmissibility</t>
+  </si>
+  <si>
+    <t>Social mitigation costs</t>
+  </si>
+  <si>
+    <t>HIV-related health care costs (excluding treatment)</t>
+  </si>
+  <si>
+    <t>Untreated HIV, acute</t>
+  </si>
+  <si>
+    <t>Disutility weights</t>
+  </si>
+  <si>
+    <t>Interactions between casual partners</t>
+  </si>
+  <si>
+    <t>Interactions between commercial partners</t>
+  </si>
+  <si>
+    <t>Interactions between regular partners</t>
+  </si>
+  <si>
+    <t>Interactions between people who inject drugs</t>
+  </si>
+  <si>
+    <t>Interaction-related transmissibility (% per act)</t>
+  </si>
+  <si>
+    <t>Treatment recovery rate (% per year)</t>
+  </si>
+  <si>
+    <t>Treatment failure rate (% per year)</t>
+  </si>
+  <si>
+    <t>Death rate (% mortality per year)</t>
+  </si>
+  <si>
+    <t>Relative transmissibility</t>
+  </si>
+  <si>
+    <t>Modeled estimate of HIV prevalence</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Injects</t>
+  </si>
+  <si>
+    <t>Men who have sex with men</t>
+  </si>
+  <si>
+    <t>FSW programs</t>
+  </si>
+  <si>
+    <t>Programs for female sex workers and clients</t>
+  </si>
+  <si>
+    <t>Needle-syringe programs</t>
+  </si>
+  <si>
+    <t>Programs for men who have sex with men</t>
+  </si>
+  <si>
+    <t>Social and behavior change communication</t>
+  </si>
+  <si>
+    <t>SBCC</t>
+  </si>
+  <si>
+    <t>Male PWID</t>
+  </si>
+  <si>
+    <t>Males who inject drugs</t>
+  </si>
+  <si>
+    <t>MSM programs</t>
+  </si>
   <si>
     <t>Age-related population transitions (average number of years before movement)</t>
   </si>
@@ -239,243 +468,17 @@
   <si>
     <t>OR</t>
   </si>
-  <si>
-    <t>Coverage</t>
-  </si>
-  <si>
-    <t>Treated HIV</t>
-  </si>
-  <si>
-    <t>Populations</t>
-  </si>
-  <si>
-    <t>HIV prevalence</t>
-  </si>
-  <si>
-    <t>Number of acts with regular partners per person per year</t>
-  </si>
-  <si>
-    <t>Number of acts with casual partners per person per year</t>
-  </si>
-  <si>
-    <t>Number of acts with commercial partners per person per year</t>
-  </si>
-  <si>
-    <t>Gross domestic product</t>
-  </si>
-  <si>
-    <t>Government revenue</t>
-  </si>
-  <si>
-    <t>Prevalence of any ulcerative STIs</t>
-  </si>
-  <si>
-    <t>Number of people initiating ART each year</t>
-  </si>
-  <si>
-    <t>Percentage of people who used a condom at last act with commercial partners</t>
-  </si>
-  <si>
-    <t>Percentage of people who receptively shared a needle at last injection</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Average</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Female sex workers</t>
-  </si>
-  <si>
-    <t>Clients</t>
-  </si>
-  <si>
-    <t>Opiate substition therapy</t>
-  </si>
-  <si>
-    <t>Antiretroviral therapy</t>
-  </si>
-  <si>
-    <t>Prevention of mother-to-child transmission</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Average</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prevalence of any discharging STIs</t>
-  </si>
-  <si>
-    <t>Percentage of people who used a condom at last act with regular partners</t>
-  </si>
-  <si>
-    <t>Average number of injections per person per year</t>
-  </si>
-  <si>
-    <t>Disease progression rate (% per year)</t>
-  </si>
-  <si>
-    <t>Mother-to-child (breastfeeding)</t>
-  </si>
-  <si>
-    <t>Mother-to-child (non-breastfeeding)</t>
-  </si>
-  <si>
-    <t>Relative disease-related transmissibility</t>
-  </si>
-  <si>
-    <t>Social mitigation costs</t>
-  </si>
-  <si>
-    <t>HIV-related health care costs (excluding treatment)</t>
-  </si>
-  <si>
-    <t>Untreated HIV, acute</t>
-  </si>
-  <si>
-    <t>Disutility weights</t>
-  </si>
-  <si>
-    <t>Interactions between casual partners</t>
-  </si>
-  <si>
-    <t>Interactions between commercial partners</t>
-  </si>
-  <si>
-    <t>Interactions between regular partners</t>
-  </si>
-  <si>
-    <t>Interactions between people who inject drugs</t>
-  </si>
-  <si>
-    <t>Interaction-related transmissibility (% per act)</t>
-  </si>
-  <si>
-    <t>Treatment recovery rate (% per year)</t>
-  </si>
-  <si>
-    <t>Treatment failure rate (% per year)</t>
-  </si>
-  <si>
-    <t>Death rate (% mortality per year)</t>
-  </si>
-  <si>
-    <t>Relative transmissibility</t>
-  </si>
-  <si>
-    <t>Modeled estimate of HIV prevalence</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Injects</t>
-  </si>
-  <si>
-    <t>Men who have sex with men</t>
-  </si>
-  <si>
-    <t>FSW programs</t>
-  </si>
-  <si>
-    <t>Programs for female sex workers and clients</t>
-  </si>
-  <si>
-    <t>Needle-syringe programs</t>
-  </si>
-  <si>
-    <t>Programs for men who have sex with men</t>
-  </si>
-  <si>
-    <t>Social and behavior change communication</t>
-  </si>
-  <si>
-    <t>SBCC</t>
-  </si>
-  <si>
-    <t>Male PWID</t>
-  </si>
-  <si>
-    <t>Males who inject drugs</t>
-  </si>
-  <si>
-    <t>MSM programs</t>
-  </si>
-  <si>
-    <t>Number of people who inject drugs who are on opiate substitution therapy</t>
-  </si>
-  <si>
-    <t>Number of women on PMTCT (Option B/B+)</t>
-  </si>
-  <si>
-    <t>Number of voluntary medical male circumcisions performed</t>
-  </si>
-  <si>
-    <t>Percentage of people covered by pre-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Percentage of people coveraged by post-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Pre-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Post-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Cost &amp; coverage</t>
-  </si>
-  <si>
-    <t>Saturating</t>
-  </si>
-  <si>
-    <t>Assumption</t>
-  </si>
-  <si>
-    <t>Injecting</t>
-  </si>
-  <si>
-    <t>Heterosexual insertive</t>
-  </si>
-  <si>
-    <t>Heterosexual receptive</t>
-  </si>
-  <si>
-    <t>Homosexual insertive</t>
-  </si>
-  <si>
-    <t>Homosexual receptive</t>
-  </si>
-  <si>
-    <t>Opiate substitution therapy</t>
-  </si>
-  <si>
-    <t>ARV treatment</t>
-  </si>
-  <si>
-    <t>Percentage of people who die from non-HIV-related causes per year</t>
-  </si>
-  <si>
-    <t>Number of HIV tests per year</t>
-  </si>
-  <si>
-    <t>Number of HIV diagnoses per year</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.00%"/>
+    <numFmt numFmtId="170" formatCode="0"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -1304,7 +1307,7 @@
     <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1414,6 +1417,14 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2409,36 +2420,36 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="21" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="C2" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="G2" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>112</v>
-      </c>
       <c r="H2" s="21" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2446,10 +2457,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>113</v>
+        <v>65</v>
       </c>
       <c r="E3" s="41" t="b">
         <v>1</v>
@@ -2478,10 +2489,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="E4" s="41" t="b">
         <v>0</v>
@@ -2510,10 +2521,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="E5" s="41" t="b">
         <v>1</v>
@@ -2542,10 +2553,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="E6" s="41" t="b">
         <v>1</v>
@@ -2574,10 +2585,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="E7" s="41" t="b">
         <v>0</v>
@@ -2606,10 +2617,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="E8" s="41" t="b">
         <v>1</v>
@@ -2644,20 +2655,20 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="21" t="s">
-        <v>59</v>
+        <v>134</v>
       </c>
       <c r="B12" s="21"/>
     </row>
     <row r="13" spans="1:11">
       <c r="B13" s="21"/>
       <c r="C13" s="21" t="s">
-        <v>63</v>
+        <v>138</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>64</v>
+        <v>139</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>132</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2665,10 +2676,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="E14" s="41" t="b">
         <v>1</v>
@@ -2679,10 +2690,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="D15" s="45" t="s">
-        <v>116</v>
+        <v>68</v>
       </c>
       <c r="E15" s="41" t="b">
         <v>1</v>
@@ -2693,10 +2704,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>47</v>
+        <v>122</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="E16" s="41" t="b">
         <v>0</v>
@@ -2707,10 +2718,10 @@
         <v>4</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>117</v>
+        <v>69</v>
       </c>
       <c r="E17" s="41" t="b">
         <v>1</v>
@@ -2721,10 +2732,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="45" t="s">
-        <v>114</v>
+        <v>66</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>115</v>
+        <v>67</v>
       </c>
       <c r="E18" s="41" t="b">
         <v>1</v>
@@ -2735,10 +2746,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>48</v>
+        <v>123</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="E19" s="41" t="b">
         <v>0</v>
@@ -2749,10 +2760,10 @@
         <v>7</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>49</v>
+        <v>124</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="E20" s="41" t="b">
         <v>0</v>
@@ -2786,7 +2797,7 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="2"/>
@@ -2939,7 +2950,7 @@
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="17" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="2"/>
@@ -3078,23 +3089,23 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="19" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1">
       <c r="C2" s="4" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" s="19" t="s">
-        <v>135</v>
+        <v>12</v>
       </c>
       <c r="C3" s="26">
         <v>4.0000000000000002E-4</v>
@@ -3104,7 +3115,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="B4" s="19" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
       <c r="C4" s="26">
         <v>1E-3</v>
@@ -3114,7 +3125,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="B5" s="19" t="s">
-        <v>137</v>
+        <v>14</v>
       </c>
       <c r="C5" s="26">
         <v>5.9999999999999995E-4</v>
@@ -3124,7 +3135,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="B6" s="19" t="s">
-        <v>138</v>
+        <v>15</v>
       </c>
       <c r="C6" s="26">
         <v>5.0000000000000001E-3</v>
@@ -3134,7 +3145,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="B7" s="19" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="C7" s="26">
         <v>3.0000000000000001E-3</v>
@@ -3144,7 +3155,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="B8" s="19" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="C8" s="25">
         <v>0.05</v>
@@ -3154,7 +3165,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="B9" s="19" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="C9" s="25">
         <v>0.03</v>
@@ -3174,23 +3185,23 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="19" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1">
       <c r="C14" s="4" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" s="19" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="C15" s="22">
         <v>10</v>
@@ -3200,7 +3211,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="B16" s="19" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="C16" s="22">
         <v>1</v>
@@ -3210,7 +3221,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="B17" s="19" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C17" s="22">
         <v>1</v>
@@ -3220,7 +3231,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="B18" s="19" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="C18" s="22">
         <v>1</v>
@@ -3230,7 +3241,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="B19" s="19" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="C19" s="22">
         <v>3.8</v>
@@ -3250,24 +3261,24 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="19" t="s">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="B23" s="19"/>
     </row>
     <row r="24" spans="1:8">
       <c r="C24" s="4" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="B25" s="19" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="C25" s="25">
         <v>1</v>
@@ -3277,7 +3288,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="B26" s="19" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C26" s="25">
         <v>0.25</v>
@@ -3287,7 +3298,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="B27" s="19" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="C27" s="25">
         <v>0.25</v>
@@ -3297,7 +3308,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="B28" s="19" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="C28" s="25">
         <v>0.5</v>
@@ -3317,23 +3328,23 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="19" t="s">
-        <v>105</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="C33" s="4" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="B34" s="19" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="C34" s="25">
         <v>0.45</v>
@@ -3343,7 +3354,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="B35" s="19" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="C35" s="25">
         <v>0.7</v>
@@ -3353,7 +3364,7 @@
     </row>
     <row r="36" spans="1:8">
       <c r="B36" s="19" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="C36" s="25">
         <v>0.36</v>
@@ -3376,23 +3387,23 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="19" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="C41" s="4" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="B42" s="19" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="C42" s="25">
         <v>0.2</v>
@@ -3406,7 +3417,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="B43" s="19" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="C43" s="25">
         <v>0.1</v>
@@ -3430,23 +3441,23 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="19" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="C48" s="4" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="B49" s="19" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="C49" s="25">
         <v>0</v>
@@ -3456,7 +3467,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="B50" s="19" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="C50" s="26">
         <v>5.0000000000000001E-4</v>
@@ -3466,7 +3477,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="B51" s="19" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="C51" s="26">
         <v>1E-3</v>
@@ -3476,7 +3487,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="B52" s="19" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="C52" s="25">
         <v>0.01</v>
@@ -3486,7 +3497,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="B53" s="19" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="C53" s="25">
         <v>0.49</v>
@@ -3496,7 +3507,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="B54" s="19" t="s">
-        <v>55</v>
+        <v>130</v>
       </c>
       <c r="C54" s="25">
         <v>0.04</v>
@@ -3506,7 +3517,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="B55" s="19" t="s">
-        <v>66</v>
+        <v>141</v>
       </c>
       <c r="C55" s="22">
         <v>2</v>
@@ -3526,23 +3537,23 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="19" t="s">
-        <v>108</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="C60" s="4" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="B61" s="19" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="C61" s="25">
         <v>0.05</v>
@@ -3552,7 +3563,7 @@
     </row>
     <row r="62" spans="1:8">
       <c r="B62" s="19" t="s">
-        <v>56</v>
+        <v>131</v>
       </c>
       <c r="C62" s="25">
         <v>0.3</v>
@@ -3562,7 +3573,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="B63" s="19" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="C63" s="25">
         <v>0.65</v>
@@ -3572,7 +3583,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="B64" s="19" t="s">
-        <v>57</v>
+        <v>132</v>
       </c>
       <c r="C64" s="25">
         <v>3.5</v>
@@ -3582,7 +3593,7 @@
     </row>
     <row r="65" spans="2:5">
       <c r="B65" s="19" t="s">
-        <v>139</v>
+        <v>16</v>
       </c>
       <c r="C65" s="25">
         <v>0.05</v>
@@ -3592,7 +3603,7 @@
     </row>
     <row r="66" spans="2:5">
       <c r="B66" s="19" t="s">
-        <v>58</v>
+        <v>133</v>
       </c>
       <c r="C66" s="25">
         <v>0.05</v>
@@ -3602,7 +3613,7 @@
     </row>
     <row r="67" spans="2:5">
       <c r="B67" s="19" t="s">
-        <v>140</v>
+        <v>17</v>
       </c>
       <c r="C67" s="25">
         <v>0.3</v>
@@ -3612,7 +3623,7 @@
     </row>
     <row r="68" spans="2:5">
       <c r="B68" s="19" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="C68" s="25">
         <v>0.5</v>
@@ -3622,7 +3633,7 @@
     </row>
     <row r="69" spans="2:5">
       <c r="B69" s="19" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="C69" s="25">
         <v>0.5</v>
@@ -3657,7 +3668,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="19" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -3668,18 +3679,18 @@
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="4" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="18" customFormat="1">
       <c r="B3" s="19" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="C3" s="24">
         <v>0.05</v>
@@ -3690,7 +3701,7 @@
     <row r="4" spans="1:8">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="C4" s="24">
         <v>0.05</v>
@@ -3701,7 +3712,7 @@
     <row r="5" spans="1:8">
       <c r="A5" s="18"/>
       <c r="B5" s="19" t="s">
-        <v>41</v>
+        <v>116</v>
       </c>
       <c r="C5" s="24">
         <v>0.1</v>
@@ -3712,7 +3723,7 @@
     <row r="6" spans="1:8">
       <c r="A6" s="18"/>
       <c r="B6" s="19" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="C6" s="24">
         <v>0.15</v>
@@ -3723,7 +3734,7 @@
     <row r="7" spans="1:8">
       <c r="A7" s="18"/>
       <c r="B7" s="19" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="C7" s="24">
         <v>0.5</v>
@@ -3734,7 +3745,7 @@
     <row r="8" spans="1:8">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="C8" s="24">
         <v>5.2999999999999999E-2</v>
@@ -3762,7 +3773,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="19" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -3773,19 +3784,19 @@
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="4" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="C14" s="22">
         <v>0</v>
@@ -3796,7 +3807,7 @@
     <row r="15" spans="1:8">
       <c r="A15" s="18"/>
       <c r="B15" s="19" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="C15" s="22">
         <v>100</v>
@@ -3807,7 +3818,7 @@
     <row r="16" spans="1:8">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="C16" s="22">
         <v>100</v>
@@ -3818,7 +3829,7 @@
     <row r="17" spans="1:5">
       <c r="A17" s="18"/>
       <c r="B17" s="19" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="C17" s="22">
         <v>200</v>
@@ -3829,7 +3840,7 @@
     <row r="18" spans="1:5">
       <c r="A18" s="18"/>
       <c r="B18" s="19" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="C18" s="22">
         <v>450</v>
@@ -3839,7 +3850,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="19" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -3850,19 +3861,19 @@
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="4" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18"/>
       <c r="B24" s="19" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="C24" s="22">
         <v>0</v>
@@ -3873,7 +3884,7 @@
     <row r="25" spans="1:5">
       <c r="A25" s="18"/>
       <c r="B25" s="19" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="C25" s="22">
         <v>100</v>
@@ -3884,7 +3895,7 @@
     <row r="26" spans="1:5">
       <c r="A26" s="18"/>
       <c r="B26" s="19" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="C26" s="22">
         <v>100</v>
@@ -3895,7 +3906,7 @@
     <row r="27" spans="1:5">
       <c r="A27" s="18"/>
       <c r="B27" s="19" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="C27" s="22">
         <v>1000</v>
@@ -3906,7 +3917,7 @@
     <row r="28" spans="1:5">
       <c r="A28" s="18"/>
       <c r="B28" s="19" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="C28" s="22">
         <v>10000</v>
@@ -3949,7 +3960,7 @@
   <sheetData>
     <row r="1" spans="1:35">
       <c r="A1" s="19" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="S1" s="18"/>
       <c r="T1" s="18"/>
@@ -4065,13 +4076,13 @@
       </c>
       <c r="AH2" s="18"/>
       <c r="AI2" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:35">
       <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C3" s="22">
         <f t="shared" ref="C3:R3" si="0">D3/(1.12)</f>
@@ -4197,7 +4208,7 @@
         <v>350405950838.15192</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="AI3" s="29"/>
     </row>
@@ -4208,7 +4219,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" s="19" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="S7" s="18"/>
       <c r="T7" s="18"/>
@@ -4324,13 +4335,13 @@
       </c>
       <c r="AH8" s="18"/>
       <c r="AI8" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:35">
       <c r="A9" s="18"/>
       <c r="B9" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C9" s="40">
         <v>30000000000</v>
@@ -4456,13 +4467,13 @@
         <v>180000000000</v>
       </c>
       <c r="AH9" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="AI9" s="29"/>
     </row>
     <row r="13" spans="1:35">
       <c r="A13" s="19" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
@@ -4578,13 +4589,13 @@
       </c>
       <c r="AH14" s="18"/>
       <c r="AI14" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:35">
       <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C15" s="22">
         <v>10000000000</v>
@@ -4710,13 +4721,13 @@
         <v>43219423751.506668</v>
       </c>
       <c r="AH15" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="AI15" s="29"/>
     </row>
     <row r="19" spans="1:35" s="18" customFormat="1">
       <c r="A19" s="19" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="B19" s="6"/>
       <c r="AI19" s="6"/>
@@ -4817,12 +4828,12 @@
         <v>2030</v>
       </c>
       <c r="AI20" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:35" s="18" customFormat="1">
       <c r="B21" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -4856,7 +4867,7 @@
       <c r="AF21" s="22"/>
       <c r="AG21" s="22"/>
       <c r="AH21" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="AI21" s="29"/>
     </row>
@@ -4874,7 +4885,7 @@
     </row>
     <row r="25" spans="1:35" s="18" customFormat="1">
       <c r="A25" s="19" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="B25" s="6"/>
       <c r="AI25" s="6"/>
@@ -4975,12 +4986,12 @@
         <v>2030</v>
       </c>
       <c r="AI26" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:35" s="18" customFormat="1">
       <c r="B27" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C27" s="22">
         <f>12%*C15</f>
@@ -5107,13 +5118,13 @@
         <v>5186330850.1808004</v>
       </c>
       <c r="AH27" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="AI27" s="29"/>
     </row>
     <row r="31" spans="1:35" s="18" customFormat="1">
       <c r="A31" s="19" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="B31" s="6"/>
       <c r="AI31" s="6"/>
@@ -5214,12 +5225,12 @@
         <v>2030</v>
       </c>
       <c r="AI32" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:35" s="18" customFormat="1">
       <c r="B33" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C33" s="22">
         <v>15000000</v>
@@ -5315,7 +5326,7 @@
         <v>18000000</v>
       </c>
       <c r="AH33" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="AI33" s="29"/>
     </row>
@@ -5333,7 +5344,7 @@
     </row>
     <row r="37" spans="1:35" s="18" customFormat="1">
       <c r="A37" s="19" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="B37" s="6"/>
       <c r="AI37" s="6"/>
@@ -5434,12 +5445,12 @@
         <v>2030</v>
       </c>
       <c r="AI38" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:35" s="18" customFormat="1">
       <c r="B39" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
@@ -5473,7 +5484,7 @@
       <c r="AF39" s="22"/>
       <c r="AG39" s="22"/>
       <c r="AH39" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="AI39" s="29"/>
     </row>
@@ -5491,7 +5502,7 @@
     </row>
     <row r="43" spans="1:35" s="18" customFormat="1">
       <c r="A43" s="19" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="B43" s="6"/>
       <c r="AI43" s="6"/>
@@ -5592,12 +5603,12 @@
         <v>2030</v>
       </c>
       <c r="AI44" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:35" s="18" customFormat="1">
       <c r="B45" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
@@ -5631,13 +5642,13 @@
       <c r="AF45" s="22"/>
       <c r="AG45" s="22"/>
       <c r="AH45" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="AI45" s="29"/>
     </row>
     <row r="49" spans="1:35" s="18" customFormat="1">
       <c r="A49" s="19" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="B49" s="6"/>
       <c r="AI49" s="6"/>
@@ -5738,12 +5749,12 @@
         <v>2030</v>
       </c>
       <c r="AI50" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:35" s="18" customFormat="1">
       <c r="B51" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
@@ -5777,7 +5788,7 @@
       <c r="AF51" s="22"/>
       <c r="AG51" s="22"/>
       <c r="AH51" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="AI51" s="29"/>
     </row>
@@ -5795,7 +5806,7 @@
     </row>
     <row r="55" spans="1:35" s="18" customFormat="1">
       <c r="A55" s="19" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="B55" s="6"/>
       <c r="AI55" s="6"/>
@@ -5896,12 +5907,12 @@
         <v>2030</v>
       </c>
       <c r="AI56" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:35" s="18" customFormat="1">
       <c r="B57" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C57" s="22"/>
       <c r="D57" s="22"/>
@@ -5935,7 +5946,7 @@
       <c r="AF57" s="22"/>
       <c r="AG57" s="22"/>
       <c r="AH57" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="AI57" s="29"/>
     </row>
@@ -5955,22 +5966,24 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.125" style="18"/>
     <col min="3" max="3" width="11" style="18" customWidth="1"/>
-    <col min="4" max="20" width="9.125" style="18"/>
+    <col min="4" max="13" width="9.125" style="18"/>
+    <col min="14" max="14" width="9.875" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="9.125" style="18"/>
     <col min="21" max="21" width="15.125" style="18" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="9.125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="19" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:22">
@@ -6023,7 +6036,7 @@
         <v>2015</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -6032,7 +6045,7 @@
         <v>SBCC</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="25">
@@ -6065,7 +6078,7 @@
       <c r="R3" s="22"/>
       <c r="S3" s="22"/>
       <c r="T3" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U3" s="25"/>
     </row>
@@ -6075,7 +6088,7 @@
         <v>SBCC</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="27">
@@ -6115,7 +6128,7 @@
       <c r="R4" s="24"/>
       <c r="S4" s="24"/>
       <c r="T4" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U4" s="37"/>
     </row>
@@ -6128,7 +6141,7 @@
         <v>NSP</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="25"/>
@@ -6147,7 +6160,7 @@
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
       <c r="T6" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U6" s="25">
         <v>0.2</v>
@@ -6159,7 +6172,7 @@
         <v>NSP</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="23"/>
@@ -6178,7 +6191,7 @@
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
       <c r="T7" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U7" s="47">
         <v>25000</v>
@@ -6193,7 +6206,7 @@
         <v>OST</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="25"/>
@@ -6214,7 +6227,7 @@
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
       <c r="T9" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U9" s="25"/>
     </row>
@@ -6225,7 +6238,7 @@
         <v>OST</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="23"/>
@@ -6247,7 +6260,7 @@
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
       <c r="T10" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U10" s="37"/>
     </row>
@@ -6262,7 +6275,7 @@
         <v>MSM programs</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="25"/>
@@ -6283,7 +6296,7 @@
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
       <c r="T12" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U12" s="25"/>
       <c r="V12" s="6"/>
@@ -6294,7 +6307,7 @@
         <v>MSM programs</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="23"/>
@@ -6315,7 +6328,7 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
       <c r="T13" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U13" s="37"/>
     </row>
@@ -6325,7 +6338,7 @@
         <v>FSW programs</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="25"/>
@@ -6346,7 +6359,7 @@
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
       <c r="T15" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U15" s="25"/>
     </row>
@@ -6356,7 +6369,7 @@
         <v>FSW programs</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
@@ -6377,7 +6390,7 @@
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
       <c r="T16" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U16" s="37"/>
     </row>
@@ -6387,7 +6400,7 @@
         <v>ART</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="25"/>
@@ -6408,7 +6421,7 @@
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
       <c r="T18" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U18" s="25"/>
     </row>
@@ -6418,7 +6431,7 @@
         <v>ART</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="23"/>
@@ -6440,7 +6453,7 @@
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
       <c r="T19" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U19" s="37"/>
     </row>
@@ -6450,7 +6463,7 @@
         <v>PMTCT</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="25"/>
@@ -6471,7 +6484,7 @@
       <c r="R21" s="22"/>
       <c r="S21" s="22"/>
       <c r="T21" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U21" s="25"/>
     </row>
@@ -6481,7 +6494,7 @@
         <v>PMTCT</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
@@ -6503,13 +6516,14 @@
       <c r="R22" s="22"/>
       <c r="S22" s="22"/>
       <c r="T22" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U22" s="37"/>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6539,7 +6553,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="19" t="s">
-        <v>60</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -6592,7 +6606,7 @@
         <v>2015</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -6601,7 +6615,7 @@
         <v>MSM</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
@@ -6620,7 +6634,7 @@
       <c r="R3" s="27"/>
       <c r="S3" s="27"/>
       <c r="T3" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U3" s="27">
         <v>37500</v>
@@ -6632,7 +6646,7 @@
         <v>MSM</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
@@ -6651,7 +6665,7 @@
       <c r="R4" s="27"/>
       <c r="S4" s="27"/>
       <c r="T4" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U4" s="27">
         <v>21000</v>
@@ -6663,7 +6677,7 @@
         <v>MSM</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
@@ -6682,7 +6696,7 @@
       <c r="R5" s="27"/>
       <c r="S5" s="27"/>
       <c r="T5" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U5" s="27">
         <v>11000</v>
@@ -6699,7 +6713,7 @@
         <v>FSW</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
@@ -6718,7 +6732,7 @@
       <c r="R7" s="27"/>
       <c r="S7" s="27"/>
       <c r="T7" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U7" s="27"/>
     </row>
@@ -6728,7 +6742,7 @@
         <v>FSW</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
@@ -6747,7 +6761,7 @@
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
       <c r="T8" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U8" s="27">
         <v>15000</v>
@@ -6759,7 +6773,7 @@
         <v>FSW</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
@@ -6778,7 +6792,7 @@
       <c r="R9" s="27"/>
       <c r="S9" s="27"/>
       <c r="T9" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U9" s="27"/>
     </row>
@@ -6809,7 +6823,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
@@ -6838,7 +6852,7 @@
       <c r="R11" s="27"/>
       <c r="S11" s="27"/>
       <c r="T11" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U11" s="27"/>
     </row>
@@ -6848,7 +6862,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
@@ -6877,7 +6891,7 @@
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
       <c r="T12" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U12" s="27"/>
     </row>
@@ -6887,7 +6901,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
@@ -6916,7 +6930,7 @@
       <c r="R13" s="27"/>
       <c r="S13" s="27"/>
       <c r="T13" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U13" s="27"/>
     </row>
@@ -6947,7 +6961,7 @@
         <v>Other males</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
@@ -6966,7 +6980,7 @@
       <c r="R15" s="27"/>
       <c r="S15" s="27"/>
       <c r="T15" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U15" s="27"/>
     </row>
@@ -6976,7 +6990,7 @@
         <v>Other males</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D16" s="22">
         <v>4227500</v>
@@ -7027,7 +7041,7 @@
         <v>6118320.6906761518</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U16" s="27"/>
     </row>
@@ -7037,7 +7051,7 @@
         <v>Other males</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
@@ -7056,7 +7070,7 @@
       <c r="R17" s="27"/>
       <c r="S17" s="27"/>
       <c r="T17" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U17" s="27"/>
     </row>
@@ -7087,7 +7101,7 @@
         <v>Other females</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
@@ -7106,7 +7120,7 @@
       <c r="R19" s="27"/>
       <c r="S19" s="27"/>
       <c r="T19" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U19" s="27"/>
     </row>
@@ -7116,7 +7130,7 @@
         <v>Other females</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D20" s="22">
         <v>4759641.7668505535</v>
@@ -7167,7 +7181,7 @@
         <v>7061706.1901886221</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U20" s="27"/>
     </row>
@@ -7177,7 +7191,7 @@
         <v>Other females</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
@@ -7196,7 +7210,7 @@
       <c r="R21" s="27"/>
       <c r="S21" s="27"/>
       <c r="T21" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U21" s="27"/>
     </row>
@@ -7227,7 +7241,7 @@
         <v>Clients</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -7246,7 +7260,7 @@
       <c r="R23" s="27"/>
       <c r="S23" s="27"/>
       <c r="T23" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U23" s="27"/>
     </row>
@@ -7256,7 +7270,7 @@
         <v>Clients</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D24" s="22">
         <v>522500</v>
@@ -7307,7 +7321,7 @@
         <v>756196.93929705245</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U24" s="27"/>
     </row>
@@ -7317,7 +7331,7 @@
         <v>Clients</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -7336,13 +7350,13 @@
       <c r="R25" s="27"/>
       <c r="S25" s="27"/>
       <c r="T25" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U25" s="27"/>
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="19" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -7395,7 +7409,7 @@
         <v>2015</v>
       </c>
       <c r="U30" s="19" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -7404,7 +7418,7 @@
         <v>MSM</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -7425,7 +7439,7 @@
       <c r="R31" s="22"/>
       <c r="S31" s="22"/>
       <c r="T31" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U31" s="26"/>
     </row>
@@ -7435,7 +7449,7 @@
         <v>MSM</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -7456,7 +7470,7 @@
       <c r="R32" s="22"/>
       <c r="S32" s="22"/>
       <c r="T32" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U32" s="26"/>
     </row>
@@ -7466,7 +7480,7 @@
         <v>MSM</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
@@ -7487,7 +7501,7 @@
       <c r="R33" s="22"/>
       <c r="S33" s="22"/>
       <c r="T33" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U33" s="26"/>
     </row>
@@ -7501,7 +7515,7 @@
         <v>FSW</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
@@ -7526,7 +7540,7 @@
       <c r="R35" s="22"/>
       <c r="S35" s="22"/>
       <c r="T35" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U35" s="26"/>
     </row>
@@ -7536,7 +7550,7 @@
         <v>FSW</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -7561,7 +7575,7 @@
       <c r="R36" s="22"/>
       <c r="S36" s="22"/>
       <c r="T36" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U36" s="26"/>
     </row>
@@ -7571,7 +7585,7 @@
         <v>FSW</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
@@ -7596,7 +7610,7 @@
       <c r="R37" s="22"/>
       <c r="S37" s="22"/>
       <c r="T37" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U37" s="26"/>
     </row>
@@ -7610,7 +7624,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
@@ -7635,7 +7649,7 @@
       <c r="R39" s="22"/>
       <c r="S39" s="22"/>
       <c r="T39" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U39" s="26"/>
     </row>
@@ -7645,7 +7659,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
@@ -7670,7 +7684,7 @@
       <c r="R40" s="22"/>
       <c r="S40" s="22"/>
       <c r="T40" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U40" s="26"/>
     </row>
@@ -7680,7 +7694,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
@@ -7705,7 +7719,7 @@
       <c r="R41" s="22"/>
       <c r="S41" s="22"/>
       <c r="T41" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U41" s="26"/>
     </row>
@@ -7719,7 +7733,7 @@
         <v>Other males</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
@@ -7738,7 +7752,7 @@
       <c r="R43" s="22"/>
       <c r="S43" s="22"/>
       <c r="T43" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U43" s="26"/>
     </row>
@@ -7748,7 +7762,7 @@
         <v>Other males</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
@@ -7767,7 +7781,7 @@
       <c r="R44" s="22"/>
       <c r="S44" s="22"/>
       <c r="T44" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U44" s="26">
         <v>5.0000000000000001E-4</v>
@@ -7779,7 +7793,7 @@
         <v>Other males</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
@@ -7798,7 +7812,7 @@
       <c r="R45" s="22"/>
       <c r="S45" s="22"/>
       <c r="T45" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U45" s="26"/>
     </row>
@@ -7812,7 +7826,7 @@
         <v>Other females</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
@@ -7831,7 +7845,7 @@
       <c r="R47" s="22"/>
       <c r="S47" s="22"/>
       <c r="T47" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U47" s="26"/>
     </row>
@@ -7841,7 +7855,7 @@
         <v>Other females</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
@@ -7868,7 +7882,7 @@
       <c r="R48" s="22"/>
       <c r="S48" s="22"/>
       <c r="T48" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U48" s="26"/>
     </row>
@@ -7878,7 +7892,7 @@
         <v>Other females</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
@@ -7897,7 +7911,7 @@
       <c r="R49" s="22"/>
       <c r="S49" s="22"/>
       <c r="T49" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U49" s="26"/>
     </row>
@@ -7911,7 +7925,7 @@
         <v>Clients</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
@@ -7930,7 +7944,7 @@
       <c r="R51" s="22"/>
       <c r="S51" s="22"/>
       <c r="T51" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U51" s="26"/>
     </row>
@@ -7940,7 +7954,7 @@
         <v>Clients</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
@@ -7959,7 +7973,7 @@
       <c r="R52" s="22"/>
       <c r="S52" s="22"/>
       <c r="T52" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U52" s="26">
         <v>0.01</v>
@@ -7971,7 +7985,7 @@
         <v>Clients</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
@@ -7990,7 +8004,7 @@
       <c r="R53" s="22"/>
       <c r="S53" s="22"/>
       <c r="T53" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="U53" s="26"/>
     </row>
@@ -8022,7 +8036,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="10" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -8095,13 +8109,13 @@
       </c>
       <c r="S2" s="9"/>
       <c r="T2" s="10" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="9"/>
       <c r="B3" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -8120,7 +8134,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T3" s="22"/>
     </row>
@@ -8132,7 +8146,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="10" t="s">
-        <v>143</v>
+        <v>20</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -8205,13 +8219,13 @@
       </c>
       <c r="S8" s="9"/>
       <c r="T8" s="10" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -8254,7 +8268,7 @@
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
       <c r="S9" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T9" s="22"/>
     </row>
@@ -8266,7 +8280,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="10" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -8339,13 +8353,13 @@
       </c>
       <c r="S14" s="9"/>
       <c r="T14" s="10" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="9"/>
       <c r="B15" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -8364,7 +8378,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T15" s="22"/>
     </row>
@@ -8376,7 +8390,7 @@
     </row>
     <row r="19" spans="1:20" s="18" customFormat="1">
       <c r="A19" s="19" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="B19" s="6"/>
     </row>
@@ -8431,12 +8445,12 @@
         <v>2015</v>
       </c>
       <c r="T20" s="19" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:20" s="18" customFormat="1">
       <c r="B21" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -8455,7 +8469,7 @@
       <c r="Q21" s="22"/>
       <c r="R21" s="22"/>
       <c r="S21" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T21" s="22"/>
     </row>
@@ -8470,7 +8484,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="10" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -8543,13 +8557,13 @@
       </c>
       <c r="S26" s="9"/>
       <c r="T26" s="10" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="9"/>
       <c r="B27" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
@@ -8568,13 +8582,13 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T27" s="22"/>
     </row>
     <row r="31" spans="1:20" s="18" customFormat="1">
       <c r="A31" s="19" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="B31" s="6"/>
     </row>
@@ -8629,12 +8643,12 @@
         <v>2015</v>
       </c>
       <c r="T32" s="19" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="2:20" s="18" customFormat="1">
       <c r="B33" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
@@ -8653,7 +8667,7 @@
       <c r="Q33" s="22"/>
       <c r="R33" s="22"/>
       <c r="S33" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T33" s="22"/>
     </row>
@@ -8684,7 +8698,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="18" customFormat="1">
       <c r="A1" s="19" t="s">
-        <v>141</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6"/>
     </row>
@@ -8739,7 +8753,7 @@
         <v>2015</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="18" customFormat="1">
@@ -8764,7 +8778,7 @@
       <c r="Q3" s="25"/>
       <c r="R3" s="25"/>
       <c r="S3" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T3" s="25">
         <v>0.01</v>
@@ -8792,7 +8806,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T4" s="25">
         <v>0.01</v>
@@ -8820,7 +8834,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T5" s="25">
         <v>0.03</v>
@@ -8848,7 +8862,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T6" s="25">
         <v>0.01</v>
@@ -8876,7 +8890,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T7" s="25">
         <v>0.01</v>
@@ -8904,7 +8918,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T8" s="25">
         <v>0.01</v>
@@ -8921,7 +8935,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="8" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -8994,7 +9008,7 @@
       </c>
       <c r="S13" s="7"/>
       <c r="T13" s="8" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -9020,7 +9034,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T14" s="25">
         <v>0</v>
@@ -9049,7 +9063,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T15" s="25">
         <v>0</v>
@@ -9078,7 +9092,7 @@
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T16" s="25">
         <v>0</v>
@@ -9107,7 +9121,7 @@
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T17" s="25">
         <v>0</v>
@@ -9136,7 +9150,7 @@
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T18" s="25">
         <v>0</v>
@@ -9165,7 +9179,7 @@
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T19" s="25">
         <v>0</v>
@@ -9182,7 +9196,7 @@
     </row>
     <row r="23" spans="1:20" s="18" customFormat="1">
       <c r="A23" s="19" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="B23" s="6"/>
     </row>
@@ -9237,7 +9251,7 @@
         <v>2015</v>
       </c>
       <c r="T24" s="19" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:20" s="18" customFormat="1">
@@ -9262,7 +9276,7 @@
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T25" s="25">
         <v>0</v>
@@ -9290,7 +9304,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T26" s="25">
         <v>0</v>
@@ -9318,7 +9332,7 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T27" s="25">
         <v>0</v>
@@ -9346,7 +9360,7 @@
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
       <c r="S28" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T28" s="25">
         <v>0</v>
@@ -9374,7 +9388,7 @@
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
       <c r="S29" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T29" s="25">
         <v>0</v>
@@ -9402,7 +9416,7 @@
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
       <c r="S30" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T30" s="25">
         <v>0</v>
@@ -9421,7 +9435,7 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="8" t="s">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -9494,7 +9508,7 @@
       </c>
       <c r="S35" s="7"/>
       <c r="T35" s="8" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -9520,7 +9534,7 @@
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
       <c r="S36" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T36" s="25">
         <v>0</v>
@@ -9548,7 +9562,7 @@
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
       <c r="S37" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T37" s="25">
         <v>0</v>
@@ -9576,7 +9590,7 @@
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
       <c r="S38" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T38" s="25">
         <v>0</v>
@@ -9604,7 +9618,7 @@
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
       <c r="S39" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T39" s="25">
         <v>0</v>
@@ -9632,7 +9646,7 @@
       <c r="Q40" s="22"/>
       <c r="R40" s="22"/>
       <c r="S40" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T40" s="25">
         <v>0</v>
@@ -9660,7 +9674,7 @@
       <c r="Q41" s="22"/>
       <c r="R41" s="22"/>
       <c r="S41" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T41" s="25">
         <v>0</v>
@@ -9670,6 +9684,7 @@
       <c r="S42" s="5"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -9685,7 +9700,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="U1" sqref="U1:AW1048576"/>
     </sheetView>
   </sheetViews>
@@ -9697,7 +9712,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="10" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -9770,7 +9785,7 @@
       </c>
       <c r="S2" s="9"/>
       <c r="T2" s="10" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -9796,7 +9811,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T3" s="25">
         <v>0.03</v>
@@ -9829,7 +9844,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T4" s="25"/>
     </row>
@@ -9862,7 +9877,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T5" s="22"/>
     </row>
@@ -9889,7 +9904,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T6" s="25">
         <v>0.01</v>
@@ -9918,7 +9933,7 @@
       <c r="Q7" s="25"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T7" s="25">
         <v>0.01</v>
@@ -9947,7 +9962,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T8" s="25">
         <v>0.05</v>
@@ -9961,7 +9976,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="10" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -10034,13 +10049,13 @@
       </c>
       <c r="S13" s="9"/>
       <c r="T13" s="10" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="9"/>
       <c r="B14" s="4" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -10059,7 +10074,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T14" s="25">
         <v>0.5</v>
@@ -10073,7 +10088,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="10" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -10146,13 +10161,13 @@
       </c>
       <c r="S19" s="9"/>
       <c r="T19" s="10" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="9"/>
       <c r="B20" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C20" s="22">
         <v>0</v>
@@ -10199,7 +10214,7 @@
       <c r="Q20" s="22"/>
       <c r="R20" s="22"/>
       <c r="S20" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T20" s="22"/>
     </row>
@@ -10211,7 +10226,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="10" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -10284,13 +10299,13 @@
       </c>
       <c r="S25" s="9"/>
       <c r="T25" s="10" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="9"/>
       <c r="B26" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C26" s="22">
         <v>0</v>
@@ -10337,7 +10352,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T26" s="22"/>
     </row>
@@ -10352,7 +10367,7 @@
     </row>
     <row r="30" spans="1:20" s="18" customFormat="1">
       <c r="A30" s="19" t="s">
-        <v>126</v>
+        <v>3</v>
       </c>
       <c r="B30" s="6"/>
     </row>
@@ -10407,7 +10422,7 @@
         <v>2015</v>
       </c>
       <c r="T31" s="19" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:20" s="18" customFormat="1">
@@ -10432,7 +10447,7 @@
       <c r="Q32" s="22"/>
       <c r="R32" s="22"/>
       <c r="S32" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T32" s="24">
         <v>0</v>
@@ -10460,7 +10475,7 @@
       <c r="Q33" s="22"/>
       <c r="R33" s="22"/>
       <c r="S33" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T33" s="24">
         <v>0</v>
@@ -10488,7 +10503,7 @@
       <c r="Q34" s="22"/>
       <c r="R34" s="22"/>
       <c r="S34" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T34" s="24">
         <v>0</v>
@@ -10516,7 +10531,7 @@
       <c r="Q35" s="22"/>
       <c r="R35" s="22"/>
       <c r="S35" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T35" s="24">
         <v>0</v>
@@ -10544,7 +10559,7 @@
       <c r="Q36" s="25"/>
       <c r="R36" s="22"/>
       <c r="S36" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T36" s="24">
         <f>2/50</f>
@@ -10573,7 +10588,7 @@
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
       <c r="S37" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T37" s="24">
         <v>0</v>
@@ -10587,7 +10602,7 @@
     </row>
     <row r="41" spans="1:20" s="18" customFormat="1">
       <c r="A41" s="19" t="s">
-        <v>127</v>
+        <v>4</v>
       </c>
       <c r="B41" s="6"/>
     </row>
@@ -10642,7 +10657,7 @@
         <v>2015</v>
       </c>
       <c r="T42" s="19" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:20" s="18" customFormat="1">
@@ -10667,7 +10682,7 @@
       <c r="Q43" s="22"/>
       <c r="R43" s="22"/>
       <c r="S43" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T43" s="24">
         <v>0</v>
@@ -10695,7 +10710,7 @@
       <c r="Q44" s="22"/>
       <c r="R44" s="22"/>
       <c r="S44" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T44" s="24">
         <v>0</v>
@@ -10723,7 +10738,7 @@
       <c r="Q45" s="22"/>
       <c r="R45" s="22"/>
       <c r="S45" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T45" s="24">
         <v>0</v>
@@ -10751,7 +10766,7 @@
       <c r="Q46" s="22"/>
       <c r="R46" s="22"/>
       <c r="S46" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T46" s="24">
         <v>0</v>
@@ -10779,7 +10794,7 @@
       <c r="Q47" s="25"/>
       <c r="R47" s="22"/>
       <c r="S47" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T47" s="24">
         <f>2/50</f>
@@ -10808,7 +10823,7 @@
       <c r="Q48" s="22"/>
       <c r="R48" s="22"/>
       <c r="S48" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T48" s="24">
         <v>0</v>
@@ -10825,7 +10840,7 @@
     </row>
     <row r="52" spans="1:20">
       <c r="A52" s="10" t="s">
-        <v>124</v>
+        <v>1</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
@@ -10898,13 +10913,13 @@
       </c>
       <c r="S53" s="9"/>
       <c r="T53" s="10" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:20">
       <c r="A54" s="9"/>
       <c r="B54" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C54" s="27"/>
       <c r="D54" s="27"/>
@@ -10933,7 +10948,7 @@
       <c r="Q54" s="27"/>
       <c r="R54" s="27"/>
       <c r="S54" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T54" s="22"/>
     </row>
@@ -10948,7 +10963,7 @@
     </row>
     <row r="58" spans="1:20" s="18" customFormat="1">
       <c r="A58" s="19" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="B58" s="6"/>
     </row>
@@ -11003,7 +11018,7 @@
         <v>2015</v>
       </c>
       <c r="T59" s="19" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:20" s="18" customFormat="1">
@@ -11028,7 +11043,7 @@
       <c r="Q60" s="22"/>
       <c r="R60" s="22"/>
       <c r="S60" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T60" s="24">
         <v>0</v>
@@ -11056,7 +11071,7 @@
       <c r="Q61" s="22"/>
       <c r="R61" s="22"/>
       <c r="S61" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T61" s="24">
         <v>0</v>
@@ -11084,7 +11099,7 @@
       <c r="Q62" s="22"/>
       <c r="R62" s="22"/>
       <c r="S62" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T62" s="24">
         <v>0</v>
@@ -11112,7 +11127,7 @@
       <c r="Q63" s="22"/>
       <c r="R63" s="22"/>
       <c r="S63" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T63" s="24">
         <v>0</v>
@@ -11140,7 +11155,7 @@
       <c r="Q64" s="25"/>
       <c r="R64" s="22"/>
       <c r="S64" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T64" s="24">
         <f>2/50</f>
@@ -11169,7 +11184,7 @@
       <c r="Q65" s="22"/>
       <c r="R65" s="22"/>
       <c r="S65" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T65" s="24">
         <v>0</v>
@@ -11177,7 +11192,7 @@
     </row>
     <row r="69" spans="1:20" s="18" customFormat="1">
       <c r="A69" s="19" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="B69" s="6"/>
     </row>
@@ -11232,12 +11247,12 @@
         <v>2015</v>
       </c>
       <c r="T70" s="19" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:20" s="18" customFormat="1">
       <c r="B71" s="4" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="C71" s="22"/>
       <c r="D71" s="22"/>
@@ -11256,13 +11271,14 @@
       <c r="Q71" s="22"/>
       <c r="R71" s="22"/>
       <c r="S71" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T71" s="25">
         <v>0.3</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -11278,8 +11294,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T85"/>
   <sheetViews>
-    <sheetView topLeftCell="J45" workbookViewId="0">
-      <selection activeCell="U45" sqref="U1:AX1048576"/>
+    <sheetView tabSelected="1" topLeftCell="H53" workbookViewId="0">
+      <selection activeCell="T87" sqref="T87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
@@ -11290,7 +11306,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="12" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -11362,7 +11378,7 @@
       </c>
       <c r="S2" s="11"/>
       <c r="T2" s="32" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -11388,7 +11404,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T3" s="33">
         <v>80</v>
@@ -11417,7 +11433,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T4" s="33">
         <v>80</v>
@@ -11446,7 +11462,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T5" s="33">
         <v>80</v>
@@ -11475,7 +11491,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T6" s="33">
         <v>80</v>
@@ -11504,7 +11520,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T7" s="33">
         <v>80</v>
@@ -11533,7 +11549,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T8" s="33">
         <v>80</v>
@@ -11549,7 +11565,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="12" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -11621,7 +11637,7 @@
       </c>
       <c r="S13" s="11"/>
       <c r="T13" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -11647,7 +11663,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T14" s="29">
         <v>10</v>
@@ -11676,7 +11692,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T15" s="29">
         <v>10</v>
@@ -11705,7 +11721,7 @@
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T16" s="29">
         <v>10</v>
@@ -11734,7 +11750,7 @@
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T17" s="29">
         <v>10</v>
@@ -11763,7 +11779,7 @@
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T18" s="29">
         <v>10</v>
@@ -11792,7 +11808,7 @@
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T19" s="29">
         <v>10</v>
@@ -11808,7 +11824,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="12" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -11880,7 +11896,7 @@
       </c>
       <c r="S24" s="11"/>
       <c r="T24" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -11906,7 +11922,7 @@
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T25" s="29">
         <v>0</v>
@@ -11935,7 +11951,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T26" s="29">
         <v>500</v>
@@ -11964,7 +11980,7 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T27" s="29">
         <v>0</v>
@@ -11993,7 +12009,7 @@
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
       <c r="S28" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T28" s="29">
         <v>0</v>
@@ -12022,7 +12038,7 @@
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
       <c r="S29" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T29" s="29">
         <v>0</v>
@@ -12051,14 +12067,83 @@
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
       <c r="S30" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T30" s="29">
         <v>10</v>
       </c>
     </row>
+    <row r="31" spans="1:20">
+      <c r="C31" s="22"/>
+      <c r="D31" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="25">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H31" s="25">
+        <v>0.17</v>
+      </c>
+      <c r="I31" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="J31" s="22"/>
+      <c r="K31" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="L31" s="22"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="25">
+        <v>0.39</v>
+      </c>
+      <c r="O31" s="22"/>
+      <c r="P31" s="25">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="22"/>
+    </row>
     <row r="32" spans="1:20" s="18" customFormat="1">
       <c r="B32" s="6"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="27">
+        <f>550000*D31</f>
+        <v>11000</v>
+      </c>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27">
+        <f t="shared" ref="G32:P32" si="0">550000*G31</f>
+        <v>77000.000000000015</v>
+      </c>
+      <c r="H32" s="27">
+        <f t="shared" si="0"/>
+        <v>93500</v>
+      </c>
+      <c r="I32" s="27">
+        <f t="shared" si="0"/>
+        <v>27500</v>
+      </c>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27">
+        <f t="shared" si="0"/>
+        <v>110000</v>
+      </c>
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
+      <c r="N32" s="27">
+        <f t="shared" si="0"/>
+        <v>214500</v>
+      </c>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27">
+        <f t="shared" si="0"/>
+        <v>154000.00000000003</v>
+      </c>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
       <c r="T32" s="31"/>
     </row>
     <row r="33" spans="1:20" s="18" customFormat="1">
@@ -12067,7 +12152,7 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="12" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -12139,7 +12224,7 @@
       </c>
       <c r="S35" s="11"/>
       <c r="T35" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -12165,7 +12250,7 @@
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
       <c r="S36" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T36" s="30">
         <v>0.4</v>
@@ -12204,7 +12289,7 @@
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
       <c r="S37" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T37" s="30"/>
     </row>
@@ -12231,7 +12316,7 @@
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
       <c r="S38" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T38" s="30">
         <v>0.05</v>
@@ -12260,7 +12345,7 @@
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
       <c r="S39" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T39" s="30">
         <v>0.05</v>
@@ -12289,7 +12374,7 @@
       <c r="Q40" s="22"/>
       <c r="R40" s="22"/>
       <c r="S40" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T40" s="30">
         <v>0.05</v>
@@ -12318,7 +12403,7 @@
       <c r="Q41" s="22"/>
       <c r="R41" s="22"/>
       <c r="S41" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T41" s="30">
         <v>7.0000000000000007E-2</v>
@@ -12334,7 +12419,7 @@
     </row>
     <row r="45" spans="1:20">
       <c r="A45" s="19" t="s">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
@@ -12406,7 +12491,7 @@
       </c>
       <c r="S46" s="11"/>
       <c r="T46" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:20">
@@ -12432,7 +12517,7 @@
       <c r="Q47" s="22"/>
       <c r="R47" s="22"/>
       <c r="S47" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T47" s="30">
         <v>0.6</v>
@@ -12471,7 +12556,7 @@
       <c r="Q48" s="22"/>
       <c r="R48" s="22"/>
       <c r="S48" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T48" s="30"/>
     </row>
@@ -12498,7 +12583,7 @@
       <c r="Q49" s="22"/>
       <c r="R49" s="22"/>
       <c r="S49" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T49" s="30">
         <v>0.5</v>
@@ -12533,7 +12618,7 @@
       <c r="Q50" s="22"/>
       <c r="R50" s="22"/>
       <c r="S50" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T50" s="30"/>
     </row>
@@ -12566,7 +12651,7 @@
       <c r="Q51" s="22"/>
       <c r="R51" s="22"/>
       <c r="S51" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T51" s="30"/>
     </row>
@@ -12593,7 +12678,7 @@
       <c r="Q52" s="22"/>
       <c r="R52" s="22"/>
       <c r="S52" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T52" s="30">
         <v>0.5</v>
@@ -12609,7 +12694,7 @@
     </row>
     <row r="56" spans="1:20">
       <c r="A56" s="19" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
@@ -12681,7 +12766,7 @@
       </c>
       <c r="S57" s="11"/>
       <c r="T57" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:20">
@@ -12707,7 +12792,7 @@
       <c r="Q58" s="22"/>
       <c r="R58" s="22"/>
       <c r="S58" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T58" s="29">
         <v>0</v>
@@ -12746,7 +12831,7 @@
       <c r="Q59" s="22"/>
       <c r="R59" s="22"/>
       <c r="S59" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T59" s="38"/>
     </row>
@@ -12773,7 +12858,7 @@
       <c r="Q60" s="22"/>
       <c r="R60" s="22"/>
       <c r="S60" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T60" s="30">
         <v>0</v>
@@ -12802,7 +12887,7 @@
       <c r="Q61" s="22"/>
       <c r="R61" s="22"/>
       <c r="S61" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T61" s="30">
         <v>0</v>
@@ -12831,7 +12916,7 @@
       <c r="Q62" s="22"/>
       <c r="R62" s="22"/>
       <c r="S62" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T62" s="29">
         <v>0</v>
@@ -12870,7 +12955,7 @@
       <c r="Q63" s="22"/>
       <c r="R63" s="22"/>
       <c r="S63" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T63" s="39"/>
     </row>
@@ -12884,7 +12969,7 @@
     </row>
     <row r="67" spans="1:20">
       <c r="A67" s="12" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
@@ -12956,7 +13041,7 @@
       </c>
       <c r="S68" s="11"/>
       <c r="T68" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:20">
@@ -12982,9 +13067,9 @@
       <c r="Q69" s="22"/>
       <c r="R69" s="22"/>
       <c r="S69" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T69" s="30">
+        <v>143</v>
+      </c>
+      <c r="T69" s="50">
         <v>0.03</v>
       </c>
     </row>
@@ -13011,9 +13096,9 @@
       <c r="Q70" s="22"/>
       <c r="R70" s="22"/>
       <c r="S70" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T70" s="29">
+        <v>143</v>
+      </c>
+      <c r="T70" s="50">
         <v>0</v>
       </c>
     </row>
@@ -13040,9 +13125,9 @@
       <c r="Q71" s="22"/>
       <c r="R71" s="22"/>
       <c r="S71" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T71" s="30">
+        <v>143</v>
+      </c>
+      <c r="T71" s="50">
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
@@ -13069,9 +13154,9 @@
       <c r="Q72" s="22"/>
       <c r="R72" s="22"/>
       <c r="S72" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T72" s="30">
+        <v>143</v>
+      </c>
+      <c r="T72" s="50">
         <v>0.03</v>
       </c>
     </row>
@@ -13098,9 +13183,9 @@
       <c r="Q73" s="22"/>
       <c r="R73" s="22"/>
       <c r="S73" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T73" s="30">
+        <v>143</v>
+      </c>
+      <c r="T73" s="50">
         <v>0</v>
       </c>
     </row>
@@ -13127,9 +13212,9 @@
       <c r="Q74" s="22"/>
       <c r="R74" s="22"/>
       <c r="S74" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T74" s="30">
+        <v>143</v>
+      </c>
+      <c r="T74" s="50">
         <v>0.03</v>
       </c>
     </row>
@@ -13147,7 +13232,7 @@
     </row>
     <row r="78" spans="1:20" s="18" customFormat="1">
       <c r="A78" s="19" t="s">
-        <v>125</v>
+        <v>2</v>
       </c>
       <c r="B78" s="6"/>
       <c r="T78" s="31"/>
@@ -13203,7 +13288,7 @@
         <v>2015</v>
       </c>
       <c r="T79" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:20" s="18" customFormat="1">
@@ -13228,10 +13313,10 @@
       <c r="Q80" s="22"/>
       <c r="R80" s="22"/>
       <c r="S80" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T80" s="30">
-        <v>0.03</v>
+        <v>143</v>
+      </c>
+      <c r="T80" s="51">
+        <v>450</v>
       </c>
     </row>
     <row r="81" spans="2:20" s="18" customFormat="1">
@@ -13256,9 +13341,9 @@
       <c r="Q81" s="22"/>
       <c r="R81" s="22"/>
       <c r="S81" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T81" s="29">
+        <v>143</v>
+      </c>
+      <c r="T81" s="51">
         <v>0</v>
       </c>
     </row>
@@ -13284,10 +13369,10 @@
       <c r="Q82" s="22"/>
       <c r="R82" s="22"/>
       <c r="S82" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T82" s="30">
-        <v>2.5999999999999999E-2</v>
+        <v>143</v>
+      </c>
+      <c r="T82" s="51">
+        <v>50</v>
       </c>
     </row>
     <row r="83" spans="2:20" s="18" customFormat="1">
@@ -13312,10 +13397,10 @@
       <c r="Q83" s="22"/>
       <c r="R83" s="22"/>
       <c r="S83" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T83" s="30">
-        <v>0.03</v>
+        <v>143</v>
+      </c>
+      <c r="T83" s="51">
+        <v>5000</v>
       </c>
     </row>
     <row r="84" spans="2:20" s="18" customFormat="1">
@@ -13340,9 +13425,9 @@
       <c r="Q84" s="22"/>
       <c r="R84" s="22"/>
       <c r="S84" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T84" s="30">
+        <v>143</v>
+      </c>
+      <c r="T84" s="51">
         <v>0</v>
       </c>
     </row>
@@ -13368,15 +13453,17 @@
       <c r="Q85" s="22"/>
       <c r="R85" s="22"/>
       <c r="S85" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T85" s="30">
-        <v>0.03</v>
+        <v>143</v>
+      </c>
+      <c r="T85" s="51">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -13402,7 +13489,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="14" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -13474,7 +13561,7 @@
       </c>
       <c r="S2" s="13"/>
       <c r="T2" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -13500,7 +13587,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T3" s="29">
         <v>0</v>
@@ -13529,7 +13616,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T4" s="29">
         <v>0</v>
@@ -13558,7 +13645,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T5" s="29">
         <v>400</v>
@@ -13587,7 +13674,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T6" s="29">
         <v>0</v>
@@ -13616,7 +13703,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T7" s="29">
         <v>0</v>
@@ -13645,7 +13732,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T8" s="29">
         <v>0</v>
@@ -13661,7 +13748,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="19" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -13733,13 +13820,13 @@
       </c>
       <c r="S13" s="13"/>
       <c r="T13" s="32" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="13"/>
       <c r="B14" s="43" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="25">
@@ -13766,7 +13853,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T14" s="38"/>
     </row>
@@ -13780,7 +13867,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="14" t="s">
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -13852,13 +13939,13 @@
       </c>
       <c r="S19" s="13"/>
       <c r="T19" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="13"/>
       <c r="B20" s="43" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="C20" s="38"/>
       <c r="D20" s="38">
@@ -13883,11 +13970,12 @@
       <c r="Q20" s="38"/>
       <c r="R20" s="38"/>
       <c r="S20" s="5" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="T20" s="38"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -13914,7 +14002,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1">
       <c r="A1" s="17" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -14218,7 +14306,7 @@
     <row r="11" spans="1:26" s="18" customFormat="1"/>
     <row r="12" spans="1:26">
       <c r="A12" s="17" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -14515,7 +14603,7 @@
     <row r="22" spans="1:26" s="18" customFormat="1"/>
     <row r="23" spans="1:26">
       <c r="A23" s="17" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -14674,7 +14762,7 @@
     <row r="33" spans="1:8" s="18" customFormat="1"/>
     <row r="34" spans="1:8">
       <c r="A34" s="17" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -14793,6 +14881,7 @@
       <c r="H41" s="34"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
small changes to model for population-specific sharing rates
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14200" tabRatio="863" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14200" tabRatio="863" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -31,166 +31,117 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="143">
   <si>
-    <t>Number of people who inject drugs who are on opiate substitution therapy</t>
+    <t>CD4(200-350) to CD4(350-500)</t>
   </si>
   <si>
-    <t>Number of women on PMTCT (Option B/B+)</t>
+    <t>CD4(&lt;200) to CD4(200-350)</t>
   </si>
   <si>
-    <t>Number of voluntary medical male circumcisions performed</t>
+    <t>First-line treatment</t>
   </si>
   <si>
-    <t>Percentage of people covered by pre-exposure prophylaxis</t>
+    <t>Second-line  treatment</t>
   </si>
   <si>
-    <t>Percentage of people coveraged by post-exposure prophylaxis</t>
+    <t>CD4(&gt;500)</t>
   </si>
   <si>
-    <t>Pre-exposure prophylaxis</t>
+    <t>CD4(350-500)</t>
   </si>
   <si>
-    <t>Post-exposure prophylaxis</t>
+    <t>CD4(&lt;200)</t>
   </si>
   <si>
-    <t>Cost</t>
+    <t>CD4(200-350) to CD4(&lt;200)</t>
   </si>
   <si>
-    <t>Cost &amp; coverage</t>
+    <t>Untreated HIV, CD4(&gt;500)</t>
   </si>
   <si>
-    <t>Saturating</t>
+    <t>Untreated HIV, CD4(350-500)</t>
   </si>
   <si>
-    <t>Assumption</t>
+    <t>Untreated HIV, CD4(200-350)</t>
   </si>
   <si>
-    <t>Injecting</t>
+    <t>Untreated HIV, CD4(&lt;200)</t>
   </si>
   <si>
-    <t>Heterosexual insertive</t>
+    <t>MSM</t>
   </si>
   <si>
-    <t>Heterosexual receptive</t>
+    <t>FSW</t>
   </si>
   <si>
-    <t>Homosexual insertive</t>
+    <t>NSP</t>
   </si>
   <si>
-    <t>Homosexual receptive</t>
+    <t>OST</t>
   </si>
   <si>
-    <t>Opiate substitution therapy</t>
+    <t>ART</t>
   </si>
   <si>
-    <t>ARV treatment</t>
+    <t>PMTCT</t>
   </si>
   <si>
-    <t>Percentage of people who die from non-HIV-related causes per year</t>
+    <t>Percentage of people who used a condom at last act with casual partners</t>
   </si>
   <si>
-    <t>Number of HIV tests per year</t>
+    <t>best</t>
   </si>
   <si>
-    <t>Number of HIV diagnoses per year</t>
+    <t>low</t>
   </si>
   <si>
-    <t>Coverage</t>
+    <t>high</t>
   </si>
   <si>
-    <t>Treated HIV</t>
+    <t>Acute infection</t>
   </si>
   <si>
-    <t>Populations</t>
+    <t>On treatment</t>
   </si>
   <si>
-    <t>HIV prevalence</t>
+    <t xml:space="preserve">Circumcision </t>
   </si>
   <si>
-    <t>Number of acts with regular partners per person per year</t>
+    <t xml:space="preserve">STI cofactor increase </t>
   </si>
   <si>
-    <t>Number of acts with casual partners per person per year</t>
+    <t xml:space="preserve">PMTCT </t>
   </si>
   <si>
-    <t>Number of acts with commercial partners per person per year</t>
+    <t>Programs</t>
   </si>
   <si>
-    <t>Gross domestic product</t>
+    <t>Population size</t>
   </si>
   <si>
-    <t>Government revenue</t>
-  </si>
-  <si>
-    <t>Prevalence of any ulcerative STIs</t>
-  </si>
-  <si>
-    <t>Number of people initiating ART each year</t>
-  </si>
-  <si>
-    <t>Percentage of people who used a condom at last act with commercial partners</t>
-  </si>
-  <si>
-    <t>Percentage of people who receptively shared a needle at last injection</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <t>Total</t>
   </si>
   <si>
     <t>Average</t>
-    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>Female sex workers</t>
+    <t>Short name</t>
   </si>
   <si>
-    <t>Clients</t>
+    <t>Long name</t>
   </si>
   <si>
-    <t>Opiate substition therapy</t>
+    <t>Tuberculosis prevalence</t>
   </si>
   <si>
-    <t>Antiretroviral therapy</t>
+    <t>Tuberculosis cofactor</t>
   </si>
   <si>
-    <t>Prevention of mother-to-child transmission</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <t>Diagnosis behavior change</t>
   </si>
   <si>
-    <t>Average</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prevalence of any discharging STIs</t>
-  </si>
-  <si>
-    <t>Percentage of people who used a condom at last act with regular partners</t>
-  </si>
-  <si>
-    <t>Average number of injections per person per year</t>
-  </si>
-  <si>
-    <t>Disease progression rate (% per year)</t>
-  </si>
-  <si>
-    <t>Mother-to-child (breastfeeding)</t>
-  </si>
-  <si>
-    <t>Mother-to-child (non-breastfeeding)</t>
-  </si>
-  <si>
-    <t>Relative disease-related transmissibility</t>
-  </si>
-  <si>
-    <t>Social mitigation costs</t>
-  </si>
-  <si>
-    <t>HIV-related health care costs (excluding treatment)</t>
-  </si>
-  <si>
-    <t>Untreated HIV, acute</t>
-  </si>
-  <si>
-    <t>Disutility weights</t>
+    <t>OR</t>
   </si>
   <si>
     <t>Interactions between casual partners</t>
@@ -358,127 +309,169 @@
     <t>CD4(350-500) to CD4(&gt;500)</t>
   </si>
   <si>
-    <t>CD4(200-350) to CD4(350-500)</t>
+    <t>Number of people who inject drugs who are on opiate substitution therapy</t>
   </si>
   <si>
-    <t>CD4(&lt;200) to CD4(200-350)</t>
+    <t>Number of women on PMTCT (Option B/B+)</t>
   </si>
   <si>
-    <t>First-line treatment</t>
+    <t>Number of voluntary medical male circumcisions performed</t>
   </si>
   <si>
-    <t>Second-line  treatment</t>
+    <t>Percentage of people covered by pre-exposure prophylaxis</t>
   </si>
   <si>
-    <t>CD4(&gt;500)</t>
+    <t>Percentage of people coveraged by post-exposure prophylaxis</t>
   </si>
   <si>
-    <t>CD4(350-500)</t>
+    <t>Pre-exposure prophylaxis</t>
   </si>
   <si>
-    <t>CD4(&lt;200)</t>
+    <t>Post-exposure prophylaxis</t>
   </si>
   <si>
-    <t>CD4(200-350) to CD4(&lt;200)</t>
+    <t>Cost</t>
   </si>
   <si>
-    <t>Untreated HIV, CD4(&gt;500)</t>
+    <t>Cost &amp; coverage</t>
   </si>
   <si>
-    <t>Untreated HIV, CD4(350-500)</t>
+    <t>Saturating</t>
   </si>
   <si>
-    <t>Untreated HIV, CD4(200-350)</t>
+    <t>Assumption</t>
   </si>
   <si>
-    <t>Untreated HIV, CD4(&lt;200)</t>
+    <t>Injecting</t>
   </si>
   <si>
-    <t>MSM</t>
+    <t>Heterosexual insertive</t>
   </si>
   <si>
-    <t>FSW</t>
+    <t>Heterosexual receptive</t>
   </si>
   <si>
-    <t>NSP</t>
+    <t>Homosexual insertive</t>
   </si>
   <si>
-    <t>OST</t>
+    <t>Homosexual receptive</t>
   </si>
   <si>
-    <t>ART</t>
+    <t>Opiate substitution therapy</t>
   </si>
   <si>
-    <t>PMTCT</t>
+    <t>ARV treatment</t>
   </si>
   <si>
-    <t>Percentage of people who used a condom at last act with casual partners</t>
+    <t>Percentage of people who die from non-HIV-related causes per year</t>
   </si>
   <si>
-    <t>best</t>
+    <t>Number of HIV tests per year</t>
   </si>
   <si>
-    <t>low</t>
+    <t>Number of HIV diagnoses per year</t>
   </si>
   <si>
-    <t>high</t>
+    <t>Coverage</t>
   </si>
   <si>
-    <t>Acute infection</t>
+    <t>Treated HIV</t>
   </si>
   <si>
-    <t>On treatment</t>
+    <t>Populations</t>
   </si>
   <si>
-    <t xml:space="preserve">Circumcision </t>
+    <t>HIV prevalence</t>
   </si>
   <si>
-    <t xml:space="preserve">STI cofactor increase </t>
+    <t>Number of acts with regular partners per person per year</t>
   </si>
   <si>
-    <t xml:space="preserve">PMTCT </t>
+    <t>Number of acts with casual partners per person per year</t>
   </si>
   <si>
-    <t>Programs</t>
+    <t>Number of acts with commercial partners per person per year</t>
   </si>
   <si>
-    <t>Population size</t>
+    <t>Gross domestic product</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Government revenue</t>
+  </si>
+  <si>
+    <t>Prevalence of any ulcerative STIs</t>
+  </si>
+  <si>
+    <t>Number of people initiating ART each year</t>
+  </si>
+  <si>
+    <t>Percentage of people who used a condom at last act with commercial partners</t>
+  </si>
+  <si>
+    <t>Percentage of people who receptively shared a needle at last injection</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Female sex workers</t>
+  </si>
+  <si>
+    <t>Clients</t>
+  </si>
+  <si>
+    <t>Opiate substition therapy</t>
+  </si>
+  <si>
+    <t>Antiretroviral therapy</t>
+  </si>
+  <si>
+    <t>Prevention of mother-to-child transmission</t>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Average</t>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>Short name</t>
+    <t>Prevalence of any discharging STIs</t>
   </si>
   <si>
-    <t>Long name</t>
+    <t>Percentage of people who used a condom at last act with regular partners</t>
   </si>
   <si>
-    <t>Tuberculosis prevalence</t>
+    <t>Average number of injections per person per year</t>
   </si>
   <si>
-    <t>Tuberculosis cofactor</t>
+    <t>Disease progression rate (% per year)</t>
   </si>
   <si>
-    <t>Diagnosis behavior change</t>
+    <t>Mother-to-child (breastfeeding)</t>
   </si>
   <si>
-    <t>OR</t>
+    <t>Mother-to-child (non-breastfeeding)</t>
+  </si>
+  <si>
+    <t>Relative disease-related transmissibility</t>
+  </si>
+  <si>
+    <t>Social mitigation costs</t>
+  </si>
+  <si>
+    <t>HIV-related health care costs (excluding treatment)</t>
+  </si>
+  <si>
+    <t>Untreated HIV, acute</t>
+  </si>
+  <si>
+    <t>Disutility weights</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="0.00%"/>
-    <numFmt numFmtId="170" formatCode="0"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -1419,11 +1412,11 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
@@ -2420,36 +2413,36 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="21" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="C2" s="21" t="s">
-        <v>138</v>
+        <v>31</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2457,10 +2450,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E3" s="41" t="b">
         <v>1</v>
@@ -2489,10 +2482,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="E4" s="41" t="b">
         <v>0</v>
@@ -2521,10 +2514,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E5" s="41" t="b">
         <v>1</v>
@@ -2553,10 +2546,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E6" s="41" t="b">
         <v>1</v>
@@ -2585,10 +2578,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="E7" s="41" t="b">
         <v>0</v>
@@ -2617,10 +2610,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E8" s="41" t="b">
         <v>1</v>
@@ -2655,20 +2648,20 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="21" t="s">
-        <v>134</v>
+        <v>27</v>
       </c>
       <c r="B12" s="21"/>
     </row>
     <row r="13" spans="1:11">
       <c r="B13" s="21"/>
       <c r="C13" s="21" t="s">
-        <v>138</v>
+        <v>31</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2676,10 +2669,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="E14" s="41" t="b">
         <v>1</v>
@@ -2690,10 +2683,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="D15" s="45" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E15" s="41" t="b">
         <v>1</v>
@@ -2704,10 +2697,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>37</v>
+        <v>128</v>
       </c>
       <c r="E16" s="41" t="b">
         <v>0</v>
@@ -2718,10 +2711,10 @@
         <v>4</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E17" s="41" t="b">
         <v>1</v>
@@ -2732,10 +2725,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="45" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="E18" s="41" t="b">
         <v>1</v>
@@ -2746,10 +2739,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>123</v>
+        <v>16</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="E19" s="41" t="b">
         <v>0</v>
@@ -2760,10 +2753,10 @@
         <v>7</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>124</v>
+        <v>17</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>39</v>
+        <v>130</v>
       </c>
       <c r="E20" s="41" t="b">
         <v>0</v>
@@ -2797,7 +2790,7 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="2"/>
@@ -2950,7 +2943,7 @@
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="17" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="2"/>
@@ -3089,23 +3082,23 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="19" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1">
       <c r="C2" s="4" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" s="19" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="C3" s="26">
         <v>4.0000000000000002E-4</v>
@@ -3115,7 +3108,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="B4" s="19" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="C4" s="26">
         <v>1E-3</v>
@@ -3125,7 +3118,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="B5" s="19" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="C5" s="26">
         <v>5.9999999999999995E-4</v>
@@ -3135,7 +3128,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="B6" s="19" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="C6" s="26">
         <v>5.0000000000000001E-3</v>
@@ -3145,7 +3138,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="B7" s="19" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="C7" s="26">
         <v>3.0000000000000001E-3</v>
@@ -3155,7 +3148,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="B8" s="19" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="C8" s="25">
         <v>0.05</v>
@@ -3165,7 +3158,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="B9" s="19" t="s">
-        <v>46</v>
+        <v>137</v>
       </c>
       <c r="C9" s="25">
         <v>0.03</v>
@@ -3185,23 +3178,23 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="19" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1">
       <c r="C14" s="4" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" s="19" t="s">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="C15" s="22">
         <v>10</v>
@@ -3211,7 +3204,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="B16" s="19" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="C16" s="22">
         <v>1</v>
@@ -3221,7 +3214,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="B17" s="19" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="C17" s="22">
         <v>1</v>
@@ -3231,7 +3224,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="B18" s="19" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C18" s="22">
         <v>1</v>
@@ -3241,7 +3234,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="B19" s="19" t="s">
-        <v>113</v>
+        <v>6</v>
       </c>
       <c r="C19" s="22">
         <v>3.8</v>
@@ -3261,24 +3254,24 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="19" t="s">
-        <v>44</v>
+        <v>135</v>
       </c>
       <c r="B23" s="19"/>
     </row>
     <row r="24" spans="1:8">
       <c r="C24" s="4" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="B25" s="19" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C25" s="25">
         <v>1</v>
@@ -3288,7 +3281,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="B26" s="19" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="C26" s="25">
         <v>0.25</v>
@@ -3298,7 +3291,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="B27" s="19" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="C27" s="25">
         <v>0.25</v>
@@ -3308,7 +3301,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="B28" s="19" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="C28" s="25">
         <v>0.5</v>
@@ -3328,23 +3321,23 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="19" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="C33" s="4" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="B34" s="19" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="C34" s="25">
         <v>0.45</v>
@@ -3354,7 +3347,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="B35" s="19" t="s">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="C35" s="25">
         <v>0.7</v>
@@ -3364,7 +3357,7 @@
     </row>
     <row r="36" spans="1:8">
       <c r="B36" s="19" t="s">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="C36" s="25">
         <v>0.36</v>
@@ -3387,23 +3380,23 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="19" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="C41" s="4" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="B42" s="19" t="s">
-        <v>109</v>
+        <v>2</v>
       </c>
       <c r="C42" s="25">
         <v>0.2</v>
@@ -3417,7 +3410,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="B43" s="19" t="s">
-        <v>110</v>
+        <v>3</v>
       </c>
       <c r="C43" s="25">
         <v>0.1</v>
@@ -3441,23 +3434,23 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="19" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="C48" s="4" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="B49" s="19" t="s">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="C49" s="25">
         <v>0</v>
@@ -3467,7 +3460,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="B50" s="19" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="C50" s="26">
         <v>5.0000000000000001E-4</v>
@@ -3477,7 +3470,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="B51" s="19" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="C51" s="26">
         <v>1E-3</v>
@@ -3487,7 +3480,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="B52" s="19" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C52" s="25">
         <v>0.01</v>
@@ -3497,7 +3490,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="B53" s="19" t="s">
-        <v>113</v>
+        <v>6</v>
       </c>
       <c r="C53" s="25">
         <v>0.49</v>
@@ -3507,7 +3500,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="B54" s="19" t="s">
-        <v>130</v>
+        <v>23</v>
       </c>
       <c r="C54" s="25">
         <v>0.04</v>
@@ -3517,7 +3510,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="B55" s="19" t="s">
-        <v>141</v>
+        <v>34</v>
       </c>
       <c r="C55" s="22">
         <v>2</v>
@@ -3537,23 +3530,23 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="19" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="C60" s="4" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="B61" s="19" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C61" s="25">
         <v>0.05</v>
@@ -3563,7 +3556,7 @@
     </row>
     <row r="62" spans="1:8">
       <c r="B62" s="19" t="s">
-        <v>131</v>
+        <v>24</v>
       </c>
       <c r="C62" s="25">
         <v>0.3</v>
@@ -3573,7 +3566,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="B63" s="19" t="s">
-        <v>142</v>
+        <v>35</v>
       </c>
       <c r="C63" s="25">
         <v>0.65</v>
@@ -3583,7 +3576,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="B64" s="19" t="s">
-        <v>132</v>
+        <v>25</v>
       </c>
       <c r="C64" s="25">
         <v>3.5</v>
@@ -3593,7 +3586,7 @@
     </row>
     <row r="65" spans="2:5">
       <c r="B65" s="19" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="C65" s="25">
         <v>0.05</v>
@@ -3603,7 +3596,7 @@
     </row>
     <row r="66" spans="2:5">
       <c r="B66" s="19" t="s">
-        <v>133</v>
+        <v>26</v>
       </c>
       <c r="C66" s="25">
         <v>0.05</v>
@@ -3613,7 +3606,7 @@
     </row>
     <row r="67" spans="2:5">
       <c r="B67" s="19" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="C67" s="25">
         <v>0.3</v>
@@ -3623,7 +3616,7 @@
     </row>
     <row r="68" spans="2:5">
       <c r="B68" s="19" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="C68" s="25">
         <v>0.5</v>
@@ -3633,7 +3626,7 @@
     </row>
     <row r="69" spans="2:5">
       <c r="B69" s="19" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="C69" s="25">
         <v>0.5</v>
@@ -3668,7 +3661,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="19" t="s">
-        <v>51</v>
+        <v>142</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -3679,18 +3672,18 @@
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="4" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="18" customFormat="1">
       <c r="B3" s="19" t="s">
-        <v>50</v>
+        <v>141</v>
       </c>
       <c r="C3" s="24">
         <v>0.05</v>
@@ -3701,7 +3694,7 @@
     <row r="4" spans="1:8">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
-        <v>115</v>
+        <v>8</v>
       </c>
       <c r="C4" s="24">
         <v>0.05</v>
@@ -3712,7 +3705,7 @@
     <row r="5" spans="1:8">
       <c r="A5" s="18"/>
       <c r="B5" s="19" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="C5" s="24">
         <v>0.1</v>
@@ -3723,7 +3716,7 @@
     <row r="6" spans="1:8">
       <c r="A6" s="18"/>
       <c r="B6" s="19" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="C6" s="24">
         <v>0.15</v>
@@ -3734,7 +3727,7 @@
     <row r="7" spans="1:8">
       <c r="A7" s="18"/>
       <c r="B7" s="19" t="s">
-        <v>118</v>
+        <v>11</v>
       </c>
       <c r="C7" s="24">
         <v>0.5</v>
@@ -3745,7 +3738,7 @@
     <row r="8" spans="1:8">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="C8" s="24">
         <v>5.2999999999999999E-2</v>
@@ -3773,7 +3766,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="19" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -3784,19 +3777,19 @@
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="4" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="C14" s="22">
         <v>0</v>
@@ -3807,7 +3800,7 @@
     <row r="15" spans="1:8">
       <c r="A15" s="18"/>
       <c r="B15" s="19" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="C15" s="22">
         <v>100</v>
@@ -3818,7 +3811,7 @@
     <row r="16" spans="1:8">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="C16" s="22">
         <v>100</v>
@@ -3829,7 +3822,7 @@
     <row r="17" spans="1:5">
       <c r="A17" s="18"/>
       <c r="B17" s="19" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C17" s="22">
         <v>200</v>
@@ -3840,7 +3833,7 @@
     <row r="18" spans="1:5">
       <c r="A18" s="18"/>
       <c r="B18" s="19" t="s">
-        <v>113</v>
+        <v>6</v>
       </c>
       <c r="C18" s="22">
         <v>450</v>
@@ -3850,7 +3843,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="19" t="s">
-        <v>48</v>
+        <v>139</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -3861,19 +3854,19 @@
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="4" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18"/>
       <c r="B24" s="19" t="s">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="C24" s="22">
         <v>0</v>
@@ -3884,7 +3877,7 @@
     <row r="25" spans="1:5">
       <c r="A25" s="18"/>
       <c r="B25" s="19" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="C25" s="22">
         <v>100</v>
@@ -3895,7 +3888,7 @@
     <row r="26" spans="1:5">
       <c r="A26" s="18"/>
       <c r="B26" s="19" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="C26" s="22">
         <v>100</v>
@@ -3906,7 +3899,7 @@
     <row r="27" spans="1:5">
       <c r="A27" s="18"/>
       <c r="B27" s="19" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C27" s="22">
         <v>1000</v>
@@ -3917,7 +3910,7 @@
     <row r="28" spans="1:5">
       <c r="A28" s="18"/>
       <c r="B28" s="19" t="s">
-        <v>113</v>
+        <v>6</v>
       </c>
       <c r="C28" s="22">
         <v>10000</v>
@@ -3960,7 +3953,7 @@
   <sheetData>
     <row r="1" spans="1:35">
       <c r="A1" s="19" t="s">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="S1" s="18"/>
       <c r="T1" s="18"/>
@@ -4076,13 +4069,13 @@
       </c>
       <c r="AH2" s="18"/>
       <c r="AI2" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:35">
       <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C3" s="22">
         <f t="shared" ref="C3:R3" si="0">D3/(1.12)</f>
@@ -4208,7 +4201,7 @@
         <v>350405950838.15192</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="AI3" s="29"/>
     </row>
@@ -4219,7 +4212,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" s="19" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="S7" s="18"/>
       <c r="T7" s="18"/>
@@ -4335,13 +4328,13 @@
       </c>
       <c r="AH8" s="18"/>
       <c r="AI8" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:35">
       <c r="A9" s="18"/>
       <c r="B9" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C9" s="40">
         <v>30000000000</v>
@@ -4467,13 +4460,13 @@
         <v>180000000000</v>
       </c>
       <c r="AH9" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="AI9" s="29"/>
     </row>
     <row r="13" spans="1:35">
       <c r="A13" s="19" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
@@ -4589,13 +4582,13 @@
       </c>
       <c r="AH14" s="18"/>
       <c r="AI14" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:35">
       <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C15" s="22">
         <v>10000000000</v>
@@ -4721,13 +4714,13 @@
         <v>43219423751.506668</v>
       </c>
       <c r="AH15" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="AI15" s="29"/>
     </row>
     <row r="19" spans="1:35" s="18" customFormat="1">
       <c r="A19" s="19" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B19" s="6"/>
       <c r="AI19" s="6"/>
@@ -4828,12 +4821,12 @@
         <v>2030</v>
       </c>
       <c r="AI20" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:35" s="18" customFormat="1">
       <c r="B21" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -4867,7 +4860,7 @@
       <c r="AF21" s="22"/>
       <c r="AG21" s="22"/>
       <c r="AH21" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="AI21" s="29"/>
     </row>
@@ -4885,7 +4878,7 @@
     </row>
     <row r="25" spans="1:35" s="18" customFormat="1">
       <c r="A25" s="19" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B25" s="6"/>
       <c r="AI25" s="6"/>
@@ -4986,12 +4979,12 @@
         <v>2030</v>
       </c>
       <c r="AI26" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:35" s="18" customFormat="1">
       <c r="B27" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C27" s="22">
         <f>12%*C15</f>
@@ -5118,13 +5111,13 @@
         <v>5186330850.1808004</v>
       </c>
       <c r="AH27" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="AI27" s="29"/>
     </row>
     <row r="31" spans="1:35" s="18" customFormat="1">
       <c r="A31" s="19" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B31" s="6"/>
       <c r="AI31" s="6"/>
@@ -5225,12 +5218,12 @@
         <v>2030</v>
       </c>
       <c r="AI32" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:35" s="18" customFormat="1">
       <c r="B33" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C33" s="22">
         <v>15000000</v>
@@ -5326,7 +5319,7 @@
         <v>18000000</v>
       </c>
       <c r="AH33" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="AI33" s="29"/>
     </row>
@@ -5344,7 +5337,7 @@
     </row>
     <row r="37" spans="1:35" s="18" customFormat="1">
       <c r="A37" s="19" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B37" s="6"/>
       <c r="AI37" s="6"/>
@@ -5445,12 +5438,12 @@
         <v>2030</v>
       </c>
       <c r="AI38" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:35" s="18" customFormat="1">
       <c r="B39" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
@@ -5484,7 +5477,7 @@
       <c r="AF39" s="22"/>
       <c r="AG39" s="22"/>
       <c r="AH39" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="AI39" s="29"/>
     </row>
@@ -5502,7 +5495,7 @@
     </row>
     <row r="43" spans="1:35" s="18" customFormat="1">
       <c r="A43" s="19" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B43" s="6"/>
       <c r="AI43" s="6"/>
@@ -5603,12 +5596,12 @@
         <v>2030</v>
       </c>
       <c r="AI44" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:35" s="18" customFormat="1">
       <c r="B45" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
@@ -5642,13 +5635,13 @@
       <c r="AF45" s="22"/>
       <c r="AG45" s="22"/>
       <c r="AH45" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="AI45" s="29"/>
     </row>
     <row r="49" spans="1:35" s="18" customFormat="1">
       <c r="A49" s="19" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B49" s="6"/>
       <c r="AI49" s="6"/>
@@ -5749,12 +5742,12 @@
         <v>2030</v>
       </c>
       <c r="AI50" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:35" s="18" customFormat="1">
       <c r="B51" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
@@ -5788,7 +5781,7 @@
       <c r="AF51" s="22"/>
       <c r="AG51" s="22"/>
       <c r="AH51" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="AI51" s="29"/>
     </row>
@@ -5806,7 +5799,7 @@
     </row>
     <row r="55" spans="1:35" s="18" customFormat="1">
       <c r="A55" s="19" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B55" s="6"/>
       <c r="AI55" s="6"/>
@@ -5907,12 +5900,12 @@
         <v>2030</v>
       </c>
       <c r="AI56" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:35" s="18" customFormat="1">
       <c r="B57" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C57" s="22"/>
       <c r="D57" s="22"/>
@@ -5946,7 +5939,7 @@
       <c r="AF57" s="22"/>
       <c r="AG57" s="22"/>
       <c r="AH57" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="AI57" s="29"/>
     </row>
@@ -5983,7 +5976,7 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="19" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:22">
@@ -6036,7 +6029,7 @@
         <v>2015</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -6045,7 +6038,7 @@
         <v>SBCC</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="25">
@@ -6078,7 +6071,7 @@
       <c r="R3" s="22"/>
       <c r="S3" s="22"/>
       <c r="T3" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U3" s="25"/>
     </row>
@@ -6088,7 +6081,7 @@
         <v>SBCC</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="27">
@@ -6128,7 +6121,7 @@
       <c r="R4" s="24"/>
       <c r="S4" s="24"/>
       <c r="T4" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U4" s="37"/>
     </row>
@@ -6141,7 +6134,7 @@
         <v>NSP</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="25"/>
@@ -6160,7 +6153,7 @@
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
       <c r="T6" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U6" s="25">
         <v>0.2</v>
@@ -6172,7 +6165,7 @@
         <v>NSP</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="23"/>
@@ -6191,7 +6184,7 @@
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
       <c r="T7" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U7" s="47">
         <v>25000</v>
@@ -6206,7 +6199,7 @@
         <v>OST</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="25"/>
@@ -6227,7 +6220,7 @@
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
       <c r="T9" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U9" s="25"/>
     </row>
@@ -6238,7 +6231,7 @@
         <v>OST</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="23"/>
@@ -6260,7 +6253,7 @@
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
       <c r="T10" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U10" s="37"/>
     </row>
@@ -6275,7 +6268,7 @@
         <v>MSM programs</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="25"/>
@@ -6296,7 +6289,7 @@
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
       <c r="T12" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U12" s="25"/>
       <c r="V12" s="6"/>
@@ -6307,7 +6300,7 @@
         <v>MSM programs</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="23"/>
@@ -6328,7 +6321,7 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
       <c r="T13" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U13" s="37"/>
     </row>
@@ -6338,7 +6331,7 @@
         <v>FSW programs</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="25"/>
@@ -6359,7 +6352,7 @@
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
       <c r="T15" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U15" s="25"/>
     </row>
@@ -6369,7 +6362,7 @@
         <v>FSW programs</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
@@ -6390,7 +6383,7 @@
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
       <c r="T16" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U16" s="37"/>
     </row>
@@ -6400,7 +6393,7 @@
         <v>ART</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="25"/>
@@ -6421,7 +6414,7 @@
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
       <c r="T18" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U18" s="25"/>
     </row>
@@ -6431,7 +6424,7 @@
         <v>ART</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="23"/>
@@ -6453,7 +6446,7 @@
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
       <c r="T19" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U19" s="37"/>
     </row>
@@ -6463,7 +6456,7 @@
         <v>PMTCT</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="25"/>
@@ -6484,7 +6477,7 @@
       <c r="R21" s="22"/>
       <c r="S21" s="22"/>
       <c r="T21" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U21" s="25"/>
     </row>
@@ -6494,7 +6487,7 @@
         <v>PMTCT</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
@@ -6516,14 +6509,13 @@
       <c r="R22" s="22"/>
       <c r="S22" s="22"/>
       <c r="T22" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U22" s="37"/>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6553,7 +6545,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="19" t="s">
-        <v>135</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -6606,7 +6598,7 @@
         <v>2015</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -6615,7 +6607,7 @@
         <v>MSM</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
@@ -6634,7 +6626,7 @@
       <c r="R3" s="27"/>
       <c r="S3" s="27"/>
       <c r="T3" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U3" s="27">
         <v>37500</v>
@@ -6646,7 +6638,7 @@
         <v>MSM</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
@@ -6665,7 +6657,7 @@
       <c r="R4" s="27"/>
       <c r="S4" s="27"/>
       <c r="T4" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U4" s="27">
         <v>21000</v>
@@ -6677,7 +6669,7 @@
         <v>MSM</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
@@ -6696,7 +6688,7 @@
       <c r="R5" s="27"/>
       <c r="S5" s="27"/>
       <c r="T5" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U5" s="27">
         <v>11000</v>
@@ -6713,7 +6705,7 @@
         <v>FSW</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
@@ -6732,7 +6724,7 @@
       <c r="R7" s="27"/>
       <c r="S7" s="27"/>
       <c r="T7" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U7" s="27"/>
     </row>
@@ -6742,7 +6734,7 @@
         <v>FSW</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
@@ -6761,7 +6753,7 @@
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
       <c r="T8" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U8" s="27">
         <v>15000</v>
@@ -6773,7 +6765,7 @@
         <v>FSW</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
@@ -6792,7 +6784,7 @@
       <c r="R9" s="27"/>
       <c r="S9" s="27"/>
       <c r="T9" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U9" s="27"/>
     </row>
@@ -6823,7 +6815,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
@@ -6852,7 +6844,7 @@
       <c r="R11" s="27"/>
       <c r="S11" s="27"/>
       <c r="T11" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U11" s="27"/>
     </row>
@@ -6862,7 +6854,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
@@ -6891,7 +6883,7 @@
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
       <c r="T12" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U12" s="27"/>
     </row>
@@ -6901,7 +6893,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
@@ -6930,7 +6922,7 @@
       <c r="R13" s="27"/>
       <c r="S13" s="27"/>
       <c r="T13" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U13" s="27"/>
     </row>
@@ -6961,7 +6953,7 @@
         <v>Other males</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
@@ -6980,7 +6972,7 @@
       <c r="R15" s="27"/>
       <c r="S15" s="27"/>
       <c r="T15" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U15" s="27"/>
     </row>
@@ -6990,7 +6982,7 @@
         <v>Other males</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D16" s="22">
         <v>4227500</v>
@@ -7041,7 +7033,7 @@
         <v>6118320.6906761518</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U16" s="27"/>
     </row>
@@ -7051,7 +7043,7 @@
         <v>Other males</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
@@ -7070,7 +7062,7 @@
       <c r="R17" s="27"/>
       <c r="S17" s="27"/>
       <c r="T17" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U17" s="27"/>
     </row>
@@ -7101,7 +7093,7 @@
         <v>Other females</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
@@ -7120,7 +7112,7 @@
       <c r="R19" s="27"/>
       <c r="S19" s="27"/>
       <c r="T19" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U19" s="27"/>
     </row>
@@ -7130,7 +7122,7 @@
         <v>Other females</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D20" s="22">
         <v>4759641.7668505535</v>
@@ -7181,7 +7173,7 @@
         <v>7061706.1901886221</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U20" s="27"/>
     </row>
@@ -7191,7 +7183,7 @@
         <v>Other females</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
@@ -7210,7 +7202,7 @@
       <c r="R21" s="27"/>
       <c r="S21" s="27"/>
       <c r="T21" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U21" s="27"/>
     </row>
@@ -7241,7 +7233,7 @@
         <v>Clients</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -7260,7 +7252,7 @@
       <c r="R23" s="27"/>
       <c r="S23" s="27"/>
       <c r="T23" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U23" s="27"/>
     </row>
@@ -7270,7 +7262,7 @@
         <v>Clients</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D24" s="22">
         <v>522500</v>
@@ -7321,7 +7313,7 @@
         <v>756196.93929705245</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U24" s="27"/>
     </row>
@@ -7331,7 +7323,7 @@
         <v>Clients</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -7350,13 +7342,13 @@
       <c r="R25" s="27"/>
       <c r="S25" s="27"/>
       <c r="T25" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U25" s="27"/>
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="19" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -7409,7 +7401,7 @@
         <v>2015</v>
       </c>
       <c r="U30" s="19" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -7418,7 +7410,7 @@
         <v>MSM</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -7439,7 +7431,7 @@
       <c r="R31" s="22"/>
       <c r="S31" s="22"/>
       <c r="T31" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U31" s="26"/>
     </row>
@@ -7449,7 +7441,7 @@
         <v>MSM</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -7470,7 +7462,7 @@
       <c r="R32" s="22"/>
       <c r="S32" s="22"/>
       <c r="T32" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U32" s="26"/>
     </row>
@@ -7480,7 +7472,7 @@
         <v>MSM</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
@@ -7501,7 +7493,7 @@
       <c r="R33" s="22"/>
       <c r="S33" s="22"/>
       <c r="T33" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U33" s="26"/>
     </row>
@@ -7515,7 +7507,7 @@
         <v>FSW</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
@@ -7540,7 +7532,7 @@
       <c r="R35" s="22"/>
       <c r="S35" s="22"/>
       <c r="T35" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U35" s="26"/>
     </row>
@@ -7550,7 +7542,7 @@
         <v>FSW</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -7575,7 +7567,7 @@
       <c r="R36" s="22"/>
       <c r="S36" s="22"/>
       <c r="T36" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U36" s="26"/>
     </row>
@@ -7585,7 +7577,7 @@
         <v>FSW</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
@@ -7610,7 +7602,7 @@
       <c r="R37" s="22"/>
       <c r="S37" s="22"/>
       <c r="T37" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U37" s="26"/>
     </row>
@@ -7624,7 +7616,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
@@ -7649,7 +7641,7 @@
       <c r="R39" s="22"/>
       <c r="S39" s="22"/>
       <c r="T39" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U39" s="26"/>
     </row>
@@ -7659,7 +7651,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
@@ -7684,7 +7676,7 @@
       <c r="R40" s="22"/>
       <c r="S40" s="22"/>
       <c r="T40" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U40" s="26"/>
     </row>
@@ -7694,7 +7686,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
@@ -7719,7 +7711,7 @@
       <c r="R41" s="22"/>
       <c r="S41" s="22"/>
       <c r="T41" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U41" s="26"/>
     </row>
@@ -7733,7 +7725,7 @@
         <v>Other males</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
@@ -7752,7 +7744,7 @@
       <c r="R43" s="22"/>
       <c r="S43" s="22"/>
       <c r="T43" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U43" s="26"/>
     </row>
@@ -7762,7 +7754,7 @@
         <v>Other males</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
@@ -7781,7 +7773,7 @@
       <c r="R44" s="22"/>
       <c r="S44" s="22"/>
       <c r="T44" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U44" s="26">
         <v>5.0000000000000001E-4</v>
@@ -7793,7 +7785,7 @@
         <v>Other males</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
@@ -7812,7 +7804,7 @@
       <c r="R45" s="22"/>
       <c r="S45" s="22"/>
       <c r="T45" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U45" s="26"/>
     </row>
@@ -7826,7 +7818,7 @@
         <v>Other females</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
@@ -7845,7 +7837,7 @@
       <c r="R47" s="22"/>
       <c r="S47" s="22"/>
       <c r="T47" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U47" s="26"/>
     </row>
@@ -7855,7 +7847,7 @@
         <v>Other females</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
@@ -7882,7 +7874,7 @@
       <c r="R48" s="22"/>
       <c r="S48" s="22"/>
       <c r="T48" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U48" s="26"/>
     </row>
@@ -7892,7 +7884,7 @@
         <v>Other females</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
@@ -7911,7 +7903,7 @@
       <c r="R49" s="22"/>
       <c r="S49" s="22"/>
       <c r="T49" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U49" s="26"/>
     </row>
@@ -7925,7 +7917,7 @@
         <v>Clients</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
@@ -7944,7 +7936,7 @@
       <c r="R51" s="22"/>
       <c r="S51" s="22"/>
       <c r="T51" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U51" s="26"/>
     </row>
@@ -7954,7 +7946,7 @@
         <v>Clients</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
@@ -7973,7 +7965,7 @@
       <c r="R52" s="22"/>
       <c r="S52" s="22"/>
       <c r="T52" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U52" s="26">
         <v>0.01</v>
@@ -7985,7 +7977,7 @@
         <v>Clients</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
@@ -8004,7 +7996,7 @@
       <c r="R53" s="22"/>
       <c r="S53" s="22"/>
       <c r="T53" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="U53" s="26"/>
     </row>
@@ -8036,7 +8028,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="10" t="s">
-        <v>19</v>
+        <v>111</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -8109,13 +8101,13 @@
       </c>
       <c r="S2" s="9"/>
       <c r="T2" s="10" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="9"/>
       <c r="B3" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -8134,7 +8126,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T3" s="22"/>
     </row>
@@ -8146,7 +8138,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="10" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -8219,13 +8211,13 @@
       </c>
       <c r="S8" s="9"/>
       <c r="T8" s="10" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -8268,7 +8260,7 @@
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
       <c r="S9" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T9" s="22"/>
     </row>
@@ -8280,7 +8272,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="10" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -8353,13 +8345,13 @@
       </c>
       <c r="S14" s="9"/>
       <c r="T14" s="10" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="9"/>
       <c r="B15" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -8378,7 +8370,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T15" s="22"/>
     </row>
@@ -8390,7 +8382,7 @@
     </row>
     <row r="19" spans="1:20" s="18" customFormat="1">
       <c r="A19" s="19" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B19" s="6"/>
     </row>
@@ -8445,12 +8437,12 @@
         <v>2015</v>
       </c>
       <c r="T20" s="19" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:20" s="18" customFormat="1">
       <c r="B21" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -8469,7 +8461,7 @@
       <c r="Q21" s="22"/>
       <c r="R21" s="22"/>
       <c r="S21" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T21" s="22"/>
     </row>
@@ -8484,7 +8476,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="10" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -8557,13 +8549,13 @@
       </c>
       <c r="S26" s="9"/>
       <c r="T26" s="10" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="9"/>
       <c r="B27" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
@@ -8582,13 +8574,13 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T27" s="22"/>
     </row>
     <row r="31" spans="1:20" s="18" customFormat="1">
       <c r="A31" s="19" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="B31" s="6"/>
     </row>
@@ -8643,12 +8635,12 @@
         <v>2015</v>
       </c>
       <c r="T32" s="19" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="2:20" s="18" customFormat="1">
       <c r="B33" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
@@ -8667,7 +8659,7 @@
       <c r="Q33" s="22"/>
       <c r="R33" s="22"/>
       <c r="S33" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T33" s="22"/>
     </row>
@@ -8698,7 +8690,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="18" customFormat="1">
       <c r="A1" s="19" t="s">
-        <v>18</v>
+        <v>110</v>
       </c>
       <c r="B1" s="6"/>
     </row>
@@ -8753,7 +8745,7 @@
         <v>2015</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="18" customFormat="1">
@@ -8778,7 +8770,7 @@
       <c r="Q3" s="25"/>
       <c r="R3" s="25"/>
       <c r="S3" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T3" s="25">
         <v>0.01</v>
@@ -8806,7 +8798,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T4" s="25">
         <v>0.01</v>
@@ -8834,7 +8826,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T5" s="25">
         <v>0.03</v>
@@ -8862,7 +8854,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T6" s="25">
         <v>0.01</v>
@@ -8890,7 +8882,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T7" s="25">
         <v>0.01</v>
@@ -8918,7 +8910,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T8" s="25">
         <v>0.01</v>
@@ -8935,7 +8927,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="8" t="s">
-        <v>30</v>
+        <v>122</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -9008,7 +9000,7 @@
       </c>
       <c r="S13" s="7"/>
       <c r="T13" s="8" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -9034,7 +9026,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T14" s="25">
         <v>0</v>
@@ -9063,7 +9055,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T15" s="25">
         <v>0</v>
@@ -9092,7 +9084,7 @@
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T16" s="25">
         <v>0</v>
@@ -9121,7 +9113,7 @@
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T17" s="25">
         <v>0</v>
@@ -9150,7 +9142,7 @@
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T18" s="25">
         <v>0</v>
@@ -9179,7 +9171,7 @@
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T19" s="25">
         <v>0</v>
@@ -9196,7 +9188,7 @@
     </row>
     <row r="23" spans="1:20" s="18" customFormat="1">
       <c r="A23" s="19" t="s">
-        <v>41</v>
+        <v>132</v>
       </c>
       <c r="B23" s="6"/>
     </row>
@@ -9251,7 +9243,7 @@
         <v>2015</v>
       </c>
       <c r="T24" s="19" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:20" s="18" customFormat="1">
@@ -9276,7 +9268,7 @@
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T25" s="25">
         <v>0</v>
@@ -9304,7 +9296,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T26" s="25">
         <v>0</v>
@@ -9332,7 +9324,7 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T27" s="25">
         <v>0</v>
@@ -9360,7 +9352,7 @@
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
       <c r="S28" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T28" s="25">
         <v>0</v>
@@ -9388,7 +9380,7 @@
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
       <c r="S29" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T29" s="25">
         <v>0</v>
@@ -9416,7 +9408,7 @@
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
       <c r="S30" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T30" s="25">
         <v>0</v>
@@ -9435,7 +9427,7 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="8" t="s">
-        <v>140</v>
+        <v>33</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -9508,7 +9500,7 @@
       </c>
       <c r="S35" s="7"/>
       <c r="T35" s="8" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -9534,7 +9526,7 @@
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
       <c r="S36" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T36" s="25">
         <v>0</v>
@@ -9562,7 +9554,7 @@
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
       <c r="S37" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T37" s="25">
         <v>0</v>
@@ -9590,7 +9582,7 @@
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
       <c r="S38" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T38" s="25">
         <v>0</v>
@@ -9618,7 +9610,7 @@
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
       <c r="S39" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T39" s="25">
         <v>0</v>
@@ -9646,7 +9638,7 @@
       <c r="Q40" s="22"/>
       <c r="R40" s="22"/>
       <c r="S40" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T40" s="25">
         <v>0</v>
@@ -9674,7 +9666,7 @@
       <c r="Q41" s="22"/>
       <c r="R41" s="22"/>
       <c r="S41" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T41" s="25">
         <v>0</v>
@@ -9684,7 +9676,6 @@
       <c r="S42" s="5"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -9712,7 +9703,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="10" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -9785,7 +9776,7 @@
       </c>
       <c r="S2" s="9"/>
       <c r="T2" s="10" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -9811,7 +9802,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T3" s="25">
         <v>0.03</v>
@@ -9844,7 +9835,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T4" s="25"/>
     </row>
@@ -9877,7 +9868,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T5" s="22"/>
     </row>
@@ -9904,7 +9895,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T6" s="25">
         <v>0.01</v>
@@ -9933,7 +9924,7 @@
       <c r="Q7" s="25"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T7" s="25">
         <v>0.01</v>
@@ -9962,7 +9953,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T8" s="25">
         <v>0.05</v>
@@ -9976,7 +9967,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="10" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -10049,13 +10040,13 @@
       </c>
       <c r="S13" s="9"/>
       <c r="T13" s="10" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="9"/>
       <c r="B14" s="4" t="s">
-        <v>137</v>
+        <v>30</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -10074,7 +10065,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T14" s="25">
         <v>0.5</v>
@@ -10088,7 +10079,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="10" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -10161,13 +10152,13 @@
       </c>
       <c r="S19" s="9"/>
       <c r="T19" s="10" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="9"/>
       <c r="B20" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C20" s="22">
         <v>0</v>
@@ -10214,7 +10205,7 @@
       <c r="Q20" s="22"/>
       <c r="R20" s="22"/>
       <c r="S20" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T20" s="22"/>
     </row>
@@ -10226,7 +10217,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="10" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -10299,13 +10290,13 @@
       </c>
       <c r="S25" s="9"/>
       <c r="T25" s="10" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="9"/>
       <c r="B26" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C26" s="22">
         <v>0</v>
@@ -10352,7 +10343,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T26" s="22"/>
     </row>
@@ -10367,7 +10358,7 @@
     </row>
     <row r="30" spans="1:20" s="18" customFormat="1">
       <c r="A30" s="19" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="B30" s="6"/>
     </row>
@@ -10422,7 +10413,7 @@
         <v>2015</v>
       </c>
       <c r="T31" s="19" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:20" s="18" customFormat="1">
@@ -10447,7 +10438,7 @@
       <c r="Q32" s="22"/>
       <c r="R32" s="22"/>
       <c r="S32" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T32" s="24">
         <v>0</v>
@@ -10475,7 +10466,7 @@
       <c r="Q33" s="22"/>
       <c r="R33" s="22"/>
       <c r="S33" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T33" s="24">
         <v>0</v>
@@ -10503,7 +10494,7 @@
       <c r="Q34" s="22"/>
       <c r="R34" s="22"/>
       <c r="S34" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T34" s="24">
         <v>0</v>
@@ -10531,7 +10522,7 @@
       <c r="Q35" s="22"/>
       <c r="R35" s="22"/>
       <c r="S35" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T35" s="24">
         <v>0</v>
@@ -10559,7 +10550,7 @@
       <c r="Q36" s="25"/>
       <c r="R36" s="22"/>
       <c r="S36" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T36" s="24">
         <f>2/50</f>
@@ -10588,7 +10579,7 @@
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
       <c r="S37" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T37" s="24">
         <v>0</v>
@@ -10602,7 +10593,7 @@
     </row>
     <row r="41" spans="1:20" s="18" customFormat="1">
       <c r="A41" s="19" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="B41" s="6"/>
     </row>
@@ -10657,7 +10648,7 @@
         <v>2015</v>
       </c>
       <c r="T42" s="19" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:20" s="18" customFormat="1">
@@ -10682,7 +10673,7 @@
       <c r="Q43" s="22"/>
       <c r="R43" s="22"/>
       <c r="S43" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T43" s="24">
         <v>0</v>
@@ -10710,7 +10701,7 @@
       <c r="Q44" s="22"/>
       <c r="R44" s="22"/>
       <c r="S44" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T44" s="24">
         <v>0</v>
@@ -10738,7 +10729,7 @@
       <c r="Q45" s="22"/>
       <c r="R45" s="22"/>
       <c r="S45" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T45" s="24">
         <v>0</v>
@@ -10766,7 +10757,7 @@
       <c r="Q46" s="22"/>
       <c r="R46" s="22"/>
       <c r="S46" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T46" s="24">
         <v>0</v>
@@ -10794,7 +10785,7 @@
       <c r="Q47" s="25"/>
       <c r="R47" s="22"/>
       <c r="S47" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T47" s="24">
         <f>2/50</f>
@@ -10823,7 +10814,7 @@
       <c r="Q48" s="22"/>
       <c r="R48" s="22"/>
       <c r="S48" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T48" s="24">
         <v>0</v>
@@ -10840,7 +10831,7 @@
     </row>
     <row r="52" spans="1:20">
       <c r="A52" s="10" t="s">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
@@ -10913,13 +10904,13 @@
       </c>
       <c r="S53" s="9"/>
       <c r="T53" s="10" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:20">
       <c r="A54" s="9"/>
       <c r="B54" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C54" s="27"/>
       <c r="D54" s="27"/>
@@ -10948,7 +10939,7 @@
       <c r="Q54" s="27"/>
       <c r="R54" s="27"/>
       <c r="S54" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T54" s="22"/>
     </row>
@@ -10963,7 +10954,7 @@
     </row>
     <row r="58" spans="1:20" s="18" customFormat="1">
       <c r="A58" s="19" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B58" s="6"/>
     </row>
@@ -11018,7 +11009,7 @@
         <v>2015</v>
       </c>
       <c r="T59" s="19" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:20" s="18" customFormat="1">
@@ -11043,7 +11034,7 @@
       <c r="Q60" s="22"/>
       <c r="R60" s="22"/>
       <c r="S60" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T60" s="24">
         <v>0</v>
@@ -11071,7 +11062,7 @@
       <c r="Q61" s="22"/>
       <c r="R61" s="22"/>
       <c r="S61" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T61" s="24">
         <v>0</v>
@@ -11099,7 +11090,7 @@
       <c r="Q62" s="22"/>
       <c r="R62" s="22"/>
       <c r="S62" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T62" s="24">
         <v>0</v>
@@ -11127,7 +11118,7 @@
       <c r="Q63" s="22"/>
       <c r="R63" s="22"/>
       <c r="S63" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T63" s="24">
         <v>0</v>
@@ -11155,7 +11146,7 @@
       <c r="Q64" s="25"/>
       <c r="R64" s="22"/>
       <c r="S64" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T64" s="24">
         <f>2/50</f>
@@ -11184,7 +11175,7 @@
       <c r="Q65" s="22"/>
       <c r="R65" s="22"/>
       <c r="S65" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T65" s="24">
         <v>0</v>
@@ -11192,7 +11183,7 @@
     </row>
     <row r="69" spans="1:20" s="18" customFormat="1">
       <c r="A69" s="19" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B69" s="6"/>
     </row>
@@ -11247,12 +11238,12 @@
         <v>2015</v>
       </c>
       <c r="T70" s="19" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:20" s="18" customFormat="1">
       <c r="B71" s="4" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="C71" s="22"/>
       <c r="D71" s="22"/>
@@ -11271,14 +11262,13 @@
       <c r="Q71" s="22"/>
       <c r="R71" s="22"/>
       <c r="S71" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T71" s="25">
         <v>0.3</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -11294,7 +11284,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H53" workbookViewId="0">
+    <sheetView topLeftCell="H53" workbookViewId="0">
       <selection activeCell="T87" sqref="T87"/>
     </sheetView>
   </sheetViews>
@@ -11306,7 +11296,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="12" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -11378,7 +11368,7 @@
       </c>
       <c r="S2" s="11"/>
       <c r="T2" s="32" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -11404,7 +11394,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T3" s="33">
         <v>80</v>
@@ -11433,7 +11423,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T4" s="33">
         <v>80</v>
@@ -11462,7 +11452,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T5" s="33">
         <v>80</v>
@@ -11491,7 +11481,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T6" s="33">
         <v>80</v>
@@ -11520,7 +11510,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T7" s="33">
         <v>80</v>
@@ -11549,7 +11539,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T8" s="33">
         <v>80</v>
@@ -11565,7 +11555,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="12" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -11637,7 +11627,7 @@
       </c>
       <c r="S13" s="11"/>
       <c r="T13" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -11663,7 +11653,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T14" s="29">
         <v>10</v>
@@ -11692,7 +11682,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T15" s="29">
         <v>10</v>
@@ -11721,7 +11711,7 @@
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T16" s="29">
         <v>10</v>
@@ -11750,7 +11740,7 @@
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T17" s="29">
         <v>10</v>
@@ -11779,7 +11769,7 @@
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T18" s="29">
         <v>10</v>
@@ -11808,7 +11798,7 @@
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T19" s="29">
         <v>10</v>
@@ -11824,7 +11814,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="12" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -11896,7 +11886,7 @@
       </c>
       <c r="S24" s="11"/>
       <c r="T24" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -11922,7 +11912,7 @@
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T25" s="29">
         <v>0</v>
@@ -11951,7 +11941,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T26" s="29">
         <v>500</v>
@@ -11980,7 +11970,7 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T27" s="29">
         <v>0</v>
@@ -12009,7 +11999,7 @@
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
       <c r="S28" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T28" s="29">
         <v>0</v>
@@ -12038,7 +12028,7 @@
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
       <c r="S29" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T29" s="29">
         <v>0</v>
@@ -12067,7 +12057,7 @@
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
       <c r="S30" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T30" s="29">
         <v>10</v>
@@ -12152,7 +12142,7 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="12" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -12224,7 +12214,7 @@
       </c>
       <c r="S35" s="11"/>
       <c r="T35" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -12250,7 +12240,7 @@
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
       <c r="S36" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T36" s="30">
         <v>0.4</v>
@@ -12289,7 +12279,7 @@
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
       <c r="S37" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T37" s="30"/>
     </row>
@@ -12316,7 +12306,7 @@
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
       <c r="S38" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T38" s="30">
         <v>0.05</v>
@@ -12345,7 +12335,7 @@
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
       <c r="S39" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T39" s="30">
         <v>0.05</v>
@@ -12374,7 +12364,7 @@
       <c r="Q40" s="22"/>
       <c r="R40" s="22"/>
       <c r="S40" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T40" s="30">
         <v>0.05</v>
@@ -12403,7 +12393,7 @@
       <c r="Q41" s="22"/>
       <c r="R41" s="22"/>
       <c r="S41" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T41" s="30">
         <v>7.0000000000000007E-2</v>
@@ -12419,7 +12409,7 @@
     </row>
     <row r="45" spans="1:20">
       <c r="A45" s="19" t="s">
-        <v>125</v>
+        <v>18</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
@@ -12491,7 +12481,7 @@
       </c>
       <c r="S46" s="11"/>
       <c r="T46" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:20">
@@ -12517,7 +12507,7 @@
       <c r="Q47" s="22"/>
       <c r="R47" s="22"/>
       <c r="S47" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T47" s="30">
         <v>0.6</v>
@@ -12556,7 +12546,7 @@
       <c r="Q48" s="22"/>
       <c r="R48" s="22"/>
       <c r="S48" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T48" s="30"/>
     </row>
@@ -12583,7 +12573,7 @@
       <c r="Q49" s="22"/>
       <c r="R49" s="22"/>
       <c r="S49" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T49" s="30">
         <v>0.5</v>
@@ -12618,7 +12608,7 @@
       <c r="Q50" s="22"/>
       <c r="R50" s="22"/>
       <c r="S50" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T50" s="30"/>
     </row>
@@ -12651,7 +12641,7 @@
       <c r="Q51" s="22"/>
       <c r="R51" s="22"/>
       <c r="S51" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T51" s="30"/>
     </row>
@@ -12678,7 +12668,7 @@
       <c r="Q52" s="22"/>
       <c r="R52" s="22"/>
       <c r="S52" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T52" s="30">
         <v>0.5</v>
@@ -12694,7 +12684,7 @@
     </row>
     <row r="56" spans="1:20">
       <c r="A56" s="19" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
@@ -12766,7 +12756,7 @@
       </c>
       <c r="S57" s="11"/>
       <c r="T57" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:20">
@@ -12792,7 +12782,7 @@
       <c r="Q58" s="22"/>
       <c r="R58" s="22"/>
       <c r="S58" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T58" s="29">
         <v>0</v>
@@ -12831,7 +12821,7 @@
       <c r="Q59" s="22"/>
       <c r="R59" s="22"/>
       <c r="S59" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T59" s="38"/>
     </row>
@@ -12858,7 +12848,7 @@
       <c r="Q60" s="22"/>
       <c r="R60" s="22"/>
       <c r="S60" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T60" s="30">
         <v>0</v>
@@ -12887,7 +12877,7 @@
       <c r="Q61" s="22"/>
       <c r="R61" s="22"/>
       <c r="S61" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T61" s="30">
         <v>0</v>
@@ -12916,7 +12906,7 @@
       <c r="Q62" s="22"/>
       <c r="R62" s="22"/>
       <c r="S62" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T62" s="29">
         <v>0</v>
@@ -12955,7 +12945,7 @@
       <c r="Q63" s="22"/>
       <c r="R63" s="22"/>
       <c r="S63" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T63" s="39"/>
     </row>
@@ -12969,7 +12959,7 @@
     </row>
     <row r="67" spans="1:20">
       <c r="A67" s="12" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
@@ -13041,7 +13031,7 @@
       </c>
       <c r="S68" s="11"/>
       <c r="T68" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:20">
@@ -13067,7 +13057,7 @@
       <c r="Q69" s="22"/>
       <c r="R69" s="22"/>
       <c r="S69" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T69" s="50">
         <v>0.03</v>
@@ -13096,7 +13086,7 @@
       <c r="Q70" s="22"/>
       <c r="R70" s="22"/>
       <c r="S70" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T70" s="50">
         <v>0</v>
@@ -13125,7 +13115,7 @@
       <c r="Q71" s="22"/>
       <c r="R71" s="22"/>
       <c r="S71" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T71" s="50">
         <v>2.5999999999999999E-2</v>
@@ -13154,7 +13144,7 @@
       <c r="Q72" s="22"/>
       <c r="R72" s="22"/>
       <c r="S72" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T72" s="50">
         <v>0.03</v>
@@ -13183,7 +13173,7 @@
       <c r="Q73" s="22"/>
       <c r="R73" s="22"/>
       <c r="S73" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T73" s="50">
         <v>0</v>
@@ -13212,7 +13202,7 @@
       <c r="Q74" s="22"/>
       <c r="R74" s="22"/>
       <c r="S74" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T74" s="50">
         <v>0.03</v>
@@ -13232,7 +13222,7 @@
     </row>
     <row r="78" spans="1:20" s="18" customFormat="1">
       <c r="A78" s="19" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="B78" s="6"/>
       <c r="T78" s="31"/>
@@ -13288,7 +13278,7 @@
         <v>2015</v>
       </c>
       <c r="T79" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" spans="1:20" s="18" customFormat="1">
@@ -13313,7 +13303,7 @@
       <c r="Q80" s="22"/>
       <c r="R80" s="22"/>
       <c r="S80" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T80" s="51">
         <v>450</v>
@@ -13341,7 +13331,7 @@
       <c r="Q81" s="22"/>
       <c r="R81" s="22"/>
       <c r="S81" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T81" s="51">
         <v>0</v>
@@ -13369,7 +13359,7 @@
       <c r="Q82" s="22"/>
       <c r="R82" s="22"/>
       <c r="S82" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T82" s="51">
         <v>50</v>
@@ -13397,7 +13387,7 @@
       <c r="Q83" s="22"/>
       <c r="R83" s="22"/>
       <c r="S83" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T83" s="51">
         <v>5000</v>
@@ -13425,7 +13415,7 @@
       <c r="Q84" s="22"/>
       <c r="R84" s="22"/>
       <c r="S84" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T84" s="51">
         <v>0</v>
@@ -13453,17 +13443,15 @@
       <c r="Q85" s="22"/>
       <c r="R85" s="22"/>
       <c r="S85" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T85" s="51">
         <v>500</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -13475,10 +13463,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z19" sqref="Z19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
@@ -13489,7 +13477,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="14" t="s">
-        <v>43</v>
+        <v>134</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -13561,7 +13549,7 @@
       </c>
       <c r="S2" s="13"/>
       <c r="T2" s="4" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -13587,7 +13575,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T3" s="29">
         <v>0</v>
@@ -13616,7 +13604,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T4" s="29">
         <v>0</v>
@@ -13645,7 +13633,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T5" s="29">
         <v>400</v>
@@ -13674,7 +13662,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T6" s="29">
         <v>0</v>
@@ -13703,7 +13691,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T7" s="29">
         <v>0</v>
@@ -13732,7 +13720,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="T8" s="29">
         <v>0</v>
@@ -13748,7 +13736,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="19" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -13820,32 +13808,25 @@
       </c>
       <c r="S13" s="13"/>
       <c r="T13" s="32" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="13"/>
-      <c r="B14" s="43" t="s">
-        <v>34</v>
+      <c r="B14" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>MSM</v>
       </c>
       <c r="C14" s="22"/>
-      <c r="D14" s="25">
-        <v>0.3</v>
-      </c>
+      <c r="D14" s="22"/>
       <c r="E14" s="22"/>
-      <c r="F14" s="25">
-        <v>0.25</v>
-      </c>
+      <c r="F14" s="22"/>
       <c r="G14" s="22"/>
-      <c r="H14" s="25">
-        <v>0.2</v>
-      </c>
+      <c r="H14" s="22"/>
       <c r="I14" s="22"/>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
-      <c r="L14" s="25">
-        <v>0.2</v>
-      </c>
+      <c r="L14" s="22"/>
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
       <c r="O14" s="22"/>
@@ -13853,131 +13834,279 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="T14" s="38"/>
+        <v>36</v>
+      </c>
+      <c r="T14" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" s="18" customFormat="1">
+      <c r="B15" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>FSW</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T15" s="29">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:20" s="18" customFormat="1">
-      <c r="B16" s="6"/>
-      <c r="T16" s="31"/>
+      <c r="B16" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>Male PWID</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="25">
+        <v>0.3</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="H16" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T16" s="38"/>
     </row>
     <row r="17" spans="1:20" s="18" customFormat="1">
-      <c r="B17" s="6"/>
-      <c r="T17" s="31"/>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18" s="14" t="s">
+      <c r="B17" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>Other males</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T17" s="29">
         <v>0</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19" s="13"/>
-      <c r="C19" s="14">
+    </row>
+    <row r="18" spans="1:20" s="18" customFormat="1">
+      <c r="B18" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Other females</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T18" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" s="18" customFormat="1">
+      <c r="B19" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$8</f>
+        <v>Clients</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T19" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" s="18" customFormat="1">
+      <c r="B21" s="6"/>
+      <c r="T21" s="31"/>
+    </row>
+    <row r="22" spans="1:20" s="18" customFormat="1">
+      <c r="B22" s="6"/>
+      <c r="T22" s="31"/>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="13"/>
+      <c r="C24" s="14">
         <v>2000</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D24" s="14">
         <v>2001</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E24" s="14">
         <v>2002</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F24" s="14">
         <v>2003</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G24" s="14">
         <v>2004</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H24" s="14">
         <v>2005</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I24" s="14">
         <v>2006</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J24" s="14">
         <v>2007</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K24" s="14">
         <v>2008</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L24" s="14">
         <v>2009</v>
       </c>
-      <c r="M19" s="14">
+      <c r="M24" s="14">
         <v>2010</v>
       </c>
-      <c r="N19" s="14">
+      <c r="N24" s="14">
         <v>2011</v>
       </c>
-      <c r="O19" s="14">
+      <c r="O24" s="14">
         <v>2012</v>
       </c>
-      <c r="P19" s="14">
+      <c r="P24" s="14">
         <v>2013</v>
       </c>
-      <c r="Q19" s="14">
+      <c r="Q24" s="14">
         <v>2014</v>
       </c>
-      <c r="R19" s="14">
+      <c r="R24" s="14">
         <v>2015</v>
       </c>
-      <c r="S19" s="13"/>
-      <c r="T19" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="A20" s="13"/>
-      <c r="B20" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38">
+      <c r="S24" s="13"/>
+      <c r="T24" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="13"/>
+      <c r="B25" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38">
         <v>50</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38">
+      <c r="E25" s="38"/>
+      <c r="F25" s="38">
         <v>70</v>
       </c>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38">
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38">
         <v>190</v>
       </c>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="T20" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T25" s="38"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -14002,7 +14131,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1">
       <c r="A1" s="17" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -14306,7 +14435,7 @@
     <row r="11" spans="1:26" s="18" customFormat="1"/>
     <row r="12" spans="1:26">
       <c r="A12" s="17" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -14603,7 +14732,7 @@
     <row r="22" spans="1:26" s="18" customFormat="1"/>
     <row r="23" spans="1:26">
       <c r="A23" s="17" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -14762,7 +14891,7 @@
     <row r="33" spans="1:8" s="18" customFormat="1"/>
     <row r="34" spans="1:8">
       <c r="A34" s="17" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -14881,7 +15010,6 @@
       <c r="H41" s="34"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
working on cd4 stratifications
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="14205" tabRatio="863" activeTab="6"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="14205" tabRatio="863" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="147">
   <si>
     <t>Number of people who inject drugs who are on opiate substitution therapy</t>
   </si>
@@ -342,9 +342,6 @@
     <t>Untreated HIV, CD4(200-350)</t>
   </si>
   <si>
-    <t>Untreated HIV, CD4(&lt;200)</t>
-  </si>
-  <si>
     <t>MSM</t>
   </si>
   <si>
@@ -472,6 +469,12 @@
   </si>
   <si>
     <t>Purchasing power parity</t>
+  </si>
+  <si>
+    <t>Untreated HIV, CD4(50-200)</t>
+  </si>
+  <si>
+    <t>Untreated HIV, CD4(&lt;50)</t>
   </si>
 </sst>
 </file>
@@ -2427,10 +2430,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>121</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>122</v>
       </c>
       <c r="E2" s="44" t="s">
         <v>50</v>
@@ -2459,7 +2462,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>53</v>
@@ -2491,7 +2494,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>24</v>
@@ -2657,17 +2660,17 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B12" s="21"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="21"/>
       <c r="C13" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="21" t="s">
         <v>121</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>122</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>7</v>
@@ -2692,7 +2695,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>56</v>
@@ -2706,7 +2709,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="41" t="s">
         <v>26</v>
@@ -2748,7 +2751,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D19" s="41" t="s">
         <v>27</v>
@@ -2762,7 +2765,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D20" s="42" t="s">
         <v>28</v>
@@ -3076,10 +3079,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3096,13 +3099,13 @@
     </row>
     <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
@@ -3112,7 +3115,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="26">
         <v>4.0000000000000002E-4</v>
@@ -3126,7 +3129,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="26">
         <v>8.0000000000000004E-4</v>
@@ -3140,7 +3143,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" s="26">
         <v>1.38E-2</v>
@@ -3154,7 +3157,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" s="26">
         <v>1.1000000000000001E-3</v>
@@ -3168,7 +3171,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" s="26">
         <v>8.0000000000000002E-3</v>
@@ -3225,18 +3228,18 @@
     </row>
     <row r="14" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C15" s="22">
         <v>26.03</v>
@@ -3292,7 +3295,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C19" s="22">
         <v>3.49</v>
@@ -3306,7 +3309,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C20" s="22">
         <v>7.17</v>
@@ -3336,13 +3339,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -3389,7 +3392,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C29" s="25">
         <v>0.27</v>
@@ -3403,7 +3406,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C30" s="25">
         <v>0.67</v>
@@ -3432,13 +3435,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3471,7 +3474,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C38" s="25">
         <v>0.47</v>
@@ -3485,7 +3488,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C39" s="25">
         <v>1.52</v>
@@ -3517,13 +3520,13 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C44" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3571,18 +3574,18 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C51" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C52" s="26">
         <v>3.5999999999999999E-3</v>
@@ -3638,7 +3641,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C56" s="26">
         <v>5.8999999999999997E-2</v>
@@ -3652,7 +3655,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B57" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C57" s="26">
         <v>0.32300000000000001</v>
@@ -3666,7 +3669,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C58" s="26">
         <v>0.23</v>
@@ -3680,7 +3683,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B59" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C59" s="22">
         <v>2.17</v>
@@ -3709,13 +3712,13 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C64" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="E64" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3734,7 +3737,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B66" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C66" s="26">
         <v>0.42</v>
@@ -3748,7 +3751,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C67" s="26">
         <v>1</v>
@@ -3762,7 +3765,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C68" s="26">
         <v>2.65</v>
@@ -3790,7 +3793,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C70" s="26">
         <v>0.105</v>
@@ -3837,13 +3840,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C77" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D77" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="E77" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3888,23 +3891,33 @@
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="19" t="s">
-        <v>102</v>
+        <v>145</v>
       </c>
       <c r="C82" s="24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D82" s="22"/>
       <c r="E82" s="22"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="19" t="s">
-        <v>14</v>
+        <v>146</v>
       </c>
       <c r="C83" s="24">
-        <v>5.2999999999999999E-2</v>
+        <v>0.6</v>
       </c>
       <c r="D83" s="22"/>
       <c r="E83" s="22"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84" s="24">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D84" s="22"/>
+      <c r="E84" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
@@ -3940,7 +3953,7 @@
   <sheetData>
     <row r="1" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B1" s="6"/>
       <c r="AI1" s="6"/>
@@ -4046,7 +4059,7 @@
     </row>
     <row r="3" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -4080,7 +4093,7 @@
       <c r="AF3" s="22"/>
       <c r="AG3" s="22"/>
       <c r="AH3" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI3" s="29"/>
     </row>
@@ -4098,7 +4111,7 @@
     </row>
     <row r="7" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B7" s="6"/>
       <c r="AI7" s="6"/>
@@ -4204,7 +4217,7 @@
     </row>
     <row r="9" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
@@ -4238,7 +4251,7 @@
       <c r="AF9" s="40"/>
       <c r="AG9" s="40"/>
       <c r="AH9" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI9" s="29"/>
     </row>
@@ -4378,7 +4391,7 @@
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" s="22">
         <f t="shared" ref="C15:R15" si="0">D15/(1.12)</f>
@@ -4504,7 +4517,7 @@
         <v>350405950838.15192</v>
       </c>
       <c r="AH15" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI15" s="29"/>
     </row>
@@ -4637,7 +4650,7 @@
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C21" s="40">
         <v>30000000000</v>
@@ -4763,7 +4776,7 @@
         <v>180000000000</v>
       </c>
       <c r="AH21" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI21" s="29"/>
     </row>
@@ -4891,7 +4904,7 @@
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C27" s="22">
         <v>10000000000</v>
@@ -5017,7 +5030,7 @@
         <v>43219423751.506668</v>
       </c>
       <c r="AH27" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI27" s="29"/>
     </row>
@@ -5129,7 +5142,7 @@
     </row>
     <row r="33" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
@@ -5163,7 +5176,7 @@
       <c r="AF33" s="22"/>
       <c r="AG33" s="22"/>
       <c r="AH33" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI33" s="29"/>
     </row>
@@ -5287,7 +5300,7 @@
     </row>
     <row r="39" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C39" s="22">
         <f>12%*C27</f>
@@ -5414,7 +5427,7 @@
         <v>5186330850.1808004</v>
       </c>
       <c r="AH39" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI39" s="29"/>
     </row>
@@ -5526,7 +5539,7 @@
     </row>
     <row r="45" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C45" s="22">
         <v>15000000</v>
@@ -5622,7 +5635,7 @@
         <v>18000000</v>
       </c>
       <c r="AH45" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI45" s="29"/>
     </row>
@@ -5746,7 +5759,7 @@
     </row>
     <row r="51" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
@@ -5780,7 +5793,7 @@
       <c r="AF51" s="22"/>
       <c r="AG51" s="22"/>
       <c r="AH51" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI51" s="29"/>
     </row>
@@ -5904,7 +5917,7 @@
     </row>
     <row r="57" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C57" s="22"/>
       <c r="D57" s="22"/>
@@ -5938,7 +5951,7 @@
       <c r="AF57" s="22"/>
       <c r="AG57" s="22"/>
       <c r="AH57" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI57" s="29"/>
     </row>
@@ -6050,7 +6063,7 @@
     </row>
     <row r="63" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C63" s="22"/>
       <c r="D63" s="22"/>
@@ -6084,7 +6097,7 @@
       <c r="AF63" s="22"/>
       <c r="AG63" s="22"/>
       <c r="AH63" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI63" s="29"/>
     </row>
@@ -6208,7 +6221,7 @@
     </row>
     <row r="69" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C69" s="22"/>
       <c r="D69" s="22"/>
@@ -6242,7 +6255,7 @@
       <c r="AF69" s="22"/>
       <c r="AG69" s="22"/>
       <c r="AH69" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI69" s="29"/>
     </row>
@@ -6356,7 +6369,7 @@
     <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75" s="18"/>
       <c r="B75" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C75" s="22">
         <v>0</v>
@@ -6392,7 +6405,7 @@
       <c r="AF75" s="22"/>
       <c r="AG75" s="22"/>
       <c r="AH75" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI75" s="29"/>
     </row>
@@ -6435,7 +6448,7 @@
       <c r="AF76" s="22"/>
       <c r="AG76" s="22"/>
       <c r="AH76" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI76" s="29"/>
     </row>
@@ -6478,7 +6491,7 @@
       <c r="AF77" s="22"/>
       <c r="AG77" s="22"/>
       <c r="AH77" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI77" s="29"/>
     </row>
@@ -6518,14 +6531,14 @@
       <c r="AF78" s="22"/>
       <c r="AG78" s="22"/>
       <c r="AH78" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI78" s="29"/>
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79" s="18"/>
       <c r="B79" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C79" s="22">
         <v>200</v>
@@ -6561,14 +6574,14 @@
       <c r="AF79" s="22"/>
       <c r="AG79" s="22"/>
       <c r="AH79" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI79" s="29"/>
     </row>
     <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80" s="18"/>
       <c r="B80" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C80" s="22">
         <v>450</v>
@@ -6604,7 +6617,7 @@
       <c r="AF80" s="22"/>
       <c r="AG80" s="22"/>
       <c r="AH80" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI80" s="29"/>
     </row>
@@ -6730,7 +6743,7 @@
     <row r="86" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A86" s="18"/>
       <c r="B86" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C86" s="22">
         <v>0</v>
@@ -6766,7 +6779,7 @@
       <c r="AF86" s="22"/>
       <c r="AG86" s="22"/>
       <c r="AH86" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI86" s="29"/>
     </row>
@@ -6809,7 +6822,7 @@
       <c r="AF87" s="22"/>
       <c r="AG87" s="22"/>
       <c r="AH87" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI87" s="29"/>
     </row>
@@ -6849,7 +6862,7 @@
       <c r="AF88" s="22"/>
       <c r="AG88" s="22"/>
       <c r="AH88" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI88" s="29"/>
     </row>
@@ -6892,14 +6905,14 @@
       <c r="AF89" s="22"/>
       <c r="AG89" s="22"/>
       <c r="AH89" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI89" s="29"/>
     </row>
     <row r="90" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A90" s="18"/>
       <c r="B90" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C90" s="22">
         <v>1000</v>
@@ -6935,14 +6948,14 @@
       <c r="AF90" s="22"/>
       <c r="AG90" s="22"/>
       <c r="AH90" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI90" s="29"/>
     </row>
     <row r="91" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A91" s="18"/>
       <c r="B91" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C91" s="22">
         <v>10000</v>
@@ -6978,7 +6991,7 @@
       <c r="AF91" s="22"/>
       <c r="AG91" s="22"/>
       <c r="AH91" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI91" s="29"/>
     </row>
@@ -7110,7 +7123,7 @@
       <c r="R3" s="22"/>
       <c r="S3" s="22"/>
       <c r="T3" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U3" s="25"/>
     </row>
@@ -7160,7 +7173,7 @@
       <c r="R4" s="24"/>
       <c r="S4" s="24"/>
       <c r="T4" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U4" s="37"/>
     </row>
@@ -7192,7 +7205,7 @@
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
       <c r="T6" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U6" s="25">
         <v>0.2</v>
@@ -7223,7 +7236,7 @@
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
       <c r="T7" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U7" s="47">
         <v>25000</v>
@@ -7259,7 +7272,7 @@
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
       <c r="T9" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U9" s="25"/>
     </row>
@@ -7292,7 +7305,7 @@
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
       <c r="T10" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U10" s="37"/>
     </row>
@@ -7328,7 +7341,7 @@
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
       <c r="T12" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U12" s="25"/>
       <c r="V12" s="6"/>
@@ -7360,7 +7373,7 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
       <c r="T13" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U13" s="37"/>
     </row>
@@ -7391,7 +7404,7 @@
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
       <c r="T15" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U15" s="25"/>
     </row>
@@ -7422,7 +7435,7 @@
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
       <c r="T16" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U16" s="37"/>
     </row>
@@ -7453,7 +7466,7 @@
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
       <c r="T18" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U18" s="25"/>
     </row>
@@ -7485,7 +7498,7 @@
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
       <c r="T19" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U19" s="37"/>
     </row>
@@ -7516,7 +7529,7 @@
       <c r="R21" s="22"/>
       <c r="S21" s="22"/>
       <c r="T21" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U21" s="25"/>
     </row>
@@ -7548,7 +7561,7 @@
       <c r="R22" s="22"/>
       <c r="S22" s="22"/>
       <c r="T22" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U22" s="37"/>
     </row>
@@ -7583,7 +7596,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -7645,7 +7658,7 @@
         <v>MSM</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
@@ -7664,7 +7677,7 @@
       <c r="R3" s="27"/>
       <c r="S3" s="27"/>
       <c r="T3" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U3" s="27">
         <v>37500</v>
@@ -7676,7 +7689,7 @@
         <v>MSM</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
@@ -7695,7 +7708,7 @@
       <c r="R4" s="27"/>
       <c r="S4" s="27"/>
       <c r="T4" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U4" s="27">
         <v>21000</v>
@@ -7707,7 +7720,7 @@
         <v>MSM</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
@@ -7726,7 +7739,7 @@
       <c r="R5" s="27"/>
       <c r="S5" s="27"/>
       <c r="T5" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U5" s="27">
         <v>11000</v>
@@ -7743,7 +7756,7 @@
         <v>FSW</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
@@ -7762,7 +7775,7 @@
       <c r="R7" s="27"/>
       <c r="S7" s="27"/>
       <c r="T7" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U7" s="27"/>
     </row>
@@ -7772,7 +7785,7 @@
         <v>FSW</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
@@ -7791,7 +7804,7 @@
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
       <c r="T8" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U8" s="27">
         <v>15000</v>
@@ -7803,7 +7816,7 @@
         <v>FSW</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
@@ -7822,7 +7835,7 @@
       <c r="R9" s="27"/>
       <c r="S9" s="27"/>
       <c r="T9" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U9" s="27"/>
     </row>
@@ -7853,7 +7866,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
@@ -7882,7 +7895,7 @@
       <c r="R11" s="27"/>
       <c r="S11" s="27"/>
       <c r="T11" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U11" s="27"/>
     </row>
@@ -7892,7 +7905,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
@@ -7921,7 +7934,7 @@
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
       <c r="T12" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U12" s="27"/>
     </row>
@@ -7931,7 +7944,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
@@ -7960,7 +7973,7 @@
       <c r="R13" s="27"/>
       <c r="S13" s="27"/>
       <c r="T13" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U13" s="27"/>
     </row>
@@ -7991,7 +8004,7 @@
         <v>Other males</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
@@ -8010,7 +8023,7 @@
       <c r="R15" s="27"/>
       <c r="S15" s="27"/>
       <c r="T15" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U15" s="27"/>
     </row>
@@ -8020,7 +8033,7 @@
         <v>Other males</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D16" s="22">
         <v>4227500</v>
@@ -8071,7 +8084,7 @@
         <v>6118320.6906761518</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U16" s="27"/>
     </row>
@@ -8081,7 +8094,7 @@
         <v>Other males</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
@@ -8100,7 +8113,7 @@
       <c r="R17" s="27"/>
       <c r="S17" s="27"/>
       <c r="T17" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U17" s="27"/>
     </row>
@@ -8131,7 +8144,7 @@
         <v>Other females</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
@@ -8150,7 +8163,7 @@
       <c r="R19" s="27"/>
       <c r="S19" s="27"/>
       <c r="T19" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U19" s="27"/>
     </row>
@@ -8160,7 +8173,7 @@
         <v>Other females</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D20" s="22">
         <v>4759641.7668505535</v>
@@ -8211,7 +8224,7 @@
         <v>7061706.1901886221</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U20" s="27"/>
     </row>
@@ -8221,7 +8234,7 @@
         <v>Other females</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
@@ -8240,7 +8253,7 @@
       <c r="R21" s="27"/>
       <c r="S21" s="27"/>
       <c r="T21" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U21" s="27"/>
     </row>
@@ -8271,7 +8284,7 @@
         <v>Clients</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -8290,7 +8303,7 @@
       <c r="R23" s="27"/>
       <c r="S23" s="27"/>
       <c r="T23" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U23" s="27"/>
     </row>
@@ -8300,7 +8313,7 @@
         <v>Clients</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24" s="22">
         <v>522500</v>
@@ -8351,7 +8364,7 @@
         <v>756196.93929705245</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U24" s="27"/>
     </row>
@@ -8361,7 +8374,7 @@
         <v>Clients</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -8380,7 +8393,7 @@
       <c r="R25" s="27"/>
       <c r="S25" s="27"/>
       <c r="T25" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U25" s="27"/>
     </row>
@@ -8448,7 +8461,7 @@
         <v>MSM</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -8469,7 +8482,7 @@
       <c r="R31" s="22"/>
       <c r="S31" s="22"/>
       <c r="T31" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U31" s="26"/>
     </row>
@@ -8479,7 +8492,7 @@
         <v>MSM</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -8500,7 +8513,7 @@
       <c r="R32" s="22"/>
       <c r="S32" s="22"/>
       <c r="T32" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U32" s="26"/>
     </row>
@@ -8510,7 +8523,7 @@
         <v>MSM</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
@@ -8531,7 +8544,7 @@
       <c r="R33" s="22"/>
       <c r="S33" s="22"/>
       <c r="T33" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U33" s="26"/>
     </row>
@@ -8545,7 +8558,7 @@
         <v>FSW</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
@@ -8570,7 +8583,7 @@
       <c r="R35" s="22"/>
       <c r="S35" s="22"/>
       <c r="T35" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U35" s="26"/>
     </row>
@@ -8580,7 +8593,7 @@
         <v>FSW</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -8605,7 +8618,7 @@
       <c r="R36" s="22"/>
       <c r="S36" s="22"/>
       <c r="T36" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U36" s="26"/>
     </row>
@@ -8615,7 +8628,7 @@
         <v>FSW</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
@@ -8640,7 +8653,7 @@
       <c r="R37" s="22"/>
       <c r="S37" s="22"/>
       <c r="T37" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U37" s="26"/>
     </row>
@@ -8654,7 +8667,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
@@ -8679,7 +8692,7 @@
       <c r="R39" s="22"/>
       <c r="S39" s="22"/>
       <c r="T39" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U39" s="26"/>
     </row>
@@ -8689,7 +8702,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
@@ -8714,7 +8727,7 @@
       <c r="R40" s="22"/>
       <c r="S40" s="22"/>
       <c r="T40" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U40" s="26"/>
     </row>
@@ -8724,7 +8737,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
@@ -8749,7 +8762,7 @@
       <c r="R41" s="22"/>
       <c r="S41" s="22"/>
       <c r="T41" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U41" s="26"/>
     </row>
@@ -8763,7 +8776,7 @@
         <v>Other males</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
@@ -8782,7 +8795,7 @@
       <c r="R43" s="22"/>
       <c r="S43" s="22"/>
       <c r="T43" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U43" s="26"/>
     </row>
@@ -8792,7 +8805,7 @@
         <v>Other males</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
@@ -8811,7 +8824,7 @@
       <c r="R44" s="22"/>
       <c r="S44" s="22"/>
       <c r="T44" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U44" s="26">
         <v>5.0000000000000001E-4</v>
@@ -8823,7 +8836,7 @@
         <v>Other males</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
@@ -8842,7 +8855,7 @@
       <c r="R45" s="22"/>
       <c r="S45" s="22"/>
       <c r="T45" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U45" s="26"/>
     </row>
@@ -8856,7 +8869,7 @@
         <v>Other females</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
@@ -8875,7 +8888,7 @@
       <c r="R47" s="22"/>
       <c r="S47" s="22"/>
       <c r="T47" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U47" s="26"/>
     </row>
@@ -8885,7 +8898,7 @@
         <v>Other females</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
@@ -8912,7 +8925,7 @@
       <c r="R48" s="22"/>
       <c r="S48" s="22"/>
       <c r="T48" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U48" s="26"/>
     </row>
@@ -8922,7 +8935,7 @@
         <v>Other females</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
@@ -8941,7 +8954,7 @@
       <c r="R49" s="22"/>
       <c r="S49" s="22"/>
       <c r="T49" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U49" s="26"/>
     </row>
@@ -8955,7 +8968,7 @@
         <v>Clients</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
@@ -8974,7 +8987,7 @@
       <c r="R51" s="22"/>
       <c r="S51" s="22"/>
       <c r="T51" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U51" s="26"/>
     </row>
@@ -8984,7 +8997,7 @@
         <v>Clients</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
@@ -9003,7 +9016,7 @@
       <c r="R52" s="22"/>
       <c r="S52" s="22"/>
       <c r="T52" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U52" s="26">
         <v>0.01</v>
@@ -9015,7 +9028,7 @@
         <v>Clients</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
@@ -9034,7 +9047,7 @@
       <c r="R53" s="22"/>
       <c r="S53" s="22"/>
       <c r="T53" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U53" s="26"/>
     </row>
@@ -9143,7 +9156,7 @@
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -9162,7 +9175,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T3" s="22"/>
     </row>
@@ -9253,7 +9266,7 @@
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -9296,7 +9309,7 @@
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
       <c r="S9" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T9" s="22"/>
     </row>
@@ -9387,7 +9400,7 @@
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -9406,7 +9419,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T15" s="22"/>
     </row>
@@ -9478,7 +9491,7 @@
     </row>
     <row r="21" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -9497,7 +9510,7 @@
       <c r="Q21" s="22"/>
       <c r="R21" s="22"/>
       <c r="S21" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T21" s="22"/>
     </row>
@@ -9591,7 +9604,7 @@
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
@@ -9610,7 +9623,7 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T27" s="22"/>
     </row>
@@ -9676,7 +9689,7 @@
     </row>
     <row r="33" spans="2:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
@@ -9695,7 +9708,7 @@
       <c r="Q33" s="22"/>
       <c r="R33" s="22"/>
       <c r="S33" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T33" s="22"/>
     </row>
@@ -9806,7 +9819,7 @@
       <c r="Q3" s="25"/>
       <c r="R3" s="25"/>
       <c r="S3" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T3" s="25">
         <v>0.01</v>
@@ -9834,7 +9847,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T4" s="25">
         <v>0.01</v>
@@ -9862,7 +9875,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T5" s="25">
         <v>0.03</v>
@@ -9890,7 +9903,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T6" s="25">
         <v>0.01</v>
@@ -9918,7 +9931,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T7" s="25">
         <v>0.01</v>
@@ -9946,7 +9959,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T8" s="25">
         <v>0.01</v>
@@ -10062,7 +10075,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T14" s="25">
         <v>0</v>
@@ -10091,7 +10104,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T15" s="25">
         <v>0</v>
@@ -10120,7 +10133,7 @@
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T16" s="25">
         <v>0</v>
@@ -10149,7 +10162,7 @@
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T17" s="25">
         <v>0</v>
@@ -10178,7 +10191,7 @@
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T18" s="25">
         <v>0</v>
@@ -10207,7 +10220,7 @@
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T19" s="25">
         <v>0</v>
@@ -10226,7 +10239,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -10325,7 +10338,7 @@
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T25" s="25">
         <v>0</v>
@@ -10353,7 +10366,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T26" s="25">
         <v>0</v>
@@ -10381,7 +10394,7 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T27" s="25">
         <v>0</v>
@@ -10409,7 +10422,7 @@
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
       <c r="S28" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T28" s="25">
         <v>0</v>
@@ -10437,7 +10450,7 @@
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
       <c r="S29" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T29" s="25">
         <v>0</v>
@@ -10465,7 +10478,7 @@
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
       <c r="S30" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T30" s="25">
         <v>0</v>
@@ -10599,7 +10612,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T3" s="25">
         <v>0.03</v>
@@ -10632,7 +10645,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T4" s="25"/>
     </row>
@@ -10665,7 +10678,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T5" s="22"/>
     </row>
@@ -10692,7 +10705,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T6" s="25">
         <v>0.01</v>
@@ -10721,7 +10734,7 @@
       <c r="Q7" s="25"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T7" s="25">
         <v>0.01</v>
@@ -10750,7 +10763,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T8" s="25">
         <v>0.05</v>
@@ -10843,7 +10856,7 @@
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -10862,7 +10875,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T14" s="25">
         <v>0.5</v>
@@ -10955,7 +10968,7 @@
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" s="22">
         <v>0</v>
@@ -11002,7 +11015,7 @@
       <c r="Q20" s="22"/>
       <c r="R20" s="22"/>
       <c r="S20" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T20" s="22"/>
     </row>
@@ -11014,7 +11027,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -11093,7 +11106,7 @@
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" s="22">
         <v>0</v>
@@ -11140,7 +11153,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T26" s="22"/>
     </row>
@@ -11155,7 +11168,7 @@
     </row>
     <row r="30" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B30" s="6"/>
     </row>
@@ -11215,7 +11228,7 @@
     </row>
     <row r="32" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C32" s="22">
         <v>350</v>
@@ -11262,7 +11275,7 @@
       <c r="Q32" s="22"/>
       <c r="R32" s="22"/>
       <c r="S32" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T32" s="22"/>
     </row>
@@ -11357,7 +11370,7 @@
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
       <c r="S38" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T38" s="24">
         <v>0</v>
@@ -11385,7 +11398,7 @@
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
       <c r="S39" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T39" s="24">
         <v>0</v>
@@ -11413,7 +11426,7 @@
       <c r="Q40" s="22"/>
       <c r="R40" s="22"/>
       <c r="S40" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T40" s="24">
         <v>0</v>
@@ -11441,7 +11454,7 @@
       <c r="Q41" s="22"/>
       <c r="R41" s="22"/>
       <c r="S41" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T41" s="24">
         <v>0</v>
@@ -11469,7 +11482,7 @@
       <c r="Q42" s="25"/>
       <c r="R42" s="22"/>
       <c r="S42" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T42" s="24">
         <f>2/50</f>
@@ -11498,7 +11511,7 @@
       <c r="Q43" s="22"/>
       <c r="R43" s="22"/>
       <c r="S43" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T43" s="24">
         <v>0</v>
@@ -11594,7 +11607,7 @@
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
       <c r="B49" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C49" s="27"/>
       <c r="D49" s="27"/>
@@ -11623,7 +11636,7 @@
       <c r="Q49" s="27"/>
       <c r="R49" s="27"/>
       <c r="S49" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T49" s="22"/>
     </row>
@@ -11718,7 +11731,7 @@
       <c r="Q55" s="22"/>
       <c r="R55" s="22"/>
       <c r="S55" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T55" s="24">
         <v>0</v>
@@ -11746,7 +11759,7 @@
       <c r="Q56" s="25"/>
       <c r="R56" s="22"/>
       <c r="S56" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T56" s="24">
         <f>2/50</f>
@@ -11815,7 +11828,7 @@
     </row>
     <row r="62" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C62" s="22"/>
       <c r="D62" s="22"/>
@@ -11834,7 +11847,7 @@
       <c r="Q62" s="22"/>
       <c r="R62" s="22"/>
       <c r="S62" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T62" s="25">
         <v>0.3</v>
@@ -11856,7 +11869,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11866,7 +11879,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -11964,7 +11977,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T3" s="33">
         <v>80</v>
@@ -11993,7 +12006,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T4" s="33">
         <v>80</v>
@@ -12022,7 +12035,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T5" s="33">
         <v>80</v>
@@ -12051,7 +12064,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T6" s="33">
         <v>80</v>
@@ -12080,7 +12093,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T7" s="33">
         <v>80</v>
@@ -12109,7 +12122,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T8" s="33">
         <v>80</v>
@@ -12125,7 +12138,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -12223,7 +12236,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T14" s="29">
         <v>10</v>
@@ -12252,7 +12265,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T15" s="29">
         <v>10</v>
@@ -12281,7 +12294,7 @@
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T16" s="29">
         <v>10</v>
@@ -12310,7 +12323,7 @@
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T17" s="29">
         <v>10</v>
@@ -12339,7 +12352,7 @@
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T18" s="29">
         <v>10</v>
@@ -12368,7 +12381,7 @@
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T19" s="29">
         <v>10</v>
@@ -12384,7 +12397,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -12482,7 +12495,7 @@
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T25" s="29">
         <v>0</v>
@@ -12511,7 +12524,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T26" s="29">
         <v>500</v>
@@ -12540,7 +12553,7 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T27" s="29">
         <v>0</v>
@@ -12569,7 +12582,7 @@
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
       <c r="S28" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T28" s="29">
         <v>0</v>
@@ -12598,7 +12611,7 @@
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
       <c r="S29" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T29" s="29">
         <v>0</v>
@@ -12627,7 +12640,7 @@
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
       <c r="S30" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T30" s="29">
         <v>10</v>
@@ -12816,7 +12829,7 @@
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
       <c r="S38" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T38" s="30">
         <v>0.4</v>
@@ -12855,7 +12868,7 @@
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
       <c r="S39" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T39" s="30"/>
     </row>
@@ -12882,7 +12895,7 @@
       <c r="Q40" s="22"/>
       <c r="R40" s="22"/>
       <c r="S40" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T40" s="30">
         <v>0.05</v>
@@ -12911,7 +12924,7 @@
       <c r="Q41" s="22"/>
       <c r="R41" s="22"/>
       <c r="S41" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T41" s="30">
         <v>0.05</v>
@@ -12940,7 +12953,7 @@
       <c r="Q42" s="22"/>
       <c r="R42" s="22"/>
       <c r="S42" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T42" s="30">
         <v>0.05</v>
@@ -12969,7 +12982,7 @@
       <c r="Q43" s="22"/>
       <c r="R43" s="22"/>
       <c r="S43" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T43" s="30">
         <v>7.0000000000000007E-2</v>
@@ -12985,7 +12998,7 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
@@ -13083,7 +13096,7 @@
       <c r="Q49" s="22"/>
       <c r="R49" s="22"/>
       <c r="S49" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T49" s="30">
         <v>0.6</v>
@@ -13122,7 +13135,7 @@
       <c r="Q50" s="22"/>
       <c r="R50" s="22"/>
       <c r="S50" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T50" s="30"/>
     </row>
@@ -13149,7 +13162,7 @@
       <c r="Q51" s="22"/>
       <c r="R51" s="22"/>
       <c r="S51" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T51" s="30">
         <v>0.5</v>
@@ -13184,7 +13197,7 @@
       <c r="Q52" s="22"/>
       <c r="R52" s="22"/>
       <c r="S52" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T52" s="30"/>
     </row>
@@ -13217,7 +13230,7 @@
       <c r="Q53" s="22"/>
       <c r="R53" s="22"/>
       <c r="S53" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T53" s="30"/>
     </row>
@@ -13244,7 +13257,7 @@
       <c r="Q54" s="22"/>
       <c r="R54" s="22"/>
       <c r="S54" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T54" s="30">
         <v>0.5</v>
@@ -13358,7 +13371,7 @@
       <c r="Q60" s="22"/>
       <c r="R60" s="22"/>
       <c r="S60" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T60" s="29">
         <v>0</v>
@@ -13397,7 +13410,7 @@
       <c r="Q61" s="22"/>
       <c r="R61" s="22"/>
       <c r="S61" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T61" s="38"/>
     </row>
@@ -13424,7 +13437,7 @@
       <c r="Q62" s="22"/>
       <c r="R62" s="22"/>
       <c r="S62" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T62" s="30">
         <v>0</v>
@@ -13453,7 +13466,7 @@
       <c r="Q63" s="22"/>
       <c r="R63" s="22"/>
       <c r="S63" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T63" s="30">
         <v>0</v>
@@ -13482,7 +13495,7 @@
       <c r="Q64" s="22"/>
       <c r="R64" s="22"/>
       <c r="S64" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T64" s="29">
         <v>0</v>
@@ -13521,7 +13534,7 @@
       <c r="Q65" s="22"/>
       <c r="R65" s="22"/>
       <c r="S65" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T65" s="39"/>
     </row>
@@ -13633,7 +13646,7 @@
       <c r="Q71" s="22"/>
       <c r="R71" s="22"/>
       <c r="S71" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T71" s="50">
         <v>0.03</v>
@@ -13662,7 +13675,7 @@
       <c r="Q72" s="22"/>
       <c r="R72" s="22"/>
       <c r="S72" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T72" s="50">
         <v>2.5999999999999999E-2</v>
@@ -13691,7 +13704,7 @@
       <c r="Q73" s="22"/>
       <c r="R73" s="22"/>
       <c r="S73" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T73" s="50">
         <v>0.03</v>
@@ -13720,7 +13733,7 @@
       <c r="Q74" s="22"/>
       <c r="R74" s="22"/>
       <c r="S74" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T74" s="50">
         <v>0.03</v>
@@ -13821,7 +13834,7 @@
       <c r="Q80" s="22"/>
       <c r="R80" s="22"/>
       <c r="S80" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T80" s="51">
         <v>450</v>
@@ -13849,7 +13862,7 @@
       <c r="Q81" s="22"/>
       <c r="R81" s="22"/>
       <c r="S81" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T81" s="51">
         <v>50</v>
@@ -13877,7 +13890,7 @@
       <c r="Q82" s="22"/>
       <c r="R82" s="22"/>
       <c r="S82" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T82" s="51">
         <v>5000</v>
@@ -13905,7 +13918,7 @@
       <c r="Q83" s="22"/>
       <c r="R83" s="22"/>
       <c r="S83" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T83" s="51">
         <v>500</v>
@@ -14038,7 +14051,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T3" s="29">
         <v>0</v>
@@ -14067,7 +14080,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T4" s="29">
         <v>0</v>
@@ -14096,7 +14109,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T5" s="29">
         <v>400</v>
@@ -14125,7 +14138,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T6" s="29">
         <v>0</v>
@@ -14154,7 +14167,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T7" s="29">
         <v>0</v>
@@ -14183,7 +14196,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T8" s="29">
         <v>0</v>
@@ -14304,7 +14317,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T14" s="38"/>
     </row>
@@ -14421,7 +14434,7 @@
       <c r="Q20" s="38"/>
       <c r="R20" s="38"/>
       <c r="S20" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T20" s="38"/>
     </row>

</xml_diff>

<commit_message>
removed saturating column from spreadsheet
</commit_message>
<xml_diff>
--- a/server/src/sim/example.xlsx
+++ b/server/src/sim/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="14205" tabRatio="863" activeTab="10"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="14205" tabRatio="863" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Populations &amp; programs" sheetId="12" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="146">
   <si>
     <t>Number of people who inject drugs who are on opiate substitution therapy</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Cost &amp; coverage</t>
-  </si>
-  <si>
-    <t>Saturating</t>
   </si>
   <si>
     <t>Assumption</t>
@@ -2407,7 +2404,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2425,36 +2422,36 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>121</v>
-      </c>
       <c r="E2" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="21" t="s">
-        <v>52</v>
-      </c>
       <c r="H2" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="J2" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="K2" s="21" t="s">
         <v>80</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2462,10 +2459,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="41" t="b">
         <v>1</v>
@@ -2494,10 +2491,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="41" t="b">
         <v>0</v>
@@ -2526,10 +2523,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="45" t="s">
         <v>60</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>61</v>
       </c>
       <c r="E5" s="41" t="b">
         <v>1</v>
@@ -2558,10 +2555,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" s="41" t="b">
         <v>1</v>
@@ -2590,10 +2587,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" s="41" t="b">
         <v>0</v>
@@ -2622,10 +2619,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E8" s="41" t="b">
         <v>1</v>
@@ -2660,20 +2657,17 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B12" s="21"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="21"/>
       <c r="C13" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="21" t="s">
         <v>120</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2681,13 +2675,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="41" t="b">
-        <v>1</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2695,13 +2686,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D15" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="41" t="b">
-        <v>1</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2709,69 +2697,54 @@
         <v>3</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="21">
         <v>4</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="41" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="21">
         <v>5</v>
       </c>
       <c r="C18" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="41" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="21">
         <v>6</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="21">
         <v>7</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="41" t="b">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2802,7 +2775,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="2"/>
@@ -2955,7 +2928,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="2"/>
@@ -3081,7 +3054,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+    <sheetView topLeftCell="A44" workbookViewId="0">
       <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
@@ -3094,18 +3067,18 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
@@ -3115,7 +3088,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" s="26">
         <v>4.0000000000000002E-4</v>
@@ -3129,7 +3102,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" s="26">
         <v>8.0000000000000004E-4</v>
@@ -3143,7 +3116,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" s="26">
         <v>1.38E-2</v>
@@ -3157,7 +3130,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="26">
         <v>1.1000000000000001E-3</v>
@@ -3171,7 +3144,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" s="26">
         <v>8.0000000000000002E-3</v>
@@ -3185,7 +3158,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="26">
         <v>0.36699999999999999</v>
@@ -3199,7 +3172,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="26">
         <v>0.20499999999999999</v>
@@ -3223,23 +3196,23 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C15" s="22">
         <v>26.03</v>
@@ -3253,7 +3226,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="22">
         <v>1</v>
@@ -3267,7 +3240,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="22">
         <v>1</v>
@@ -3281,7 +3254,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" s="22">
         <v>1</v>
@@ -3295,7 +3268,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C19" s="22">
         <v>3.49</v>
@@ -3309,7 +3282,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C20" s="22">
         <v>7.17</v>
@@ -3333,24 +3306,24 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="19"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" s="25">
         <v>4.1399999999999997</v>
@@ -3364,7 +3337,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="25">
         <v>1.05</v>
@@ -3378,7 +3351,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C28" s="25">
         <v>0.33</v>
@@ -3392,7 +3365,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C29" s="25">
         <v>0.27</v>
@@ -3406,7 +3379,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C30" s="25">
         <v>0.67</v>
@@ -3430,23 +3403,23 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C36" s="25">
         <v>0.45</v>
@@ -3460,7 +3433,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C37" s="25">
         <v>0.7</v>
@@ -3474,7 +3447,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C38" s="25">
         <v>0.47</v>
@@ -3488,7 +3461,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C39" s="25">
         <v>1.52</v>
@@ -3515,23 +3488,23 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C44" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C45" s="25">
         <v>0.1</v>
@@ -3545,7 +3518,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C46" s="25">
         <v>0.16</v>
@@ -3569,23 +3542,23 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C51" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C52" s="26">
         <v>3.5999999999999999E-3</v>
@@ -3599,7 +3572,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C53" s="26">
         <v>3.5999999999999999E-3</v>
@@ -3613,7 +3586,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C54" s="26">
         <v>5.7999999999999996E-3</v>
@@ -3627,7 +3600,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C55" s="26">
         <v>8.8000000000000005E-3</v>
@@ -3641,7 +3614,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C56" s="26">
         <v>5.8999999999999997E-2</v>
@@ -3655,7 +3628,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B57" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C57" s="26">
         <v>0.32300000000000001</v>
@@ -3669,7 +3642,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C58" s="26">
         <v>0.23</v>
@@ -3683,7 +3656,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B59" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C59" s="22">
         <v>2.17</v>
@@ -3707,23 +3680,23 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C64" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="E64" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B65" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C65" s="26">
         <v>0.05</v>
@@ -3737,7 +3710,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B66" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C66" s="26">
         <v>0.42</v>
@@ -3751,7 +3724,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C67" s="26">
         <v>1</v>
@@ -3765,7 +3738,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C68" s="26">
         <v>2.65</v>
@@ -3779,7 +3752,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B69" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C69" s="26">
         <v>0.46</v>
@@ -3793,7 +3766,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C70" s="26">
         <v>0.105</v>
@@ -3807,7 +3780,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C71" s="26">
         <v>0.3</v>
@@ -3835,23 +3808,23 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C77" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D77" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="E77" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C78" s="24">
         <v>0.05</v>
@@ -3861,7 +3834,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B79" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C79" s="24">
         <v>0.05</v>
@@ -3871,7 +3844,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B80" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C80" s="24">
         <v>0.1</v>
@@ -3881,7 +3854,7 @@
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C81" s="24">
         <v>0.15</v>
@@ -3891,7 +3864,7 @@
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C82" s="24">
         <v>0.4</v>
@@ -3901,7 +3874,7 @@
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C83" s="24">
         <v>0.6</v>
@@ -3911,7 +3884,7 @@
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C84" s="24">
         <v>5.2999999999999999E-2</v>
@@ -3953,7 +3926,7 @@
   <sheetData>
     <row r="1" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" s="6"/>
       <c r="AI1" s="6"/>
@@ -4054,12 +4027,12 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -4093,7 +4066,7 @@
       <c r="AF3" s="22"/>
       <c r="AG3" s="22"/>
       <c r="AH3" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI3" s="29"/>
     </row>
@@ -4111,7 +4084,7 @@
     </row>
     <row r="7" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" s="6"/>
       <c r="AI7" s="6"/>
@@ -4212,12 +4185,12 @@
         <v>2030</v>
       </c>
       <c r="AI8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
@@ -4251,7 +4224,7 @@
       <c r="AF9" s="40"/>
       <c r="AG9" s="40"/>
       <c r="AH9" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI9" s="29"/>
     </row>
@@ -4269,7 +4242,7 @@
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
@@ -4385,13 +4358,13 @@
       </c>
       <c r="AH14" s="18"/>
       <c r="AI14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="22">
         <f t="shared" ref="C15:R15" si="0">D15/(1.12)</f>
@@ -4517,7 +4490,7 @@
         <v>350405950838.15192</v>
       </c>
       <c r="AH15" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI15" s="29"/>
     </row>
@@ -4528,7 +4501,7 @@
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="S19" s="18"/>
       <c r="T19" s="18"/>
@@ -4644,13 +4617,13 @@
       </c>
       <c r="AH20" s="18"/>
       <c r="AI20" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" s="40">
         <v>30000000000</v>
@@ -4776,13 +4749,13 @@
         <v>180000000000</v>
       </c>
       <c r="AH21" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI21" s="29"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S25" s="18"/>
       <c r="T25" s="18"/>
@@ -4898,13 +4871,13 @@
       </c>
       <c r="AH26" s="18"/>
       <c r="AI26" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" s="22">
         <v>10000000000</v>
@@ -5030,13 +5003,13 @@
         <v>43219423751.506668</v>
       </c>
       <c r="AH27" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI27" s="29"/>
     </row>
     <row r="31" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="6"/>
       <c r="AI31" s="6"/>
@@ -5137,12 +5110,12 @@
         <v>2030</v>
       </c>
       <c r="AI32" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
@@ -5176,7 +5149,7 @@
       <c r="AF33" s="22"/>
       <c r="AG33" s="22"/>
       <c r="AH33" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI33" s="29"/>
     </row>
@@ -5194,7 +5167,7 @@
     </row>
     <row r="37" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" s="6"/>
       <c r="AI37" s="6"/>
@@ -5295,12 +5268,12 @@
         <v>2030</v>
       </c>
       <c r="AI38" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C39" s="22">
         <f>12%*C27</f>
@@ -5427,13 +5400,13 @@
         <v>5186330850.1808004</v>
       </c>
       <c r="AH39" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI39" s="29"/>
     </row>
     <row r="43" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B43" s="6"/>
       <c r="AI43" s="6"/>
@@ -5534,12 +5507,12 @@
         <v>2030</v>
       </c>
       <c r="AI44" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C45" s="22">
         <v>15000000</v>
@@ -5635,7 +5608,7 @@
         <v>18000000</v>
       </c>
       <c r="AH45" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI45" s="29"/>
     </row>
@@ -5653,7 +5626,7 @@
     </row>
     <row r="49" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B49" s="6"/>
       <c r="AI49" s="6"/>
@@ -5754,12 +5727,12 @@
         <v>2030</v>
       </c>
       <c r="AI50" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
@@ -5793,7 +5766,7 @@
       <c r="AF51" s="22"/>
       <c r="AG51" s="22"/>
       <c r="AH51" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI51" s="29"/>
     </row>
@@ -5811,7 +5784,7 @@
     </row>
     <row r="55" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B55" s="6"/>
       <c r="AI55" s="6"/>
@@ -5912,12 +5885,12 @@
         <v>2030</v>
       </c>
       <c r="AI56" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C57" s="22"/>
       <c r="D57" s="22"/>
@@ -5951,13 +5924,13 @@
       <c r="AF57" s="22"/>
       <c r="AG57" s="22"/>
       <c r="AH57" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI57" s="29"/>
     </row>
     <row r="61" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B61" s="6"/>
       <c r="AI61" s="6"/>
@@ -6058,12 +6031,12 @@
         <v>2030</v>
       </c>
       <c r="AI62" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C63" s="22"/>
       <c r="D63" s="22"/>
@@ -6097,7 +6070,7 @@
       <c r="AF63" s="22"/>
       <c r="AG63" s="22"/>
       <c r="AH63" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI63" s="29"/>
     </row>
@@ -6115,7 +6088,7 @@
     </row>
     <row r="67" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B67" s="6"/>
       <c r="AI67" s="6"/>
@@ -6216,12 +6189,12 @@
         <v>2030</v>
       </c>
       <c r="AI68" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C69" s="22"/>
       <c r="D69" s="22"/>
@@ -6255,13 +6228,13 @@
       <c r="AF69" s="22"/>
       <c r="AG69" s="22"/>
       <c r="AH69" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI69" s="29"/>
     </row>
     <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B73" s="18"/>
     </row>
@@ -6363,13 +6336,13 @@
       </c>
       <c r="AH74" s="18"/>
       <c r="AI74" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75" s="18"/>
       <c r="B75" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C75" s="22">
         <v>0</v>
@@ -6405,14 +6378,14 @@
       <c r="AF75" s="22"/>
       <c r="AG75" s="22"/>
       <c r="AH75" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI75" s="29"/>
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76" s="18"/>
       <c r="B76" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C76" s="22">
         <v>100</v>
@@ -6448,14 +6421,14 @@
       <c r="AF76" s="22"/>
       <c r="AG76" s="22"/>
       <c r="AH76" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI76" s="29"/>
     </row>
     <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77" s="18"/>
       <c r="B77" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C77" s="22">
         <v>100</v>
@@ -6491,13 +6464,13 @@
       <c r="AF77" s="22"/>
       <c r="AG77" s="22"/>
       <c r="AH77" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI77" s="29"/>
     </row>
     <row r="78" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C78" s="22"/>
       <c r="D78" s="22"/>
@@ -6531,14 +6504,14 @@
       <c r="AF78" s="22"/>
       <c r="AG78" s="22"/>
       <c r="AH78" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI78" s="29"/>
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79" s="18"/>
       <c r="B79" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C79" s="22">
         <v>200</v>
@@ -6574,14 +6547,14 @@
       <c r="AF79" s="22"/>
       <c r="AG79" s="22"/>
       <c r="AH79" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI79" s="29"/>
     </row>
     <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80" s="18"/>
       <c r="B80" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C80" s="22">
         <v>450</v>
@@ -6617,7 +6590,7 @@
       <c r="AF80" s="22"/>
       <c r="AG80" s="22"/>
       <c r="AH80" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI80" s="29"/>
     </row>
@@ -6635,7 +6608,7 @@
     </row>
     <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B84" s="18"/>
     </row>
@@ -6737,13 +6710,13 @@
       </c>
       <c r="AH85" s="18"/>
       <c r="AI85" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A86" s="18"/>
       <c r="B86" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C86" s="22">
         <v>0</v>
@@ -6779,14 +6752,14 @@
       <c r="AF86" s="22"/>
       <c r="AG86" s="22"/>
       <c r="AH86" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI86" s="29"/>
     </row>
     <row r="87" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A87" s="18"/>
       <c r="B87" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C87" s="22">
         <v>100</v>
@@ -6822,13 +6795,13 @@
       <c r="AF87" s="22"/>
       <c r="AG87" s="22"/>
       <c r="AH87" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI87" s="29"/>
     </row>
     <row r="88" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C88" s="22"/>
       <c r="D88" s="22"/>
@@ -6862,14 +6835,14 @@
       <c r="AF88" s="22"/>
       <c r="AG88" s="22"/>
       <c r="AH88" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI88" s="29"/>
     </row>
     <row r="89" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A89" s="18"/>
       <c r="B89" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C89" s="22">
         <v>100</v>
@@ -6905,14 +6878,14 @@
       <c r="AF89" s="22"/>
       <c r="AG89" s="22"/>
       <c r="AH89" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI89" s="29"/>
     </row>
     <row r="90" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A90" s="18"/>
       <c r="B90" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C90" s="22">
         <v>1000</v>
@@ -6948,14 +6921,14 @@
       <c r="AF90" s="22"/>
       <c r="AG90" s="22"/>
       <c r="AH90" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI90" s="29"/>
     </row>
     <row r="91" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A91" s="18"/>
       <c r="B91" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C91" s="22">
         <v>10000</v>
@@ -6991,7 +6964,7 @@
       <c r="AF91" s="22"/>
       <c r="AG91" s="22"/>
       <c r="AH91" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AI91" s="29"/>
     </row>
@@ -7081,7 +7054,7 @@
         <v>2015</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -7090,7 +7063,7 @@
         <v>SBCC</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="25">
@@ -7123,7 +7096,7 @@
       <c r="R3" s="22"/>
       <c r="S3" s="22"/>
       <c r="T3" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U3" s="25"/>
     </row>
@@ -7173,7 +7146,7 @@
       <c r="R4" s="24"/>
       <c r="S4" s="24"/>
       <c r="T4" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U4" s="37"/>
     </row>
@@ -7186,7 +7159,7 @@
         <v>NSP</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="25"/>
@@ -7205,7 +7178,7 @@
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
       <c r="T6" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U6" s="25">
         <v>0.2</v>
@@ -7236,7 +7209,7 @@
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
       <c r="T7" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U7" s="47">
         <v>25000</v>
@@ -7251,7 +7224,7 @@
         <v>OST</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="25"/>
@@ -7272,7 +7245,7 @@
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
       <c r="T9" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U9" s="25"/>
     </row>
@@ -7305,7 +7278,7 @@
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
       <c r="T10" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U10" s="37"/>
     </row>
@@ -7320,7 +7293,7 @@
         <v>MSM programs</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="25"/>
@@ -7341,7 +7314,7 @@
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
       <c r="T12" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U12" s="25"/>
       <c r="V12" s="6"/>
@@ -7373,7 +7346,7 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
       <c r="T13" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U13" s="37"/>
     </row>
@@ -7383,7 +7356,7 @@
         <v>FSW programs</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="25"/>
@@ -7404,7 +7377,7 @@
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
       <c r="T15" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U15" s="25"/>
     </row>
@@ -7435,7 +7408,7 @@
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
       <c r="T16" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U16" s="37"/>
     </row>
@@ -7445,7 +7418,7 @@
         <v>ART</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="25"/>
@@ -7466,7 +7439,7 @@
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
       <c r="T18" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U18" s="25"/>
     </row>
@@ -7498,7 +7471,7 @@
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
       <c r="T19" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U19" s="37"/>
     </row>
@@ -7508,7 +7481,7 @@
         <v>PMTCT</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="25"/>
@@ -7529,7 +7502,7 @@
       <c r="R21" s="22"/>
       <c r="S21" s="22"/>
       <c r="T21" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U21" s="25"/>
     </row>
@@ -7561,7 +7534,7 @@
       <c r="R22" s="22"/>
       <c r="S22" s="22"/>
       <c r="T22" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U22" s="37"/>
     </row>
@@ -7582,7 +7555,9 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W24" sqref="W24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7596,7 +7571,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -7649,7 +7624,7 @@
         <v>2015</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -7658,7 +7633,7 @@
         <v>MSM</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
@@ -7677,7 +7652,7 @@
       <c r="R3" s="27"/>
       <c r="S3" s="27"/>
       <c r="T3" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U3" s="27">
         <v>37500</v>
@@ -7689,7 +7664,7 @@
         <v>MSM</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
@@ -7708,7 +7683,7 @@
       <c r="R4" s="27"/>
       <c r="S4" s="27"/>
       <c r="T4" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U4" s="27">
         <v>21000</v>
@@ -7720,7 +7695,7 @@
         <v>MSM</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
@@ -7739,7 +7714,7 @@
       <c r="R5" s="27"/>
       <c r="S5" s="27"/>
       <c r="T5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U5" s="27">
         <v>11000</v>
@@ -7756,7 +7731,7 @@
         <v>FSW</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
@@ -7775,7 +7750,7 @@
       <c r="R7" s="27"/>
       <c r="S7" s="27"/>
       <c r="T7" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U7" s="27"/>
     </row>
@@ -7785,7 +7760,7 @@
         <v>FSW</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
@@ -7804,7 +7779,7 @@
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
       <c r="T8" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U8" s="27">
         <v>15000</v>
@@ -7816,7 +7791,7 @@
         <v>FSW</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
@@ -7835,7 +7810,7 @@
       <c r="R9" s="27"/>
       <c r="S9" s="27"/>
       <c r="T9" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U9" s="27"/>
     </row>
@@ -7866,7 +7841,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
@@ -7895,7 +7870,7 @@
       <c r="R11" s="27"/>
       <c r="S11" s="27"/>
       <c r="T11" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U11" s="27"/>
     </row>
@@ -7905,7 +7880,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
@@ -7934,7 +7909,7 @@
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
       <c r="T12" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U12" s="27"/>
     </row>
@@ -7944,7 +7919,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
@@ -7973,7 +7948,7 @@
       <c r="R13" s="27"/>
       <c r="S13" s="27"/>
       <c r="T13" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U13" s="27"/>
     </row>
@@ -8004,7 +7979,7 @@
         <v>Other males</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
@@ -8023,7 +7998,7 @@
       <c r="R15" s="27"/>
       <c r="S15" s="27"/>
       <c r="T15" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U15" s="27"/>
     </row>
@@ -8033,7 +8008,7 @@
         <v>Other males</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D16" s="22">
         <v>4227500</v>
@@ -8084,7 +8059,7 @@
         <v>6118320.6906761518</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U16" s="27"/>
     </row>
@@ -8094,7 +8069,7 @@
         <v>Other males</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
@@ -8113,7 +8088,7 @@
       <c r="R17" s="27"/>
       <c r="S17" s="27"/>
       <c r="T17" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U17" s="27"/>
     </row>
@@ -8144,7 +8119,7 @@
         <v>Other females</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
@@ -8163,7 +8138,7 @@
       <c r="R19" s="27"/>
       <c r="S19" s="27"/>
       <c r="T19" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U19" s="27"/>
     </row>
@@ -8173,7 +8148,7 @@
         <v>Other females</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D20" s="22">
         <v>4759641.7668505535</v>
@@ -8224,7 +8199,7 @@
         <v>7061706.1901886221</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U20" s="27"/>
     </row>
@@ -8234,7 +8209,7 @@
         <v>Other females</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
@@ -8253,7 +8228,7 @@
       <c r="R21" s="27"/>
       <c r="S21" s="27"/>
       <c r="T21" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U21" s="27"/>
     </row>
@@ -8284,7 +8259,7 @@
         <v>Clients</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -8303,7 +8278,7 @@
       <c r="R23" s="27"/>
       <c r="S23" s="27"/>
       <c r="T23" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U23" s="27"/>
     </row>
@@ -8313,7 +8288,7 @@
         <v>Clients</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D24" s="22">
         <v>522500</v>
@@ -8364,7 +8339,7 @@
         <v>756196.93929705245</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U24" s="27"/>
     </row>
@@ -8374,7 +8349,7 @@
         <v>Clients</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -8393,13 +8368,13 @@
       <c r="R25" s="27"/>
       <c r="S25" s="27"/>
       <c r="T25" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U25" s="27"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -8452,7 +8427,7 @@
         <v>2015</v>
       </c>
       <c r="U30" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -8461,7 +8436,7 @@
         <v>MSM</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -8482,7 +8457,7 @@
       <c r="R31" s="22"/>
       <c r="S31" s="22"/>
       <c r="T31" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U31" s="26"/>
     </row>
@@ -8492,7 +8467,7 @@
         <v>MSM</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -8513,7 +8488,7 @@
       <c r="R32" s="22"/>
       <c r="S32" s="22"/>
       <c r="T32" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U32" s="26"/>
     </row>
@@ -8523,7 +8498,7 @@
         <v>MSM</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
@@ -8544,7 +8519,7 @@
       <c r="R33" s="22"/>
       <c r="S33" s="22"/>
       <c r="T33" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U33" s="26"/>
     </row>
@@ -8558,7 +8533,7 @@
         <v>FSW</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
@@ -8583,7 +8558,7 @@
       <c r="R35" s="22"/>
       <c r="S35" s="22"/>
       <c r="T35" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U35" s="26"/>
     </row>
@@ -8593,7 +8568,7 @@
         <v>FSW</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -8618,7 +8593,7 @@
       <c r="R36" s="22"/>
       <c r="S36" s="22"/>
       <c r="T36" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U36" s="26"/>
     </row>
@@ -8628,7 +8603,7 @@
         <v>FSW</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
@@ -8653,7 +8628,7 @@
       <c r="R37" s="22"/>
       <c r="S37" s="22"/>
       <c r="T37" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U37" s="26"/>
     </row>
@@ -8667,7 +8642,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
@@ -8692,7 +8667,7 @@
       <c r="R39" s="22"/>
       <c r="S39" s="22"/>
       <c r="T39" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U39" s="26"/>
     </row>
@@ -8702,7 +8677,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
@@ -8727,7 +8702,7 @@
       <c r="R40" s="22"/>
       <c r="S40" s="22"/>
       <c r="T40" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U40" s="26"/>
     </row>
@@ -8737,7 +8712,7 @@
         <v>Male PWID</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
@@ -8762,7 +8737,7 @@
       <c r="R41" s="22"/>
       <c r="S41" s="22"/>
       <c r="T41" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U41" s="26"/>
     </row>
@@ -8776,7 +8751,7 @@
         <v>Other males</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
@@ -8795,7 +8770,7 @@
       <c r="R43" s="22"/>
       <c r="S43" s="22"/>
       <c r="T43" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U43" s="26"/>
     </row>
@@ -8805,7 +8780,7 @@
         <v>Other males</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
@@ -8824,7 +8799,7 @@
       <c r="R44" s="22"/>
       <c r="S44" s="22"/>
       <c r="T44" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U44" s="26">
         <v>5.0000000000000001E-4</v>
@@ -8836,7 +8811,7 @@
         <v>Other males</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
@@ -8855,7 +8830,7 @@
       <c r="R45" s="22"/>
       <c r="S45" s="22"/>
       <c r="T45" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U45" s="26"/>
     </row>
@@ -8869,7 +8844,7 @@
         <v>Other females</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
@@ -8888,7 +8863,7 @@
       <c r="R47" s="22"/>
       <c r="S47" s="22"/>
       <c r="T47" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U47" s="26"/>
     </row>
@@ -8898,7 +8873,7 @@
         <v>Other females</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
@@ -8925,7 +8900,7 @@
       <c r="R48" s="22"/>
       <c r="S48" s="22"/>
       <c r="T48" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U48" s="26"/>
     </row>
@@ -8935,7 +8910,7 @@
         <v>Other females</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
@@ -8954,7 +8929,7 @@
       <c r="R49" s="22"/>
       <c r="S49" s="22"/>
       <c r="T49" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U49" s="26"/>
     </row>
@@ -8968,7 +8943,7 @@
         <v>Clients</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
@@ -8987,7 +8962,7 @@
       <c r="R51" s="22"/>
       <c r="S51" s="22"/>
       <c r="T51" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U51" s="26"/>
     </row>
@@ -8997,7 +8972,7 @@
         <v>Clients</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
@@ -9016,7 +8991,7 @@
       <c r="R52" s="22"/>
       <c r="S52" s="22"/>
       <c r="T52" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U52" s="26">
         <v>0.01</v>
@@ -9028,7 +9003,7 @@
         <v>Clients</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
@@ -9047,7 +9022,7 @@
       <c r="R53" s="22"/>
       <c r="S53" s="22"/>
       <c r="T53" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U53" s="26"/>
     </row>
@@ -9077,7 +9052,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -9150,13 +9125,13 @@
       </c>
       <c r="S2" s="9"/>
       <c r="T2" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -9175,7 +9150,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T3" s="22"/>
     </row>
@@ -9187,7 +9162,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -9260,13 +9235,13 @@
       </c>
       <c r="S8" s="9"/>
       <c r="T8" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -9309,7 +9284,7 @@
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
       <c r="S9" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T9" s="22"/>
     </row>
@@ -9321,7 +9296,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -9394,13 +9369,13 @@
       </c>
       <c r="S14" s="9"/>
       <c r="T14" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -9419,7 +9394,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T15" s="22"/>
     </row>
@@ -9431,7 +9406,7 @@
     </row>
     <row r="19" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="6"/>
     </row>
@@ -9486,12 +9461,12 @@
         <v>2015</v>
       </c>
       <c r="T20" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -9510,7 +9485,7 @@
       <c r="Q21" s="22"/>
       <c r="R21" s="22"/>
       <c r="S21" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T21" s="22"/>
     </row>
@@ -9525,7 +9500,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -9598,13 +9573,13 @@
       </c>
       <c r="S26" s="9"/>
       <c r="T26" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
@@ -9623,13 +9598,13 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T27" s="22"/>
     </row>
     <row r="31" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" s="6"/>
     </row>
@@ -9684,12 +9659,12 @@
         <v>2015</v>
       </c>
       <c r="T32" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="2:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
@@ -9708,7 +9683,7 @@
       <c r="Q33" s="22"/>
       <c r="R33" s="22"/>
       <c r="S33" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T33" s="22"/>
     </row>
@@ -9728,9 +9703,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9739,7 +9712,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="6"/>
     </row>
@@ -9794,7 +9767,7 @@
         <v>2015</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -9819,7 +9792,7 @@
       <c r="Q3" s="25"/>
       <c r="R3" s="25"/>
       <c r="S3" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T3" s="25">
         <v>0.01</v>
@@ -9847,7 +9820,7 @@
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T4" s="25">
         <v>0.01</v>
@@ -9875,7 +9848,7 @@
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T5" s="25">
         <v>0.03</v>
@@ -9903,7 +9876,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T6" s="25">
         <v>0.01</v>
@@ -9931,7 +9904,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T7" s="25">
         <v>0.01</v>
@@ -9959,7 +9932,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T8" s="25">
         <v>0.01</v>
@@ -9976,7 +9949,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -10049,7 +10022,7 @@
       </c>
       <c r="S13" s="7"/>
       <c r="T13" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -10075,7 +10048,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="5" t="